<commit_message>
Jimmy removed the minimum build constraint on everything except nuclear and added comments about it in windsun.mod.
</commit_message>
<xml_diff>
--- a/DatabasePrep/GeneratorInfo/generator_costs.xlsx
+++ b/DatabasePrep/GeneratorInfo/generator_costs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="15880" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="15880" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Chart_revise" sheetId="4" r:id="rId1"/>
@@ -24,6 +24,268 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="103">
   <si>
+    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, EIA says minimum learning by 2025 is 20%, so this is a 1.1% declination rate, capital cost multipulier from EIA,http://graysharboroceanenergy.com/Documents/LIPA%20Offshore%20Wind%20rept.pdf for total outage rate of 3%, distributed by guess</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cost Declination Rate (%/yr)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resultant Capital Costs ($2007/MW) in Investment Period Years</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to gas combustion turbine</t>
+  </si>
+  <si>
+    <t>Geothermal_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCGT_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_4_cost_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_5_cost_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_6_cost_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, outage rates from Mathias</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>technology</t>
+  </si>
+  <si>
+    <t>overnight_cost_change</t>
+  </si>
+  <si>
+    <t>intermittent</t>
+  </si>
+  <si>
+    <t>resource_limited</t>
+  </si>
+  <si>
+    <t>baseload</t>
+  </si>
+  <si>
+    <t>min_build_capacity</t>
+  </si>
+  <si>
+    <t>startup_fuel_mbtu</t>
+  </si>
+  <si>
+    <t>nonfuel_startup_cost</t>
+  </si>
+  <si>
+    <t>$year_of_costs</t>
+  </si>
+  <si>
+    <t>cost_for_which_year?</t>
+  </si>
+  <si>
+    <t>ReEDs Sheet, nukes run for 40 years at least, so the 30 year ReEDs lifetime was changed to 40, also the cost declination rate was set to 0.55% as nukes don't really obey the laws of mass production because they aren't mass produced</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCGT</t>
+  </si>
+  <si>
+    <t>ReEDs Sheet</t>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Distributed_PV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Central_PV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>construction_cost_multipulier</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed_o_m</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var_o_m</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>overnight_cost_$2007</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed_o_m_$2007</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var_o_m_$2007</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>construction_time_years</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>forced_outage_rate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>scheduled_outage_rate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>connect_cost_generic_$2007_per_mw</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fuel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>price_and_dollar_year</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_ramp_rate_mw_per_hour</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Uranium</t>
+  </si>
+  <si>
+    <t>DOE Solar Program Costs, took 2020 value for fixed O+M, 10% added to capital costs to go from utility to distributed, but also assumed a 5% declination rate, , outage rates from Mathias</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>overnight_cost</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Solar</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Solid</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Uranium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>interest_between_price_year_and_cost_year</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Residential_PV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Geothermal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compressed_Air_Energy_Storage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>source - all dispatch data from TEPPC_Generator_Categories</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>technology_id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_age_years</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Solar</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Gas</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, assumed to run for 40 years, not 60</t>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine</t>
+  </si>
+  <si>
+    <t>Nuclear</t>
+  </si>
+  <si>
+    <t>Geothermal</t>
+  </si>
+  <si>
+    <t>tech_name_again</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Solar Vision Study (see PV_Cost_Calc.xlsx) for costs, ReEDs sheet for construction cost multiplier and cost fractions, Matthias for forced outage rate </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>Compressed_Air_Energy_storage</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -141,275 +403,17 @@
   <si>
     <t>min_downtime_hours</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, nukes run for 40 years at least, so the 30 year ReEDs lifetime was changed to 40, also the cost declination rate was set to 0.55% as nukes don't really obey the laws of mass production because they aren't mass produced</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCGT</t>
-  </si>
-  <si>
-    <t>ReEDs Sheet</t>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine</t>
-  </si>
-  <si>
-    <t>Wind</t>
-  </si>
-  <si>
-    <t>Distributed_PV</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Central_PV</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>construction_cost_multipulier</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed_o_m</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var_o_m</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>overnight_cost_$2007</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed_o_m_$2007</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var_o_m_$2007</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>construction_time_years</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>forced_outage_rate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>scheduled_outage_rate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>connect_cost_generic_$2007_per_mw</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>fuel</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wind</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>price_and_dollar_year</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_ramp_rate_mw_per_hour</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas</t>
-  </si>
-  <si>
-    <t>Coal</t>
-  </si>
-  <si>
-    <t>Uranium</t>
-  </si>
-  <si>
-    <t>DOE Solar Program Costs, took 2020 value for fixed O+M, 10% added to capital costs to go from utility to distributed, but also assumed a 5% declination rate, , outage rates from Mathias</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>overnight_cost</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Solar</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bio_Solid</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Uranium</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>interest_between_price_year_and_cost_year</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Residential_PV</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Geothermal</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Compressed_Air_Energy_Storage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>source - all dispatch data from TEPPC_Generator_Categories</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>technology_id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_age_years</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Solar</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bio_Gas</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, assumed to run for 40 years, not 60</t>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine</t>
-  </si>
-  <si>
-    <t>Nuclear</t>
-  </si>
-  <si>
-    <t>Geothermal</t>
-  </si>
-  <si>
-    <t>tech_name_again</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Solar Vision Study (see PV_Cost_Calc.xlsx) for costs, ReEDs sheet for construction cost multiplier and cost fractions, Matthias for forced outage rate </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, EIA says minimum learning by 2025 is 20%, so this is a 1.1% declination rate, capital cost multipulier from EIA,http://graysharboroceanenergy.com/Documents/LIPA%20Offshore%20Wind%20rept.pdf for total outage rate of 3%, distributed by guess</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cost Declination Rate (%/yr)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resultant Capital Costs ($2007/MW) in Investment Period Years</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to gas combustion turbine</t>
-  </si>
-  <si>
-    <t>Geothermal_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCGT_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wind_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wind</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_4_cost_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_5_cost_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_6_cost_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, outage rates from Mathias</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>technology</t>
-  </si>
-  <si>
-    <t>overnight_cost_change</t>
-  </si>
-  <si>
-    <t>intermittent</t>
-  </si>
-  <si>
-    <t>resource_limited</t>
-  </si>
-  <si>
-    <t>baseload</t>
-  </si>
-  <si>
-    <t>min_build_capacity</t>
-  </si>
-  <si>
-    <t>startup_fuel_mbtu</t>
-  </si>
-  <si>
-    <t>nonfuel_startup_cost</t>
-  </si>
-  <si>
-    <t>$year_of_costs</t>
-  </si>
-  <si>
-    <t>cost_for_which_year?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3">
@@ -1325,7 +1329,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>#REF!</c:v>
+                  <c:v>Gas_Combustion_Turbine_EP</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1401,11 +1405,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="547111704"/>
-        <c:axId val="547120808"/>
+        <c:axId val="495116376"/>
+        <c:axId val="495125400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="547111704"/>
+        <c:axId val="495116376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1439,14 +1443,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="547120808"/>
+        <c:crossAx val="495125400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="547120808"/>
+        <c:axId val="495125400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="7.0"/>
@@ -1482,7 +1486,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="547111704"/>
+        <c:crossAx val="495116376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1866,11 +1870,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:AP57"/>
+  <dimension ref="A1:AP56"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="X1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A57" sqref="A57:XFD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1901,130 +1905,130 @@
   <sheetData>
     <row r="1" spans="1:42">
       <c r="A1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN1" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO1" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P1" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>48</v>
-      </c>
-      <c r="R1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN1" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="AO1" s="12" t="s">
-        <v>77</v>
-      </c>
       <c r="AP1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:42">
@@ -2032,7 +2036,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C2" s="5">
         <v>2007</v>
@@ -2041,7 +2045,7 @@
         <v>2010</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F2">
         <v>2004</v>
@@ -2156,7 +2160,7 @@
         <v>CCGT</v>
       </c>
       <c r="AP2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:42">
@@ -2164,7 +2168,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C3" s="5">
         <v>2007</v>
@@ -2173,7 +2177,7 @@
         <v>2010</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F3">
         <v>2004</v>
@@ -2288,7 +2292,7 @@
         <v>Gas_Combustion_Turbine</v>
       </c>
       <c r="AP3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:42">
@@ -2296,7 +2300,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C4" s="5">
         <v>2007</v>
@@ -2305,7 +2309,7 @@
         <v>2010</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F4">
         <v>2004</v>
@@ -2420,7 +2424,7 @@
         <v>Wind</v>
       </c>
       <c r="AP4" t="s">
-        <v>92</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:42">
@@ -2428,7 +2432,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="C5" s="5">
         <v>2007</v>
@@ -2437,7 +2441,7 @@
         <v>2010</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F5">
         <v>2004</v>
@@ -2552,7 +2556,7 @@
         <v>Offshore_Wind</v>
       </c>
       <c r="AP5" t="s">
-        <v>79</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:42">
@@ -2560,7 +2564,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C6" s="5">
         <v>2007</v>
@@ -2569,7 +2573,7 @@
         <v>2010</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F6">
         <v>2009</v>
@@ -2685,7 +2689,7 @@
         <v>Residential_PV</v>
       </c>
       <c r="AP6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:42" s="11" customFormat="1">
@@ -2693,7 +2697,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>25</v>
+        <v>96</v>
       </c>
       <c r="C7" s="11">
         <v>2007</v>
@@ -2702,7 +2706,7 @@
         <v>2012</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F7" s="11">
         <v>2010</v>
@@ -2813,10 +2817,10 @@
         <v>0</v>
       </c>
       <c r="AO7" s="11" t="s">
-        <v>25</v>
+        <v>96</v>
       </c>
       <c r="AP7" s="11" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:42">
@@ -2824,7 +2828,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="C8" s="5">
         <v>2007</v>
@@ -2833,7 +2837,7 @@
         <v>2010</v>
       </c>
       <c r="E8" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="F8">
         <v>2007</v>
@@ -2948,7 +2952,7 @@
         <v>Bio_Gas</v>
       </c>
       <c r="AP8" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:42">
@@ -2956,7 +2960,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="C9" s="5">
         <v>2007</v>
@@ -2965,7 +2969,7 @@
         <v>2010</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F9">
         <v>2004</v>
@@ -3080,7 +3084,7 @@
         <v>Biomass_Steam_Turbine</v>
       </c>
       <c r="AP9" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:42">
@@ -3088,7 +3092,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="C10" s="5">
         <v>2007</v>
@@ -3097,7 +3101,7 @@
         <v>2012</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F10">
         <v>2007</v>
@@ -3212,7 +3216,7 @@
         <v>Biomass_IGCC</v>
       </c>
       <c r="AP10" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:42">
@@ -3220,7 +3224,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="C11" s="5">
         <v>2007</v>
@@ -3229,7 +3233,7 @@
         <v>2010</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F11">
         <v>2004</v>
@@ -3344,7 +3348,7 @@
         <v>Coal_IGCC</v>
       </c>
       <c r="AP11" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:42">
@@ -3352,7 +3356,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C12" s="5">
         <v>2007</v>
@@ -3361,7 +3365,7 @@
         <v>2010</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F12">
         <v>2004</v>
@@ -3476,7 +3480,7 @@
         <v>Coal_Steam_Turbine</v>
       </c>
       <c r="AP12" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:42">
@@ -3484,7 +3488,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C13" s="5">
         <v>2007</v>
@@ -3493,7 +3497,7 @@
         <v>2010</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F13">
         <v>2004</v>
@@ -3608,7 +3612,7 @@
         <v>Nuclear</v>
       </c>
       <c r="AP13" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:42">
@@ -3616,7 +3620,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C14" s="5">
         <v>2007</v>
@@ -3625,7 +3629,7 @@
         <v>2010</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F14">
         <v>2004</v>
@@ -3740,7 +3744,7 @@
         <v>Geothermal</v>
       </c>
       <c r="AP14" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:42">
@@ -3748,7 +3752,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="C15" s="5">
         <v>2007</v>
@@ -3757,7 +3761,7 @@
         <v>2010</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="F15" s="5">
         <v>2004</v>
@@ -3872,7 +3876,7 @@
         <v>Hydro_NonPumped</v>
       </c>
       <c r="AP15" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:42">
@@ -3880,7 +3884,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="C16" s="5">
         <v>2007</v>
@@ -3889,7 +3893,7 @@
         <v>2010</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="F16" s="5">
         <v>2004</v>
@@ -4004,31 +4008,37 @@
         <v>Hydro_Pumped</v>
       </c>
       <c r="AP16" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:42" s="19" customFormat="1">
-      <c r="A17" s="19">
+    <row r="17" spans="1:42" s="18" customFormat="1">
+      <c r="A17" s="18">
         <v>17</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>87</v>
+      <c r="B17" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="AM17" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN17" s="18">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:42" s="5" customFormat="1">
       <c r="A18">
         <v>18</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>12</v>
+      <c r="B18" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G18" s="11"/>
       <c r="M18" s="11"/>
@@ -4045,13 +4055,13 @@
       <c r="A19">
         <v>19</v>
       </c>
-      <c r="B19" s="18" t="s">
-        <v>13</v>
+      <c r="B19" s="17" t="s">
+        <v>84</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G19" s="11"/>
       <c r="M19" s="11"/>
@@ -4068,13 +4078,13 @@
       <c r="A20">
         <v>20</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>84</v>
+      <c r="B20" s="18" t="s">
+        <v>5</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G20" s="11"/>
       <c r="M20" s="11"/>
@@ -4092,12 +4102,12 @@
         <v>21</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
       <c r="C21" s="21"/>
       <c r="D21"/>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G21" s="11"/>
       <c r="M21" s="11"/>
@@ -4114,13 +4124,13 @@
       <c r="A22">
         <v>22</v>
       </c>
-      <c r="B22" s="18" t="s">
-        <v>14</v>
+      <c r="B22" s="17" t="s">
+        <v>85</v>
       </c>
       <c r="C22"/>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="G22" s="11"/>
       <c r="M22" s="11"/>
@@ -4133,15 +4143,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:42" s="19" customFormat="1">
-      <c r="A23" s="19">
+    <row r="23" spans="1:42" s="18" customFormat="1">
+      <c r="A23" s="18">
         <v>23</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>88</v>
+      <c r="B23" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="AM23" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN23" s="18">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:42" s="8" customFormat="1">
@@ -4149,7 +4165,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="C24" s="8">
         <v>2007</v>
@@ -4158,7 +4174,7 @@
         <v>2010</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F24" s="8">
         <v>2009</v>
@@ -4269,10 +4285,10 @@
         <v>0</v>
       </c>
       <c r="AO24" s="9" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="AP24" s="9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:42" s="8" customFormat="1">
@@ -4280,7 +4296,7 @@
         <v>26</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C25" s="8">
         <v>2007</v>
@@ -4289,7 +4305,7 @@
         <v>2010</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F25" s="8">
         <v>2009</v>
@@ -4400,10 +4416,10 @@
         <v>0</v>
       </c>
       <c r="AO25" s="9" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="AP25" s="9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:42" s="5" customFormat="1">
@@ -4411,7 +4427,7 @@
         <v>27</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="C26" s="5">
         <v>2007</v>
@@ -4420,7 +4436,7 @@
         <v>2010</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F26" s="5">
         <v>2010</v>
@@ -4531,10 +4547,10 @@
         <v>0</v>
       </c>
       <c r="AO26" s="9" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="AP26" s="9" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:42" s="9" customFormat="1">
@@ -4542,7 +4558,7 @@
         <v>28</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C27" s="9">
         <v>2007</v>
@@ -4551,7 +4567,7 @@
         <v>2010</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F27" s="9">
         <v>2010</v>
@@ -4662,10 +4678,10 @@
         <v>1</v>
       </c>
       <c r="AO27" s="14" t="s">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="AP27" s="14" t="s">
-        <v>1</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:42" s="5" customFormat="1">
@@ -4675,12 +4691,12 @@
     </row>
     <row r="29" spans="1:42" s="6" customFormat="1">
       <c r="A29" s="6" t="s">
-        <v>81</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:42">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="B30">
         <v>2010</v>
@@ -4697,8 +4713,8 @@
       <c r="F30">
         <v>2026</v>
       </c>
-      <c r="H30" t="s">
-        <v>80</v>
+      <c r="G30" t="s">
+        <v>1</v>
       </c>
       <c r="S30" s="5"/>
       <c r="Y30"/>
@@ -4728,9 +4744,8 @@
         <f t="shared" si="10"/>
         <v>0.84732302571340368</v>
       </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="2">
-        <f t="shared" ref="H31:H45" si="11">-P2*100</f>
+      <c r="G31" s="2">
+        <f>-P2*100</f>
         <v>1.35</v>
       </c>
       <c r="S31" s="5"/>
@@ -4761,9 +4776,8 @@
         <f t="shared" si="10"/>
         <v>0.5373949539554197</v>
       </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="2">
-        <f t="shared" si="11"/>
+      <c r="G32" s="2">
+        <f t="shared" ref="G32:G56" si="11">-P3*100</f>
         <v>1.44</v>
       </c>
       <c r="S32" s="5"/>
@@ -4794,8 +4808,7 @@
         <f t="shared" si="10"/>
         <v>1.6980921160796985</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="2">
+      <c r="G33" s="2">
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
@@ -4827,8 +4840,7 @@
         <f t="shared" si="10"/>
         <v>2.8495848614886108</v>
       </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="2">
+      <c r="G34" s="2">
         <f t="shared" si="11"/>
         <v>1.3</v>
       </c>
@@ -4860,8 +4872,7 @@
         <f t="shared" si="10"/>
         <v>2.1545565356234837</v>
       </c>
-      <c r="G35" s="1"/>
-      <c r="H35" s="2">
+      <c r="G35" s="2">
         <f t="shared" si="11"/>
         <v>4.3999999999999995</v>
       </c>
@@ -4893,8 +4904,7 @@
         <f t="shared" si="10"/>
         <v>3.2883466482033623</v>
       </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="2">
+      <c r="G36" s="2">
         <f t="shared" si="11"/>
         <v>4.5</v>
       </c>
@@ -4926,8 +4936,7 @@
         <f t="shared" si="10"/>
         <v>1.9585533298471325</v>
       </c>
-      <c r="G37" s="1"/>
-      <c r="H37" s="2">
+      <c r="G37" s="2">
         <f t="shared" si="11"/>
         <v>1.44</v>
       </c>
@@ -4959,8 +4968,7 @@
         <f t="shared" si="10"/>
         <v>2.8940804939190024</v>
       </c>
-      <c r="G38" s="1"/>
-      <c r="H38" s="2">
+      <c r="G38" s="2">
         <f t="shared" si="11"/>
         <v>0.54999999999999993</v>
       </c>
@@ -4992,8 +5000,7 @@
         <f t="shared" si="10"/>
         <v>2.858765685081833</v>
       </c>
-      <c r="G39" s="1"/>
-      <c r="H39" s="2">
+      <c r="G39" s="2">
         <f t="shared" si="11"/>
         <v>1.48</v>
       </c>
@@ -5025,8 +5032,7 @@
         <f t="shared" si="10"/>
         <v>2.1906568125359844</v>
       </c>
-      <c r="G40" s="1"/>
-      <c r="H40" s="2">
+      <c r="G40" s="2">
         <f t="shared" si="11"/>
         <v>1.48</v>
       </c>
@@ -5058,8 +5064,7 @@
         <f t="shared" si="10"/>
         <v>1.8686997855157279</v>
       </c>
-      <c r="G41" s="1"/>
-      <c r="H41" s="2">
+      <c r="G41" s="2">
         <f t="shared" si="11"/>
         <v>1.1900000000000002</v>
       </c>
@@ -5091,8 +5096,7 @@
         <f t="shared" si="10"/>
         <v>3.1349761419194406</v>
       </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="2">
+      <c r="G42" s="2">
         <f t="shared" si="11"/>
         <v>1.48</v>
       </c>
@@ -5124,8 +5128,7 @@
         <f t="shared" si="10"/>
         <v>3.1247016636575049</v>
       </c>
-      <c r="G43" s="1"/>
-      <c r="H43" s="2">
+      <c r="G43" s="2">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
@@ -5157,8 +5160,7 @@
         <f t="shared" si="10"/>
         <v>2.3773825018890866</v>
       </c>
-      <c r="G44" s="1"/>
-      <c r="H44" s="2">
+      <c r="G44" s="2">
         <f t="shared" si="11"/>
         <v>0.77</v>
       </c>
@@ -5190,8 +5192,7 @@
         <f t="shared" si="10"/>
         <v>3.6707659988132098</v>
       </c>
-      <c r="G45" s="1"/>
-      <c r="H45" s="2">
+      <c r="G45" s="2">
         <f t="shared" si="11"/>
         <v>1.44</v>
       </c>
@@ -5199,370 +5200,333 @@
       <c r="Y45"/>
     </row>
     <row r="46" spans="1:25">
-      <c r="A46" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B46" s="1" t="e">
-        <f>#REF!*(1+#REF!)^(B$30-2007)/1000000</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C46" s="1" t="e">
-        <f>#REF!*(1+#REF!)^(C$30-2007)/1000000</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D46" s="1" t="e">
-        <f>#REF!*(1+#REF!)^(D$30-2007)/1000000</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E46" s="1" t="e">
-        <f>#REF!*(1+#REF!)^(E$30-2007)/1000000</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F46" s="1" t="e">
-        <f>#REF!*(1+#REF!)^(F$30-2007)/1000000</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G46" s="1"/>
-      <c r="H46" s="2" t="e">
-        <f>-#REF!*100</f>
-        <v>#REF!</v>
+      <c r="A46" s="20" t="str">
+        <f t="shared" ref="A46:A56" si="12">B17</f>
+        <v>Gas_Combustion_Turbine_EP</v>
+      </c>
+      <c r="B46" s="1">
+        <f t="shared" ref="B46:F46" si="13">$M17*(1+$P17)^(B$30-2007)/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="C46" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="D46" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="E46" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G46" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:25">
-      <c r="A47" s="8" t="str">
-        <f>B18</f>
+      <c r="A47" s="20" t="str">
+        <f t="shared" si="12"/>
         <v>Coal_Steam_Turbine_EP</v>
       </c>
       <c r="B47" s="1">
-        <f t="shared" ref="B47:F51" si="12">$M18*(1+$P18)^(B$30-2007)/1000000</f>
+        <f t="shared" ref="B47:F47" si="14">$M18*(1+$P18)^(B$30-2007)/1000000</f>
         <v>0</v>
       </c>
       <c r="C47" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D47" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="E47" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="F47" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="G47" s="1"/>
-      <c r="H47" s="2">
-        <f>-P18*100</f>
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G47" s="2">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:25">
-      <c r="A48" s="8" t="str">
-        <f>B19</f>
+      <c r="A48" s="20" t="str">
+        <f t="shared" si="12"/>
         <v>Gas_Steam_Turbine_EP</v>
       </c>
       <c r="B48" s="1">
+        <f t="shared" ref="B48:F48" si="15">$M19*(1+$P19)^(B$30-2007)/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="C48" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="D48" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="G48" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="20" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="C48" s="1">
+        <v>CCGT_EP</v>
+      </c>
+      <c r="B49" s="1">
+        <f t="shared" ref="B49:F49" si="16">$M20*(1+$P20)^(B$30-2007)/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="C49" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="D49" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="E49" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="G49" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="20" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="D48" s="1">
+        <v>Geothermal_EP</v>
+      </c>
+      <c r="B50" s="1">
+        <f t="shared" ref="B50:F50" si="17">$M21*(1+$P21)^(B$30-2007)/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="C50" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="D50" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="E50" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="G50" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="20" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="E48" s="1">
+        <v>Nuclear_EP</v>
+      </c>
+      <c r="B51" s="1">
+        <f t="shared" ref="B51:F51" si="18">$M22*(1+$P22)^(B$30-2007)/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="C51" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="D51" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="E51" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G51" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="20" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="F48" s="1">
+        <v>Wind_EP</v>
+      </c>
+      <c r="B52" s="1">
+        <f t="shared" ref="B52:F52" si="19">$M23*(1+$P23)^(B$30-2007)/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="C52" s="1">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="D52" s="1">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="G52" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="20" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="G48" s="1"/>
-      <c r="H48" s="2">
-        <f>-P19*100</f>
-        <v>0</v>
+        <v>Commercial_PV</v>
+      </c>
+      <c r="B53" s="1">
+        <f t="shared" ref="B53:F53" si="20">$M24*(1+$P24)^(B$30-2007)/1000000</f>
+        <v>4.1718955072971022</v>
+      </c>
+      <c r="C53" s="1">
+        <f t="shared" si="20"/>
+        <v>3.4846967579028645</v>
+      </c>
+      <c r="D53" s="1">
+        <f t="shared" si="20"/>
+        <v>2.9106940653952389</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="20"/>
+        <v>2.4312416634570249</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="20"/>
+        <v>2.0307651348190192</v>
+      </c>
+      <c r="G53" s="2">
+        <f t="shared" si="11"/>
+        <v>4.3999999999999995</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="8" t="str">
-        <f>B20</f>
-        <v>CCGT_EP</v>
-      </c>
-      <c r="B49" s="1">
+    <row r="54" spans="1:7">
+      <c r="A54" s="20" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="C49" s="1">
+        <v>Central_PV</v>
+      </c>
+      <c r="B54" s="1">
+        <f t="shared" ref="B54:F54" si="21">$M25*(1+$P25)^(B$30-2007)/1000000</f>
+        <v>3.9491243879754125</v>
+      </c>
+      <c r="C54" s="1">
+        <f t="shared" si="21"/>
+        <v>3.298620717432323</v>
+      </c>
+      <c r="D54" s="1">
+        <f t="shared" si="21"/>
+        <v>2.7552686541362692</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="21"/>
+        <v>2.3014180794860186</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="21"/>
+        <v>1.9223262198529554</v>
+      </c>
+      <c r="G54" s="2">
+        <f t="shared" si="11"/>
+        <v>4.3999999999999995</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="20" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="D49" s="1">
+        <v>CSP_Trough_No_Storage</v>
+      </c>
+      <c r="B55" s="1">
+        <f t="shared" ref="B55:F55" si="22">$M26*(1+$P26)^(B$30-2007)/1000000</f>
+        <v>4.2780161826030145</v>
+      </c>
+      <c r="C55" s="1">
+        <f t="shared" si="22"/>
+        <v>3.8659914201161327</v>
+      </c>
+      <c r="D55" s="1">
+        <f t="shared" si="22"/>
+        <v>3.4936496316190953</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="22"/>
+        <v>3.1571688661806681</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="22"/>
+        <v>2.8530952730257311</v>
+      </c>
+      <c r="G55" s="2">
+        <f t="shared" si="11"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="20" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="E49" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="F49" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="G49" s="1"/>
-      <c r="H49" s="2">
-        <f>-P20*100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="8" t="str">
-        <f>B21</f>
-        <v>Geothermal_EP</v>
-      </c>
-      <c r="B50" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="C50" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="D50" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="E50" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="F50" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="G50" s="1"/>
-      <c r="H50" s="2">
-        <f>-P21*100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="8" t="str">
-        <f>B22</f>
-        <v>Nuclear_EP</v>
-      </c>
-      <c r="B51" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="C51" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="D51" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="E51" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="F51" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="G51" s="1"/>
-      <c r="H51" s="2">
-        <f>-P22*100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B52" s="1" t="e">
-        <f>#REF!*(1+#REF!)^(B$30-2007)/1000000</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C52" s="1" t="e">
-        <f>#REF!*(1+#REF!)^(C$30-2007)/1000000</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D52" s="1" t="e">
-        <f>#REF!*(1+#REF!)^(D$30-2007)/1000000</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E52" s="1" t="e">
-        <f>#REF!*(1+#REF!)^(E$30-2007)/1000000</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F52" s="1" t="e">
-        <f>#REF!*(1+#REF!)^(F$30-2007)/1000000</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G52" s="1"/>
-      <c r="H52" s="2" t="e">
-        <f>-#REF!*100</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B53" s="1" t="e">
-        <f>#REF!*(1+#REF!)^(B$30-2007)/1000000</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C53" s="1" t="e">
-        <f>#REF!*(1+#REF!)^(C$30-2007)/1000000</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D53" s="1" t="e">
-        <f>#REF!*(1+#REF!)^(D$30-2007)/1000000</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E53" s="1" t="e">
-        <f>#REF!*(1+#REF!)^(E$30-2007)/1000000</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F53" s="1" t="e">
-        <f>#REF!*(1+#REF!)^(F$30-2007)/1000000</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G53" s="1"/>
-      <c r="H53" s="2" t="e">
-        <f>-#REF!*100</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="8" t="str">
-        <f>B24</f>
-        <v>Commercial_PV</v>
-      </c>
-      <c r="B54" s="1">
-        <f t="shared" ref="B54:F57" si="13">$M24*(1+$P24)^(B$30-2007)/1000000</f>
-        <v>4.1718955072971022</v>
-      </c>
-      <c r="C54" s="1">
-        <f t="shared" si="13"/>
-        <v>3.4846967579028645</v>
-      </c>
-      <c r="D54" s="1">
-        <f t="shared" si="13"/>
-        <v>2.9106940653952389</v>
-      </c>
-      <c r="E54" s="1">
-        <f t="shared" si="13"/>
-        <v>2.4312416634570249</v>
-      </c>
-      <c r="F54" s="1">
-        <f t="shared" si="13"/>
-        <v>2.0307651348190192</v>
-      </c>
-      <c r="G54" s="1"/>
-      <c r="H54" s="2">
-        <f t="shared" ref="H54:H55" si="14">-P24*100</f>
-        <v>4.3999999999999995</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="8" t="str">
-        <f>B25</f>
-        <v>Central_PV</v>
-      </c>
-      <c r="B55" s="1">
-        <f t="shared" si="13"/>
-        <v>3.9491243879754125</v>
-      </c>
-      <c r="C55" s="1">
-        <f t="shared" si="13"/>
-        <v>3.298620717432323</v>
-      </c>
-      <c r="D55" s="1">
-        <f t="shared" si="13"/>
-        <v>2.7552686541362692</v>
-      </c>
-      <c r="E55" s="1">
-        <f t="shared" si="13"/>
-        <v>2.3014180794860186</v>
-      </c>
-      <c r="F55" s="1">
-        <f t="shared" si="13"/>
-        <v>1.9223262198529554</v>
-      </c>
-      <c r="G55" s="1"/>
-      <c r="H55" s="2">
-        <f t="shared" si="14"/>
-        <v>4.3999999999999995</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="9" t="str">
-        <f>B26</f>
-        <v>CSP_Trough_No_Storage</v>
+        <v>Compressed_Air_Energy_Storage</v>
       </c>
       <c r="B56" s="1">
-        <f t="shared" si="13"/>
-        <v>4.2780161826030145</v>
+        <f t="shared" ref="B56:F56" si="23">$M27*(1+$P27)^(B$30-2007)/1000000</f>
+        <v>1.3974549825990654</v>
       </c>
       <c r="C56" s="1">
-        <f t="shared" si="13"/>
-        <v>3.8659914201161327</v>
+        <f t="shared" si="23"/>
+        <v>1.3907592630373287</v>
       </c>
       <c r="D56" s="1">
-        <f t="shared" si="13"/>
-        <v>3.4936496316190953</v>
+        <f t="shared" si="23"/>
+        <v>1.384095625124738</v>
       </c>
       <c r="E56" s="1">
-        <f t="shared" si="13"/>
-        <v>3.1571688661806681</v>
+        <f t="shared" si="23"/>
+        <v>1.3774639151463415</v>
       </c>
       <c r="F56" s="1">
-        <f t="shared" si="13"/>
-        <v>2.8530952730257311</v>
-      </c>
-      <c r="G56" s="1"/>
-      <c r="H56" s="2">
-        <f>-P26*100</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="17" t="str">
-        <f>B27</f>
-        <v>Compressed_Air_Energy_Storage</v>
-      </c>
-      <c r="B57" s="1">
-        <f t="shared" si="13"/>
-        <v>1.3974549825990654</v>
-      </c>
-      <c r="C57" s="1">
-        <f t="shared" si="13"/>
-        <v>1.3907592630373287</v>
-      </c>
-      <c r="D57" s="1">
-        <f t="shared" si="13"/>
-        <v>1.384095625124738</v>
-      </c>
-      <c r="E57" s="1">
-        <f t="shared" si="13"/>
-        <v>1.3774639151463415</v>
-      </c>
-      <c r="F57" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="23"/>
         <v>1.3708639801236917</v>
+      </c>
+      <c r="G56" s="2">
+        <f t="shared" si="11"/>
+        <v>0.12</v>
       </c>
     </row>
   </sheetData>
@@ -5584,8 +5548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:AG27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W23" sqref="W23"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -5829,8 +5793,7 @@
         <v>0</v>
       </c>
       <c r="Y2" s="5">
-        <f>'generator_costs_04-08-2010'!AF2</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="Z2" s="5">
         <f>'generator_costs_04-08-2010'!AG2</f>
@@ -7035,8 +6998,7 @@
         <v>1</v>
       </c>
       <c r="Y11" s="11">
-        <f>'generator_costs_04-08-2010'!AF11</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="Z11" s="11">
         <f>'generator_costs_04-08-2010'!AG11</f>
@@ -7169,8 +7131,7 @@
         <v>1</v>
       </c>
       <c r="Y12" s="11">
-        <f>'generator_costs_04-08-2010'!AF12</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Z12" s="11">
         <f>'generator_costs_04-08-2010'!AG12</f>
@@ -7742,1475 +7703,1475 @@
       </c>
     </row>
     <row r="17" spans="1:33">
-      <c r="A17" s="20">
+      <c r="A17" s="19">
         <f>'generator_costs_04-08-2010'!A17</f>
         <v>17</v>
       </c>
-      <c r="B17" s="20" t="str">
+      <c r="B17" s="19" t="str">
         <f>'generator_costs_04-08-2010'!B17</f>
         <v>Gas_Combustion_Turbine_EP</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="19">
         <f>'generator_costs_04-08-2010'!C17</f>
         <v>0</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="19">
         <f>'generator_costs_04-08-2010'!D17</f>
         <v>0</v>
       </c>
-      <c r="E17" s="20" t="str">
+      <c r="E17" s="19" t="str">
         <f>'generator_costs_04-08-2010'!E17</f>
         <v>Gas</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="19">
         <f>'generator_costs_04-08-2010'!M17</f>
         <v>0</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="19">
         <f>'generator_costs_04-08-2010'!N17</f>
         <v>0</v>
       </c>
-      <c r="H17" s="20">
+      <c r="H17" s="19">
         <f>'generator_costs_04-08-2010'!O17</f>
         <v>0</v>
       </c>
-      <c r="I17" s="20">
+      <c r="I17" s="19">
         <f>'generator_costs_04-08-2010'!P17</f>
         <v>0</v>
       </c>
-      <c r="J17" s="20">
+      <c r="J17" s="19">
         <f>'generator_costs_04-08-2010'!Q17</f>
         <v>0</v>
       </c>
-      <c r="K17" s="20">
+      <c r="K17" s="19">
         <f>'generator_costs_04-08-2010'!R17</f>
         <v>0</v>
       </c>
-      <c r="L17" s="20">
+      <c r="L17" s="19">
         <f>'generator_costs_04-08-2010'!S17</f>
         <v>0</v>
       </c>
-      <c r="M17" s="20">
+      <c r="M17" s="19">
         <f>'generator_costs_04-08-2010'!T17</f>
         <v>0</v>
       </c>
-      <c r="N17" s="20">
+      <c r="N17" s="19">
         <f>'generator_costs_04-08-2010'!U17</f>
         <v>0</v>
       </c>
-      <c r="O17" s="20">
+      <c r="O17" s="19">
         <f>'generator_costs_04-08-2010'!V17</f>
         <v>0</v>
       </c>
-      <c r="P17" s="20">
+      <c r="P17" s="19">
         <f>'generator_costs_04-08-2010'!W17</f>
         <v>0</v>
       </c>
-      <c r="Q17" s="20">
+      <c r="Q17" s="19">
         <f>'generator_costs_04-08-2010'!X17</f>
         <v>0</v>
       </c>
-      <c r="R17" s="20">
+      <c r="R17" s="19">
         <f>'generator_costs_04-08-2010'!Y17</f>
         <v>0</v>
       </c>
-      <c r="S17" s="20">
+      <c r="S17" s="19">
         <f>'generator_costs_04-08-2010'!Z17</f>
         <v>0</v>
       </c>
-      <c r="T17" s="20">
+      <c r="T17" s="19">
         <f>'generator_costs_04-08-2010'!AA17</f>
         <v>0</v>
       </c>
-      <c r="U17" s="20">
+      <c r="U17" s="19">
         <f>'generator_costs_04-08-2010'!AB17</f>
         <v>0</v>
       </c>
-      <c r="V17" s="20">
+      <c r="V17" s="19">
         <f>'generator_costs_04-08-2010'!AC17</f>
         <v>0</v>
       </c>
-      <c r="W17" s="20">
+      <c r="W17" s="19">
         <f>'generator_costs_04-08-2010'!AD17</f>
         <v>0</v>
       </c>
-      <c r="X17" s="20">
+      <c r="X17" s="19">
         <f>'generator_costs_04-08-2010'!AE17</f>
         <v>0</v>
       </c>
-      <c r="Y17" s="20">
+      <c r="Y17" s="19">
         <f>'generator_costs_04-08-2010'!AF17</f>
         <v>0</v>
       </c>
-      <c r="Z17" s="20">
+      <c r="Z17" s="19">
         <f>'generator_costs_04-08-2010'!AG17</f>
         <v>0</v>
       </c>
-      <c r="AA17" s="20">
+      <c r="AA17" s="19">
         <f>'generator_costs_04-08-2010'!AH17</f>
         <v>0</v>
       </c>
-      <c r="AB17" s="20">
+      <c r="AB17" s="19">
         <f>'generator_costs_04-08-2010'!AI17</f>
         <v>0</v>
       </c>
-      <c r="AC17" s="20">
+      <c r="AC17" s="19">
         <f>'generator_costs_04-08-2010'!AJ17</f>
         <v>0</v>
       </c>
-      <c r="AD17" s="20">
+      <c r="AD17" s="19">
         <f>'generator_costs_04-08-2010'!AK17</f>
         <v>0</v>
       </c>
-      <c r="AE17" s="20">
+      <c r="AE17" s="19">
         <f>'generator_costs_04-08-2010'!AL17</f>
         <v>0</v>
       </c>
-      <c r="AF17" s="20">
+      <c r="AF17" s="19">
         <f>'generator_costs_04-08-2010'!AM17</f>
         <v>0</v>
       </c>
-      <c r="AG17" s="20">
+      <c r="AG17" s="19">
         <f>'generator_costs_04-08-2010'!AN17</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:33">
-      <c r="A18" s="20">
+      <c r="A18" s="19">
         <f>'generator_costs_04-08-2010'!A18</f>
         <v>18</v>
       </c>
-      <c r="B18" s="20" t="str">
+      <c r="B18" s="19" t="str">
         <f>'generator_costs_04-08-2010'!B18</f>
         <v>Coal_Steam_Turbine_EP</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="19">
         <f>'generator_costs_04-08-2010'!C18</f>
         <v>0</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D18" s="19">
         <f>'generator_costs_04-08-2010'!D18</f>
         <v>0</v>
       </c>
-      <c r="E18" s="20" t="str">
+      <c r="E18" s="19" t="str">
         <f>'generator_costs_04-08-2010'!E18</f>
         <v>Coal</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="19">
         <f>'generator_costs_04-08-2010'!M18</f>
         <v>0</v>
       </c>
-      <c r="G18" s="20">
+      <c r="G18" s="19">
         <f>'generator_costs_04-08-2010'!N18</f>
         <v>0</v>
       </c>
-      <c r="H18" s="20">
+      <c r="H18" s="19">
         <f>'generator_costs_04-08-2010'!O18</f>
         <v>0</v>
       </c>
-      <c r="I18" s="20">
+      <c r="I18" s="19">
         <f>'generator_costs_04-08-2010'!P18</f>
         <v>0</v>
       </c>
-      <c r="J18" s="20">
+      <c r="J18" s="19">
         <f>'generator_costs_04-08-2010'!Q18</f>
         <v>0</v>
       </c>
-      <c r="K18" s="20">
+      <c r="K18" s="19">
         <f>'generator_costs_04-08-2010'!R18</f>
         <v>0</v>
       </c>
-      <c r="L18" s="20">
+      <c r="L18" s="19">
         <f>'generator_costs_04-08-2010'!S18</f>
         <v>0</v>
       </c>
-      <c r="M18" s="20">
+      <c r="M18" s="19">
         <f>'generator_costs_04-08-2010'!T18</f>
         <v>0</v>
       </c>
-      <c r="N18" s="20">
+      <c r="N18" s="19">
         <f>'generator_costs_04-08-2010'!U18</f>
         <v>0</v>
       </c>
-      <c r="O18" s="20">
+      <c r="O18" s="19">
         <f>'generator_costs_04-08-2010'!V18</f>
         <v>0</v>
       </c>
-      <c r="P18" s="20">
+      <c r="P18" s="19">
         <f>'generator_costs_04-08-2010'!W18</f>
         <v>0</v>
       </c>
-      <c r="Q18" s="20">
+      <c r="Q18" s="19">
         <f>'generator_costs_04-08-2010'!X18</f>
         <v>0</v>
       </c>
-      <c r="R18" s="20">
+      <c r="R18" s="19">
         <f>'generator_costs_04-08-2010'!Y18</f>
         <v>0</v>
       </c>
-      <c r="S18" s="20">
+      <c r="S18" s="19">
         <f>'generator_costs_04-08-2010'!Z18</f>
         <v>0</v>
       </c>
-      <c r="T18" s="20">
+      <c r="T18" s="19">
         <f>'generator_costs_04-08-2010'!AA18</f>
         <v>0</v>
       </c>
-      <c r="U18" s="20">
+      <c r="U18" s="19">
         <f>'generator_costs_04-08-2010'!AB18</f>
         <v>0</v>
       </c>
-      <c r="V18" s="20">
+      <c r="V18" s="19">
         <f>'generator_costs_04-08-2010'!AC18</f>
         <v>0</v>
       </c>
-      <c r="W18" s="20">
+      <c r="W18" s="19">
         <f>'generator_costs_04-08-2010'!AD18</f>
         <v>0</v>
       </c>
-      <c r="X18" s="20">
+      <c r="X18" s="19">
         <f>'generator_costs_04-08-2010'!AE18</f>
         <v>0</v>
       </c>
-      <c r="Y18" s="20">
+      <c r="Y18" s="19">
         <f>'generator_costs_04-08-2010'!AF18</f>
         <v>0</v>
       </c>
-      <c r="Z18" s="20">
+      <c r="Z18" s="19">
         <f>'generator_costs_04-08-2010'!AG18</f>
         <v>0</v>
       </c>
-      <c r="AA18" s="20">
+      <c r="AA18" s="19">
         <f>'generator_costs_04-08-2010'!AH18</f>
         <v>0</v>
       </c>
-      <c r="AB18" s="20">
+      <c r="AB18" s="19">
         <f>'generator_costs_04-08-2010'!AI18</f>
         <v>0</v>
       </c>
-      <c r="AC18" s="20">
+      <c r="AC18" s="19">
         <f>'generator_costs_04-08-2010'!AJ18</f>
         <v>0</v>
       </c>
-      <c r="AD18" s="20">
+      <c r="AD18" s="19">
         <f>'generator_costs_04-08-2010'!AK18</f>
         <v>0</v>
       </c>
-      <c r="AE18" s="20">
+      <c r="AE18" s="19">
         <f>'generator_costs_04-08-2010'!AL18</f>
         <v>0</v>
       </c>
-      <c r="AF18" s="20">
+      <c r="AF18" s="19">
         <f>'generator_costs_04-08-2010'!AM18</f>
         <v>0</v>
       </c>
-      <c r="AG18" s="20">
+      <c r="AG18" s="19">
         <f>'generator_costs_04-08-2010'!AN18</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:33">
-      <c r="A19" s="20">
+      <c r="A19" s="19">
         <f>'generator_costs_04-08-2010'!A19</f>
         <v>19</v>
       </c>
-      <c r="B19" s="20" t="str">
+      <c r="B19" s="19" t="str">
         <f>'generator_costs_04-08-2010'!B19</f>
         <v>Gas_Steam_Turbine_EP</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="19">
         <f>'generator_costs_04-08-2010'!C19</f>
         <v>0</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="19">
         <f>'generator_costs_04-08-2010'!D19</f>
         <v>0</v>
       </c>
-      <c r="E19" s="20" t="str">
+      <c r="E19" s="19" t="str">
         <f>'generator_costs_04-08-2010'!E19</f>
         <v>Gas</v>
       </c>
-      <c r="F19" s="20">
+      <c r="F19" s="19">
         <f>'generator_costs_04-08-2010'!M19</f>
         <v>0</v>
       </c>
-      <c r="G19" s="20">
+      <c r="G19" s="19">
         <f>'generator_costs_04-08-2010'!N19</f>
         <v>0</v>
       </c>
-      <c r="H19" s="20">
+      <c r="H19" s="19">
         <f>'generator_costs_04-08-2010'!O19</f>
         <v>0</v>
       </c>
-      <c r="I19" s="20">
+      <c r="I19" s="19">
         <f>'generator_costs_04-08-2010'!P19</f>
         <v>0</v>
       </c>
-      <c r="J19" s="20">
+      <c r="J19" s="19">
         <f>'generator_costs_04-08-2010'!Q19</f>
         <v>0</v>
       </c>
-      <c r="K19" s="20">
+      <c r="K19" s="19">
         <f>'generator_costs_04-08-2010'!R19</f>
         <v>0</v>
       </c>
-      <c r="L19" s="20">
+      <c r="L19" s="19">
         <f>'generator_costs_04-08-2010'!S19</f>
         <v>0</v>
       </c>
-      <c r="M19" s="20">
+      <c r="M19" s="19">
         <f>'generator_costs_04-08-2010'!T19</f>
         <v>0</v>
       </c>
-      <c r="N19" s="20">
+      <c r="N19" s="19">
         <f>'generator_costs_04-08-2010'!U19</f>
         <v>0</v>
       </c>
-      <c r="O19" s="20">
+      <c r="O19" s="19">
         <f>'generator_costs_04-08-2010'!V19</f>
         <v>0</v>
       </c>
-      <c r="P19" s="20">
+      <c r="P19" s="19">
         <f>'generator_costs_04-08-2010'!W19</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="20">
+      <c r="Q19" s="19">
         <f>'generator_costs_04-08-2010'!X19</f>
         <v>0</v>
       </c>
-      <c r="R19" s="20">
+      <c r="R19" s="19">
         <f>'generator_costs_04-08-2010'!Y19</f>
         <v>0</v>
       </c>
-      <c r="S19" s="20">
+      <c r="S19" s="19">
         <f>'generator_costs_04-08-2010'!Z19</f>
         <v>0</v>
       </c>
-      <c r="T19" s="20">
+      <c r="T19" s="19">
         <f>'generator_costs_04-08-2010'!AA19</f>
         <v>0</v>
       </c>
-      <c r="U19" s="20">
+      <c r="U19" s="19">
         <f>'generator_costs_04-08-2010'!AB19</f>
         <v>0</v>
       </c>
-      <c r="V19" s="20">
+      <c r="V19" s="19">
         <f>'generator_costs_04-08-2010'!AC19</f>
         <v>0</v>
       </c>
-      <c r="W19" s="20">
+      <c r="W19" s="19">
         <f>'generator_costs_04-08-2010'!AD19</f>
         <v>0</v>
       </c>
-      <c r="X19" s="20">
+      <c r="X19" s="19">
         <f>'generator_costs_04-08-2010'!AE19</f>
         <v>0</v>
       </c>
-      <c r="Y19" s="20">
+      <c r="Y19" s="19">
         <f>'generator_costs_04-08-2010'!AF19</f>
         <v>0</v>
       </c>
-      <c r="Z19" s="20">
+      <c r="Z19" s="19">
         <f>'generator_costs_04-08-2010'!AG19</f>
         <v>0</v>
       </c>
-      <c r="AA19" s="20">
+      <c r="AA19" s="19">
         <f>'generator_costs_04-08-2010'!AH19</f>
         <v>0</v>
       </c>
-      <c r="AB19" s="20">
+      <c r="AB19" s="19">
         <f>'generator_costs_04-08-2010'!AI19</f>
         <v>0</v>
       </c>
-      <c r="AC19" s="20">
+      <c r="AC19" s="19">
         <f>'generator_costs_04-08-2010'!AJ19</f>
         <v>0</v>
       </c>
-      <c r="AD19" s="20">
+      <c r="AD19" s="19">
         <f>'generator_costs_04-08-2010'!AK19</f>
         <v>0</v>
       </c>
-      <c r="AE19" s="20">
+      <c r="AE19" s="19">
         <f>'generator_costs_04-08-2010'!AL19</f>
         <v>0</v>
       </c>
-      <c r="AF19" s="20">
+      <c r="AF19" s="19">
         <f>'generator_costs_04-08-2010'!AM19</f>
         <v>0</v>
       </c>
-      <c r="AG19" s="20">
+      <c r="AG19" s="19">
         <f>'generator_costs_04-08-2010'!AN19</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:33">
-      <c r="A20" s="20">
+      <c r="A20" s="19">
         <f>'generator_costs_04-08-2010'!A20</f>
         <v>20</v>
       </c>
-      <c r="B20" s="20" t="str">
+      <c r="B20" s="19" t="str">
         <f>'generator_costs_04-08-2010'!B20</f>
         <v>CCGT_EP</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="19">
         <f>'generator_costs_04-08-2010'!C20</f>
         <v>0</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="19">
         <f>'generator_costs_04-08-2010'!D20</f>
         <v>0</v>
       </c>
-      <c r="E20" s="20" t="str">
+      <c r="E20" s="19" t="str">
         <f>'generator_costs_04-08-2010'!E20</f>
         <v>Gas</v>
       </c>
-      <c r="F20" s="20">
+      <c r="F20" s="19">
         <f>'generator_costs_04-08-2010'!M20</f>
         <v>0</v>
       </c>
-      <c r="G20" s="20">
+      <c r="G20" s="19">
         <f>'generator_costs_04-08-2010'!N20</f>
         <v>0</v>
       </c>
-      <c r="H20" s="20">
+      <c r="H20" s="19">
         <f>'generator_costs_04-08-2010'!O20</f>
         <v>0</v>
       </c>
-      <c r="I20" s="20">
+      <c r="I20" s="19">
         <f>'generator_costs_04-08-2010'!P20</f>
         <v>0</v>
       </c>
-      <c r="J20" s="20">
+      <c r="J20" s="19">
         <f>'generator_costs_04-08-2010'!Q20</f>
         <v>0</v>
       </c>
-      <c r="K20" s="20">
+      <c r="K20" s="19">
         <f>'generator_costs_04-08-2010'!R20</f>
         <v>0</v>
       </c>
-      <c r="L20" s="20">
+      <c r="L20" s="19">
         <f>'generator_costs_04-08-2010'!S20</f>
         <v>0</v>
       </c>
-      <c r="M20" s="20">
+      <c r="M20" s="19">
         <f>'generator_costs_04-08-2010'!T20</f>
         <v>0</v>
       </c>
-      <c r="N20" s="20">
+      <c r="N20" s="19">
         <f>'generator_costs_04-08-2010'!U20</f>
         <v>0</v>
       </c>
-      <c r="O20" s="20">
+      <c r="O20" s="19">
         <f>'generator_costs_04-08-2010'!V20</f>
         <v>0</v>
       </c>
-      <c r="P20" s="20">
+      <c r="P20" s="19">
         <f>'generator_costs_04-08-2010'!W20</f>
         <v>0</v>
       </c>
-      <c r="Q20" s="20">
+      <c r="Q20" s="19">
         <f>'generator_costs_04-08-2010'!X20</f>
         <v>0</v>
       </c>
-      <c r="R20" s="20">
+      <c r="R20" s="19">
         <f>'generator_costs_04-08-2010'!Y20</f>
         <v>0</v>
       </c>
-      <c r="S20" s="20">
+      <c r="S20" s="19">
         <f>'generator_costs_04-08-2010'!Z20</f>
         <v>0</v>
       </c>
-      <c r="T20" s="20">
+      <c r="T20" s="19">
         <f>'generator_costs_04-08-2010'!AA20</f>
         <v>0</v>
       </c>
-      <c r="U20" s="20">
+      <c r="U20" s="19">
         <f>'generator_costs_04-08-2010'!AB20</f>
         <v>0</v>
       </c>
-      <c r="V20" s="20">
+      <c r="V20" s="19">
         <f>'generator_costs_04-08-2010'!AC20</f>
         <v>0</v>
       </c>
-      <c r="W20" s="20">
+      <c r="W20" s="19">
         <f>'generator_costs_04-08-2010'!AD20</f>
         <v>0</v>
       </c>
-      <c r="X20" s="20">
+      <c r="X20" s="19">
         <f>'generator_costs_04-08-2010'!AE20</f>
         <v>0</v>
       </c>
-      <c r="Y20" s="20">
+      <c r="Y20" s="19">
         <f>'generator_costs_04-08-2010'!AF20</f>
         <v>0</v>
       </c>
-      <c r="Z20" s="20">
+      <c r="Z20" s="19">
         <f>'generator_costs_04-08-2010'!AG20</f>
         <v>0</v>
       </c>
-      <c r="AA20" s="20">
+      <c r="AA20" s="19">
         <f>'generator_costs_04-08-2010'!AH20</f>
         <v>0</v>
       </c>
-      <c r="AB20" s="20">
+      <c r="AB20" s="19">
         <f>'generator_costs_04-08-2010'!AI20</f>
         <v>0</v>
       </c>
-      <c r="AC20" s="20">
+      <c r="AC20" s="19">
         <f>'generator_costs_04-08-2010'!AJ20</f>
         <v>0</v>
       </c>
-      <c r="AD20" s="20">
+      <c r="AD20" s="19">
         <f>'generator_costs_04-08-2010'!AK20</f>
         <v>0</v>
       </c>
-      <c r="AE20" s="20">
+      <c r="AE20" s="19">
         <f>'generator_costs_04-08-2010'!AL20</f>
         <v>0</v>
       </c>
-      <c r="AF20" s="20">
+      <c r="AF20" s="19">
         <f>'generator_costs_04-08-2010'!AM20</f>
         <v>0</v>
       </c>
-      <c r="AG20" s="20">
+      <c r="AG20" s="19">
         <f>'generator_costs_04-08-2010'!AN20</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:33">
-      <c r="A21" s="20">
+      <c r="A21" s="19">
         <f>'generator_costs_04-08-2010'!A21</f>
         <v>21</v>
       </c>
-      <c r="B21" s="20" t="str">
+      <c r="B21" s="19" t="str">
         <f>'generator_costs_04-08-2010'!B21</f>
         <v>Geothermal_EP</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="19">
         <f>'generator_costs_04-08-2010'!C21</f>
         <v>0</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="19">
         <f>'generator_costs_04-08-2010'!D21</f>
         <v>0</v>
       </c>
-      <c r="E21" s="20" t="str">
+      <c r="E21" s="19" t="str">
         <f>'generator_costs_04-08-2010'!E21</f>
         <v>Geothermal</v>
       </c>
-      <c r="F21" s="20">
+      <c r="F21" s="19">
         <f>'generator_costs_04-08-2010'!M21</f>
         <v>0</v>
       </c>
-      <c r="G21" s="20">
+      <c r="G21" s="19">
         <f>'generator_costs_04-08-2010'!N21</f>
         <v>0</v>
       </c>
-      <c r="H21" s="20">
+      <c r="H21" s="19">
         <f>'generator_costs_04-08-2010'!O21</f>
         <v>0</v>
       </c>
-      <c r="I21" s="20">
+      <c r="I21" s="19">
         <f>'generator_costs_04-08-2010'!P21</f>
         <v>0</v>
       </c>
-      <c r="J21" s="20">
+      <c r="J21" s="19">
         <f>'generator_costs_04-08-2010'!Q21</f>
         <v>0</v>
       </c>
-      <c r="K21" s="20">
+      <c r="K21" s="19">
         <f>'generator_costs_04-08-2010'!R21</f>
         <v>0</v>
       </c>
-      <c r="L21" s="20">
+      <c r="L21" s="19">
         <f>'generator_costs_04-08-2010'!S21</f>
         <v>0</v>
       </c>
-      <c r="M21" s="20">
+      <c r="M21" s="19">
         <f>'generator_costs_04-08-2010'!T21</f>
         <v>0</v>
       </c>
-      <c r="N21" s="20">
+      <c r="N21" s="19">
         <f>'generator_costs_04-08-2010'!U21</f>
         <v>0</v>
       </c>
-      <c r="O21" s="20">
+      <c r="O21" s="19">
         <f>'generator_costs_04-08-2010'!V21</f>
         <v>0</v>
       </c>
-      <c r="P21" s="20">
+      <c r="P21" s="19">
         <f>'generator_costs_04-08-2010'!W21</f>
         <v>0</v>
       </c>
-      <c r="Q21" s="20">
+      <c r="Q21" s="19">
         <f>'generator_costs_04-08-2010'!X21</f>
         <v>0</v>
       </c>
-      <c r="R21" s="20">
+      <c r="R21" s="19">
         <f>'generator_costs_04-08-2010'!Y21</f>
         <v>0</v>
       </c>
-      <c r="S21" s="20">
+      <c r="S21" s="19">
         <f>'generator_costs_04-08-2010'!Z21</f>
         <v>0</v>
       </c>
-      <c r="T21" s="20">
+      <c r="T21" s="19">
         <f>'generator_costs_04-08-2010'!AA21</f>
         <v>0</v>
       </c>
-      <c r="U21" s="20">
+      <c r="U21" s="19">
         <f>'generator_costs_04-08-2010'!AB21</f>
         <v>0</v>
       </c>
-      <c r="V21" s="20">
+      <c r="V21" s="19">
         <f>'generator_costs_04-08-2010'!AC21</f>
         <v>0</v>
       </c>
-      <c r="W21" s="20">
+      <c r="W21" s="19">
         <f>'generator_costs_04-08-2010'!AD21</f>
         <v>0</v>
       </c>
-      <c r="X21" s="20">
+      <c r="X21" s="19">
         <f>'generator_costs_04-08-2010'!AE21</f>
         <v>0</v>
       </c>
-      <c r="Y21" s="20">
+      <c r="Y21" s="19">
         <f>'generator_costs_04-08-2010'!AF21</f>
         <v>0</v>
       </c>
-      <c r="Z21" s="20">
+      <c r="Z21" s="19">
         <f>'generator_costs_04-08-2010'!AG21</f>
         <v>0</v>
       </c>
-      <c r="AA21" s="20">
+      <c r="AA21" s="19">
         <f>'generator_costs_04-08-2010'!AH21</f>
         <v>0</v>
       </c>
-      <c r="AB21" s="20">
+      <c r="AB21" s="19">
         <f>'generator_costs_04-08-2010'!AI21</f>
         <v>0</v>
       </c>
-      <c r="AC21" s="20">
+      <c r="AC21" s="19">
         <f>'generator_costs_04-08-2010'!AJ21</f>
         <v>0</v>
       </c>
-      <c r="AD21" s="20">
+      <c r="AD21" s="19">
         <f>'generator_costs_04-08-2010'!AK21</f>
         <v>0</v>
       </c>
-      <c r="AE21" s="20">
+      <c r="AE21" s="19">
         <f>'generator_costs_04-08-2010'!AL21</f>
         <v>0</v>
       </c>
-      <c r="AF21" s="20">
+      <c r="AF21" s="19">
         <f>'generator_costs_04-08-2010'!AM21</f>
         <v>0</v>
       </c>
-      <c r="AG21" s="20">
+      <c r="AG21" s="19">
         <f>'generator_costs_04-08-2010'!AN21</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:33">
-      <c r="A22" s="20">
+      <c r="A22" s="19">
         <f>'generator_costs_04-08-2010'!A22</f>
         <v>22</v>
       </c>
-      <c r="B22" s="20" t="str">
+      <c r="B22" s="19" t="str">
         <f>'generator_costs_04-08-2010'!B22</f>
         <v>Nuclear_EP</v>
       </c>
-      <c r="C22" s="20">
+      <c r="C22" s="19">
         <f>'generator_costs_04-08-2010'!C22</f>
         <v>0</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="19">
         <f>'generator_costs_04-08-2010'!D22</f>
         <v>0</v>
       </c>
-      <c r="E22" s="20" t="str">
+      <c r="E22" s="19" t="str">
         <f>'generator_costs_04-08-2010'!E22</f>
         <v>Uranium</v>
       </c>
-      <c r="F22" s="20">
+      <c r="F22" s="19">
         <f>'generator_costs_04-08-2010'!M22</f>
         <v>0</v>
       </c>
-      <c r="G22" s="20">
+      <c r="G22" s="19">
         <f>'generator_costs_04-08-2010'!N22</f>
         <v>0</v>
       </c>
-      <c r="H22" s="20">
+      <c r="H22" s="19">
         <f>'generator_costs_04-08-2010'!O22</f>
         <v>0</v>
       </c>
-      <c r="I22" s="20">
+      <c r="I22" s="19">
         <f>'generator_costs_04-08-2010'!P22</f>
         <v>0</v>
       </c>
-      <c r="J22" s="20">
+      <c r="J22" s="19">
         <f>'generator_costs_04-08-2010'!Q22</f>
         <v>0</v>
       </c>
-      <c r="K22" s="20">
+      <c r="K22" s="19">
         <f>'generator_costs_04-08-2010'!R22</f>
         <v>0</v>
       </c>
-      <c r="L22" s="20">
+      <c r="L22" s="19">
         <f>'generator_costs_04-08-2010'!S22</f>
         <v>0</v>
       </c>
-      <c r="M22" s="20">
+      <c r="M22" s="19">
         <f>'generator_costs_04-08-2010'!T22</f>
         <v>0</v>
       </c>
-      <c r="N22" s="20">
+      <c r="N22" s="19">
         <f>'generator_costs_04-08-2010'!U22</f>
         <v>0</v>
       </c>
-      <c r="O22" s="20">
+      <c r="O22" s="19">
         <f>'generator_costs_04-08-2010'!V22</f>
         <v>0</v>
       </c>
-      <c r="P22" s="20">
+      <c r="P22" s="19">
         <f>'generator_costs_04-08-2010'!W22</f>
         <v>0</v>
       </c>
-      <c r="Q22" s="20">
+      <c r="Q22" s="19">
         <f>'generator_costs_04-08-2010'!X22</f>
         <v>0</v>
       </c>
-      <c r="R22" s="20">
+      <c r="R22" s="19">
         <f>'generator_costs_04-08-2010'!Y22</f>
         <v>0</v>
       </c>
-      <c r="S22" s="20">
+      <c r="S22" s="19">
         <f>'generator_costs_04-08-2010'!Z22</f>
         <v>0</v>
       </c>
-      <c r="T22" s="20">
+      <c r="T22" s="19">
         <f>'generator_costs_04-08-2010'!AA22</f>
         <v>0</v>
       </c>
-      <c r="U22" s="20">
+      <c r="U22" s="19">
         <f>'generator_costs_04-08-2010'!AB22</f>
         <v>0</v>
       </c>
-      <c r="V22" s="20">
+      <c r="V22" s="19">
         <f>'generator_costs_04-08-2010'!AC22</f>
         <v>0</v>
       </c>
-      <c r="W22" s="20">
+      <c r="W22" s="19">
         <f>'generator_costs_04-08-2010'!AD22</f>
         <v>0</v>
       </c>
-      <c r="X22" s="20">
+      <c r="X22" s="19">
         <f>'generator_costs_04-08-2010'!AE22</f>
         <v>0</v>
       </c>
-      <c r="Y22" s="20">
+      <c r="Y22" s="19">
         <f>'generator_costs_04-08-2010'!AF22</f>
         <v>0</v>
       </c>
-      <c r="Z22" s="20">
+      <c r="Z22" s="19">
         <f>'generator_costs_04-08-2010'!AG22</f>
         <v>0</v>
       </c>
-      <c r="AA22" s="20">
+      <c r="AA22" s="19">
         <f>'generator_costs_04-08-2010'!AH22</f>
         <v>0</v>
       </c>
-      <c r="AB22" s="20">
+      <c r="AB22" s="19">
         <f>'generator_costs_04-08-2010'!AI22</f>
         <v>0</v>
       </c>
-      <c r="AC22" s="20">
+      <c r="AC22" s="19">
         <f>'generator_costs_04-08-2010'!AJ22</f>
         <v>0</v>
       </c>
-      <c r="AD22" s="20">
+      <c r="AD22" s="19">
         <f>'generator_costs_04-08-2010'!AK22</f>
         <v>0</v>
       </c>
-      <c r="AE22" s="20">
+      <c r="AE22" s="19">
         <f>'generator_costs_04-08-2010'!AL22</f>
         <v>0</v>
       </c>
-      <c r="AF22" s="20">
+      <c r="AF22" s="19">
         <f>'generator_costs_04-08-2010'!AM22</f>
         <v>0</v>
       </c>
-      <c r="AG22" s="20">
+      <c r="AG22" s="19">
         <f>'generator_costs_04-08-2010'!AN22</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:33">
-      <c r="A23" s="20">
+      <c r="A23" s="19">
         <f>'generator_costs_04-08-2010'!A23</f>
         <v>23</v>
       </c>
-      <c r="B23" s="20" t="str">
+      <c r="B23" s="19" t="str">
         <f>'generator_costs_04-08-2010'!B23</f>
         <v>Wind_EP</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="19">
         <f>'generator_costs_04-08-2010'!C23</f>
         <v>0</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="19">
         <f>'generator_costs_04-08-2010'!D23</f>
         <v>0</v>
       </c>
-      <c r="E23" s="20" t="str">
+      <c r="E23" s="19" t="str">
         <f>'generator_costs_04-08-2010'!E23</f>
         <v>Wind</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="19">
         <f>'generator_costs_04-08-2010'!M23</f>
         <v>0</v>
       </c>
-      <c r="G23" s="20">
+      <c r="G23" s="19">
         <f>'generator_costs_04-08-2010'!N23</f>
         <v>0</v>
       </c>
-      <c r="H23" s="20">
+      <c r="H23" s="19">
         <f>'generator_costs_04-08-2010'!O23</f>
         <v>0</v>
       </c>
-      <c r="I23" s="20">
+      <c r="I23" s="19">
         <f>'generator_costs_04-08-2010'!P23</f>
         <v>0</v>
       </c>
-      <c r="J23" s="20">
+      <c r="J23" s="19">
         <f>'generator_costs_04-08-2010'!Q23</f>
         <v>0</v>
       </c>
-      <c r="K23" s="20">
+      <c r="K23" s="19">
         <f>'generator_costs_04-08-2010'!R23</f>
         <v>0</v>
       </c>
-      <c r="L23" s="20">
+      <c r="L23" s="19">
         <f>'generator_costs_04-08-2010'!S23</f>
         <v>0</v>
       </c>
-      <c r="M23" s="20">
+      <c r="M23" s="19">
         <f>'generator_costs_04-08-2010'!T23</f>
         <v>0</v>
       </c>
-      <c r="N23" s="20">
+      <c r="N23" s="19">
         <f>'generator_costs_04-08-2010'!U23</f>
         <v>0</v>
       </c>
-      <c r="O23" s="20">
+      <c r="O23" s="19">
         <f>'generator_costs_04-08-2010'!V23</f>
         <v>0</v>
       </c>
-      <c r="P23" s="20">
+      <c r="P23" s="19">
         <f>'generator_costs_04-08-2010'!W23</f>
         <v>0</v>
       </c>
-      <c r="Q23" s="20">
+      <c r="Q23" s="19">
         <f>'generator_costs_04-08-2010'!X23</f>
         <v>0</v>
       </c>
-      <c r="R23" s="20">
+      <c r="R23" s="19">
         <f>'generator_costs_04-08-2010'!Y23</f>
         <v>0</v>
       </c>
-      <c r="S23" s="20">
+      <c r="S23" s="19">
         <f>'generator_costs_04-08-2010'!Z23</f>
         <v>0</v>
       </c>
-      <c r="T23" s="20">
+      <c r="T23" s="19">
         <f>'generator_costs_04-08-2010'!AA23</f>
         <v>0</v>
       </c>
-      <c r="U23" s="20">
+      <c r="U23" s="19">
         <f>'generator_costs_04-08-2010'!AB23</f>
         <v>0</v>
       </c>
-      <c r="V23" s="20">
+      <c r="V23" s="19">
         <f>'generator_costs_04-08-2010'!AC23</f>
         <v>0</v>
       </c>
-      <c r="W23" s="20">
+      <c r="W23" s="19">
         <f>'generator_costs_04-08-2010'!AD23</f>
         <v>0</v>
       </c>
-      <c r="X23" s="20">
+      <c r="X23" s="19">
         <f>'generator_costs_04-08-2010'!AE23</f>
         <v>0</v>
       </c>
-      <c r="Y23" s="20">
+      <c r="Y23" s="19">
         <f>'generator_costs_04-08-2010'!AF23</f>
         <v>0</v>
       </c>
-      <c r="Z23" s="20">
+      <c r="Z23" s="19">
         <f>'generator_costs_04-08-2010'!AG23</f>
         <v>0</v>
       </c>
-      <c r="AA23" s="20">
+      <c r="AA23" s="19">
         <f>'generator_costs_04-08-2010'!AH23</f>
         <v>0</v>
       </c>
-      <c r="AB23" s="20">
+      <c r="AB23" s="19">
         <f>'generator_costs_04-08-2010'!AI23</f>
         <v>0</v>
       </c>
-      <c r="AC23" s="20">
+      <c r="AC23" s="19">
         <f>'generator_costs_04-08-2010'!AJ23</f>
         <v>0</v>
       </c>
-      <c r="AD23" s="20">
+      <c r="AD23" s="19">
         <f>'generator_costs_04-08-2010'!AK23</f>
         <v>0</v>
       </c>
-      <c r="AE23" s="20">
+      <c r="AE23" s="19">
         <f>'generator_costs_04-08-2010'!AL23</f>
         <v>0</v>
       </c>
-      <c r="AF23" s="20">
+      <c r="AF23" s="19">
         <f>'generator_costs_04-08-2010'!AM23</f>
         <v>0</v>
       </c>
-      <c r="AG23" s="20">
+      <c r="AG23" s="19">
         <f>'generator_costs_04-08-2010'!AN23</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:33">
-      <c r="A24" s="20">
+      <c r="A24" s="19">
         <f>'generator_costs_04-08-2010'!A24</f>
         <v>25</v>
       </c>
-      <c r="B24" s="20" t="str">
+      <c r="B24" s="19" t="str">
         <f>'generator_costs_04-08-2010'!B24</f>
         <v>Commercial_PV</v>
       </c>
-      <c r="C24" s="20">
+      <c r="C24" s="19">
         <f>'generator_costs_04-08-2010'!C24</f>
         <v>2007</v>
       </c>
-      <c r="D24" s="20">
+      <c r="D24" s="19">
         <f>'generator_costs_04-08-2010'!D24</f>
         <v>2010</v>
       </c>
-      <c r="E24" s="20" t="str">
+      <c r="E24" s="19" t="str">
         <f>'generator_costs_04-08-2010'!E24</f>
         <v>Solar</v>
       </c>
-      <c r="F24" s="20">
+      <c r="F24" s="19">
         <f>'generator_costs_04-08-2010'!M24</f>
         <v>4774850.1365644811</v>
       </c>
-      <c r="G24" s="20">
+      <c r="G24" s="19">
         <f>'generator_costs_04-08-2010'!N24</f>
         <v>10210.219999999999</v>
       </c>
-      <c r="H24" s="20">
+      <c r="H24" s="19">
         <f>'generator_costs_04-08-2010'!O24</f>
         <v>0</v>
       </c>
-      <c r="I24" s="20">
+      <c r="I24" s="19">
         <f>'generator_costs_04-08-2010'!P24</f>
         <v>-4.3999999999999997E-2</v>
       </c>
-      <c r="J24" s="20">
+      <c r="J24" s="19">
         <f>'generator_costs_04-08-2010'!Q24</f>
         <v>0</v>
       </c>
-      <c r="K24" s="20">
+      <c r="K24" s="19">
         <f>'generator_costs_04-08-2010'!R24</f>
         <v>0</v>
       </c>
-      <c r="L24" s="20">
+      <c r="L24" s="19">
         <f>'generator_costs_04-08-2010'!S24</f>
         <v>1</v>
       </c>
-      <c r="M24" s="20">
+      <c r="M24" s="19">
         <f>'generator_costs_04-08-2010'!T24</f>
         <v>1</v>
       </c>
-      <c r="N24" s="20">
+      <c r="N24" s="19">
         <f>'generator_costs_04-08-2010'!U24</f>
         <v>0</v>
       </c>
-      <c r="O24" s="20">
+      <c r="O24" s="19">
         <f>'generator_costs_04-08-2010'!V24</f>
         <v>0</v>
       </c>
-      <c r="P24" s="20">
+      <c r="P24" s="19">
         <f>'generator_costs_04-08-2010'!W24</f>
         <v>0</v>
       </c>
-      <c r="Q24" s="20">
+      <c r="Q24" s="19">
         <f>'generator_costs_04-08-2010'!X24</f>
         <v>0</v>
       </c>
-      <c r="R24" s="20">
+      <c r="R24" s="19">
         <f>'generator_costs_04-08-2010'!Y24</f>
         <v>0</v>
       </c>
-      <c r="S24" s="20">
+      <c r="S24" s="19">
         <f>'generator_costs_04-08-2010'!Z24</f>
         <v>30</v>
       </c>
-      <c r="T24" s="20">
+      <c r="T24" s="19">
         <f>'generator_costs_04-08-2010'!AA24</f>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="U24" s="20">
+      <c r="U24" s="19">
         <f>'generator_costs_04-08-2010'!AB24</f>
         <v>0</v>
       </c>
-      <c r="V24" s="20">
+      <c r="V24" s="19">
         <f>'generator_costs_04-08-2010'!AC24</f>
         <v>1</v>
       </c>
-      <c r="W24" s="20">
+      <c r="W24" s="19">
         <f>'generator_costs_04-08-2010'!AD24</f>
         <v>1</v>
       </c>
-      <c r="X24" s="20">
+      <c r="X24" s="19">
         <f>'generator_costs_04-08-2010'!AE24</f>
         <v>0</v>
       </c>
-      <c r="Y24" s="20">
+      <c r="Y24" s="19">
         <f>'generator_costs_04-08-2010'!AF24</f>
         <v>0</v>
       </c>
-      <c r="Z24" s="20">
+      <c r="Z24" s="19">
         <f>'generator_costs_04-08-2010'!AG24</f>
         <v>0</v>
       </c>
-      <c r="AA24" s="20">
+      <c r="AA24" s="19">
         <f>'generator_costs_04-08-2010'!AH24</f>
         <v>0</v>
       </c>
-      <c r="AB24" s="20">
+      <c r="AB24" s="19">
         <f>'generator_costs_04-08-2010'!AI24</f>
         <v>0</v>
       </c>
-      <c r="AC24" s="20">
+      <c r="AC24" s="19">
         <f>'generator_costs_04-08-2010'!AJ24</f>
         <v>0</v>
       </c>
-      <c r="AD24" s="20">
+      <c r="AD24" s="19">
         <f>'generator_costs_04-08-2010'!AK24</f>
         <v>0</v>
       </c>
-      <c r="AE24" s="20">
+      <c r="AE24" s="19">
         <f>'generator_costs_04-08-2010'!AL24</f>
         <v>0</v>
       </c>
-      <c r="AF24" s="20">
+      <c r="AF24" s="19">
         <f>'generator_costs_04-08-2010'!AM24</f>
         <v>1</v>
       </c>
-      <c r="AG24" s="20">
+      <c r="AG24" s="19">
         <f>'generator_costs_04-08-2010'!AN24</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:33">
-      <c r="A25" s="20">
+      <c r="A25" s="19">
         <f>'generator_costs_04-08-2010'!A25</f>
         <v>26</v>
       </c>
-      <c r="B25" s="20" t="str">
+      <c r="B25" s="19" t="str">
         <f>'generator_costs_04-08-2010'!B25</f>
         <v>Central_PV</v>
       </c>
-      <c r="C25" s="20">
+      <c r="C25" s="19">
         <f>'generator_costs_04-08-2010'!C25</f>
         <v>2007</v>
       </c>
-      <c r="D25" s="20">
+      <c r="D25" s="19">
         <f>'generator_costs_04-08-2010'!D25</f>
         <v>2010</v>
       </c>
-      <c r="E25" s="20" t="str">
+      <c r="E25" s="19" t="str">
         <f>'generator_costs_04-08-2010'!E25</f>
         <v>Solar</v>
       </c>
-      <c r="F25" s="20">
+      <c r="F25" s="19">
         <f>'generator_costs_04-08-2010'!M25</f>
         <v>4519882.4108256008</v>
       </c>
-      <c r="G25" s="20">
+      <c r="G25" s="19">
         <f>'generator_costs_04-08-2010'!N25</f>
         <v>10210.219999999999</v>
       </c>
-      <c r="H25" s="20">
+      <c r="H25" s="19">
         <f>'generator_costs_04-08-2010'!O25</f>
         <v>0</v>
       </c>
-      <c r="I25" s="20">
+      <c r="I25" s="19">
         <f>'generator_costs_04-08-2010'!P25</f>
         <v>-4.3999999999999997E-2</v>
       </c>
-      <c r="J25" s="20">
+      <c r="J25" s="19">
         <f>'generator_costs_04-08-2010'!Q25</f>
         <v>65639</v>
       </c>
-      <c r="K25" s="20">
+      <c r="K25" s="19">
         <f>'generator_costs_04-08-2010'!R25</f>
         <v>0</v>
       </c>
-      <c r="L25" s="20">
+      <c r="L25" s="19">
         <f>'generator_costs_04-08-2010'!S25</f>
         <v>3</v>
       </c>
-      <c r="M25" s="20">
+      <c r="M25" s="19">
         <f>'generator_costs_04-08-2010'!T25</f>
         <v>0.8</v>
       </c>
-      <c r="N25" s="20">
+      <c r="N25" s="19">
         <f>'generator_costs_04-08-2010'!U25</f>
         <v>0.1</v>
       </c>
-      <c r="O25" s="20">
+      <c r="O25" s="19">
         <f>'generator_costs_04-08-2010'!V25</f>
         <v>0.1</v>
       </c>
-      <c r="P25" s="20">
+      <c r="P25" s="19">
         <f>'generator_costs_04-08-2010'!W25</f>
         <v>0</v>
       </c>
-      <c r="Q25" s="20">
+      <c r="Q25" s="19">
         <f>'generator_costs_04-08-2010'!X25</f>
         <v>0</v>
       </c>
-      <c r="R25" s="20">
+      <c r="R25" s="19">
         <f>'generator_costs_04-08-2010'!Y25</f>
         <v>0</v>
       </c>
-      <c r="S25" s="20">
+      <c r="S25" s="19">
         <f>'generator_costs_04-08-2010'!Z25</f>
         <v>30</v>
       </c>
-      <c r="T25" s="20">
+      <c r="T25" s="19">
         <f>'generator_costs_04-08-2010'!AA25</f>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="U25" s="20">
+      <c r="U25" s="19">
         <f>'generator_costs_04-08-2010'!AB25</f>
         <v>0</v>
       </c>
-      <c r="V25" s="20">
+      <c r="V25" s="19">
         <f>'generator_costs_04-08-2010'!AC25</f>
         <v>1</v>
       </c>
-      <c r="W25" s="20">
+      <c r="W25" s="19">
         <f>'generator_costs_04-08-2010'!AD25</f>
         <v>1</v>
       </c>
-      <c r="X25" s="20">
+      <c r="X25" s="19">
         <f>'generator_costs_04-08-2010'!AE25</f>
         <v>0</v>
       </c>
-      <c r="Y25" s="20">
+      <c r="Y25" s="19">
         <f>'generator_costs_04-08-2010'!AF25</f>
         <v>0</v>
       </c>
-      <c r="Z25" s="20">
+      <c r="Z25" s="19">
         <f>'generator_costs_04-08-2010'!AG25</f>
         <v>0</v>
       </c>
-      <c r="AA25" s="20">
+      <c r="AA25" s="19">
         <f>'generator_costs_04-08-2010'!AH25</f>
         <v>0</v>
       </c>
-      <c r="AB25" s="20">
+      <c r="AB25" s="19">
         <f>'generator_costs_04-08-2010'!AI25</f>
         <v>0</v>
       </c>
-      <c r="AC25" s="20">
+      <c r="AC25" s="19">
         <f>'generator_costs_04-08-2010'!AJ25</f>
         <v>0</v>
       </c>
-      <c r="AD25" s="20">
+      <c r="AD25" s="19">
         <f>'generator_costs_04-08-2010'!AK25</f>
         <v>0</v>
       </c>
-      <c r="AE25" s="20">
+      <c r="AE25" s="19">
         <f>'generator_costs_04-08-2010'!AL25</f>
         <v>0</v>
       </c>
-      <c r="AF25" s="20">
+      <c r="AF25" s="19">
         <f>'generator_costs_04-08-2010'!AM25</f>
         <v>1</v>
       </c>
-      <c r="AG25" s="20">
+      <c r="AG25" s="19">
         <f>'generator_costs_04-08-2010'!AN25</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:33">
-      <c r="A26" s="20">
+      <c r="A26" s="19">
         <f>'generator_costs_04-08-2010'!A26</f>
         <v>27</v>
       </c>
-      <c r="B26" s="20" t="str">
+      <c r="B26" s="19" t="str">
         <f>'generator_costs_04-08-2010'!B26</f>
         <v>CSP_Trough_No_Storage</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C26" s="19">
         <f>'generator_costs_04-08-2010'!C26</f>
         <v>2007</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D26" s="19">
         <f>'generator_costs_04-08-2010'!D26</f>
         <v>2010</v>
       </c>
-      <c r="E26" s="20" t="str">
+      <c r="E26" s="19" t="str">
         <f>'generator_costs_04-08-2010'!E26</f>
         <v>Solar</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F26" s="19">
         <f>'generator_costs_04-08-2010'!M26</f>
         <v>4615604.3710546866</v>
       </c>
-      <c r="G26" s="20">
+      <c r="G26" s="19">
         <f>'generator_costs_04-08-2010'!N26</f>
         <v>42817.049999999996</v>
       </c>
-      <c r="H26" s="20">
+      <c r="H26" s="19">
         <f>'generator_costs_04-08-2010'!O26</f>
         <v>0</v>
       </c>
-      <c r="I26" s="20">
+      <c r="I26" s="19">
         <f>'generator_costs_04-08-2010'!P26</f>
         <v>-2.5000000000000001E-2</v>
       </c>
-      <c r="J26" s="20">
+      <c r="J26" s="19">
         <f>'generator_costs_04-08-2010'!Q26</f>
         <v>65639</v>
       </c>
-      <c r="K26" s="20">
+      <c r="K26" s="19">
         <f>'generator_costs_04-08-2010'!R26</f>
         <v>0</v>
       </c>
-      <c r="L26" s="20">
+      <c r="L26" s="19">
         <f>'generator_costs_04-08-2010'!S26</f>
         <v>3</v>
       </c>
-      <c r="M26" s="20">
+      <c r="M26" s="19">
         <f>'generator_costs_04-08-2010'!T26</f>
         <v>0.8</v>
       </c>
-      <c r="N26" s="20">
+      <c r="N26" s="19">
         <f>'generator_costs_04-08-2010'!U26</f>
         <v>0.1</v>
       </c>
-      <c r="O26" s="20">
+      <c r="O26" s="19">
         <f>'generator_costs_04-08-2010'!V26</f>
         <v>0.1</v>
       </c>
-      <c r="P26" s="20">
+      <c r="P26" s="19">
         <f>'generator_costs_04-08-2010'!W26</f>
         <v>0</v>
       </c>
-      <c r="Q26" s="20">
+      <c r="Q26" s="19">
         <f>'generator_costs_04-08-2010'!X26</f>
         <v>0</v>
       </c>
-      <c r="R26" s="20">
+      <c r="R26" s="19">
         <f>'generator_costs_04-08-2010'!Y26</f>
         <v>0</v>
       </c>
-      <c r="S26" s="20">
+      <c r="S26" s="19">
         <f>'generator_costs_04-08-2010'!Z26</f>
         <v>30</v>
       </c>
-      <c r="T26" s="20">
+      <c r="T26" s="19">
         <f>'generator_costs_04-08-2010'!AA26</f>
         <v>0.05</v>
       </c>
-      <c r="U26" s="20">
+      <c r="U26" s="19">
         <f>'generator_costs_04-08-2010'!AB26</f>
         <v>0.05</v>
       </c>
-      <c r="V26" s="20">
+      <c r="V26" s="19">
         <f>'generator_costs_04-08-2010'!AC26</f>
         <v>1</v>
       </c>
-      <c r="W26" s="20">
+      <c r="W26" s="19">
         <f>'generator_costs_04-08-2010'!AD26</f>
         <v>1</v>
       </c>
-      <c r="X26" s="20">
+      <c r="X26" s="19">
         <f>'generator_costs_04-08-2010'!AE26</f>
         <v>0</v>
       </c>
-      <c r="Y26" s="20">
+      <c r="Y26" s="19">
         <f>'generator_costs_04-08-2010'!AF26</f>
         <v>0</v>
       </c>
-      <c r="Z26" s="20">
+      <c r="Z26" s="19">
         <f>'generator_costs_04-08-2010'!AG26</f>
         <v>0</v>
       </c>
-      <c r="AA26" s="20">
+      <c r="AA26" s="19">
         <f>'generator_costs_04-08-2010'!AH26</f>
         <v>0</v>
       </c>
-      <c r="AB26" s="20">
+      <c r="AB26" s="19">
         <f>'generator_costs_04-08-2010'!AI26</f>
         <v>0</v>
       </c>
-      <c r="AC26" s="20">
+      <c r="AC26" s="19">
         <f>'generator_costs_04-08-2010'!AJ26</f>
         <v>0</v>
       </c>
-      <c r="AD26" s="20">
+      <c r="AD26" s="19">
         <f>'generator_costs_04-08-2010'!AK26</f>
         <v>0</v>
       </c>
-      <c r="AE26" s="20">
+      <c r="AE26" s="19">
         <f>'generator_costs_04-08-2010'!AL26</f>
         <v>0</v>
       </c>
-      <c r="AF26" s="20">
+      <c r="AF26" s="19">
         <f>'generator_costs_04-08-2010'!AM26</f>
         <v>1</v>
       </c>
-      <c r="AG26" s="20">
+      <c r="AG26" s="19">
         <f>'generator_costs_04-08-2010'!AN26</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:33">
-      <c r="A27" s="20">
+      <c r="A27" s="19">
         <f>'generator_costs_04-08-2010'!A27</f>
         <v>28</v>
       </c>
-      <c r="B27" s="20" t="str">
+      <c r="B27" s="19" t="str">
         <f>'generator_costs_04-08-2010'!B27</f>
         <v>Compressed_Air_Energy_Storage</v>
       </c>
-      <c r="C27" s="20">
+      <c r="C27" s="19">
         <f>'generator_costs_04-08-2010'!C27</f>
         <v>2007</v>
       </c>
-      <c r="D27" s="20">
+      <c r="D27" s="19">
         <f>'generator_costs_04-08-2010'!D27</f>
         <v>2010</v>
       </c>
-      <c r="E27" s="20" t="str">
+      <c r="E27" s="19" t="str">
         <f>'generator_costs_04-08-2010'!E27</f>
         <v>Gas</v>
       </c>
-      <c r="F27" s="20">
+      <c r="F27" s="19">
         <f>'generator_costs_04-08-2010'!M27</f>
         <v>1402497.9187390334</v>
       </c>
-      <c r="G27" s="20">
+      <c r="G27" s="19">
         <f>'generator_costs_04-08-2010'!N27</f>
         <v>9949.15</v>
       </c>
-      <c r="H27" s="20">
+      <c r="H27" s="19">
         <f>'generator_costs_04-08-2010'!O27</f>
         <v>2.9914999999999998</v>
       </c>
-      <c r="I27" s="20">
+      <c r="I27" s="19">
         <f>'generator_costs_04-08-2010'!P27</f>
         <v>-1.1999999999999999E-3</v>
       </c>
-      <c r="J27" s="20">
+      <c r="J27" s="19">
         <f>'generator_costs_04-08-2010'!Q27</f>
         <v>91289</v>
       </c>
-      <c r="K27" s="20">
+      <c r="K27" s="19">
         <f>'generator_costs_04-08-2010'!R27</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="L27" s="20">
+      <c r="L27" s="19">
         <f>'generator_costs_04-08-2010'!S27</f>
         <v>6</v>
       </c>
-      <c r="M27" s="20">
+      <c r="M27" s="19">
         <f>'generator_costs_04-08-2010'!T27</f>
         <v>0.1</v>
       </c>
-      <c r="N27" s="20">
+      <c r="N27" s="19">
         <f>'generator_costs_04-08-2010'!U27</f>
         <v>0.2</v>
       </c>
-      <c r="O27" s="20">
+      <c r="O27" s="19">
         <f>'generator_costs_04-08-2010'!V27</f>
         <v>0.2</v>
       </c>
-      <c r="P27" s="20">
+      <c r="P27" s="19">
         <f>'generator_costs_04-08-2010'!W27</f>
         <v>0.2</v>
       </c>
-      <c r="Q27" s="20">
+      <c r="Q27" s="19">
         <f>'generator_costs_04-08-2010'!X27</f>
         <v>0.2</v>
       </c>
-      <c r="R27" s="20">
+      <c r="R27" s="19">
         <f>'generator_costs_04-08-2010'!Y27</f>
         <v>0.1</v>
       </c>
-      <c r="S27" s="20">
+      <c r="S27" s="19">
         <f>'generator_costs_04-08-2010'!Z27</f>
         <v>30</v>
       </c>
-      <c r="T27" s="20">
+      <c r="T27" s="19">
         <f>'generator_costs_04-08-2010'!AA27</f>
         <v>0.03</v>
       </c>
-      <c r="U27" s="20">
+      <c r="U27" s="19">
         <f>'generator_costs_04-08-2010'!AB27</f>
         <v>0.04</v>
       </c>
-      <c r="V27" s="20">
+      <c r="V27" s="19">
         <f>'generator_costs_04-08-2010'!AC27</f>
         <v>0</v>
       </c>
-      <c r="W27" s="20">
+      <c r="W27" s="19">
         <f>'generator_costs_04-08-2010'!AD27</f>
         <v>1</v>
       </c>
-      <c r="X27" s="20">
+      <c r="X27" s="19">
         <f>'generator_costs_04-08-2010'!AE27</f>
         <v>0</v>
       </c>
-      <c r="Y27" s="20">
+      <c r="Y27" s="19">
         <f>'generator_costs_04-08-2010'!AF27</f>
         <v>0</v>
       </c>
-      <c r="Z27" s="20">
+      <c r="Z27" s="19">
         <f>'generator_costs_04-08-2010'!AG27</f>
         <v>0</v>
       </c>
-      <c r="AA27" s="20">
+      <c r="AA27" s="19">
         <f>'generator_costs_04-08-2010'!AH27</f>
         <v>0</v>
       </c>
-      <c r="AB27" s="20">
+      <c r="AB27" s="19">
         <f>'generator_costs_04-08-2010'!AI27</f>
         <v>0</v>
       </c>
-      <c r="AC27" s="20">
+      <c r="AC27" s="19">
         <f>'generator_costs_04-08-2010'!AJ27</f>
         <v>0</v>
       </c>
-      <c r="AD27" s="20">
+      <c r="AD27" s="19">
         <f>'generator_costs_04-08-2010'!AK27</f>
         <v>0</v>
       </c>
-      <c r="AE27" s="20">
+      <c r="AE27" s="19">
         <f>'generator_costs_04-08-2010'!AL27</f>
         <v>0</v>
       </c>
-      <c r="AF27" s="20">
+      <c r="AF27" s="19">
         <f>'generator_costs_04-08-2010'!AM27</f>
         <v>1</v>
       </c>
-      <c r="AG27" s="20">
+      <c r="AG27" s="19">
         <f>'generator_costs_04-08-2010'!AN27</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Jimmy added technologies for each existing cogen / fuel type combination.
</commit_message>
<xml_diff>
--- a/DatabasePrep/GeneratorInfo/generator_costs.xlsx
+++ b/DatabasePrep/GeneratorInfo/generator_costs.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="15880" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="34700" windowHeight="19300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Chart_revise" sheetId="4" r:id="rId1"/>
     <sheet name="generator_costs_04-08-2010" sheetId="1" r:id="rId2"/>
     <sheet name="Cost CSV For Export" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +21,232 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="107">
+  <si>
+    <t>ReEDs Sheet, cost declination rate assumed to be between ST and other techs (@1%).  EIA has minimum learning by 2025 as 10%, so this is roughly consistent</t>
+  </si>
+  <si>
+    <t>storage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Offshore_Wind</t>
+  </si>
+  <si>
+    <t>Bio_Gas</t>
+  </si>
+  <si>
+    <t>year_1_cost_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_2_cost_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_3_cost_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CapEx from SAM with Solar Field area = 800000m^2 and 6h TES, construction cost mulitplier and yearly cost fraction from CSP on ReEDs sheet- it's unclear how much these change with storage... assumed to be the same here, cost declination rate and fixed OM from Mark Mehos estimate on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSP_Trough_No_Storage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSP_Trough_6h_Storage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>heat_rate_mbtu_per_mwh</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commercial_PV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>min_build_year</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>min_dispatch_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>min_runtime_hours</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>min_downtime_hours</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_Cogen_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_Cogen_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Steam_Turbine_Cogen_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCGT_Cogen_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Uranium</t>
+  </si>
+  <si>
+    <t>DOE Solar Program Costs, took 2020 value for fixed O+M, 10% added to capital costs to go from utility to distributed, but also assumed a 5% declination rate, , outage rates from Mathias</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>overnight_cost</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Solar</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Solid</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Uranium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>interest_between_price_year_and_cost_year</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Residential_PV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Geothermal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compressed_Air_Energy_Storage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>source - all dispatch data from TEPPC_Generator_Categories</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>technology_id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_age_years</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Solar</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Gas</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, assumed to run for 40 years, not 60</t>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine</t>
+  </si>
+  <si>
+    <t>Nuclear</t>
+  </si>
+  <si>
+    <t>Geothermal</t>
+  </si>
+  <si>
+    <t>tech_name_again</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Solar Vision Study (see PV_Cost_Calc.xlsx) for costs, ReEDs sheet for construction cost multiplier and cost fractions, Matthias for forced outage rate </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compressed_Air_Energy_storage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet; also Sullivan et al (2008), NREL/CP-670-43510 Conference Paper for o&amp;m costs, declanation rate, etc; $1,200,000 taken as capital cost in 2010 rather than 2004 based on conversation with Hernandez</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biomass_Steam_Turbine</t>
+  </si>
+  <si>
+    <t>Hydro_NonPumped</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hydro_Pumped</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Water</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Water</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, cost declination rate assumed to be that of a gas steam turbine</t>
+  </si>
+  <si>
+    <t>Biomass_IGCC</t>
+  </si>
+  <si>
+    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to coal IGCC</t>
+  </si>
+  <si>
+    <t>Coal_IGCC</t>
+  </si>
+  <si>
+    <t>can_build_new</t>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Steam_Turbine_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nuclear_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CapEx from SAM with Solar Field area = 600000m^2, construction cost mulitplier and yearly cost fraction from ReEDs sheet, cost declination rate and fixed OM from DOE solar program costs on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, EIA says minimum learning by 2025 is 20%, so this is a 1.1% declination rate, capital cost multipulier from EIA,http://graysharboroceanenergy.com/Documents/LIPA%20Offshore%20Wind%20rept.pdf for total outage rate of 3%, distributed by guess</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -194,215 +418,6 @@
   </si>
   <si>
     <t>Gas</t>
-  </si>
-  <si>
-    <t>Coal</t>
-  </si>
-  <si>
-    <t>Uranium</t>
-  </si>
-  <si>
-    <t>DOE Solar Program Costs, took 2020 value for fixed O+M, 10% added to capital costs to go from utility to distributed, but also assumed a 5% declination rate, , outage rates from Mathias</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>overnight_cost</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Solar</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bio_Solid</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Uranium</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>interest_between_price_year_and_cost_year</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Residential_PV</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Geothermal</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Compressed_Air_Energy_Storage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>source - all dispatch data from TEPPC_Generator_Categories</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>technology_id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_age_years</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Solar</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bio_Gas</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, assumed to run for 40 years, not 60</t>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine</t>
-  </si>
-  <si>
-    <t>Nuclear</t>
-  </si>
-  <si>
-    <t>Geothermal</t>
-  </si>
-  <si>
-    <t>tech_name_again</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Solar Vision Study (see PV_Cost_Calc.xlsx) for costs, ReEDs sheet for construction cost multiplier and cost fractions, Matthias for forced outage rate </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Compressed_Air_Energy_storage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet; also Sullivan et al (2008), NREL/CP-670-43510 Conference Paper for o&amp;m costs, declanation rate, etc; $1,200,000 taken as capital cost in 2010 rather than 2004 based on conversation with Hernandez</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biomass_Steam_Turbine</t>
-  </si>
-  <si>
-    <t>Hydro_NonPumped</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hydro_Pumped</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Water</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Water</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, cost declination rate assumed to be that of a gas steam turbine</t>
-  </si>
-  <si>
-    <t>Biomass_IGCC</t>
-  </si>
-  <si>
-    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to coal IGCC</t>
-  </si>
-  <si>
-    <t>Coal_IGCC</t>
-  </si>
-  <si>
-    <t>can_build_new</t>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nuclear_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CapEx from SAM with Solar Field area = 600000m^2, construction cost mulitplier and yearly cost fraction from ReEDs sheet, cost declination rate and fixed OM from DOE solar program costs on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, cost declination rate assumed to be between ST and other techs (@1%).  EIA has minimum learning by 2025 as 10%, so this is roughly consistent</t>
-  </si>
-  <si>
-    <t>storage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Offshore_Wind</t>
-  </si>
-  <si>
-    <t>Bio_Gas</t>
-  </si>
-  <si>
-    <t>year_1_cost_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_2_cost_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_3_cost_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CapEx from SAM with Solar Field area = 800000m^2 and 6h TES, construction cost mulitplier and yearly cost fraction from CSP on ReEDs sheet- it's unclear how much these change with storage... assumed to be the same here, cost declination rate and fixed OM from Mark Mehos estimate on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSP_Trough_No_Storage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSP_Trough_6h_Storage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>heat_rate_mbtu_per_mwh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Commercial_PV</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>min_build_year</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>min_dispatch_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>min_runtime_hours</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>min_downtime_hours</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -414,7 +429,7 @@
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -451,14 +466,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -508,7 +524,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'generator_costs_04-08-2010'!$A$30</c:f>
+              <c:f>'generator_costs_04-08-2010'!$A$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -531,7 +547,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'generator_costs_04-08-2010'!$B$30:$F$30</c:f>
+              <c:f>'generator_costs_04-08-2010'!$B$34:$F$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -559,7 +575,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'generator_costs_04-08-2010'!$A$31</c:f>
+              <c:f>'generator_costs_04-08-2010'!$A$35</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -582,7 +598,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'generator_costs_04-08-2010'!$B$31:$F$31</c:f>
+              <c:f>'generator_costs_04-08-2010'!$B$35:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -610,7 +626,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'generator_costs_04-08-2010'!$A$32</c:f>
+              <c:f>'generator_costs_04-08-2010'!$A$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -633,7 +649,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'generator_costs_04-08-2010'!$B$32:$F$32</c:f>
+              <c:f>'generator_costs_04-08-2010'!$B$36:$F$36</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -701,7 +717,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'generator_costs_04-08-2010'!$A$33</c:f>
+              <c:f>'generator_costs_04-08-2010'!$A$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -725,7 +741,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'generator_costs_04-08-2010'!$B$33:$F$33</c:f>
+              <c:f>'generator_costs_04-08-2010'!$B$37:$F$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -753,7 +769,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'generator_costs_04-08-2010'!$A$34</c:f>
+              <c:f>'generator_costs_04-08-2010'!$A$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -774,7 +790,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'generator_costs_04-08-2010'!$B$34:$F$34</c:f>
+              <c:f>'generator_costs_04-08-2010'!$B$38:$F$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -802,7 +818,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'generator_costs_04-08-2010'!$A$35</c:f>
+              <c:f>'generator_costs_04-08-2010'!$A$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -825,7 +841,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'generator_costs_04-08-2010'!$B$35:$F$35</c:f>
+              <c:f>'generator_costs_04-08-2010'!$B$39:$F$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -853,7 +869,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'generator_costs_04-08-2010'!$A$36</c:f>
+              <c:f>'generator_costs_04-08-2010'!$A$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -867,7 +883,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'generator_costs_04-08-2010'!$B$36:$F$36</c:f>
+              <c:f>'generator_costs_04-08-2010'!$B$40:$F$40</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -895,7 +911,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>'generator_costs_04-08-2010'!$A$37</c:f>
+              <c:f>'generator_costs_04-08-2010'!$A$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -918,7 +934,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'generator_costs_04-08-2010'!$B$37:$F$37</c:f>
+              <c:f>'generator_costs_04-08-2010'!$B$41:$F$41</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -946,7 +962,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>'generator_costs_04-08-2010'!$A$38</c:f>
+              <c:f>'generator_costs_04-08-2010'!$A$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -969,7 +985,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'generator_costs_04-08-2010'!$B$38:$F$38</c:f>
+              <c:f>'generator_costs_04-08-2010'!$B$42:$F$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -997,7 +1013,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>'generator_costs_04-08-2010'!$A$39</c:f>
+              <c:f>'generator_costs_04-08-2010'!$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1020,7 +1036,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'generator_costs_04-08-2010'!$B$39:$F$39</c:f>
+              <c:f>'generator_costs_04-08-2010'!$B$43:$F$43</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1048,7 +1064,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>'generator_costs_04-08-2010'!$A$40</c:f>
+              <c:f>'generator_costs_04-08-2010'!$A$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1071,7 +1087,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'generator_costs_04-08-2010'!$B$40:$F$40</c:f>
+              <c:f>'generator_costs_04-08-2010'!$B$44:$F$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1099,7 +1115,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>'generator_costs_04-08-2010'!$A$41</c:f>
+              <c:f>'generator_costs_04-08-2010'!$A$45</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1122,7 +1138,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'generator_costs_04-08-2010'!$B$41:$F$41</c:f>
+              <c:f>'generator_costs_04-08-2010'!$B$45:$F$45</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1150,7 +1166,7 @@
           <c:order val="13"/>
           <c:tx>
             <c:strRef>
-              <c:f>'generator_costs_04-08-2010'!$A$42</c:f>
+              <c:f>'generator_costs_04-08-2010'!$A$46</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1171,7 +1187,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'generator_costs_04-08-2010'!$B$42:$F$42</c:f>
+              <c:f>'generator_costs_04-08-2010'!$B$46:$F$46</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1199,179 +1215,11 @@
           <c:order val="14"/>
           <c:tx>
             <c:strRef>
-              <c:f>'generator_costs_04-08-2010'!$A$43</c:f>
+              <c:f>'generator_costs_04-08-2010'!$A$47</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>Geothermal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'generator_costs_04-08-2010'!$B$43:$F$43</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>3.669825762045137</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.525219984415768</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.386312251402048</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.252878037310924</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.124701663657505</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="15"/>
-          <c:order val="15"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'generator_costs_04-08-2010'!$A$44</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Hydro_NonPumped</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'generator_costs_04-08-2010'!$B$44:$F$44</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>2.690364973631826</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.608453899375566</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.529036696453335</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.452037436252461</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.377382501889087</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="16"/>
-          <c:order val="16"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'generator_costs_04-08-2010'!$A$45</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Hydro_Pumped</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'generator_costs_04-08-2010'!$B$45:$F$45</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>4.629622533609614</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.368661169995165</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.12240960891972</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.890038692044511</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.67076599881321</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="17"/>
-          <c:order val="17"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'generator_costs_04-08-2010'!$A$46</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Gas_Combustion_Turbine_EP</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'generator_costs_04-08-2010'!$B$46:$F$46</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="18"/>
-          <c:order val="18"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'generator_costs_04-08-2010'!$A$47</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Coal_Steam_Turbine_EP</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1386,6 +1234,174 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>3.669825762045137</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.525219984415768</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.386312251402048</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.252878037310924</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.124701663657505</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="15"/>
+          <c:order val="15"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'generator_costs_04-08-2010'!$A$48</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hydro_NonPumped</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'generator_costs_04-08-2010'!$B$48:$F$48</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.690364973631826</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.608453899375566</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.529036696453335</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.452037436252461</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.377382501889087</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="16"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'generator_costs_04-08-2010'!$A$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hydro_Pumped</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'generator_costs_04-08-2010'!$B$49:$F$49</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.629622533609614</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.368661169995165</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.12240960891972</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.890038692044511</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.67076599881321</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="17"/>
+          <c:order val="17"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'generator_costs_04-08-2010'!$A$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gas_Combustion_Turbine_EP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'generator_costs_04-08-2010'!$B$50:$F$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="18"/>
+          <c:order val="18"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'generator_costs_04-08-2010'!$A$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Coal_Steam_Turbine_EP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'generator_costs_04-08-2010'!$B$51:$F$51</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -1405,11 +1421,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="495116376"/>
-        <c:axId val="495125400"/>
+        <c:axId val="522658088"/>
+        <c:axId val="522667192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="495116376"/>
+        <c:axId val="522658088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1430,6 +1446,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -1443,14 +1460,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="495125400"/>
+        <c:crossAx val="522667192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="495125400"/>
+        <c:axId val="522667192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="7.0"/>
@@ -1473,6 +1490,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
@@ -1486,7 +1504,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="495116376"/>
+        <c:crossAx val="522658088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1870,11 +1888,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:AP56"/>
+  <dimension ref="A1:AP60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A57" sqref="A57:XFD57"/>
+      <selection pane="topRight" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1905,130 +1923,130 @@
   <sheetData>
     <row r="1" spans="1:42">
       <c r="A1" s="5" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N1" t="s">
+        <v>95</v>
+      </c>
+      <c r="O1" t="s">
+        <v>96</v>
+      </c>
+      <c r="P1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>100</v>
+      </c>
+      <c r="R1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" t="s">
+        <v>97</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="11" t="s">
+      <c r="AI1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM1" t="s">
         <v>55</v>
       </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="AN1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AP1" t="s">
         <v>33</v>
-      </c>
-      <c r="M1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>40</v>
-      </c>
-      <c r="R1" t="s">
-        <v>97</v>
-      </c>
-      <c r="S1" t="s">
-        <v>37</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN1" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="AO1" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:42">
@@ -2036,7 +2054,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="C2" s="5">
         <v>2007</v>
@@ -2045,7 +2063,7 @@
         <v>2010</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
       <c r="F2">
         <v>2004</v>
@@ -2160,7 +2178,7 @@
         <v>CCGT</v>
       </c>
       <c r="AP2" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:42">
@@ -2168,7 +2186,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="C3" s="5">
         <v>2007</v>
@@ -2177,7 +2195,7 @@
         <v>2010</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
       <c r="F3">
         <v>2004</v>
@@ -2292,7 +2310,7 @@
         <v>Gas_Combustion_Turbine</v>
       </c>
       <c r="AP3" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:42">
@@ -2300,7 +2318,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="C4" s="5">
         <v>2007</v>
@@ -2309,7 +2327,7 @@
         <v>2010</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="F4">
         <v>2004</v>
@@ -2424,7 +2442,7 @@
         <v>Wind</v>
       </c>
       <c r="AP4" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:42">
@@ -2432,7 +2450,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="C5" s="5">
         <v>2007</v>
@@ -2441,7 +2459,7 @@
         <v>2010</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="F5">
         <v>2004</v>
@@ -2556,7 +2574,7 @@
         <v>Offshore_Wind</v>
       </c>
       <c r="AP5" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:42">
@@ -2564,7 +2582,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C6" s="5">
         <v>2007</v>
@@ -2573,7 +2591,7 @@
         <v>2010</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="F6">
         <v>2009</v>
@@ -2689,7 +2707,7 @@
         <v>Residential_PV</v>
       </c>
       <c r="AP6" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:42" s="11" customFormat="1">
@@ -2697,7 +2715,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="C7" s="11">
         <v>2007</v>
@@ -2706,7 +2724,7 @@
         <v>2012</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="F7" s="11">
         <v>2010</v>
@@ -2817,10 +2835,10 @@
         <v>0</v>
       </c>
       <c r="AO7" s="11" t="s">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="AP7" s="11" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:42">
@@ -2828,7 +2846,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="C8" s="5">
         <v>2007</v>
@@ -2837,7 +2855,7 @@
         <v>2010</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="F8">
         <v>2007</v>
@@ -2952,7 +2970,7 @@
         <v>Bio_Gas</v>
       </c>
       <c r="AP8" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:42">
@@ -2960,7 +2978,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="C9" s="5">
         <v>2007</v>
@@ -2969,7 +2987,7 @@
         <v>2010</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="F9">
         <v>2004</v>
@@ -3084,7 +3102,7 @@
         <v>Biomass_Steam_Turbine</v>
       </c>
       <c r="AP9" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:42">
@@ -3092,7 +3110,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="C10" s="5">
         <v>2007</v>
@@ -3101,7 +3119,7 @@
         <v>2012</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="F10">
         <v>2007</v>
@@ -3216,7 +3234,7 @@
         <v>Biomass_IGCC</v>
       </c>
       <c r="AP10" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:42">
@@ -3224,7 +3242,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="C11" s="5">
         <v>2007</v>
@@ -3233,7 +3251,7 @@
         <v>2010</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="F11">
         <v>2004</v>
@@ -3348,7 +3366,7 @@
         <v>Coal_IGCC</v>
       </c>
       <c r="AP11" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:42">
@@ -3356,7 +3374,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="C12" s="5">
         <v>2007</v>
@@ -3365,7 +3383,7 @@
         <v>2010</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="F12">
         <v>2004</v>
@@ -3480,7 +3498,7 @@
         <v>Coal_Steam_Turbine</v>
       </c>
       <c r="AP12" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:42">
@@ -3488,7 +3506,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="C13" s="5">
         <v>2007</v>
@@ -3497,7 +3515,7 @@
         <v>2010</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="F13">
         <v>2004</v>
@@ -3612,7 +3630,7 @@
         <v>Nuclear</v>
       </c>
       <c r="AP13" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:42">
@@ -3620,7 +3638,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="C14" s="5">
         <v>2007</v>
@@ -3629,7 +3647,7 @@
         <v>2010</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="F14">
         <v>2004</v>
@@ -3744,7 +3762,7 @@
         <v>Geothermal</v>
       </c>
       <c r="AP14" t="s">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:42">
@@ -3752,7 +3770,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="C15" s="5">
         <v>2007</v>
@@ -3761,7 +3779,7 @@
         <v>2010</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="F15" s="5">
         <v>2004</v>
@@ -3876,7 +3894,7 @@
         <v>Hydro_NonPumped</v>
       </c>
       <c r="AP15" s="5" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:42">
@@ -3884,7 +3902,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="C16" s="5">
         <v>2007</v>
@@ -3893,7 +3911,7 @@
         <v>2010</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="F16" s="5">
         <v>2004</v>
@@ -4008,7 +4026,7 @@
         <v>Hydro_Pumped</v>
       </c>
       <c r="AP16" s="5" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:42" s="18" customFormat="1">
@@ -4016,10 +4034,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="AM17" s="18">
         <v>0</v>
@@ -4033,12 +4051,12 @@
         <v>18</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="G18" s="11"/>
       <c r="M18" s="11"/>
@@ -4056,12 +4074,12 @@
         <v>19</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="G19" s="11"/>
       <c r="M19" s="11"/>
@@ -4079,12 +4097,12 @@
         <v>20</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="G20" s="11"/>
       <c r="M20" s="11"/>
@@ -4101,13 +4119,13 @@
       <c r="A21">
         <v>21</v>
       </c>
-      <c r="B21" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="21"/>
+      <c r="B21" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="22"/>
       <c r="D21"/>
       <c r="E21" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="G21" s="11"/>
       <c r="M21" s="11"/>
@@ -4125,12 +4143,12 @@
         <v>22</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="C22"/>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="G22" s="11"/>
       <c r="M22" s="11"/>
@@ -4148,10 +4166,10 @@
         <v>23</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="AM23" s="18">
         <v>0</v>
@@ -4165,7 +4183,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>98</v>
+        <v>11</v>
       </c>
       <c r="C24" s="8">
         <v>2007</v>
@@ -4174,7 +4192,7 @@
         <v>2010</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="F24" s="8">
         <v>2009</v>
@@ -4285,10 +4303,10 @@
         <v>0</v>
       </c>
       <c r="AO24" s="9" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="AP24" s="9" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:42" s="8" customFormat="1">
@@ -4296,7 +4314,7 @@
         <v>26</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="C25" s="8">
         <v>2007</v>
@@ -4305,7 +4323,7 @@
         <v>2010</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="F25" s="8">
         <v>2009</v>
@@ -4416,10 +4434,10 @@
         <v>0</v>
       </c>
       <c r="AO25" s="9" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="AP25" s="9" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:42" s="5" customFormat="1">
@@ -4427,7 +4445,7 @@
         <v>27</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="C26" s="5">
         <v>2007</v>
@@ -4436,7 +4454,7 @@
         <v>2010</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="F26" s="5">
         <v>2010</v>
@@ -4547,10 +4565,10 @@
         <v>0</v>
       </c>
       <c r="AO26" s="9" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="AP26" s="9" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:42" s="9" customFormat="1">
@@ -4558,7 +4576,7 @@
         <v>28</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="C27" s="9">
         <v>2007</v>
@@ -4567,7 +4585,7 @@
         <v>2010</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="F27" s="9">
         <v>2010</v>
@@ -4678,203 +4696,143 @@
         <v>1</v>
       </c>
       <c r="AO27" s="14" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="AP27" s="14" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:42" s="5" customFormat="1">
-      <c r="G28" s="11"/>
-      <c r="AM28" s="12"/>
-      <c r="AN28" s="15"/>
+    <row r="28" spans="1:42" s="21" customFormat="1">
+      <c r="A28" s="21">
+        <v>29</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM28" s="21">
+        <v>0</v>
+      </c>
+      <c r="AN28" s="21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:42" s="6" customFormat="1">
-      <c r="A29" s="6" t="s">
-        <v>2</v>
+    <row r="29" spans="1:42" s="21" customFormat="1">
+      <c r="A29" s="21">
+        <v>30</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="AM29" s="21">
+        <v>0</v>
+      </c>
+      <c r="AN29" s="21">
+        <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:42">
-      <c r="A30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30">
-        <v>2010</v>
-      </c>
-      <c r="C30">
-        <v>2014</v>
-      </c>
-      <c r="D30">
-        <v>2018</v>
-      </c>
-      <c r="E30">
-        <v>2022</v>
-      </c>
-      <c r="F30">
-        <v>2026</v>
-      </c>
-      <c r="G30" t="s">
-        <v>1</v>
-      </c>
-      <c r="S30" s="5"/>
-      <c r="Y30"/>
+    <row r="30" spans="1:42" s="21" customFormat="1">
+      <c r="A30" s="21">
+        <v>31</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="AM30" s="21">
+        <v>0</v>
+      </c>
+      <c r="AN30" s="21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:42">
-      <c r="A31" s="5" t="str">
-        <f t="shared" ref="A31:A45" si="9">B2</f>
-        <v>CCGT</v>
-      </c>
-      <c r="B31" s="1">
-        <f t="shared" ref="B31:F45" si="10">$M2*(1+$P2)^(B$30-2007)/1000000</f>
-        <v>1.0531629563645977</v>
-      </c>
-      <c r="C31" s="1">
-        <f t="shared" si="10"/>
-        <v>0.99743346069133265</v>
-      </c>
-      <c r="D31" s="1">
-        <f t="shared" si="10"/>
-        <v>0.94465296419167832</v>
-      </c>
-      <c r="E31" s="1">
-        <f t="shared" si="10"/>
-        <v>0.89466541671623157</v>
-      </c>
-      <c r="F31" s="1">
-        <f t="shared" si="10"/>
-        <v>0.84732302571340368</v>
-      </c>
-      <c r="G31" s="2">
-        <f>-P2*100</f>
-        <v>1.35</v>
-      </c>
-      <c r="S31" s="5"/>
-      <c r="Y31"/>
+    <row r="31" spans="1:42" s="21" customFormat="1">
+      <c r="A31" s="21">
+        <v>32</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="AM31" s="21">
+        <v>0</v>
+      </c>
+      <c r="AN31" s="21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:42">
-      <c r="A32" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>Gas_Combustion_Turbine</v>
-      </c>
-      <c r="B32" s="1">
-        <f t="shared" si="10"/>
-        <v>0.67777019539912997</v>
-      </c>
-      <c r="C32" s="1">
-        <f t="shared" si="10"/>
-        <v>0.63956582060948919</v>
-      </c>
-      <c r="D32" s="1">
-        <f t="shared" si="10"/>
-        <v>0.60351494012068285</v>
-      </c>
-      <c r="E32" s="1">
-        <f t="shared" si="10"/>
-        <v>0.56949616632385003</v>
-      </c>
-      <c r="F32" s="1">
-        <f t="shared" si="10"/>
-        <v>0.5373949539554197</v>
-      </c>
-      <c r="G32" s="2">
-        <f t="shared" ref="G32:G56" si="11">-P3*100</f>
-        <v>1.44</v>
-      </c>
-      <c r="S32" s="5"/>
-      <c r="Y32"/>
+    <row r="32" spans="1:42" s="5" customFormat="1">
+      <c r="G32" s="11"/>
+      <c r="AM32" s="12"/>
+      <c r="AN32" s="15"/>
     </row>
-    <row r="33" spans="1:25">
-      <c r="A33" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>Wind</v>
-      </c>
-      <c r="B33" s="1">
-        <f t="shared" si="10"/>
-        <v>1.8398904013200241</v>
-      </c>
-      <c r="C33" s="1">
-        <f t="shared" si="10"/>
-        <v>1.8033676580585525</v>
-      </c>
-      <c r="D33" s="1">
-        <f t="shared" si="10"/>
-        <v>1.767569909489366</v>
-      </c>
-      <c r="E33" s="1">
-        <f t="shared" si="10"/>
-        <v>1.7324827641057787</v>
-      </c>
-      <c r="F33" s="1">
-        <f t="shared" si="10"/>
-        <v>1.6980921160796985</v>
-      </c>
-      <c r="G33" s="2">
-        <f t="shared" si="11"/>
-        <v>0.5</v>
-      </c>
-      <c r="S33" s="5"/>
-      <c r="Y33"/>
+    <row r="33" spans="1:25" s="6" customFormat="1">
+      <c r="A33" s="6" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="34" spans="1:25">
-      <c r="A34" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>Offshore_Wind</v>
-      </c>
-      <c r="B34" s="1">
-        <f t="shared" si="10"/>
-        <v>3.513234607835245</v>
-      </c>
-      <c r="C34" s="1">
-        <f t="shared" si="10"/>
-        <v>3.3340780541559165</v>
-      </c>
-      <c r="D34" s="1">
-        <f t="shared" si="10"/>
-        <v>3.1640575458333862</v>
-      </c>
-      <c r="E34" s="1">
-        <f t="shared" si="10"/>
-        <v>3.0027071924324598</v>
-      </c>
-      <c r="F34" s="1">
-        <f t="shared" si="10"/>
-        <v>2.8495848614886108</v>
-      </c>
-      <c r="G34" s="2">
-        <f t="shared" si="11"/>
-        <v>1.3</v>
+      <c r="A34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34">
+        <v>2010</v>
+      </c>
+      <c r="C34">
+        <v>2014</v>
+      </c>
+      <c r="D34">
+        <v>2018</v>
+      </c>
+      <c r="E34">
+        <v>2022</v>
+      </c>
+      <c r="F34">
+        <v>2026</v>
+      </c>
+      <c r="G34" t="s">
+        <v>61</v>
       </c>
       <c r="S34" s="5"/>
       <c r="Y34"/>
     </row>
     <row r="35" spans="1:25">
       <c r="A35" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>Residential_PV</v>
+        <f t="shared" ref="A35:A49" si="9">B2</f>
+        <v>CCGT</v>
       </c>
       <c r="B35" s="1">
-        <f t="shared" si="10"/>
-        <v>4.4262059541347591</v>
+        <f>$M2*(1+$P2)^(B$34-2007)/1000000</f>
+        <v>1.0531629563645977</v>
       </c>
       <c r="C35" s="1">
-        <f t="shared" si="10"/>
-        <v>3.6971169367031149</v>
+        <f>$M2*(1+$P2)^(C$34-2007)/1000000</f>
+        <v>0.99743346069133265</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="10"/>
-        <v>3.0881241824927677</v>
+        <f>$M2*(1+$P2)^(D$34-2007)/1000000</f>
+        <v>0.94465296419167832</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" si="10"/>
-        <v>2.5794453163823263</v>
+        <f>$M2*(1+$P2)^(E$34-2007)/1000000</f>
+        <v>0.89466541671623157</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" si="10"/>
-        <v>2.1545565356234837</v>
+        <f>$M2*(1+$P2)^(F$34-2007)/1000000</f>
+        <v>0.84732302571340368</v>
       </c>
       <c r="G35" s="2">
-        <f t="shared" si="11"/>
-        <v>4.3999999999999995</v>
+        <f>-P2*100</f>
+        <v>1.35</v>
       </c>
       <c r="S35" s="5"/>
       <c r="Y35"/>
@@ -4882,31 +4840,31 @@
     <row r="36" spans="1:25">
       <c r="A36" s="5" t="str">
         <f t="shared" si="9"/>
-        <v>CSP_Trough_6h_Storage</v>
+        <v>Gas_Combustion_Turbine</v>
       </c>
       <c r="B36" s="1">
-        <f t="shared" si="10"/>
-        <v>6.8694765926520924</v>
+        <f>$M3*(1+$P3)^(B$34-2007)/1000000</f>
+        <v>0.67777019539912997</v>
       </c>
       <c r="C36" s="1">
-        <f t="shared" si="10"/>
-        <v>5.7139591915048698</v>
+        <f>$M3*(1+$P3)^(C$34-2007)/1000000</f>
+        <v>0.63956582060948919</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="10"/>
-        <v>4.7528118338893828</v>
+        <f>$M3*(1+$P3)^(D$34-2007)/1000000</f>
+        <v>0.60351494012068285</v>
       </c>
       <c r="E36" s="1">
-        <f t="shared" si="10"/>
-        <v>3.9533394571566234</v>
+        <f>$M3*(1+$P3)^(E$34-2007)/1000000</f>
+        <v>0.56949616632385003</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" si="10"/>
-        <v>3.2883466482033623</v>
+        <f>$M3*(1+$P3)^(F$34-2007)/1000000</f>
+        <v>0.5373949539554197</v>
       </c>
       <c r="G36" s="2">
-        <f t="shared" si="11"/>
-        <v>4.5</v>
+        <f t="shared" ref="G36:G60" si="10">-P3*100</f>
+        <v>1.44</v>
       </c>
       <c r="S36" s="5"/>
       <c r="Y36"/>
@@ -4914,31 +4872,31 @@
     <row r="37" spans="1:25">
       <c r="A37" s="5" t="str">
         <f t="shared" si="9"/>
-        <v>Bio_Gas</v>
+        <v>Wind</v>
       </c>
       <c r="B37" s="1">
+        <f>$M4*(1+$P4)^(B$34-2007)/1000000</f>
+        <v>1.8398904013200241</v>
+      </c>
+      <c r="C37" s="1">
+        <f>$M4*(1+$P4)^(C$34-2007)/1000000</f>
+        <v>1.8033676580585525</v>
+      </c>
+      <c r="D37" s="1">
+        <f>$M4*(1+$P4)^(D$34-2007)/1000000</f>
+        <v>1.767569909489366</v>
+      </c>
+      <c r="E37" s="1">
+        <f>$M4*(1+$P4)^(E$34-2007)/1000000</f>
+        <v>1.7324827641057787</v>
+      </c>
+      <c r="F37" s="1">
+        <f>$M4*(1+$P4)^(F$34-2007)/1000000</f>
+        <v>1.6980921160796985</v>
+      </c>
+      <c r="G37" s="2">
         <f t="shared" si="10"/>
-        <v>2.4701554476825773</v>
-      </c>
-      <c r="C37" s="1">
-        <f t="shared" si="10"/>
-        <v>2.3309183653314354</v>
-      </c>
-      <c r="D37" s="1">
-        <f t="shared" si="10"/>
-        <v>2.1995297627672028</v>
-      </c>
-      <c r="E37" s="1">
-        <f t="shared" si="10"/>
-        <v>2.0755472389144938</v>
-      </c>
-      <c r="F37" s="1">
-        <f t="shared" si="10"/>
-        <v>1.9585533298471325</v>
-      </c>
-      <c r="G37" s="2">
-        <f t="shared" si="11"/>
-        <v>1.44</v>
+        <v>0.5</v>
       </c>
       <c r="S37" s="5"/>
       <c r="Y37"/>
@@ -4946,31 +4904,31 @@
     <row r="38" spans="1:25">
       <c r="A38" s="5" t="str">
         <f t="shared" si="9"/>
-        <v>Biomass_Steam_Turbine</v>
+        <v>Offshore_Wind</v>
       </c>
       <c r="B38" s="1">
+        <f>$M5*(1+$P5)^(B$34-2007)/1000000</f>
+        <v>3.513234607835245</v>
+      </c>
+      <c r="C38" s="1">
+        <f>$M5*(1+$P5)^(C$34-2007)/1000000</f>
+        <v>3.3340780541559165</v>
+      </c>
+      <c r="D38" s="1">
+        <f>$M5*(1+$P5)^(D$34-2007)/1000000</f>
+        <v>3.1640575458333862</v>
+      </c>
+      <c r="E38" s="1">
+        <f>$M5*(1+$P5)^(E$34-2007)/1000000</f>
+        <v>3.0027071924324598</v>
+      </c>
+      <c r="F38" s="1">
+        <f>$M5*(1+$P5)^(F$34-2007)/1000000</f>
+        <v>2.8495848614886108</v>
+      </c>
+      <c r="G38" s="2">
         <f t="shared" si="10"/>
-        <v>3.1610692256114468</v>
-      </c>
-      <c r="C38" s="1">
-        <f t="shared" si="10"/>
-        <v>3.0920973359134503</v>
-      </c>
-      <c r="D38" s="1">
-        <f t="shared" si="10"/>
-        <v>3.024630355228509</v>
-      </c>
-      <c r="E38" s="1">
-        <f t="shared" si="10"/>
-        <v>2.958635447699181</v>
-      </c>
-      <c r="F38" s="1">
-        <f t="shared" si="10"/>
-        <v>2.8940804939190024</v>
-      </c>
-      <c r="G38" s="2">
-        <f t="shared" si="11"/>
-        <v>0.54999999999999993</v>
+        <v>1.3</v>
       </c>
       <c r="S38" s="5"/>
       <c r="Y38"/>
@@ -4978,31 +4936,31 @@
     <row r="39" spans="1:25">
       <c r="A39" s="5" t="str">
         <f t="shared" si="9"/>
-        <v>Biomass_IGCC</v>
+        <v>Residential_PV</v>
       </c>
       <c r="B39" s="1">
+        <f>$M6*(1+$P6)^(B$34-2007)/1000000</f>
+        <v>4.4262059541347591</v>
+      </c>
+      <c r="C39" s="1">
+        <f>$M6*(1+$P6)^(C$34-2007)/1000000</f>
+        <v>3.6971169367031149</v>
+      </c>
+      <c r="D39" s="1">
+        <f>$M6*(1+$P6)^(D$34-2007)/1000000</f>
+        <v>3.0881241824927677</v>
+      </c>
+      <c r="E39" s="1">
+        <f>$M6*(1+$P6)^(E$34-2007)/1000000</f>
+        <v>2.5794453163823263</v>
+      </c>
+      <c r="F39" s="1">
+        <f>$M6*(1+$P6)^(F$34-2007)/1000000</f>
+        <v>2.1545565356234837</v>
+      </c>
+      <c r="G39" s="2">
         <f t="shared" si="10"/>
-        <v>3.6290095391050952</v>
-      </c>
-      <c r="C39" s="1">
-        <f t="shared" si="10"/>
-        <v>3.4188946800248909</v>
-      </c>
-      <c r="D39" s="1">
-        <f t="shared" si="10"/>
-        <v>3.2209451937635145</v>
-      </c>
-      <c r="E39" s="1">
-        <f t="shared" si="10"/>
-        <v>3.0344567213029081</v>
-      </c>
-      <c r="F39" s="1">
-        <f t="shared" si="10"/>
-        <v>2.858765685081833</v>
-      </c>
-      <c r="G39" s="2">
-        <f t="shared" si="11"/>
-        <v>1.48</v>
+        <v>4.3999999999999995</v>
       </c>
       <c r="S39" s="5"/>
       <c r="Y39"/>
@@ -5010,31 +4968,31 @@
     <row r="40" spans="1:25">
       <c r="A40" s="5" t="str">
         <f t="shared" si="9"/>
-        <v>Coal_IGCC</v>
+        <v>CSP_Trough_6h_Storage</v>
       </c>
       <c r="B40" s="1">
+        <f>$M7*(1+$P7)^(B$34-2007)/1000000</f>
+        <v>6.8694765926520924</v>
+      </c>
+      <c r="C40" s="1">
+        <f>$M7*(1+$P7)^(C$34-2007)/1000000</f>
+        <v>5.7139591915048698</v>
+      </c>
+      <c r="D40" s="1">
+        <f>$M7*(1+$P7)^(D$34-2007)/1000000</f>
+        <v>4.7528118338893828</v>
+      </c>
+      <c r="E40" s="1">
+        <f>$M7*(1+$P7)^(E$34-2007)/1000000</f>
+        <v>3.9533394571566234</v>
+      </c>
+      <c r="F40" s="1">
+        <f>$M7*(1+$P7)^(F$34-2007)/1000000</f>
+        <v>3.2883466482033623</v>
+      </c>
+      <c r="G40" s="2">
         <f t="shared" si="10"/>
-        <v>2.7808905469533363</v>
-      </c>
-      <c r="C40" s="1">
-        <f t="shared" si="10"/>
-        <v>2.6198806573142313</v>
-      </c>
-      <c r="D40" s="1">
-        <f t="shared" si="10"/>
-        <v>2.4681930276216737</v>
-      </c>
-      <c r="E40" s="1">
-        <f t="shared" si="10"/>
-        <v>2.325287911337699</v>
-      </c>
-      <c r="F40" s="1">
-        <f t="shared" si="10"/>
-        <v>2.1906568125359844</v>
-      </c>
-      <c r="G40" s="2">
-        <f t="shared" si="11"/>
-        <v>1.48</v>
+        <v>4.5</v>
       </c>
       <c r="S40" s="5"/>
       <c r="Y40"/>
@@ -5042,31 +5000,31 @@
     <row r="41" spans="1:25">
       <c r="A41" s="5" t="str">
         <f t="shared" si="9"/>
-        <v>Coal_Steam_Turbine</v>
+        <v>Bio_Gas</v>
       </c>
       <c r="B41" s="1">
+        <f>$M8*(1+$P8)^(B$34-2007)/1000000</f>
+        <v>2.4701554476825773</v>
+      </c>
+      <c r="C41" s="1">
+        <f>$M8*(1+$P8)^(C$34-2007)/1000000</f>
+        <v>2.3309183653314354</v>
+      </c>
+      <c r="D41" s="1">
+        <f>$M8*(1+$P8)^(D$34-2007)/1000000</f>
+        <v>2.1995297627672028</v>
+      </c>
+      <c r="E41" s="1">
+        <f>$M8*(1+$P8)^(E$34-2007)/1000000</f>
+        <v>2.0755472389144938</v>
+      </c>
+      <c r="F41" s="1">
+        <f>$M8*(1+$P8)^(F$34-2007)/1000000</f>
+        <v>1.9585533298471325</v>
+      </c>
+      <c r="G41" s="2">
         <f t="shared" si="10"/>
-        <v>2.2632115302709024</v>
-      </c>
-      <c r="C41" s="1">
-        <f t="shared" si="10"/>
-        <v>2.1573904116387688</v>
-      </c>
-      <c r="D41" s="1">
-        <f t="shared" si="10"/>
-        <v>2.0565171774614375</v>
-      </c>
-      <c r="E41" s="1">
-        <f t="shared" si="10"/>
-        <v>1.9603604792056992</v>
-      </c>
-      <c r="F41" s="1">
-        <f t="shared" si="10"/>
-        <v>1.8686997855157279</v>
-      </c>
-      <c r="G41" s="2">
-        <f t="shared" si="11"/>
-        <v>1.1900000000000002</v>
+        <v>1.44</v>
       </c>
       <c r="S41" s="5"/>
       <c r="Y41"/>
@@ -5074,31 +5032,31 @@
     <row r="42" spans="1:25">
       <c r="A42" s="5" t="str">
         <f t="shared" si="9"/>
-        <v>Nuclear</v>
+        <v>Biomass_Steam_Turbine</v>
       </c>
       <c r="B42" s="1">
+        <f>$M9*(1+$P9)^(B$34-2007)/1000000</f>
+        <v>3.1610692256114468</v>
+      </c>
+      <c r="C42" s="1">
+        <f>$M9*(1+$P9)^(C$34-2007)/1000000</f>
+        <v>3.0920973359134503</v>
+      </c>
+      <c r="D42" s="1">
+        <f>$M9*(1+$P9)^(D$34-2007)/1000000</f>
+        <v>3.024630355228509</v>
+      </c>
+      <c r="E42" s="1">
+        <f>$M9*(1+$P9)^(E$34-2007)/1000000</f>
+        <v>2.958635447699181</v>
+      </c>
+      <c r="F42" s="1">
+        <f>$M9*(1+$P9)^(F$34-2007)/1000000</f>
+        <v>2.8940804939190024</v>
+      </c>
+      <c r="G42" s="2">
         <f t="shared" si="10"/>
-        <v>3.979640018509202</v>
-      </c>
-      <c r="C42" s="1">
-        <f t="shared" si="10"/>
-        <v>3.7492241177879264</v>
-      </c>
-      <c r="D42" s="1">
-        <f t="shared" si="10"/>
-        <v>3.5321489933826671</v>
-      </c>
-      <c r="E42" s="1">
-        <f t="shared" si="10"/>
-        <v>3.3276422319653642</v>
-      </c>
-      <c r="F42" s="1">
-        <f t="shared" si="10"/>
-        <v>3.1349761419194406</v>
-      </c>
-      <c r="G42" s="2">
-        <f t="shared" si="11"/>
-        <v>1.48</v>
+        <v>0.54999999999999993</v>
       </c>
       <c r="S42" s="5"/>
       <c r="Y42"/>
@@ -5106,31 +5064,31 @@
     <row r="43" spans="1:25">
       <c r="A43" s="5" t="str">
         <f t="shared" si="9"/>
-        <v>Geothermal</v>
+        <v>Biomass_IGCC</v>
       </c>
       <c r="B43" s="1">
+        <f>$M10*(1+$P10)^(B$34-2007)/1000000</f>
+        <v>3.6290095391050952</v>
+      </c>
+      <c r="C43" s="1">
+        <f>$M10*(1+$P10)^(C$34-2007)/1000000</f>
+        <v>3.4188946800248909</v>
+      </c>
+      <c r="D43" s="1">
+        <f>$M10*(1+$P10)^(D$34-2007)/1000000</f>
+        <v>3.2209451937635145</v>
+      </c>
+      <c r="E43" s="1">
+        <f>$M10*(1+$P10)^(E$34-2007)/1000000</f>
+        <v>3.0344567213029081</v>
+      </c>
+      <c r="F43" s="1">
+        <f>$M10*(1+$P10)^(F$34-2007)/1000000</f>
+        <v>2.858765685081833</v>
+      </c>
+      <c r="G43" s="2">
         <f t="shared" si="10"/>
-        <v>3.6698257620451371</v>
-      </c>
-      <c r="C43" s="1">
-        <f t="shared" si="10"/>
-        <v>3.5252199844157683</v>
-      </c>
-      <c r="D43" s="1">
-        <f t="shared" si="10"/>
-        <v>3.3863122514020483</v>
-      </c>
-      <c r="E43" s="1">
-        <f t="shared" si="10"/>
-        <v>3.2528780373109245</v>
-      </c>
-      <c r="F43" s="1">
-        <f t="shared" si="10"/>
-        <v>3.1247016636575049</v>
-      </c>
-      <c r="G43" s="2">
-        <f t="shared" si="11"/>
-        <v>1</v>
+        <v>1.48</v>
       </c>
       <c r="S43" s="5"/>
       <c r="Y43"/>
@@ -5138,31 +5096,31 @@
     <row r="44" spans="1:25">
       <c r="A44" s="5" t="str">
         <f t="shared" si="9"/>
-        <v>Hydro_NonPumped</v>
+        <v>Coal_IGCC</v>
       </c>
       <c r="B44" s="1">
+        <f>$M11*(1+$P11)^(B$34-2007)/1000000</f>
+        <v>2.7808905469533363</v>
+      </c>
+      <c r="C44" s="1">
+        <f>$M11*(1+$P11)^(C$34-2007)/1000000</f>
+        <v>2.6198806573142313</v>
+      </c>
+      <c r="D44" s="1">
+        <f>$M11*(1+$P11)^(D$34-2007)/1000000</f>
+        <v>2.4681930276216737</v>
+      </c>
+      <c r="E44" s="1">
+        <f>$M11*(1+$P11)^(E$34-2007)/1000000</f>
+        <v>2.325287911337699</v>
+      </c>
+      <c r="F44" s="1">
+        <f>$M11*(1+$P11)^(F$34-2007)/1000000</f>
+        <v>2.1906568125359844</v>
+      </c>
+      <c r="G44" s="2">
         <f t="shared" si="10"/>
-        <v>2.690364973631826</v>
-      </c>
-      <c r="C44" s="1">
-        <f t="shared" si="10"/>
-        <v>2.6084538993755664</v>
-      </c>
-      <c r="D44" s="1">
-        <f t="shared" si="10"/>
-        <v>2.5290366964533346</v>
-      </c>
-      <c r="E44" s="1">
-        <f t="shared" si="10"/>
-        <v>2.4520374362524606</v>
-      </c>
-      <c r="F44" s="1">
-        <f t="shared" si="10"/>
-        <v>2.3773825018890866</v>
-      </c>
-      <c r="G44" s="2">
-        <f t="shared" si="11"/>
-        <v>0.77</v>
+        <v>1.48</v>
       </c>
       <c r="S44" s="5"/>
       <c r="Y44"/>
@@ -5170,367 +5128,494 @@
     <row r="45" spans="1:25">
       <c r="A45" s="5" t="str">
         <f t="shared" si="9"/>
-        <v>Hydro_Pumped</v>
+        <v>Coal_Steam_Turbine</v>
       </c>
       <c r="B45" s="1">
+        <f>$M12*(1+$P12)^(B$34-2007)/1000000</f>
+        <v>2.2632115302709024</v>
+      </c>
+      <c r="C45" s="1">
+        <f>$M12*(1+$P12)^(C$34-2007)/1000000</f>
+        <v>2.1573904116387688</v>
+      </c>
+      <c r="D45" s="1">
+        <f>$M12*(1+$P12)^(D$34-2007)/1000000</f>
+        <v>2.0565171774614375</v>
+      </c>
+      <c r="E45" s="1">
+        <f>$M12*(1+$P12)^(E$34-2007)/1000000</f>
+        <v>1.9603604792056992</v>
+      </c>
+      <c r="F45" s="1">
+        <f>$M12*(1+$P12)^(F$34-2007)/1000000</f>
+        <v>1.8686997855157279</v>
+      </c>
+      <c r="G45" s="2">
         <f t="shared" si="10"/>
-        <v>4.6296225336096137</v>
-      </c>
-      <c r="C45" s="1">
-        <f t="shared" si="10"/>
-        <v>4.3686611699951658</v>
-      </c>
-      <c r="D45" s="1">
-        <f t="shared" si="10"/>
-        <v>4.1224096089197202</v>
-      </c>
-      <c r="E45" s="1">
-        <f t="shared" si="10"/>
-        <v>3.8900386920445111</v>
-      </c>
-      <c r="F45" s="1">
-        <f t="shared" si="10"/>
-        <v>3.6707659988132098</v>
-      </c>
-      <c r="G45" s="2">
-        <f t="shared" si="11"/>
-        <v>1.44</v>
+        <v>1.1900000000000002</v>
       </c>
       <c r="S45" s="5"/>
       <c r="Y45"/>
     </row>
     <row r="46" spans="1:25">
-      <c r="A46" s="20" t="str">
-        <f t="shared" ref="A46:A56" si="12">B17</f>
-        <v>Gas_Combustion_Turbine_EP</v>
+      <c r="A46" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Nuclear</v>
       </c>
       <c r="B46" s="1">
-        <f t="shared" ref="B46:F46" si="13">$M17*(1+$P17)^(B$30-2007)/1000000</f>
-        <v>0</v>
+        <f>$M13*(1+$P13)^(B$34-2007)/1000000</f>
+        <v>3.979640018509202</v>
       </c>
       <c r="C46" s="1">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f>$M13*(1+$P13)^(C$34-2007)/1000000</f>
+        <v>3.7492241177879264</v>
       </c>
       <c r="D46" s="1">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f>$M13*(1+$P13)^(D$34-2007)/1000000</f>
+        <v>3.5321489933826671</v>
       </c>
       <c r="E46" s="1">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f>$M13*(1+$P13)^(E$34-2007)/1000000</f>
+        <v>3.3276422319653642</v>
       </c>
       <c r="F46" s="1">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f>$M13*(1+$P13)^(F$34-2007)/1000000</f>
+        <v>3.1349761419194406</v>
       </c>
       <c r="G46" s="2">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
+        <f t="shared" si="10"/>
+        <v>1.48</v>
+      </c>
+      <c r="S46" s="5"/>
+      <c r="Y46"/>
     </row>
     <row r="47" spans="1:25">
-      <c r="A47" s="20" t="str">
-        <f t="shared" si="12"/>
-        <v>Coal_Steam_Turbine_EP</v>
+      <c r="A47" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Geothermal</v>
       </c>
       <c r="B47" s="1">
-        <f t="shared" ref="B47:F47" si="14">$M18*(1+$P18)^(B$30-2007)/1000000</f>
-        <v>0</v>
+        <f>$M14*(1+$P14)^(B$34-2007)/1000000</f>
+        <v>3.6698257620451371</v>
       </c>
       <c r="C47" s="1">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f>$M14*(1+$P14)^(C$34-2007)/1000000</f>
+        <v>3.5252199844157683</v>
       </c>
       <c r="D47" s="1">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f>$M14*(1+$P14)^(D$34-2007)/1000000</f>
+        <v>3.3863122514020483</v>
       </c>
       <c r="E47" s="1">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f>$M14*(1+$P14)^(E$34-2007)/1000000</f>
+        <v>3.2528780373109245</v>
       </c>
       <c r="F47" s="1">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f>$M14*(1+$P14)^(F$34-2007)/1000000</f>
+        <v>3.1247016636575049</v>
       </c>
       <c r="G47" s="2">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="S47" s="5"/>
+      <c r="Y47"/>
     </row>
     <row r="48" spans="1:25">
-      <c r="A48" s="20" t="str">
+      <c r="A48" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Hydro_NonPumped</v>
+      </c>
+      <c r="B48" s="1">
+        <f>$M15*(1+$P15)^(B$34-2007)/1000000</f>
+        <v>2.690364973631826</v>
+      </c>
+      <c r="C48" s="1">
+        <f>$M15*(1+$P15)^(C$34-2007)/1000000</f>
+        <v>2.6084538993755664</v>
+      </c>
+      <c r="D48" s="1">
+        <f>$M15*(1+$P15)^(D$34-2007)/1000000</f>
+        <v>2.5290366964533346</v>
+      </c>
+      <c r="E48" s="1">
+        <f>$M15*(1+$P15)^(E$34-2007)/1000000</f>
+        <v>2.4520374362524606</v>
+      </c>
+      <c r="F48" s="1">
+        <f>$M15*(1+$P15)^(F$34-2007)/1000000</f>
+        <v>2.3773825018890866</v>
+      </c>
+      <c r="G48" s="2">
+        <f t="shared" si="10"/>
+        <v>0.77</v>
+      </c>
+      <c r="S48" s="5"/>
+      <c r="Y48"/>
+    </row>
+    <row r="49" spans="1:25">
+      <c r="A49" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>Hydro_Pumped</v>
+      </c>
+      <c r="B49" s="1">
+        <f>$M16*(1+$P16)^(B$34-2007)/1000000</f>
+        <v>4.6296225336096137</v>
+      </c>
+      <c r="C49" s="1">
+        <f>$M16*(1+$P16)^(C$34-2007)/1000000</f>
+        <v>4.3686611699951658</v>
+      </c>
+      <c r="D49" s="1">
+        <f>$M16*(1+$P16)^(D$34-2007)/1000000</f>
+        <v>4.1224096089197202</v>
+      </c>
+      <c r="E49" s="1">
+        <f>$M16*(1+$P16)^(E$34-2007)/1000000</f>
+        <v>3.8900386920445111</v>
+      </c>
+      <c r="F49" s="1">
+        <f>$M16*(1+$P16)^(F$34-2007)/1000000</f>
+        <v>3.6707659988132098</v>
+      </c>
+      <c r="G49" s="2">
+        <f t="shared" si="10"/>
+        <v>1.44</v>
+      </c>
+      <c r="S49" s="5"/>
+      <c r="Y49"/>
+    </row>
+    <row r="50" spans="1:25">
+      <c r="A50" s="20" t="str">
+        <f t="shared" ref="A50:A60" si="11">B17</f>
+        <v>Gas_Combustion_Turbine_EP</v>
+      </c>
+      <c r="B50" s="1">
+        <f t="shared" ref="B50:F50" si="12">$M17*(1+$P17)^(B$34-2007)/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="C50" s="1">
         <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="D50" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="E50" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="G50" s="2">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25">
+      <c r="A51" s="20" t="str">
+        <f t="shared" si="11"/>
+        <v>Coal_Steam_Turbine_EP</v>
+      </c>
+      <c r="B51" s="1">
+        <f t="shared" ref="B51:F51" si="13">$M18*(1+$P18)^(B$34-2007)/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="C51" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="D51" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="E51" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G51" s="2">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25">
+      <c r="A52" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Gas_Steam_Turbine_EP</v>
       </c>
-      <c r="B48" s="1">
-        <f t="shared" ref="B48:F48" si="15">$M19*(1+$P19)^(B$30-2007)/1000000</f>
-        <v>0</v>
-      </c>
-      <c r="C48" s="1">
+      <c r="B52" s="1">
+        <f t="shared" ref="B52:F52" si="14">$M19*(1+$P19)^(B$34-2007)/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="C52" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="D52" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G52" s="2">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25">
+      <c r="A53" s="20" t="str">
+        <f t="shared" si="11"/>
+        <v>CCGT_EP</v>
+      </c>
+      <c r="B53" s="1">
+        <f t="shared" ref="B53:F53" si="15">$M20*(1+$P20)^(B$34-2007)/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="C53" s="1">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D53" s="1">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E53" s="1">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F53" s="1">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="G48" s="2">
+      <c r="G53" s="2">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25">
+      <c r="A54" s="20" t="str">
         <f t="shared" si="11"/>
+        <v>Geothermal_EP</v>
+      </c>
+      <c r="B54" s="1">
+        <f t="shared" ref="B54:F54" si="16">$M21*(1+$P21)^(B$34-2007)/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="C54" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="D54" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="G54" s="2">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="20" t="str">
-        <f t="shared" si="12"/>
-        <v>CCGT_EP</v>
-      </c>
-      <c r="B49" s="1">
-        <f t="shared" ref="B49:F49" si="16">$M20*(1+$P20)^(B$30-2007)/1000000</f>
-        <v>0</v>
-      </c>
-      <c r="C49" s="1">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="D49" s="1">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="E49" s="1">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="F49" s="1">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="G49" s="2">
+    <row r="55" spans="1:25">
+      <c r="A55" s="20" t="str">
         <f t="shared" si="11"/>
+        <v>Nuclear_EP</v>
+      </c>
+      <c r="B55" s="1">
+        <f t="shared" ref="B55:F55" si="17">$M22*(1+$P22)^(B$34-2007)/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="C55" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="D55" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="G55" s="2">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="20" t="str">
-        <f t="shared" si="12"/>
-        <v>Geothermal_EP</v>
-      </c>
-      <c r="B50" s="1">
-        <f t="shared" ref="B50:F50" si="17">$M21*(1+$P21)^(B$30-2007)/1000000</f>
-        <v>0</v>
-      </c>
-      <c r="C50" s="1">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="D50" s="1">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="E50" s="1">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="F50" s="1">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="G50" s="2">
+    <row r="56" spans="1:25">
+      <c r="A56" s="20" t="str">
         <f t="shared" si="11"/>
+        <v>Wind_EP</v>
+      </c>
+      <c r="B56" s="1">
+        <f t="shared" ref="B56:F56" si="18">$M23*(1+$P23)^(B$34-2007)/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="C56" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="D56" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G56" s="2">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="20" t="str">
-        <f t="shared" si="12"/>
-        <v>Nuclear_EP</v>
-      </c>
-      <c r="B51" s="1">
-        <f t="shared" ref="B51:F51" si="18">$M22*(1+$P22)^(B$30-2007)/1000000</f>
-        <v>0</v>
-      </c>
-      <c r="C51" s="1">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="D51" s="1">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="E51" s="1">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="F51" s="1">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="G51" s="2">
+    <row r="57" spans="1:25">
+      <c r="A57" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>Commercial_PV</v>
+      </c>
+      <c r="B57" s="1">
+        <f t="shared" ref="B57:F57" si="19">$M24*(1+$P24)^(B$34-2007)/1000000</f>
+        <v>4.1718955072971022</v>
+      </c>
+      <c r="C57" s="1">
+        <f t="shared" si="19"/>
+        <v>3.4846967579028645</v>
+      </c>
+      <c r="D57" s="1">
+        <f t="shared" si="19"/>
+        <v>2.9106940653952389</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="19"/>
+        <v>2.4312416634570249</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="19"/>
+        <v>2.0307651348190192</v>
+      </c>
+      <c r="G57" s="2">
+        <f t="shared" si="10"/>
+        <v>4.3999999999999995</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="20" t="str">
-        <f t="shared" si="12"/>
-        <v>Wind_EP</v>
-      </c>
-      <c r="B52" s="1">
-        <f t="shared" ref="B52:F52" si="19">$M23*(1+$P23)^(B$30-2007)/1000000</f>
-        <v>0</v>
-      </c>
-      <c r="C52" s="1">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="D52" s="1">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="E52" s="1">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="F52" s="1">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="G52" s="2">
+    <row r="58" spans="1:25">
+      <c r="A58" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>Central_PV</v>
+      </c>
+      <c r="B58" s="1">
+        <f t="shared" ref="B58:F58" si="20">$M25*(1+$P25)^(B$34-2007)/1000000</f>
+        <v>3.9491243879754125</v>
+      </c>
+      <c r="C58" s="1">
+        <f t="shared" si="20"/>
+        <v>3.298620717432323</v>
+      </c>
+      <c r="D58" s="1">
+        <f t="shared" si="20"/>
+        <v>2.7552686541362692</v>
+      </c>
+      <c r="E58" s="1">
+        <f t="shared" si="20"/>
+        <v>2.3014180794860186</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="20"/>
+        <v>1.9223262198529554</v>
+      </c>
+      <c r="G58" s="2">
+        <f t="shared" si="10"/>
+        <v>4.3999999999999995</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
-      <c r="A53" s="20" t="str">
-        <f t="shared" si="12"/>
-        <v>Commercial_PV</v>
-      </c>
-      <c r="B53" s="1">
-        <f t="shared" ref="B53:F53" si="20">$M24*(1+$P24)^(B$30-2007)/1000000</f>
-        <v>4.1718955072971022</v>
-      </c>
-      <c r="C53" s="1">
-        <f t="shared" si="20"/>
-        <v>3.4846967579028645</v>
-      </c>
-      <c r="D53" s="1">
-        <f t="shared" si="20"/>
-        <v>2.9106940653952389</v>
-      </c>
-      <c r="E53" s="1">
-        <f t="shared" si="20"/>
-        <v>2.4312416634570249</v>
-      </c>
-      <c r="F53" s="1">
-        <f t="shared" si="20"/>
-        <v>2.0307651348190192</v>
-      </c>
-      <c r="G53" s="2">
+    <row r="59" spans="1:25">
+      <c r="A59" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>4.3999999999999995</v>
+        <v>CSP_Trough_No_Storage</v>
+      </c>
+      <c r="B59" s="1">
+        <f t="shared" ref="B59:F59" si="21">$M26*(1+$P26)^(B$34-2007)/1000000</f>
+        <v>4.2780161826030145</v>
+      </c>
+      <c r="C59" s="1">
+        <f t="shared" si="21"/>
+        <v>3.8659914201161327</v>
+      </c>
+      <c r="D59" s="1">
+        <f t="shared" si="21"/>
+        <v>3.4936496316190953</v>
+      </c>
+      <c r="E59" s="1">
+        <f t="shared" si="21"/>
+        <v>3.1571688661806681</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="21"/>
+        <v>2.8530952730257311</v>
+      </c>
+      <c r="G59" s="2">
+        <f t="shared" si="10"/>
+        <v>2.5</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
-      <c r="A54" s="20" t="str">
-        <f t="shared" si="12"/>
-        <v>Central_PV</v>
-      </c>
-      <c r="B54" s="1">
-        <f t="shared" ref="B54:F54" si="21">$M25*(1+$P25)^(B$30-2007)/1000000</f>
-        <v>3.9491243879754125</v>
-      </c>
-      <c r="C54" s="1">
-        <f t="shared" si="21"/>
-        <v>3.298620717432323</v>
-      </c>
-      <c r="D54" s="1">
-        <f t="shared" si="21"/>
-        <v>2.7552686541362692</v>
-      </c>
-      <c r="E54" s="1">
-        <f t="shared" si="21"/>
-        <v>2.3014180794860186</v>
-      </c>
-      <c r="F54" s="1">
-        <f t="shared" si="21"/>
-        <v>1.9223262198529554</v>
-      </c>
-      <c r="G54" s="2">
+    <row r="60" spans="1:25">
+      <c r="A60" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>4.3999999999999995</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55" s="20" t="str">
-        <f t="shared" si="12"/>
-        <v>CSP_Trough_No_Storage</v>
-      </c>
-      <c r="B55" s="1">
-        <f t="shared" ref="B55:F55" si="22">$M26*(1+$P26)^(B$30-2007)/1000000</f>
-        <v>4.2780161826030145</v>
-      </c>
-      <c r="C55" s="1">
+        <v>Compressed_Air_Energy_Storage</v>
+      </c>
+      <c r="B60" s="1">
+        <f t="shared" ref="B60:F60" si="22">$M27*(1+$P27)^(B$34-2007)/1000000</f>
+        <v>1.3974549825990654</v>
+      </c>
+      <c r="C60" s="1">
         <f t="shared" si="22"/>
-        <v>3.8659914201161327</v>
-      </c>
-      <c r="D55" s="1">
+        <v>1.3907592630373287</v>
+      </c>
+      <c r="D60" s="1">
         <f t="shared" si="22"/>
-        <v>3.4936496316190953</v>
-      </c>
-      <c r="E55" s="1">
+        <v>1.384095625124738</v>
+      </c>
+      <c r="E60" s="1">
         <f t="shared" si="22"/>
-        <v>3.1571688661806681</v>
-      </c>
-      <c r="F55" s="1">
+        <v>1.3774639151463415</v>
+      </c>
+      <c r="F60" s="1">
         <f t="shared" si="22"/>
-        <v>2.8530952730257311</v>
-      </c>
-      <c r="G55" s="2">
-        <f t="shared" si="11"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56" s="20" t="str">
-        <f t="shared" si="12"/>
-        <v>Compressed_Air_Energy_Storage</v>
-      </c>
-      <c r="B56" s="1">
-        <f t="shared" ref="B56:F56" si="23">$M27*(1+$P27)^(B$30-2007)/1000000</f>
-        <v>1.3974549825990654</v>
-      </c>
-      <c r="C56" s="1">
-        <f t="shared" si="23"/>
-        <v>1.3907592630373287</v>
-      </c>
-      <c r="D56" s="1">
-        <f t="shared" si="23"/>
-        <v>1.384095625124738</v>
-      </c>
-      <c r="E56" s="1">
-        <f t="shared" si="23"/>
-        <v>1.3774639151463415</v>
-      </c>
-      <c r="F56" s="1">
-        <f t="shared" si="23"/>
         <v>1.3708639801236917</v>
       </c>
-      <c r="G56" s="2">
-        <f t="shared" si="11"/>
+      <c r="G60" s="2">
+        <f t="shared" si="10"/>
         <v>0.12</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="1">
     <mergeCell ref="B21:C21"/>
   </mergeCells>
@@ -5546,10 +5631,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:AG27"/>
+  <dimension ref="A1:AG31"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:AG31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -9176,8 +9261,543 @@
         <v>1</v>
       </c>
     </row>
+    <row r="28" spans="1:33">
+      <c r="A28" s="21">
+        <f>'generator_costs_04-08-2010'!A28</f>
+        <v>29</v>
+      </c>
+      <c r="B28" s="21" t="str">
+        <f>'generator_costs_04-08-2010'!B28</f>
+        <v>Gas_Combustion_Turbine_Cogen_EP</v>
+      </c>
+      <c r="C28" s="21">
+        <f>'generator_costs_04-08-2010'!C28</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="21">
+        <f>'generator_costs_04-08-2010'!D28</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="21" t="str">
+        <f>'generator_costs_04-08-2010'!E28</f>
+        <v>Gas</v>
+      </c>
+      <c r="F28" s="21">
+        <f>'generator_costs_04-08-2010'!M28</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="21">
+        <f>'generator_costs_04-08-2010'!N28</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="21">
+        <f>'generator_costs_04-08-2010'!O28</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="21">
+        <f>'generator_costs_04-08-2010'!P28</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="21">
+        <f>'generator_costs_04-08-2010'!Q28</f>
+        <v>0</v>
+      </c>
+      <c r="K28" s="21">
+        <f>'generator_costs_04-08-2010'!R28</f>
+        <v>0</v>
+      </c>
+      <c r="L28" s="21">
+        <f>'generator_costs_04-08-2010'!S28</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="21">
+        <f>'generator_costs_04-08-2010'!T28</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="21">
+        <f>'generator_costs_04-08-2010'!U28</f>
+        <v>0</v>
+      </c>
+      <c r="O28" s="21">
+        <f>'generator_costs_04-08-2010'!V28</f>
+        <v>0</v>
+      </c>
+      <c r="P28" s="21">
+        <f>'generator_costs_04-08-2010'!W28</f>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="21">
+        <f>'generator_costs_04-08-2010'!X28</f>
+        <v>0</v>
+      </c>
+      <c r="R28" s="21">
+        <f>'generator_costs_04-08-2010'!Y28</f>
+        <v>0</v>
+      </c>
+      <c r="S28" s="21">
+        <f>'generator_costs_04-08-2010'!Z28</f>
+        <v>0</v>
+      </c>
+      <c r="T28" s="21">
+        <f>'generator_costs_04-08-2010'!AA28</f>
+        <v>0</v>
+      </c>
+      <c r="U28" s="21">
+        <f>'generator_costs_04-08-2010'!AB28</f>
+        <v>0</v>
+      </c>
+      <c r="V28" s="21">
+        <f>'generator_costs_04-08-2010'!AC28</f>
+        <v>0</v>
+      </c>
+      <c r="W28" s="21">
+        <f>'generator_costs_04-08-2010'!AD28</f>
+        <v>0</v>
+      </c>
+      <c r="X28" s="21">
+        <f>'generator_costs_04-08-2010'!AE28</f>
+        <v>0</v>
+      </c>
+      <c r="Y28" s="21">
+        <f>'generator_costs_04-08-2010'!AF28</f>
+        <v>0</v>
+      </c>
+      <c r="Z28" s="21">
+        <f>'generator_costs_04-08-2010'!AG28</f>
+        <v>0</v>
+      </c>
+      <c r="AA28" s="21">
+        <f>'generator_costs_04-08-2010'!AH28</f>
+        <v>0</v>
+      </c>
+      <c r="AB28" s="21">
+        <f>'generator_costs_04-08-2010'!AI28</f>
+        <v>0</v>
+      </c>
+      <c r="AC28" s="21">
+        <f>'generator_costs_04-08-2010'!AJ28</f>
+        <v>0</v>
+      </c>
+      <c r="AD28" s="21">
+        <f>'generator_costs_04-08-2010'!AK28</f>
+        <v>0</v>
+      </c>
+      <c r="AE28" s="21">
+        <f>'generator_costs_04-08-2010'!AL28</f>
+        <v>0</v>
+      </c>
+      <c r="AF28" s="21">
+        <f>'generator_costs_04-08-2010'!AM28</f>
+        <v>0</v>
+      </c>
+      <c r="AG28" s="21">
+        <f>'generator_costs_04-08-2010'!AN28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33">
+      <c r="A29" s="21">
+        <f>'generator_costs_04-08-2010'!A29</f>
+        <v>30</v>
+      </c>
+      <c r="B29" s="21" t="str">
+        <f>'generator_costs_04-08-2010'!B29</f>
+        <v>Coal_Steam_Turbine_Cogen_EP</v>
+      </c>
+      <c r="C29" s="21">
+        <f>'generator_costs_04-08-2010'!C29</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="21">
+        <f>'generator_costs_04-08-2010'!D29</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="21" t="str">
+        <f>'generator_costs_04-08-2010'!E29</f>
+        <v>Coal</v>
+      </c>
+      <c r="F29" s="21">
+        <f>'generator_costs_04-08-2010'!M29</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="21">
+        <f>'generator_costs_04-08-2010'!N29</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="21">
+        <f>'generator_costs_04-08-2010'!O29</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="21">
+        <f>'generator_costs_04-08-2010'!P29</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="21">
+        <f>'generator_costs_04-08-2010'!Q29</f>
+        <v>0</v>
+      </c>
+      <c r="K29" s="21">
+        <f>'generator_costs_04-08-2010'!R29</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="21">
+        <f>'generator_costs_04-08-2010'!S29</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="21">
+        <f>'generator_costs_04-08-2010'!T29</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="21">
+        <f>'generator_costs_04-08-2010'!U29</f>
+        <v>0</v>
+      </c>
+      <c r="O29" s="21">
+        <f>'generator_costs_04-08-2010'!V29</f>
+        <v>0</v>
+      </c>
+      <c r="P29" s="21">
+        <f>'generator_costs_04-08-2010'!W29</f>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="21">
+        <f>'generator_costs_04-08-2010'!X29</f>
+        <v>0</v>
+      </c>
+      <c r="R29" s="21">
+        <f>'generator_costs_04-08-2010'!Y29</f>
+        <v>0</v>
+      </c>
+      <c r="S29" s="21">
+        <f>'generator_costs_04-08-2010'!Z29</f>
+        <v>0</v>
+      </c>
+      <c r="T29" s="21">
+        <f>'generator_costs_04-08-2010'!AA29</f>
+        <v>0</v>
+      </c>
+      <c r="U29" s="21">
+        <f>'generator_costs_04-08-2010'!AB29</f>
+        <v>0</v>
+      </c>
+      <c r="V29" s="21">
+        <f>'generator_costs_04-08-2010'!AC29</f>
+        <v>0</v>
+      </c>
+      <c r="W29" s="21">
+        <f>'generator_costs_04-08-2010'!AD29</f>
+        <v>0</v>
+      </c>
+      <c r="X29" s="21">
+        <f>'generator_costs_04-08-2010'!AE29</f>
+        <v>0</v>
+      </c>
+      <c r="Y29" s="21">
+        <f>'generator_costs_04-08-2010'!AF29</f>
+        <v>0</v>
+      </c>
+      <c r="Z29" s="21">
+        <f>'generator_costs_04-08-2010'!AG29</f>
+        <v>0</v>
+      </c>
+      <c r="AA29" s="21">
+        <f>'generator_costs_04-08-2010'!AH29</f>
+        <v>0</v>
+      </c>
+      <c r="AB29" s="21">
+        <f>'generator_costs_04-08-2010'!AI29</f>
+        <v>0</v>
+      </c>
+      <c r="AC29" s="21">
+        <f>'generator_costs_04-08-2010'!AJ29</f>
+        <v>0</v>
+      </c>
+      <c r="AD29" s="21">
+        <f>'generator_costs_04-08-2010'!AK29</f>
+        <v>0</v>
+      </c>
+      <c r="AE29" s="21">
+        <f>'generator_costs_04-08-2010'!AL29</f>
+        <v>0</v>
+      </c>
+      <c r="AF29" s="21">
+        <f>'generator_costs_04-08-2010'!AM29</f>
+        <v>0</v>
+      </c>
+      <c r="AG29" s="21">
+        <f>'generator_costs_04-08-2010'!AN29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33">
+      <c r="A30" s="21">
+        <f>'generator_costs_04-08-2010'!A30</f>
+        <v>31</v>
+      </c>
+      <c r="B30" s="21" t="str">
+        <f>'generator_costs_04-08-2010'!B30</f>
+        <v>Gas_Steam_Turbine_Cogen_EP</v>
+      </c>
+      <c r="C30" s="21">
+        <f>'generator_costs_04-08-2010'!C30</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="21">
+        <f>'generator_costs_04-08-2010'!D30</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="21" t="str">
+        <f>'generator_costs_04-08-2010'!E30</f>
+        <v>Gas</v>
+      </c>
+      <c r="F30" s="21">
+        <f>'generator_costs_04-08-2010'!M30</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="21">
+        <f>'generator_costs_04-08-2010'!N30</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="21">
+        <f>'generator_costs_04-08-2010'!O30</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="21">
+        <f>'generator_costs_04-08-2010'!P30</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="21">
+        <f>'generator_costs_04-08-2010'!Q30</f>
+        <v>0</v>
+      </c>
+      <c r="K30" s="21">
+        <f>'generator_costs_04-08-2010'!R30</f>
+        <v>0</v>
+      </c>
+      <c r="L30" s="21">
+        <f>'generator_costs_04-08-2010'!S30</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="21">
+        <f>'generator_costs_04-08-2010'!T30</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="21">
+        <f>'generator_costs_04-08-2010'!U30</f>
+        <v>0</v>
+      </c>
+      <c r="O30" s="21">
+        <f>'generator_costs_04-08-2010'!V30</f>
+        <v>0</v>
+      </c>
+      <c r="P30" s="21">
+        <f>'generator_costs_04-08-2010'!W30</f>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="21">
+        <f>'generator_costs_04-08-2010'!X30</f>
+        <v>0</v>
+      </c>
+      <c r="R30" s="21">
+        <f>'generator_costs_04-08-2010'!Y30</f>
+        <v>0</v>
+      </c>
+      <c r="S30" s="21">
+        <f>'generator_costs_04-08-2010'!Z30</f>
+        <v>0</v>
+      </c>
+      <c r="T30" s="21">
+        <f>'generator_costs_04-08-2010'!AA30</f>
+        <v>0</v>
+      </c>
+      <c r="U30" s="21">
+        <f>'generator_costs_04-08-2010'!AB30</f>
+        <v>0</v>
+      </c>
+      <c r="V30" s="21">
+        <f>'generator_costs_04-08-2010'!AC30</f>
+        <v>0</v>
+      </c>
+      <c r="W30" s="21">
+        <f>'generator_costs_04-08-2010'!AD30</f>
+        <v>0</v>
+      </c>
+      <c r="X30" s="21">
+        <f>'generator_costs_04-08-2010'!AE30</f>
+        <v>0</v>
+      </c>
+      <c r="Y30" s="21">
+        <f>'generator_costs_04-08-2010'!AF30</f>
+        <v>0</v>
+      </c>
+      <c r="Z30" s="21">
+        <f>'generator_costs_04-08-2010'!AG30</f>
+        <v>0</v>
+      </c>
+      <c r="AA30" s="21">
+        <f>'generator_costs_04-08-2010'!AH30</f>
+        <v>0</v>
+      </c>
+      <c r="AB30" s="21">
+        <f>'generator_costs_04-08-2010'!AI30</f>
+        <v>0</v>
+      </c>
+      <c r="AC30" s="21">
+        <f>'generator_costs_04-08-2010'!AJ30</f>
+        <v>0</v>
+      </c>
+      <c r="AD30" s="21">
+        <f>'generator_costs_04-08-2010'!AK30</f>
+        <v>0</v>
+      </c>
+      <c r="AE30" s="21">
+        <f>'generator_costs_04-08-2010'!AL30</f>
+        <v>0</v>
+      </c>
+      <c r="AF30" s="21">
+        <f>'generator_costs_04-08-2010'!AM30</f>
+        <v>0</v>
+      </c>
+      <c r="AG30" s="21">
+        <f>'generator_costs_04-08-2010'!AN30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33">
+      <c r="A31" s="21">
+        <f>'generator_costs_04-08-2010'!A31</f>
+        <v>32</v>
+      </c>
+      <c r="B31" s="21" t="str">
+        <f>'generator_costs_04-08-2010'!B31</f>
+        <v>CCGT_Cogen_EP</v>
+      </c>
+      <c r="C31" s="21">
+        <f>'generator_costs_04-08-2010'!C31</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="21">
+        <f>'generator_costs_04-08-2010'!D31</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="21" t="str">
+        <f>'generator_costs_04-08-2010'!E31</f>
+        <v>Gas</v>
+      </c>
+      <c r="F31" s="21">
+        <f>'generator_costs_04-08-2010'!M31</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="21">
+        <f>'generator_costs_04-08-2010'!N31</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="21">
+        <f>'generator_costs_04-08-2010'!O31</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="21">
+        <f>'generator_costs_04-08-2010'!P31</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="21">
+        <f>'generator_costs_04-08-2010'!Q31</f>
+        <v>0</v>
+      </c>
+      <c r="K31" s="21">
+        <f>'generator_costs_04-08-2010'!R31</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="21">
+        <f>'generator_costs_04-08-2010'!S31</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="21">
+        <f>'generator_costs_04-08-2010'!T31</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="21">
+        <f>'generator_costs_04-08-2010'!U31</f>
+        <v>0</v>
+      </c>
+      <c r="O31" s="21">
+        <f>'generator_costs_04-08-2010'!V31</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="21">
+        <f>'generator_costs_04-08-2010'!W31</f>
+        <v>0</v>
+      </c>
+      <c r="Q31" s="21">
+        <f>'generator_costs_04-08-2010'!X31</f>
+        <v>0</v>
+      </c>
+      <c r="R31" s="21">
+        <f>'generator_costs_04-08-2010'!Y31</f>
+        <v>0</v>
+      </c>
+      <c r="S31" s="21">
+        <f>'generator_costs_04-08-2010'!Z31</f>
+        <v>0</v>
+      </c>
+      <c r="T31" s="21">
+        <f>'generator_costs_04-08-2010'!AA31</f>
+        <v>0</v>
+      </c>
+      <c r="U31" s="21">
+        <f>'generator_costs_04-08-2010'!AB31</f>
+        <v>0</v>
+      </c>
+      <c r="V31" s="21">
+        <f>'generator_costs_04-08-2010'!AC31</f>
+        <v>0</v>
+      </c>
+      <c r="W31" s="21">
+        <f>'generator_costs_04-08-2010'!AD31</f>
+        <v>0</v>
+      </c>
+      <c r="X31" s="21">
+        <f>'generator_costs_04-08-2010'!AE31</f>
+        <v>0</v>
+      </c>
+      <c r="Y31" s="21">
+        <f>'generator_costs_04-08-2010'!AF31</f>
+        <v>0</v>
+      </c>
+      <c r="Z31" s="21">
+        <f>'generator_costs_04-08-2010'!AG31</f>
+        <v>0</v>
+      </c>
+      <c r="AA31" s="21">
+        <f>'generator_costs_04-08-2010'!AH31</f>
+        <v>0</v>
+      </c>
+      <c r="AB31" s="21">
+        <f>'generator_costs_04-08-2010'!AI31</f>
+        <v>0</v>
+      </c>
+      <c r="AC31" s="21">
+        <f>'generator_costs_04-08-2010'!AJ31</f>
+        <v>0</v>
+      </c>
+      <c r="AD31" s="21">
+        <f>'generator_costs_04-08-2010'!AK31</f>
+        <v>0</v>
+      </c>
+      <c r="AE31" s="21">
+        <f>'generator_costs_04-08-2010'!AL31</f>
+        <v>0</v>
+      </c>
+      <c r="AF31" s="21">
+        <f>'generator_costs_04-08-2010'!AM31</f>
+        <v>0</v>
+      </c>
+      <c r="AG31" s="21">
+        <f>'generator_costs_04-08-2010'!AN31</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -9186,24 +9806,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added compressed air energy storage
Updated geothermal lifetimes

Changed how construction costs are paid for

Updated pumped hydro efficiency

Finished intermittent project subsampling (TOY)

*bug: infeasible transmission optimization, see previous versions(?)*
</commit_message>
<xml_diff>
--- a/DatabasePrep/GeneratorInfo/generator_costs.xlsx
+++ b/DatabasePrep/GeneratorInfo/generator_costs.xlsx
@@ -23,6 +23,236 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="107">
   <si>
+    <t>heat_rate_mbtu_per_mwh</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commercial_PV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>min_build_year</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>min_dispatch_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>min_runtime_hours</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>min_downtime_hours</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_Cogen_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_Cogen_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Steam_Turbine_Cogen_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCGT_Cogen_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Uranium</t>
+  </si>
+  <si>
+    <t>DOE Solar Program Costs, took 2020 value for fixed O+M, 10% added to capital costs to go from utility to distributed, but also assumed a 5% declination rate, , outage rates from Mathias</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>overnight_cost</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Solar</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Solid</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Uranium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>interest_between_price_year_and_cost_year</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Residential_PV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Geothermal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compressed_Air_Energy_Storage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>source - all dispatch data from TEPPC_Generator_Categories</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>technology_id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_age_years</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Solar</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Gas</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, assumed to run for 40 years, not 60</t>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine</t>
+  </si>
+  <si>
+    <t>Nuclear</t>
+  </si>
+  <si>
+    <t>Geothermal</t>
+  </si>
+  <si>
+    <t>tech_name_again</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Steam_Turbine_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nuclear_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CapEx from SAM with Solar Field area = 600000m^2, construction cost mulitplier and yearly cost fraction from ReEDs sheet, cost declination rate and fixed OM from DOE solar program costs on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, EIA says minimum learning by 2025 is 20%, so this is a 1.1% declination rate, capital cost multipulier from EIA,http://graysharboroceanenergy.com/Documents/LIPA%20Offshore%20Wind%20rept.pdf for total outage rate of 3%, distributed by guess</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cost Declination Rate (%/yr)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resultant Capital Costs ($2007/MW) in Investment Period Years</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to gas combustion turbine</t>
+  </si>
+  <si>
+    <t>Geothermal_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCGT_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_4_cost_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_5_cost_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_6_cost_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, cost declination rate assumed to be between ST and other techs (@1%).  EIA has minimum learning by 2025 as 10%, so this is roughly consistent</t>
+  </si>
+  <si>
+    <t>storage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Offshore_Wind</t>
+  </si>
+  <si>
+    <t>Bio_Gas</t>
+  </si>
+  <si>
+    <t>year_1_cost_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_2_cost_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_3_cost_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CapEx from SAM with Solar Field area = 800000m^2 and 6h TES, construction cost mulitplier and yearly cost fraction from CSP on ReEDs sheet- it's unclear how much these change with storage... assumed to be the same here, cost declination rate and fixed OM from Mark Mehos estimate on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSP_Trough_No_Storage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSP_Trough_6h_Storage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, outage rates from Mathias</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -188,248 +418,13 @@
   </si>
   <si>
     <t>can_build_new</t>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nuclear_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CapEx from SAM with Solar Field area = 600000m^2, construction cost mulitplier and yearly cost fraction from ReEDs sheet, cost declination rate and fixed OM from DOE solar program costs on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, EIA says minimum learning by 2025 is 20%, so this is a 1.1% declination rate, capital cost multipulier from EIA,http://graysharboroceanenergy.com/Documents/LIPA%20Offshore%20Wind%20rept.pdf for total outage rate of 3%, distributed by guess</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cost Declination Rate (%/yr)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resultant Capital Costs ($2007/MW) in Investment Period Years</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to gas combustion turbine</t>
-  </si>
-  <si>
-    <t>Geothermal_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCGT_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wind_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wind</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_4_cost_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_5_cost_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_6_cost_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, cost declination rate assumed to be between ST and other techs (@1%).  EIA has minimum learning by 2025 as 10%, so this is roughly consistent</t>
-  </si>
-  <si>
-    <t>storage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Offshore_Wind</t>
-  </si>
-  <si>
-    <t>Bio_Gas</t>
-  </si>
-  <si>
-    <t>year_1_cost_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_2_cost_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_3_cost_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CapEx from SAM with Solar Field area = 800000m^2 and 6h TES, construction cost mulitplier and yearly cost fraction from CSP on ReEDs sheet- it's unclear how much these change with storage... assumed to be the same here, cost declination rate and fixed OM from Mark Mehos estimate on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSP_Trough_No_Storage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSP_Trough_6h_Storage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>heat_rate_mbtu_per_mwh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Commercial_PV</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>min_build_year</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>min_dispatch_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>min_runtime_hours</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>min_downtime_hours</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine_Cogen_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_Cogen_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_Cogen_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCGT_Cogen_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal</t>
-  </si>
-  <si>
-    <t>Uranium</t>
-  </si>
-  <si>
-    <t>DOE Solar Program Costs, took 2020 value for fixed O+M, 10% added to capital costs to go from utility to distributed, but also assumed a 5% declination rate, , outage rates from Mathias</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>overnight_cost</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Solar</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bio_Solid</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Uranium</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>interest_between_price_year_and_cost_year</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Residential_PV</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Geothermal</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Compressed_Air_Energy_Storage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>source - all dispatch data from TEPPC_Generator_Categories</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>technology_id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_age_years</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Solar</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bio_Gas</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, assumed to run for 40 years, not 60</t>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine</t>
-  </si>
-  <si>
-    <t>Nuclear</t>
-  </si>
-  <si>
-    <t>Geothermal</t>
-  </si>
-  <si>
-    <t>tech_name_again</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3">
@@ -1423,11 +1418,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="490389656"/>
-        <c:axId val="490398760"/>
+        <c:axId val="654756952"/>
+        <c:axId val="654766056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="490389656"/>
+        <c:axId val="654756952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1448,7 +1443,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -1462,14 +1456,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="490398760"/>
+        <c:crossAx val="654766056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="490398760"/>
+        <c:axId val="654766056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="7.0"/>
@@ -1492,7 +1486,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
@@ -1506,7 +1499,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="490389656"/>
+        <c:crossAx val="654756952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1894,7 +1887,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane xSplit="2" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T19" sqref="T19"/>
+      <selection pane="topRight" activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1925,130 +1918,130 @@
   <sheetData>
     <row r="1" spans="1:42">
       <c r="A1" s="5" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="D1" t="s">
-        <v>76</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="G1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" t="s">
+        <v>83</v>
+      </c>
+      <c r="P1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>87</v>
+      </c>
+      <c r="R1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" t="s">
+        <v>84</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>92</v>
       </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="AK1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AN1" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP1" t="s">
         <v>23</v>
-      </c>
-      <c r="P1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R1" t="s">
-        <v>74</v>
-      </c>
-      <c r="S1" t="s">
-        <v>24</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AN1" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="AO1" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:42">
@@ -2056,7 +2049,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="C2" s="5">
         <v>2007</v>
@@ -2065,7 +2058,7 @@
         <v>2010</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="F2">
         <v>2004</v>
@@ -2180,7 +2173,7 @@
         <v>CCGT</v>
       </c>
       <c r="AP2" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:42">
@@ -2188,7 +2181,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C3" s="5">
         <v>2007</v>
@@ -2197,7 +2190,7 @@
         <v>2010</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="F3">
         <v>2004</v>
@@ -2312,7 +2305,7 @@
         <v>Gas_Combustion_Turbine</v>
       </c>
       <c r="AP3" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:42">
@@ -2320,7 +2313,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="C4" s="5">
         <v>2007</v>
@@ -2329,7 +2322,7 @@
         <v>2010</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="F4">
         <v>2004</v>
@@ -2444,7 +2437,7 @@
         <v>Wind</v>
       </c>
       <c r="AP4" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:42">
@@ -2452,7 +2445,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C5" s="5">
         <v>2007</v>
@@ -2461,7 +2454,7 @@
         <v>2010</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="F5">
         <v>2004</v>
@@ -2576,7 +2569,7 @@
         <v>Offshore_Wind</v>
       </c>
       <c r="AP5" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:42">
@@ -2584,7 +2577,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>93</v>
+        <v>19</v>
       </c>
       <c r="C6" s="5">
         <v>2007</v>
@@ -2593,7 +2586,7 @@
         <v>2010</v>
       </c>
       <c r="E6" t="s">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="F6">
         <v>2009</v>
@@ -2709,7 +2702,7 @@
         <v>Residential_PV</v>
       </c>
       <c r="AP6" t="s">
-        <v>86</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:42" s="11" customFormat="1">
@@ -2717,7 +2710,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C7" s="11">
         <v>2007</v>
@@ -2726,7 +2719,7 @@
         <v>2012</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="F7" s="11">
         <v>2010</v>
@@ -2837,10 +2830,10 @@
         <v>0</v>
       </c>
       <c r="AO7" s="11" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="AP7" s="11" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:42">
@@ -2848,7 +2841,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C8" s="5">
         <v>2007</v>
@@ -2857,7 +2850,7 @@
         <v>2010</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="F8">
         <v>2007</v>
@@ -2972,7 +2965,7 @@
         <v>Bio_Gas</v>
       </c>
       <c r="AP8" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:42">
@@ -2980,7 +2973,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="C9" s="5">
         <v>2007</v>
@@ -2989,7 +2982,7 @@
         <v>2010</v>
       </c>
       <c r="E9" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="F9">
         <v>2004</v>
@@ -3104,7 +3097,7 @@
         <v>Biomass_Steam_Turbine</v>
       </c>
       <c r="AP9" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:42">
@@ -3112,7 +3105,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="C10" s="5">
         <v>2007</v>
@@ -3121,7 +3114,7 @@
         <v>2012</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="F10">
         <v>2007</v>
@@ -3236,7 +3229,7 @@
         <v>Biomass_IGCC</v>
       </c>
       <c r="AP10" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:42">
@@ -3244,7 +3237,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C11" s="5">
         <v>2007</v>
@@ -3253,7 +3246,7 @@
         <v>2010</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="F11">
         <v>2004</v>
@@ -3368,7 +3361,7 @@
         <v>Coal_IGCC</v>
       </c>
       <c r="AP11" t="s">
-        <v>102</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:42">
@@ -3376,7 +3369,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="C12" s="5">
         <v>2007</v>
@@ -3385,7 +3378,7 @@
         <v>2010</v>
       </c>
       <c r="E12" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="F12">
         <v>2004</v>
@@ -3500,7 +3493,7 @@
         <v>Coal_Steam_Turbine</v>
       </c>
       <c r="AP12" t="s">
-        <v>102</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:42">
@@ -3508,7 +3501,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="C13" s="5">
         <v>2007</v>
@@ -3517,7 +3510,7 @@
         <v>2010</v>
       </c>
       <c r="E13" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="F13">
         <v>2004</v>
@@ -3632,7 +3625,7 @@
         <v>Nuclear</v>
       </c>
       <c r="AP13" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:42">
@@ -3640,7 +3633,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>105</v>
+        <v>31</v>
       </c>
       <c r="C14" s="5">
         <v>2007</v>
@@ -3649,7 +3642,7 @@
         <v>2010</v>
       </c>
       <c r="E14" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="F14">
         <v>2004</v>
@@ -3715,7 +3708,7 @@
         <v>0</v>
       </c>
       <c r="Z14">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="AA14">
         <v>7.4999999999999997E-3</v>
@@ -3764,7 +3757,7 @@
         <v>Geothermal</v>
       </c>
       <c r="AP14" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:42">
@@ -3772,7 +3765,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="C15" s="5">
         <v>2007</v>
@@ -3781,7 +3774,7 @@
         <v>2010</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="F15" s="5">
         <v>2004</v>
@@ -3896,7 +3889,7 @@
         <v>Hydro_NonPumped</v>
       </c>
       <c r="AP15" s="5" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:42">
@@ -3904,7 +3897,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="C16" s="5">
         <v>2007</v>
@@ -3913,7 +3906,7 @@
         <v>2010</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="F16" s="5">
         <v>2004</v>
@@ -4028,7 +4021,7 @@
         <v>Hydro_Pumped</v>
       </c>
       <c r="AP16" s="5" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:42" s="18" customFormat="1">
@@ -4036,10 +4029,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="S17" s="22">
         <v>3</v>
@@ -4074,12 +4067,12 @@
         <v>18</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="G18" s="11"/>
       <c r="M18" s="11"/>
@@ -4118,12 +4111,12 @@
         <v>19</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="G19" s="11"/>
       <c r="M19" s="11"/>
@@ -4162,12 +4155,12 @@
         <v>20</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="G20" s="11"/>
       <c r="M20" s="11"/>
@@ -4206,12 +4199,12 @@
         <v>21</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21"/>
       <c r="E21" t="s">
-        <v>105</v>
+        <v>31</v>
       </c>
       <c r="G21" s="11"/>
       <c r="M21" s="11"/>
@@ -4250,12 +4243,12 @@
         <v>22</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C22"/>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="G22" s="11"/>
       <c r="M22" s="11"/>
@@ -4294,10 +4287,10 @@
         <v>23</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="S23" s="22">
         <v>3</v>
@@ -4332,7 +4325,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>75</v>
+        <v>1</v>
       </c>
       <c r="C24" s="8">
         <v>2007</v>
@@ -4341,7 +4334,7 @@
         <v>2010</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="F24" s="8">
         <v>2009</v>
@@ -4452,10 +4445,10 @@
         <v>0</v>
       </c>
       <c r="AO24" s="9" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="AP24" s="9" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:42" s="8" customFormat="1">
@@ -4463,7 +4456,7 @@
         <v>26</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C25" s="8">
         <v>2007</v>
@@ -4472,7 +4465,7 @@
         <v>2010</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="F25" s="8">
         <v>2009</v>
@@ -4583,10 +4576,10 @@
         <v>0</v>
       </c>
       <c r="AO25" s="9" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="AP25" s="9" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:42" s="5" customFormat="1">
@@ -4594,7 +4587,7 @@
         <v>27</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C26" s="5">
         <v>2007</v>
@@ -4603,7 +4596,7 @@
         <v>2010</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="F26" s="5">
         <v>2010</v>
@@ -4714,10 +4707,10 @@
         <v>0</v>
       </c>
       <c r="AO26" s="9" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="AP26" s="9" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:42" s="9" customFormat="1">
@@ -4725,7 +4718,7 @@
         <v>28</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>95</v>
+        <v>21</v>
       </c>
       <c r="C27" s="9">
         <v>2007</v>
@@ -4734,7 +4727,7 @@
         <v>2010</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="F27" s="9">
         <v>2010</v>
@@ -4845,10 +4838,10 @@
         <v>1</v>
       </c>
       <c r="AO27" s="14" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="AP27" s="14" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:42" s="21" customFormat="1">
@@ -4856,10 +4849,10 @@
         <v>29</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="S28" s="22">
         <v>3</v>
@@ -4894,10 +4887,10 @@
         <v>30</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="S29" s="22">
         <v>4</v>
@@ -4932,10 +4925,10 @@
         <v>31</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="S30" s="22">
         <v>3</v>
@@ -4970,10 +4963,10 @@
         <v>32</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="S31" s="22">
         <v>3</v>
@@ -5010,12 +5003,12 @@
     </row>
     <row r="33" spans="1:25" s="6" customFormat="1">
       <c r="A33" s="6" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:25">
       <c r="A34" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="B34">
         <v>2010</v>
@@ -5033,7 +5026,7 @@
         <v>2026</v>
       </c>
       <c r="G34" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="S34" s="5"/>
       <c r="Y34"/>
@@ -7694,7 +7687,7 @@
       </c>
       <c r="S14" s="11">
         <f>'generator_costs_04-08-2010'!Z14</f>
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="T14" s="11">
         <f>'generator_costs_04-08-2010'!AA14</f>

</xml_diff>

<commit_message>
- Added a carbon cap - Added units and carbon cap printouts to basicstats - Fixed biomass resource potentials and constrained biomass CCS to these potentials - Made the CCS min build year to be 2014 - Changed the export of proposed_projects.tab to eliminate less promising renewable sites, included wind in this selection - Added battery storage - Fixed a bug in run_switch.sh that didn't print out basicstats or record_results
</commit_message>
<xml_diff>
--- a/DatabasePrep/GeneratorInfo/generator_costs.xlsx
+++ b/DatabasePrep/GeneratorInfo/generator_costs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="-80" windowWidth="34700" windowHeight="19300" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="540" yWindow="-80" windowWidth="23960" windowHeight="15880" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Chart_revise" sheetId="4" r:id="rId1"/>
@@ -24,42 +24,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="138">
   <si>
-    <t>Wind</t>
+    <t>Bio_Solid_CCS</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>price_and_dollar_year</t>
+    <t>DOE Solar Program Costs, took 2020 value for fixed O+M, 10% added to capital costs to go from utility to distributed, but also assumed a 5% declination rate, , outage rates from Mathias</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Gas</t>
-  </si>
-  <si>
-    <t>year_4_cost_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_5_cost_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_6_cost_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, EIA says minimum learning by 2025 is 20%, so this is a 1.1% declination rate, capital cost multipulier from EIA,http://graysharboroceanenergy.com/Documents/LIPA%20Offshore%20Wind%20rept.pdf for total outage rate of 3%, distributed by guess</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cost Declination Rate (%/yr)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resultant Capital Costs ($2007/MW) in Investment Period Years</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Concentrating_PV</t>
+    <t>overnight_cost</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -67,261 +40,23 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>(in 2010 $)</t>
+    <t>Bio_Solid</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>year</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>Gas_Combustion_Turbine_EP</t>
   </si>
   <si>
-    <t>$/Wp</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>Coal_Steam_Turbine_EP</t>
   </si>
   <si>
-    <t>CPV Consortium numbers (It's more or less SolFocus)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>Gas_Steam_Turbine_EP</t>
   </si>
   <si>
-    <t>cost declination rate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CapEx from SAM with Solar Field area = 800000m^2 and 6h TES, construction cost mulitplier and yearly cost fraction from CSP on ReEDs sheet- it's unclear how much these change with storage... assumed to be the same here, cost declination rate and fixed OM from Mark Mehos estimate on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSP_Trough_No_Storage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSP_Trough_6h_Storage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wind</t>
-  </si>
-  <si>
-    <t>Central_PV</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>construction_cost_multipulier</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed_o_m</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var_o_m</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>overnight_cost_$2007</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed_o_m_$2007</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>heat_rate_mbtu_per_mwh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Commercial_PV</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>min_build_year</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>CCGT_EP</t>
   </si>
   <si>
     <t>Gas_Combustion_Turbine_Cogen_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_Cogen_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_Cogen_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCGT_Cogen_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal</t>
-  </si>
-  <si>
-    <t>Uranium</t>
-  </si>
-  <si>
-    <t>storage_efficiency</t>
-  </si>
-  <si>
-    <t>max_store_rate</t>
-  </si>
-  <si>
-    <t>ccs</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Uranium</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var_o_m_$2007</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>construction_time_years</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>forced_outage_rate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>scheduled_outage_rate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>connect_cost_generic_$2007_per_mw</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>fuel</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_CCS_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_CCS_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Solar Vision Study (see PV_Cost_Calc.xlsx) for costs, ReEDs sheet for construction cost multiplier and cost fractions, Matthias for forced outage rate </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>interest_between_price_year_and_cost_year</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Residential_PV</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Geothermal</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Compressed_Air_Energy_Storage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>source - all dispatch data from TEPPC_Generator_Categories</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>technology_id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_age_years</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Solar</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bio_Gas</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, assumed to run for 40 years, not 60</t>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine</t>
-  </si>
-  <si>
-    <t>Nuclear</t>
-  </si>
-  <si>
-    <t>Geothermal</t>
-  </si>
-  <si>
-    <t>tech_name_again</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nuclear_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet; also Sullivan et al (2008), NREL/CP-670-43510 Conference Paper for o&amp;m costs, declanation rate, etc; $1,200,000 taken as capital cost in 2010 rather than 2004 based on conversation with Hernandez</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biomass_Steam_Turbine</t>
-  </si>
-  <si>
-    <t>Hydro_NonPumped</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hydro_Pumped</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Water</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Water</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, cost declination rate assumed to be that of a gas steam turbine</t>
-  </si>
-  <si>
-    <t>Biomass_IGCC</t>
-  </si>
-  <si>
-    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to coal IGCC</t>
-  </si>
-  <si>
-    <t>Coal_IGCC</t>
-  </si>
-  <si>
-    <t>can_build_new</t>
   </si>
   <si>
     <t>CapEx from SAM with Solar Field area = 600000m^2, construction cost mulitplier and yearly cost fraction from ReEDs sheet, cost declination rate and fixed OM from DOE solar program costs on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
@@ -335,15 +70,10 @@
     <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to gas combustion turbine</t>
   </si>
   <si>
-    <t>Geothermal_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>CCGT_Cogen_EP</t>
   </si>
   <si>
-    <t>CCGT_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine_EP</t>
+    <t>Gas_Combustion_Turbine_CCS_EP</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -489,39 +219,72 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Bio_Solid_CCS</t>
+    <t>overnight_cost_$2007</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>DOE Solar Program Costs, took 2020 value for fixed O+M, 10% added to capital costs to go from utility to distributed, but also assumed a 5% declination rate, , outage rates from Mathias</t>
+    <t>fixed_o_m_$2007</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>overnight_cost</t>
+    <t>heat_rate_mbtu_per_mwh</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Solar</t>
+    <t>Commercial_PV</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Bio_Solid</t>
+    <t>min_build_year</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Gas_Combustion_Turbine_EP</t>
+    <t>Gas_Combustion_Turbine_Cogen_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Coal_Steam_Turbine_EP</t>
+    <t>Coal_Steam_Turbine_Cogen_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Gas_Steam_Turbine_EP</t>
+    <t>Gas_Steam_Turbine_Cogen_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>CCGT_EP</t>
+    <t>CCGT_Cogen_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Gas_Combustion_Turbine_Cogen_EP</t>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Uranium</t>
+  </si>
+  <si>
+    <t>storage_efficiency</t>
+  </si>
+  <si>
+    <t>max_store_rate</t>
+  </si>
+  <si>
+    <t>ccs</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Uranium</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var_o_m_$2007</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>construction_time_years</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Coal_Steam_Turbine_Cogen_EP</t>
@@ -530,10 +293,248 @@
     <t>Gas_Steam_Turbine_Cogen_EP</t>
   </si>
   <si>
-    <t>CCGT_Cogen_EP</t>
+    <t>connect_cost_generic_$2007_per_mw</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Gas_Combustion_Turbine_CCS_EP</t>
+    <t>fuel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_CCS_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Steam_Turbine_CCS_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Solar Vision Study (see PV_Cost_Calc.xlsx) for costs, ReEDs sheet for construction cost multiplier and cost fractions, Matthias for forced outage rate </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>interest_between_price_year_and_cost_year</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Residential_PV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Geothermal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compressed_Air_Energy_Storage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>source - all dispatch data from TEPPC_Generator_Categories</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>technology_id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_age_years</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Solar</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Gas</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, assumed to run for 40 years, not 60</t>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine</t>
+  </si>
+  <si>
+    <t>Nuclear</t>
+  </si>
+  <si>
+    <t>Geothermal</t>
+  </si>
+  <si>
+    <t>tech_name_again</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Steam_Turbine_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nuclear_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biomass_Steam_Turbine</t>
+  </si>
+  <si>
+    <t>Hydro_NonPumped</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hydro_Pumped</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Water</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Water</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, cost declination rate assumed to be that of a gas steam turbine</t>
+  </si>
+  <si>
+    <t>Biomass_IGCC</t>
+  </si>
+  <si>
+    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to coal IGCC</t>
+  </si>
+  <si>
+    <t>Coal_IGCC</t>
+  </si>
+  <si>
+    <t>can_build_new</t>
+  </si>
+  <si>
+    <t>forced_outage_rate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>scheduled_outage_rate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ReEDs Sheet; also Sullivan et al (2008), NREL/CP-670-43510 Conference Paper for o&amp;m costs, declanation rate, etc; $1,200,000 taken as capital cost in 2010 rather than 2004 based on conversation with Hernandez, also The storage efficiency of the the storage phase of compressed air energy storage from Samir Succar and Robert H. Williams: Compressed Air Energy Storage: Theory, Resources, And Applications For Wind Power, p. 39
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Geothermal_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCGT_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>price_and_dollar_year</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>year_4_cost_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_5_cost_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_6_cost_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, EIA says minimum learning by 2025 is 20%, so this is a 1.1% declination rate, capital cost multipulier from EIA,http://graysharboroceanenergy.com/Documents/LIPA%20Offshore%20Wind%20rept.pdf for total outage rate of 3%, distributed by guess</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cost Declination Rate (%/yr)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resultant Capital Costs ($2007/MW) in Investment Period Years</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Concentrating_PV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Solar</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(in 2010 $)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>year</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$/Wp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPV Consortium numbers (It's more or less SolFocus)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cost declination rate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CapEx from SAM with Solar Field area = 800000m^2 and 6h TES, construction cost mulitplier and yearly cost fraction from CSP on ReEDs sheet- it's unclear how much these change with storage... assumed to be the same here, cost declination rate and fixed OM from Mark Mehos estimate on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSP_Trough_No_Storage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSP_Trough_6h_Storage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Central_PV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>construction_cost_multipulier</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed_o_m</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var_o_m</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -541,15 +542,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  <numFmts count="6">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -586,10 +585,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -613,13 +612,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1528,11 +1532,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="96269096"/>
-        <c:axId val="96066872"/>
+        <c:axId val="95933544"/>
+        <c:axId val="96260568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96269096"/>
+        <c:axId val="95933544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1566,14 +1570,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96066872"/>
+        <c:crossAx val="96260568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96066872"/>
+        <c:axId val="96260568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="7.0"/>
@@ -1609,7 +1613,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96269096"/>
+        <c:crossAx val="95933544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1995,9 +1999,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:AM90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="125" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q41" sqref="Q41:Q48"/>
+    <sheetView topLeftCell="A17" zoomScale="125" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D34" sqref="D34:D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2028,121 +2032,121 @@
   <sheetData>
     <row r="1" spans="1:39">
       <c r="A1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>135</v>
+      </c>
+      <c r="K1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L1" t="s">
+        <v>137</v>
+      </c>
+      <c r="M1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="S1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I1" t="s">
-        <v>126</v>
-      </c>
-      <c r="J1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="V1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH1" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="N1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P1" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH1" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI1" s="15" t="s">
+      <c r="AJ1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL1" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="AJ1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL1" s="12" t="s">
-        <v>64</v>
-      </c>
       <c r="AM1" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:39">
@@ -2150,7 +2154,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>43</v>
       </c>
       <c r="C2" s="5">
         <v>2007</v>
@@ -2159,7 +2163,7 @@
         <v>2010</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="F2">
         <v>2004</v>
@@ -2265,7 +2269,7 @@
         <v>CCGT</v>
       </c>
       <c r="AM2" t="s">
-        <v>114</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:39">
@@ -2273,7 +2277,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="C3" s="5">
         <v>2007</v>
@@ -2282,7 +2286,7 @@
         <v>2010</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="F3">
         <v>2004</v>
@@ -2388,7 +2392,7 @@
         <v>Gas_Combustion_Turbine</v>
       </c>
       <c r="AM3" t="s">
-        <v>114</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:39" s="24" customFormat="1">
@@ -2396,7 +2400,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="C4" s="24">
         <v>2007</v>
@@ -2405,7 +2409,7 @@
         <v>2010</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>10</v>
+        <v>124</v>
       </c>
       <c r="F4" s="24">
         <v>2010</v>
@@ -2512,7 +2516,7 @@
         <v>Concentrating_PV</v>
       </c>
       <c r="AM4" s="24" t="s">
-        <v>14</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:39">
@@ -2520,7 +2524,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="C5" s="5">
         <v>2007</v>
@@ -2529,7 +2533,7 @@
         <v>2010</v>
       </c>
       <c r="E5" t="s">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="F5">
         <v>2004</v>
@@ -2635,7 +2639,7 @@
         <v>Wind</v>
       </c>
       <c r="AM5" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:39">
@@ -2643,7 +2647,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="C6" s="5">
         <v>2007</v>
@@ -2652,7 +2656,7 @@
         <v>2010</v>
       </c>
       <c r="E6" t="s">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="F6">
         <v>2004</v>
@@ -2758,7 +2762,7 @@
         <v>Offshore_Wind</v>
       </c>
       <c r="AM6" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:39">
@@ -2766,7 +2770,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="C7" s="5">
         <v>2007</v>
@@ -2775,7 +2779,7 @@
         <v>2010</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="F7">
         <v>2009</v>
@@ -2882,7 +2886,7 @@
         <v>Residential_PV</v>
       </c>
       <c r="AM7" t="s">
-        <v>125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:39" s="11" customFormat="1">
@@ -2890,7 +2894,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>18</v>
+        <v>132</v>
       </c>
       <c r="C8" s="11">
         <v>2007</v>
@@ -2899,7 +2903,7 @@
         <v>2012</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>127</v>
+        <v>3</v>
       </c>
       <c r="F8" s="11">
         <v>2010</v>
@@ -3005,7 +3009,7 @@
         <v>CSP_Trough_6h_Storage</v>
       </c>
       <c r="AM8" s="11" t="s">
-        <v>16</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:39">
@@ -3013,7 +3017,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>26</v>
       </c>
       <c r="C9" s="5">
         <v>2007</v>
@@ -3022,7 +3026,7 @@
         <v>2010</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="F9">
         <v>2007</v>
@@ -3128,7 +3132,7 @@
         <v>Bio_Gas</v>
       </c>
       <c r="AM9" t="s">
-        <v>81</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:39">
@@ -3136,7 +3140,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="C10" s="5">
         <v>2007</v>
@@ -3145,7 +3149,7 @@
         <v>2010</v>
       </c>
       <c r="E10" t="s">
-        <v>128</v>
+        <v>4</v>
       </c>
       <c r="F10">
         <v>2004</v>
@@ -3251,7 +3255,7 @@
         <v>Biomass_Steam_Turbine</v>
       </c>
       <c r="AM10" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:39">
@@ -3259,7 +3263,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="C11" s="5">
         <v>2007</v>
@@ -3268,7 +3272,7 @@
         <v>2012</v>
       </c>
       <c r="E11" t="s">
-        <v>128</v>
+        <v>4</v>
       </c>
       <c r="F11">
         <v>2007</v>
@@ -3374,7 +3378,7 @@
         <v>Biomass_IGCC</v>
       </c>
       <c r="AM11" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:39">
@@ -3382,7 +3386,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="C12" s="5">
         <v>2007</v>
@@ -3391,7 +3395,7 @@
         <v>2010</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="F12">
         <v>2004</v>
@@ -3497,7 +3501,7 @@
         <v>Coal_IGCC</v>
       </c>
       <c r="AM12" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:39">
@@ -3505,7 +3509,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="C13" s="5">
         <v>2007</v>
@@ -3514,7 +3518,7 @@
         <v>2010</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="F13">
         <v>2004</v>
@@ -3620,7 +3624,7 @@
         <v>Coal_Steam_Turbine</v>
       </c>
       <c r="AM13" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:39">
@@ -3628,7 +3632,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="C14" s="5">
         <v>2007</v>
@@ -3637,7 +3641,7 @@
         <v>2010</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="F14">
         <v>2004</v>
@@ -3743,7 +3747,7 @@
         <v>Nuclear</v>
       </c>
       <c r="AM14" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:39">
@@ -3751,7 +3755,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="C15" s="5">
         <v>2007</v>
@@ -3760,7 +3764,7 @@
         <v>2010</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="F15">
         <v>2004</v>
@@ -3866,7 +3870,7 @@
         <v>Geothermal</v>
       </c>
       <c r="AM15" t="s">
-        <v>93</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:39">
@@ -3874,7 +3878,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="C16" s="5">
         <v>2007</v>
@@ -3883,7 +3887,7 @@
         <v>2010</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="F16" s="5">
         <v>2004</v>
@@ -3989,7 +3993,7 @@
         <v>Hydro_NonPumped</v>
       </c>
       <c r="AM16" s="5" t="s">
-        <v>114</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:39">
@@ -3997,7 +4001,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="C17" s="5">
         <v>2007</v>
@@ -4006,7 +4010,7 @@
         <v>2010</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="F17" s="5">
         <v>2004</v>
@@ -4112,7 +4116,7 @@
         <v>Hydro_Pumped</v>
       </c>
       <c r="AM17" s="5" t="s">
-        <v>114</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:39" s="18" customFormat="1">
@@ -4120,10 +4124,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="M18" s="23"/>
       <c r="S18" s="22">
@@ -4172,12 +4176,12 @@
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="G19" s="11"/>
       <c r="M19" s="23"/>
@@ -4229,12 +4233,12 @@
         <v>19</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>2</v>
+        <v>116</v>
       </c>
       <c r="G20" s="11"/>
       <c r="M20" s="23"/>
@@ -4286,12 +4290,12 @@
         <v>20</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21" t="s">
-        <v>2</v>
+        <v>116</v>
       </c>
       <c r="G21" s="11"/>
       <c r="M21" s="23"/>
@@ -4342,13 +4346,13 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" s="33"/>
+      <c r="B22" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="36"/>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="G22" s="11"/>
       <c r="M22" s="23"/>
@@ -4400,12 +4404,12 @@
         <v>22</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="G23" s="11"/>
       <c r="M23" s="23"/>
@@ -4457,10 +4461,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="M24" s="23"/>
       <c r="S24" s="22">
@@ -4509,7 +4513,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="C25" s="8">
         <v>2007</v>
@@ -4518,7 +4522,7 @@
         <v>2010</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>127</v>
+        <v>3</v>
       </c>
       <c r="F25" s="8">
         <v>2009</v>
@@ -4624,7 +4628,7 @@
         <v>Commercial_PV</v>
       </c>
       <c r="AM25" s="9" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:39" s="8" customFormat="1">
@@ -4632,7 +4636,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>20</v>
+        <v>134</v>
       </c>
       <c r="C26" s="8">
         <v>2007</v>
@@ -4641,7 +4645,7 @@
         <v>2010</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>127</v>
+        <v>3</v>
       </c>
       <c r="F26" s="8">
         <v>2009</v>
@@ -4747,7 +4751,7 @@
         <v>Central_PV</v>
       </c>
       <c r="AM26" s="9" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:39" s="5" customFormat="1">
@@ -4755,7 +4759,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>17</v>
+        <v>131</v>
       </c>
       <c r="C27" s="5">
         <v>2007</v>
@@ -4764,7 +4768,7 @@
         <v>2010</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>127</v>
+        <v>3</v>
       </c>
       <c r="F27" s="5">
         <v>2010</v>
@@ -4870,15 +4874,15 @@
         <v>CSP_Trough_No_Storage</v>
       </c>
       <c r="AM27" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:39" s="9" customFormat="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A28" s="10">
         <v>28</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="C28" s="9">
         <v>2007</v>
@@ -4887,7 +4891,7 @@
         <v>2010</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="F28" s="9">
         <v>2010</v>
@@ -4992,8 +4996,8 @@
         <f t="shared" si="3"/>
         <v>Compressed_Air_Energy_Storage</v>
       </c>
-      <c r="AM28" s="14" t="s">
-        <v>68</v>
+      <c r="AM28" s="35" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:39" s="21" customFormat="1">
@@ -5001,10 +5005,10 @@
         <v>29</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="M29" s="25"/>
       <c r="N29" s="25"/>
@@ -5055,10 +5059,10 @@
         <v>30</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="M30" s="25"/>
       <c r="N30" s="25"/>
@@ -5109,10 +5113,10 @@
         <v>31</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>2</v>
+        <v>116</v>
       </c>
       <c r="M31" s="25"/>
       <c r="N31" s="25"/>
@@ -5163,10 +5167,10 @@
         <v>32</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>2</v>
+        <v>116</v>
       </c>
       <c r="M32" s="25"/>
       <c r="N32" s="25"/>
@@ -5217,7 +5221,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="C33" s="25">
         <v>2007</v>
@@ -5226,7 +5230,7 @@
         <v>2010</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>101</v>
+        <v>31</v>
       </c>
       <c r="F33" s="25">
         <v>2004</v>
@@ -5332,7 +5336,7 @@
         <v>Battery_Storage</v>
       </c>
       <c r="AM33" s="25" t="s">
-        <v>102</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:39" s="29" customFormat="1">
@@ -5340,16 +5344,16 @@
         <v>34</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>116</v>
+        <v>46</v>
       </c>
       <c r="C34" s="29">
         <v>2007</v>
       </c>
       <c r="D34" s="29">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>123</v>
+        <v>53</v>
       </c>
       <c r="F34" s="29">
         <v>2004</v>
@@ -5465,16 +5469,16 @@
         <v>35</v>
       </c>
       <c r="B35" s="29" t="s">
-        <v>117</v>
+        <v>47</v>
       </c>
       <c r="C35" s="29">
         <v>2007</v>
       </c>
-      <c r="D35" s="29">
-        <v>2010</v>
+      <c r="D35" s="34">
+        <v>2014</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>123</v>
+        <v>53</v>
       </c>
       <c r="F35" s="29">
         <v>2004</v>
@@ -5591,16 +5595,16 @@
         <v>36</v>
       </c>
       <c r="B36" s="29" t="s">
-        <v>118</v>
+        <v>48</v>
       </c>
       <c r="C36" s="29">
         <v>2007</v>
       </c>
-      <c r="D36" s="29">
-        <v>2010</v>
+      <c r="D36" s="34">
+        <v>2014</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>118</v>
+        <v>48</v>
       </c>
       <c r="F36" s="29">
         <v>2004</v>
@@ -5717,16 +5721,16 @@
         <v>37</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>119</v>
+        <v>49</v>
       </c>
       <c r="C37" s="29">
         <v>2007</v>
       </c>
-      <c r="D37" s="29">
-        <v>2010</v>
+      <c r="D37" s="34">
+        <v>2014</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>124</v>
+        <v>0</v>
       </c>
       <c r="F37" s="29">
         <v>2004</v>
@@ -5843,16 +5847,16 @@
         <v>38</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="C38" s="29">
         <v>2007</v>
       </c>
-      <c r="D38" s="29">
-        <v>2010</v>
+      <c r="D38" s="34">
+        <v>2014</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="F38" s="29">
         <v>2004</v>
@@ -5967,16 +5971,16 @@
         <v>39</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>121</v>
+        <v>51</v>
       </c>
       <c r="C39" s="29">
         <v>2007</v>
       </c>
-      <c r="D39" s="29">
-        <v>2010</v>
+      <c r="D39" s="34">
+        <v>2014</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="F39" s="29">
         <v>2004</v>
@@ -6093,16 +6097,16 @@
         <v>40</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>122</v>
+        <v>52</v>
       </c>
       <c r="C40" s="29">
         <v>2007</v>
       </c>
-      <c r="D40" s="29">
-        <v>2010</v>
+      <c r="D40" s="34">
+        <v>2014</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>123</v>
+        <v>53</v>
       </c>
       <c r="F40" s="29">
         <v>2004</v>
@@ -6219,16 +6223,16 @@
         <v>41</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>137</v>
+        <v>14</v>
       </c>
       <c r="C41" s="31">
         <v>2007</v>
       </c>
-      <c r="D41" s="31">
-        <v>2010</v>
-      </c>
-      <c r="E41" s="31" t="s">
-        <v>2</v>
+      <c r="D41" s="34">
+        <v>2014</v>
+      </c>
+      <c r="E41" s="33" t="s">
+        <v>53</v>
       </c>
       <c r="F41" s="31">
         <v>2004</v>
@@ -6334,7 +6338,7 @@
         <v>0</v>
       </c>
       <c r="AL41" s="31" t="s">
-        <v>129</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:39" s="31" customFormat="1">
@@ -6342,16 +6346,16 @@
         <v>42</v>
       </c>
       <c r="B42" s="31" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="C42" s="31">
         <v>2007</v>
       </c>
-      <c r="D42" s="31">
-        <v>2010</v>
-      </c>
-      <c r="E42" s="31" t="s">
-        <v>33</v>
+      <c r="D42" s="34">
+        <v>2014</v>
+      </c>
+      <c r="E42" s="33" t="s">
+        <v>11</v>
       </c>
       <c r="F42" s="31">
         <v>2004</v>
@@ -6456,7 +6460,7 @@
         <v>0</v>
       </c>
       <c r="AL42" s="31" t="s">
-        <v>130</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:39" s="31" customFormat="1">
@@ -6464,16 +6468,16 @@
         <v>43</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="C43" s="31">
         <v>2007</v>
       </c>
-      <c r="D43" s="31">
-        <v>2010</v>
-      </c>
-      <c r="E43" s="31" t="s">
-        <v>2</v>
+      <c r="D43" s="34">
+        <v>2014</v>
+      </c>
+      <c r="E43" s="33" t="s">
+        <v>53</v>
       </c>
       <c r="F43" s="31">
         <v>2004</v>
@@ -6579,7 +6583,7 @@
         <v>0</v>
       </c>
       <c r="AL43" s="31" t="s">
-        <v>131</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:39" s="31" customFormat="1">
@@ -6587,16 +6591,16 @@
         <v>44</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>88</v>
+        <v>18</v>
       </c>
       <c r="C44" s="31">
         <v>2007</v>
       </c>
-      <c r="D44" s="31">
-        <v>2010</v>
-      </c>
-      <c r="E44" s="31" t="s">
-        <v>2</v>
+      <c r="D44" s="34">
+        <v>2014</v>
+      </c>
+      <c r="E44" s="33" t="s">
+        <v>53</v>
       </c>
       <c r="F44" s="31">
         <v>2004</v>
@@ -6701,7 +6705,7 @@
         <v>0</v>
       </c>
       <c r="AL44" s="31" t="s">
-        <v>132</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:39" s="31" customFormat="1">
@@ -6709,16 +6713,16 @@
         <v>45</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="C45" s="31">
         <v>2007</v>
       </c>
-      <c r="D45" s="31">
-        <v>2010</v>
-      </c>
-      <c r="E45" s="31" t="s">
-        <v>2</v>
+      <c r="D45" s="34">
+        <v>2014</v>
+      </c>
+      <c r="E45" s="33" t="s">
+        <v>53</v>
       </c>
       <c r="F45" s="31">
         <v>2004</v>
@@ -6826,7 +6830,7 @@
         <v>0</v>
       </c>
       <c r="AL45" s="31" t="s">
-        <v>133</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:39" s="31" customFormat="1">
@@ -6834,16 +6838,16 @@
         <v>46</v>
       </c>
       <c r="B46" s="31" t="s">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="C46" s="31">
         <v>2007</v>
       </c>
-      <c r="D46" s="31">
-        <v>2010</v>
-      </c>
-      <c r="E46" s="31" t="s">
-        <v>33</v>
+      <c r="D46" s="34">
+        <v>2014</v>
+      </c>
+      <c r="E46" s="33" t="s">
+        <v>11</v>
       </c>
       <c r="F46" s="31">
         <v>2004</v>
@@ -6951,7 +6955,7 @@
         <v>0</v>
       </c>
       <c r="AL46" s="31" t="s">
-        <v>134</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:39" s="31" customFormat="1">
@@ -6959,16 +6963,16 @@
         <v>47</v>
       </c>
       <c r="B47" s="31" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="C47" s="31">
         <v>2007</v>
       </c>
-      <c r="D47" s="31">
-        <v>2010</v>
-      </c>
-      <c r="E47" s="31" t="s">
-        <v>2</v>
+      <c r="D47" s="34">
+        <v>2014</v>
+      </c>
+      <c r="E47" s="33" t="s">
+        <v>53</v>
       </c>
       <c r="F47" s="31">
         <v>2004</v>
@@ -7076,7 +7080,7 @@
         <v>0</v>
       </c>
       <c r="AL47" s="31" t="s">
-        <v>135</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:39" s="31" customFormat="1">
@@ -7084,16 +7088,16 @@
         <v>48</v>
       </c>
       <c r="B48" s="31" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="C48" s="31">
         <v>2007</v>
       </c>
-      <c r="D48" s="31">
-        <v>2010</v>
-      </c>
-      <c r="E48" s="31" t="s">
-        <v>2</v>
+      <c r="D48" s="34">
+        <v>2014</v>
+      </c>
+      <c r="E48" s="33" t="s">
+        <v>53</v>
       </c>
       <c r="F48" s="31">
         <v>2004</v>
@@ -7201,7 +7205,7 @@
         <v>0</v>
       </c>
       <c r="AL48" s="31" t="s">
-        <v>136</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:37" s="5" customFormat="1">
@@ -7214,12 +7218,12 @@
     </row>
     <row r="50" spans="1:37" s="6" customFormat="1">
       <c r="A50" s="6" t="s">
-        <v>8</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="1:37">
       <c r="A51" t="s">
-        <v>104</v>
+        <v>34</v>
       </c>
       <c r="B51">
         <v>2010</v>
@@ -7237,7 +7241,7 @@
         <v>2026</v>
       </c>
       <c r="G51" t="s">
-        <v>7</v>
+        <v>121</v>
       </c>
       <c r="I51" s="28"/>
       <c r="S51" s="5"/>
@@ -7570,7 +7574,7 @@
         <v>Coal_IGCC</v>
       </c>
       <c r="B62" s="1">
-        <f t="shared" ref="B62:F71" si="12">$M12*(1+$P12)^(B$51-2007)/1000000</f>
+        <f t="shared" ref="B62:F67" si="12">$M12*(1+$P12)^(B$51-2007)/1000000</f>
         <v>2.7827187265800002</v>
       </c>
       <c r="C62" s="1">
@@ -8438,6 +8442,7 @@
       <c r="AK90"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="1">
     <mergeCell ref="B22:C22"/>
   </mergeCells>
@@ -8455,7 +8460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:AD48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
@@ -12507,7 +12512,7 @@
       </c>
       <c r="D34" s="30">
         <f>generator_costs!D34</f>
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="E34" s="30" t="str">
         <f>generator_costs!E34</f>
@@ -12629,7 +12634,7 @@
       </c>
       <c r="D35" s="30">
         <f>generator_costs!D35</f>
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="E35" s="30" t="str">
         <f>generator_costs!E35</f>
@@ -12751,7 +12756,7 @@
       </c>
       <c r="D36" s="30">
         <f>generator_costs!D36</f>
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="E36" s="30" t="str">
         <f>generator_costs!E36</f>
@@ -12873,7 +12878,7 @@
       </c>
       <c r="D37" s="30">
         <f>generator_costs!D37</f>
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="E37" s="30" t="str">
         <f>generator_costs!E37</f>
@@ -12995,7 +13000,7 @@
       </c>
       <c r="D38" s="30">
         <f>generator_costs!D38</f>
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="E38" s="30" t="str">
         <f>generator_costs!E38</f>
@@ -13117,7 +13122,7 @@
       </c>
       <c r="D39" s="30">
         <f>generator_costs!D39</f>
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="E39" s="30" t="str">
         <f>generator_costs!E39</f>
@@ -13239,7 +13244,7 @@
       </c>
       <c r="D40" s="30">
         <f>generator_costs!D40</f>
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="E40" s="30" t="str">
         <f>generator_costs!E40</f>
@@ -13361,11 +13366,11 @@
       </c>
       <c r="D41" s="31">
         <f>generator_costs!D41</f>
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="E41" s="31" t="str">
         <f>generator_costs!E41</f>
-        <v>Gas</v>
+        <v>Gas_CCS</v>
       </c>
       <c r="F41" s="31">
         <f>generator_costs!M41</f>
@@ -13483,11 +13488,11 @@
       </c>
       <c r="D42" s="31">
         <f>generator_costs!D42</f>
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="E42" s="31" t="str">
         <f>generator_costs!E42</f>
-        <v>Coal</v>
+        <v>Coal_CCS</v>
       </c>
       <c r="F42" s="31">
         <f>generator_costs!M42</f>
@@ -13605,11 +13610,11 @@
       </c>
       <c r="D43" s="31">
         <f>generator_costs!D43</f>
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="E43" s="31" t="str">
         <f>generator_costs!E43</f>
-        <v>Gas</v>
+        <v>Gas_CCS</v>
       </c>
       <c r="F43" s="31">
         <f>generator_costs!M43</f>
@@ -13727,11 +13732,11 @@
       </c>
       <c r="D44" s="31">
         <f>generator_costs!D44</f>
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="E44" s="31" t="str">
         <f>generator_costs!E44</f>
-        <v>Gas</v>
+        <v>Gas_CCS</v>
       </c>
       <c r="F44" s="31">
         <f>generator_costs!M44</f>
@@ -13849,11 +13854,11 @@
       </c>
       <c r="D45" s="31">
         <f>generator_costs!D45</f>
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="E45" s="31" t="str">
         <f>generator_costs!E45</f>
-        <v>Gas</v>
+        <v>Gas_CCS</v>
       </c>
       <c r="F45" s="31">
         <f>generator_costs!M45</f>
@@ -13971,11 +13976,11 @@
       </c>
       <c r="D46" s="31">
         <f>generator_costs!D46</f>
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="E46" s="31" t="str">
         <f>generator_costs!E46</f>
-        <v>Coal</v>
+        <v>Coal_CCS</v>
       </c>
       <c r="F46" s="31">
         <f>generator_costs!M46</f>
@@ -14093,11 +14098,11 @@
       </c>
       <c r="D47" s="31">
         <f>generator_costs!D47</f>
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="E47" s="31" t="str">
         <f>generator_costs!E47</f>
-        <v>Gas</v>
+        <v>Gas_CCS</v>
       </c>
       <c r="F47" s="31">
         <f>generator_costs!M47</f>
@@ -14215,11 +14220,11 @@
       </c>
       <c r="D48" s="31">
         <f>generator_costs!D48</f>
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="E48" s="31" t="str">
         <f>generator_costs!E48</f>
-        <v>Gas</v>
+        <v>Gas_CCS</v>
       </c>
       <c r="F48" s="31">
         <f>generator_costs!M48</f>
@@ -14323,6 +14328,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -14345,15 +14351,15 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="24" t="s">
-        <v>11</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="24" t="s">
-        <v>12</v>
+        <v>126</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>13</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="24" customFormat="1">
@@ -14381,7 +14387,7 @@
         <v>3.3</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>15</v>
+        <v>129</v>
       </c>
       <c r="E5" s="24"/>
     </row>
@@ -14534,6 +14540,7 @@
       <c r="E21" s="24"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
- forced existing wind plants to run (no more OperateEPDuringPeriod for existing wind)
- fixed an error that put the 'can_build_new' flag of hydro to 1, which caused it's costs to not be printed out in power_cost_cc in the results

- basic stats now prints out the policy options of the scenario
- broke out storage from other fuels for dispatch display
- updated baseline 1990 WECC emissions
- added CCS costs to the power cost calculation in the results database
- added a seperate storage column in the power cost table in results
</commit_message>
<xml_diff>
--- a/DatabasePrep/GeneratorInfo/generator_costs.xlsx
+++ b/DatabasePrep/GeneratorInfo/generator_costs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="-80" windowWidth="23960" windowHeight="15880" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="540" yWindow="-80" windowWidth="23960" windowHeight="15880" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Chart_revise" sheetId="4" r:id="rId1"/>
@@ -24,15 +24,136 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="138">
   <si>
-    <t>Bio_Solid_CCS</t>
+    <t>CapEx from SAM with Solar Field area = 800000m^2 and 6h TES, construction cost mulitplier and yearly cost fraction from CSP on ReEDs sheet- it's unclear how much these change with storage... assumed to be the same here, cost declination rate and fixed OM from Mark Mehos estimate on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>DOE Solar Program Costs, took 2020 value for fixed O+M, 10% added to capital costs to go from utility to distributed, but also assumed a 5% declination rate, , outage rates from Mathias</t>
+    <t>CSP_Trough_No_Storage</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>overnight_cost</t>
+    <t>CSP_Trough_6h_Storage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Central_PV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>construction_cost_multipulier</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed_o_m</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var_o_m</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nuclear_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biomass_Steam_Turbine</t>
+  </si>
+  <si>
+    <t>Hydro_NonPumped</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hydro_Pumped</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Water</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Water</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, cost declination rate assumed to be that of a gas steam turbine</t>
+  </si>
+  <si>
+    <t>Biomass_IGCC</t>
+  </si>
+  <si>
+    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to coal IGCC</t>
+  </si>
+  <si>
+    <t>Coal_IGCC</t>
+  </si>
+  <si>
+    <t>can_build_new</t>
+  </si>
+  <si>
+    <t>forced_outage_rate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>scheduled_outage_rate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ReEDs Sheet; also Sullivan et al (2008), NREL/CP-670-43510 Conference Paper for o&amp;m costs, declanation rate, etc; $1,200,000 taken as capital cost in 2010 rather than 2004 based on conversation with Hernandez, also The storage efficiency of the the storage phase of compressed air energy storage from Samir Succar and Robert H. Williams: Compressed Air Energy Storage: Theory, Resources, And Applications For Wind Power, p. 39
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Geothermal_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCGT_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>price_and_dollar_year</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>year_4_cost_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_5_cost_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_6_cost_fraction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, EIA says minimum learning by 2025 is 20%, so this is a 1.1% declination rate, capital cost multipulier from EIA,http://graysharboroceanenergy.com/Documents/LIPA%20Offshore%20Wind%20rept.pdf for total outage rate of 3%, distributed by guess</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cost Declination Rate (%/yr)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resultant Capital Costs ($2007/MW) in Investment Period Years</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Concentrating_PV</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -40,138 +161,24 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Bio_Solid</t>
+    <t>(in 2010 $)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Gas_Combustion_Turbine_EP</t>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_EP</t>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_EP</t>
-  </si>
-  <si>
-    <t>CCGT_EP</t>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine_Cogen_EP</t>
-  </si>
-  <si>
-    <t>CapEx from SAM with Solar Field area = 600000m^2, construction cost mulitplier and yearly cost fraction from ReEDs sheet, cost declination rate and fixed OM from DOE solar program costs on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
+    <t>year</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Coal_CCS</t>
+    <t>$/Wp</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to gas combustion turbine</t>
-  </si>
-  <si>
-    <t>CCGT_Cogen_EP</t>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine_CCS_EP</t>
+    <t>CPV Consortium numbers (It's more or less SolFocus)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Wind_EP</t>
+    <t>cost declination rate</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wind</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCGT_CCS_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine_Cogen_CCS_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_Cogen_CCS_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_Cogen_CCS_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCGT_Cogen_CCS_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, cost declination rate assumed to be between ST and other techs (@1%).  EIA has minimum learning by 2025 as 10%, so this is roughly consistent</t>
-  </si>
-  <si>
-    <t>storage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Offshore_Wind</t>
-  </si>
-  <si>
-    <t>Bio_Gas</t>
-  </si>
-  <si>
-    <t>year_1_cost_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_2_cost_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_3_cost_fraction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Battery_Storage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Storage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, outage rates from Mathias</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>technology</t>
-  </si>
-  <si>
-    <t>overnight_cost_change</t>
-  </si>
-  <si>
-    <t>intermittent</t>
-  </si>
-  <si>
-    <t>resource_limited</t>
-  </si>
-  <si>
-    <t>baseload</t>
-  </si>
-  <si>
-    <t>min_build_capacity</t>
-  </si>
-  <si>
-    <t>$year_of_costs</t>
-  </si>
-  <si>
-    <t>cost_for_which_year?</t>
   </si>
   <si>
     <t>ReEDs Sheet, nukes run for 40 years at least, so the 30 year ReEDs lifetime was changed to 40, also the cost declination rate was set to 0.55% as nukes don't really obey the laws of mass production because they aren't mass produced</t>
@@ -381,66 +388,64 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Nuclear_EP</t>
+    <t>Bio_Solid_CCS</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Biomass_Steam_Turbine</t>
-  </si>
-  <si>
-    <t>Hydro_NonPumped</t>
+    <t>DOE Solar Program Costs, took 2020 value for fixed O+M, 10% added to capital costs to go from utility to distributed, but also assumed a 5% declination rate, , outage rates from Mathias</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Hydro_Pumped</t>
+    <t>overnight_cost</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Water</t>
+    <t>Solar</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Water</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, cost declination rate assumed to be that of a gas steam turbine</t>
-  </si>
-  <si>
-    <t>Biomass_IGCC</t>
-  </si>
-  <si>
-    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to coal IGCC</t>
-  </si>
-  <si>
-    <t>Coal_IGCC</t>
-  </si>
-  <si>
-    <t>can_build_new</t>
-  </si>
-  <si>
-    <t>forced_outage_rate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>scheduled_outage_rate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ReEDs Sheet; also Sullivan et al (2008), NREL/CP-670-43510 Conference Paper for o&amp;m costs, declanation rate, etc; $1,200,000 taken as capital cost in 2010 rather than 2004 based on conversation with Hernandez, also The storage efficiency of the the storage phase of compressed air energy storage from Samir Succar and Robert H. Williams: Compressed Air Energy Storage: Theory, Resources, And Applications For Wind Power, p. 39
-</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Geothermal_EP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCGT_EP</t>
+    <t>Bio_Solid</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Gas_Combustion_Turbine_EP</t>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_EP</t>
+  </si>
+  <si>
+    <t>Gas_Steam_Turbine_EP</t>
+  </si>
+  <si>
+    <t>CCGT_EP</t>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_Cogen_EP</t>
+  </si>
+  <si>
+    <t>CapEx from SAM with Solar Field area = 600000m^2, construction cost mulitplier and yearly cost fraction from ReEDs sheet, cost declination rate and fixed OM from DOE solar program costs on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_CCS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to gas combustion turbine</t>
+  </si>
+  <si>
+    <t>CCGT_Cogen_EP</t>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_CCS_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind_EP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -448,94 +453,89 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>price_and_dollar_year</t>
+    <t>CCGT_CCS_EP</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Gas</t>
-  </si>
-  <si>
-    <t>year_4_cost_fraction</t>
+    <t>Gas_Combustion_Turbine_Cogen_CCS_EP</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>year_5_cost_fraction</t>
+    <t>Coal_Steam_Turbine_Cogen_CCS_EP</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>year_6_cost_fraction</t>
+    <t>Gas_Steam_Turbine_Cogen_CCS_EP</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, EIA says minimum learning by 2025 is 20%, so this is a 1.1% declination rate, capital cost multipulier from EIA,http://graysharboroceanenergy.com/Documents/LIPA%20Offshore%20Wind%20rept.pdf for total outage rate of 3%, distributed by guess</t>
+    <t>CCGT_Cogen_CCS_EP</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Cost Declination Rate (%/yr)</t>
+    <t>ReEDs Sheet, cost declination rate assumed to be between ST and other techs (@1%).  EIA has minimum learning by 2025 as 10%, so this is roughly consistent</t>
+  </si>
+  <si>
+    <t>storage</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Resultant Capital Costs ($2007/MW) in Investment Period Years</t>
+    <t>Offshore_Wind</t>
+  </si>
+  <si>
+    <t>Bio_Gas</t>
+  </si>
+  <si>
+    <t>year_1_cost_fraction</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Concentrating_PV</t>
+    <t>year_2_cost_fraction</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Solar</t>
+    <t>year_3_cost_fraction</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>(in 2010 $)</t>
+    <t>Battery_Storage</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>year</t>
+    <t>Storage</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>$/Wp</t>
+    <t>ReEDs Sheet</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>CPV Consortium numbers (It's more or less SolFocus)</t>
+    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, outage rates from Mathias</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>cost declination rate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>technology</t>
   </si>
   <si>
-    <t>CapEx from SAM with Solar Field area = 800000m^2 and 6h TES, construction cost mulitplier and yearly cost fraction from CSP on ReEDs sheet- it's unclear how much these change with storage... assumed to be the same here, cost declination rate and fixed OM from Mark Mehos estimate on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>overnight_cost_change</t>
   </si>
   <si>
-    <t>CSP_Trough_No_Storage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>intermittent</t>
   </si>
   <si>
-    <t>CSP_Trough_6h_Storage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>resource_limited</t>
   </si>
   <si>
-    <t>Wind</t>
+    <t>baseload</t>
   </si>
   <si>
-    <t>Central_PV</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>min_build_capacity</t>
   </si>
   <si>
-    <t>construction_cost_multipulier</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>$year_of_costs</t>
   </si>
   <si>
-    <t>fixed_o_m</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var_o_m</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>cost_for_which_year?</t>
   </si>
 </sst>
 </file>
@@ -548,7 +548,7 @@
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -588,7 +588,7 @@
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1532,11 +1532,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="95933544"/>
-        <c:axId val="96260568"/>
+        <c:axId val="579649896"/>
+        <c:axId val="579168888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95933544"/>
+        <c:axId val="579649896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1570,14 +1570,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96260568"/>
+        <c:crossAx val="579168888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96260568"/>
+        <c:axId val="579168888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="7.0"/>
@@ -1613,7 +1613,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95933544"/>
+        <c:crossAx val="579649896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1999,9 +1999,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:AM90"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="125" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D34" sqref="D34:D48"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="AB1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AG18" sqref="AG18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2032,121 +2032,121 @@
   <sheetData>
     <row r="1" spans="1:39">
       <c r="A1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P1" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>73</v>
+      </c>
+      <c r="R1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S1" t="s">
+        <v>70</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z1" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="H1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="AA1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AF1" t="s">
         <v>135</v>
       </c>
-      <c r="K1" t="s">
-        <v>136</v>
-      </c>
-      <c r="L1" t="s">
-        <v>137</v>
-      </c>
-      <c r="M1" t="s">
-        <v>54</v>
-      </c>
-      <c r="N1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O1" t="s">
-        <v>70</v>
-      </c>
-      <c r="P1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>74</v>
-      </c>
-      <c r="R1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S1" t="s">
-        <v>71</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>39</v>
-      </c>
       <c r="AG1" t="s">
-        <v>107</v>
+        <v>18</v>
       </c>
       <c r="AH1" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI1" s="15" t="s">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="AJ1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK1" t="s">
         <v>65</v>
       </c>
-      <c r="AK1" t="s">
-        <v>66</v>
-      </c>
       <c r="AL1" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AM1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:39">
@@ -2154,7 +2154,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="5">
         <v>2007</v>
@@ -2163,7 +2163,7 @@
         <v>2010</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F2">
         <v>2004</v>
@@ -2269,7 +2269,7 @@
         <v>CCGT</v>
       </c>
       <c r="AM2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:39">
@@ -2277,7 +2277,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="5">
         <v>2007</v>
@@ -2286,7 +2286,7 @@
         <v>2010</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F3">
         <v>2004</v>
@@ -2392,7 +2392,7 @@
         <v>Gas_Combustion_Turbine</v>
       </c>
       <c r="AM3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:39" s="24" customFormat="1">
@@ -2400,7 +2400,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>123</v>
+        <v>34</v>
       </c>
       <c r="C4" s="24">
         <v>2007</v>
@@ -2409,7 +2409,7 @@
         <v>2010</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>124</v>
+        <v>35</v>
       </c>
       <c r="F4" s="24">
         <v>2010</v>
@@ -2516,7 +2516,7 @@
         <v>Concentrating_PV</v>
       </c>
       <c r="AM4" s="24" t="s">
-        <v>128</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:39">
@@ -2524,7 +2524,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>3</v>
       </c>
       <c r="C5" s="5">
         <v>2007</v>
@@ -2533,7 +2533,7 @@
         <v>2010</v>
       </c>
       <c r="E5" t="s">
-        <v>114</v>
+        <v>25</v>
       </c>
       <c r="F5">
         <v>2004</v>
@@ -2639,7 +2639,7 @@
         <v>Wind</v>
       </c>
       <c r="AM5" t="s">
-        <v>33</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:39">
@@ -2647,7 +2647,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>121</v>
       </c>
       <c r="C6" s="5">
         <v>2007</v>
@@ -2656,7 +2656,7 @@
         <v>2010</v>
       </c>
       <c r="E6" t="s">
-        <v>114</v>
+        <v>25</v>
       </c>
       <c r="F6">
         <v>2004</v>
@@ -2762,7 +2762,7 @@
         <v>Offshore_Wind</v>
       </c>
       <c r="AM6" t="s">
-        <v>120</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:39">
@@ -2770,7 +2770,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="5">
         <v>2007</v>
@@ -2779,7 +2779,7 @@
         <v>2010</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F7">
         <v>2009</v>
@@ -2886,7 +2886,7 @@
         <v>Residential_PV</v>
       </c>
       <c r="AM7" t="s">
-        <v>1</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:39" s="11" customFormat="1">
@@ -2894,7 +2894,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>132</v>
+        <v>2</v>
       </c>
       <c r="C8" s="11">
         <v>2007</v>
@@ -2903,7 +2903,7 @@
         <v>2012</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="F8" s="11">
         <v>2010</v>
@@ -3009,7 +3009,7 @@
         <v>CSP_Trough_6h_Storage</v>
       </c>
       <c r="AM8" s="11" t="s">
-        <v>130</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:39">
@@ -3017,7 +3017,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>122</v>
       </c>
       <c r="C9" s="5">
         <v>2007</v>
@@ -3026,7 +3026,7 @@
         <v>2010</v>
       </c>
       <c r="E9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F9">
         <v>2007</v>
@@ -3132,7 +3132,7 @@
         <v>Bio_Gas</v>
       </c>
       <c r="AM9" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:39">
@@ -3140,7 +3140,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="C10" s="5">
         <v>2007</v>
@@ -3149,7 +3149,7 @@
         <v>2010</v>
       </c>
       <c r="E10" t="s">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="F10">
         <v>2004</v>
@@ -3255,7 +3255,7 @@
         <v>Biomass_Steam_Turbine</v>
       </c>
       <c r="AM10" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:39">
@@ -3263,7 +3263,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>15</v>
       </c>
       <c r="C11" s="5">
         <v>2007</v>
@@ -3272,7 +3272,7 @@
         <v>2012</v>
       </c>
       <c r="E11" t="s">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="F11">
         <v>2007</v>
@@ -3378,7 +3378,7 @@
         <v>Biomass_IGCC</v>
       </c>
       <c r="AM11" t="s">
-        <v>105</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:39">
@@ -3386,7 +3386,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>17</v>
       </c>
       <c r="C12" s="5">
         <v>2007</v>
@@ -3395,7 +3395,7 @@
         <v>2010</v>
       </c>
       <c r="E12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F12">
         <v>2004</v>
@@ -3501,7 +3501,7 @@
         <v>Coal_IGCC</v>
       </c>
       <c r="AM12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:39">
@@ -3509,7 +3509,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C13" s="5">
         <v>2007</v>
@@ -3518,7 +3518,7 @@
         <v>2010</v>
       </c>
       <c r="E13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F13">
         <v>2004</v>
@@ -3624,7 +3624,7 @@
         <v>Coal_Steam_Turbine</v>
       </c>
       <c r="AM13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:39">
@@ -3632,7 +3632,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" s="5">
         <v>2007</v>
@@ -3641,7 +3641,7 @@
         <v>2010</v>
       </c>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F14">
         <v>2004</v>
@@ -3747,7 +3747,7 @@
         <v>Nuclear</v>
       </c>
       <c r="AM14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:39">
@@ -3755,7 +3755,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15" s="5">
         <v>2007</v>
@@ -3764,7 +3764,7 @@
         <v>2010</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F15">
         <v>2004</v>
@@ -3870,7 +3870,7 @@
         <v>Geothermal</v>
       </c>
       <c r="AM15" t="s">
-        <v>23</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:39">
@@ -3878,7 +3878,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="C16" s="5">
         <v>2007</v>
@@ -3887,7 +3887,7 @@
         <v>2010</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="F16" s="5">
         <v>2004</v>
@@ -3974,7 +3974,7 @@
         <v>0</v>
       </c>
       <c r="AG16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH16" s="30">
         <v>0</v>
@@ -3993,7 +3993,7 @@
         <v>Hydro_NonPumped</v>
       </c>
       <c r="AM16" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:39">
@@ -4001,7 +4001,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="C17" s="5">
         <v>2007</v>
@@ -4010,7 +4010,7 @@
         <v>2010</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="F17" s="5">
         <v>2004</v>
@@ -4097,7 +4097,7 @@
         <v>0</v>
       </c>
       <c r="AG17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH17" s="30">
         <v>0</v>
@@ -4116,7 +4116,7 @@
         <v>Hydro_Pumped</v>
       </c>
       <c r="AM17" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:39" s="18" customFormat="1">
@@ -4124,10 +4124,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="M18" s="23"/>
       <c r="S18" s="22">
@@ -4176,12 +4176,12 @@
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G19" s="11"/>
       <c r="M19" s="23"/>
@@ -4233,12 +4233,12 @@
         <v>19</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>116</v>
+        <v>27</v>
       </c>
       <c r="G20" s="11"/>
       <c r="M20" s="23"/>
@@ -4290,12 +4290,12 @@
         <v>20</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>112</v>
+        <v>23</v>
       </c>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21" t="s">
-        <v>116</v>
+        <v>27</v>
       </c>
       <c r="G21" s="11"/>
       <c r="M21" s="23"/>
@@ -4347,12 +4347,12 @@
         <v>21</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>111</v>
+        <v>22</v>
       </c>
       <c r="C22" s="36"/>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G22" s="11"/>
       <c r="M22" s="23"/>
@@ -4404,12 +4404,12 @@
         <v>22</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G23" s="11"/>
       <c r="M23" s="23"/>
@@ -4461,10 +4461,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="M24" s="23"/>
       <c r="S24" s="22">
@@ -4513,7 +4513,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" s="8">
         <v>2007</v>
@@ -4522,7 +4522,7 @@
         <v>2010</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="F25" s="8">
         <v>2009</v>
@@ -4628,7 +4628,7 @@
         <v>Commercial_PV</v>
       </c>
       <c r="AM25" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:39" s="8" customFormat="1">
@@ -4636,7 +4636,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>134</v>
+        <v>4</v>
       </c>
       <c r="C26" s="8">
         <v>2007</v>
@@ -4645,7 +4645,7 @@
         <v>2010</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="F26" s="8">
         <v>2009</v>
@@ -4751,7 +4751,7 @@
         <v>Central_PV</v>
       </c>
       <c r="AM26" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:39" s="5" customFormat="1">
@@ -4759,7 +4759,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
       <c r="C27" s="5">
         <v>2007</v>
@@ -4768,7 +4768,7 @@
         <v>2010</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="F27" s="5">
         <v>2010</v>
@@ -4874,7 +4874,7 @@
         <v>CSP_Trough_No_Storage</v>
       </c>
       <c r="AM27" s="9" t="s">
-        <v>10</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:39" s="9" customFormat="1" ht="15" customHeight="1">
@@ -4882,7 +4882,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C28" s="9">
         <v>2007</v>
@@ -4891,7 +4891,7 @@
         <v>2010</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F28" s="9">
         <v>2010</v>
@@ -4997,7 +4997,7 @@
         <v>Compressed_Air_Energy_Storage</v>
       </c>
       <c r="AM28" s="35" t="s">
-        <v>110</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:39" s="21" customFormat="1">
@@ -5005,10 +5005,10 @@
         <v>29</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="M29" s="25"/>
       <c r="N29" s="25"/>
@@ -5059,10 +5059,10 @@
         <v>30</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M30" s="25"/>
       <c r="N30" s="25"/>
@@ -5113,10 +5113,10 @@
         <v>31</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>116</v>
+        <v>27</v>
       </c>
       <c r="M31" s="25"/>
       <c r="N31" s="25"/>
@@ -5167,10 +5167,10 @@
         <v>32</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>116</v>
+        <v>27</v>
       </c>
       <c r="M32" s="25"/>
       <c r="N32" s="25"/>
@@ -5221,7 +5221,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>30</v>
+        <v>126</v>
       </c>
       <c r="C33" s="25">
         <v>2007</v>
@@ -5230,7 +5230,7 @@
         <v>2010</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>31</v>
+        <v>127</v>
       </c>
       <c r="F33" s="25">
         <v>2004</v>
@@ -5336,7 +5336,7 @@
         <v>Battery_Storage</v>
       </c>
       <c r="AM33" s="25" t="s">
-        <v>32</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:39" s="29" customFormat="1">
@@ -5344,7 +5344,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34" s="29">
         <v>2007</v>
@@ -5353,7 +5353,7 @@
         <v>2014</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F34" s="29">
         <v>2004</v>
@@ -5469,7 +5469,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C35" s="29">
         <v>2007</v>
@@ -5478,7 +5478,7 @@
         <v>2014</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F35" s="29">
         <v>2004</v>
@@ -5595,7 +5595,7 @@
         <v>36</v>
       </c>
       <c r="B36" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C36" s="29">
         <v>2007</v>
@@ -5604,7 +5604,7 @@
         <v>2014</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F36" s="29">
         <v>2004</v>
@@ -5721,7 +5721,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C37" s="29">
         <v>2007</v>
@@ -5730,7 +5730,7 @@
         <v>2014</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="F37" s="29">
         <v>2004</v>
@@ -5847,7 +5847,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C38" s="29">
         <v>2007</v>
@@ -5856,7 +5856,7 @@
         <v>2014</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="F38" s="29">
         <v>2004</v>
@@ -5971,7 +5971,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C39" s="29">
         <v>2007</v>
@@ -5980,7 +5980,7 @@
         <v>2014</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="F39" s="29">
         <v>2004</v>
@@ -6097,7 +6097,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C40" s="29">
         <v>2007</v>
@@ -6106,7 +6106,7 @@
         <v>2014</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F40" s="29">
         <v>2004</v>
@@ -6223,7 +6223,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="C41" s="31">
         <v>2007</v>
@@ -6232,7 +6232,7 @@
         <v>2014</v>
       </c>
       <c r="E41" s="33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F41" s="31">
         <v>2004</v>
@@ -6338,7 +6338,7 @@
         <v>0</v>
       </c>
       <c r="AL41" s="31" t="s">
-        <v>5</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:39" s="31" customFormat="1">
@@ -6346,7 +6346,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C42" s="31">
         <v>2007</v>
@@ -6355,7 +6355,7 @@
         <v>2014</v>
       </c>
       <c r="E42" s="33" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="F42" s="31">
         <v>2004</v>
@@ -6460,7 +6460,7 @@
         <v>0</v>
       </c>
       <c r="AL42" s="31" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:39" s="31" customFormat="1">
@@ -6468,7 +6468,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C43" s="31">
         <v>2007</v>
@@ -6477,7 +6477,7 @@
         <v>2014</v>
       </c>
       <c r="E43" s="33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F43" s="31">
         <v>2004</v>
@@ -6583,7 +6583,7 @@
         <v>0</v>
       </c>
       <c r="AL43" s="31" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:39" s="31" customFormat="1">
@@ -6591,7 +6591,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>18</v>
+        <v>114</v>
       </c>
       <c r="C44" s="31">
         <v>2007</v>
@@ -6600,7 +6600,7 @@
         <v>2014</v>
       </c>
       <c r="E44" s="33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F44" s="31">
         <v>2004</v>
@@ -6705,7 +6705,7 @@
         <v>0</v>
       </c>
       <c r="AL44" s="31" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:39" s="31" customFormat="1">
@@ -6713,7 +6713,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>19</v>
+        <v>115</v>
       </c>
       <c r="C45" s="31">
         <v>2007</v>
@@ -6722,7 +6722,7 @@
         <v>2014</v>
       </c>
       <c r="E45" s="33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F45" s="31">
         <v>2004</v>
@@ -6830,7 +6830,7 @@
         <v>0</v>
       </c>
       <c r="AL45" s="31" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:39" s="31" customFormat="1">
@@ -6838,7 +6838,7 @@
         <v>46</v>
       </c>
       <c r="B46" s="31" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
       <c r="C46" s="31">
         <v>2007</v>
@@ -6847,7 +6847,7 @@
         <v>2014</v>
       </c>
       <c r="E46" s="33" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="F46" s="31">
         <v>2004</v>
@@ -6955,7 +6955,7 @@
         <v>0</v>
       </c>
       <c r="AL46" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:39" s="31" customFormat="1">
@@ -6963,7 +6963,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="31" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
       <c r="C47" s="31">
         <v>2007</v>
@@ -6972,7 +6972,7 @@
         <v>2014</v>
       </c>
       <c r="E47" s="33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F47" s="31">
         <v>2004</v>
@@ -7080,7 +7080,7 @@
         <v>0</v>
       </c>
       <c r="AL47" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:39" s="31" customFormat="1">
@@ -7088,7 +7088,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="31" t="s">
-        <v>22</v>
+        <v>118</v>
       </c>
       <c r="C48" s="31">
         <v>2007</v>
@@ -7097,7 +7097,7 @@
         <v>2014</v>
       </c>
       <c r="E48" s="33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F48" s="31">
         <v>2004</v>
@@ -7205,7 +7205,7 @@
         <v>0</v>
       </c>
       <c r="AL48" s="31" t="s">
-        <v>13</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:37" s="5" customFormat="1">
@@ -7218,12 +7218,12 @@
     </row>
     <row r="50" spans="1:37" s="6" customFormat="1">
       <c r="A50" s="6" t="s">
-        <v>122</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:37">
       <c r="A51" t="s">
-        <v>34</v>
+        <v>130</v>
       </c>
       <c r="B51">
         <v>2010</v>
@@ -7241,7 +7241,7 @@
         <v>2026</v>
       </c>
       <c r="G51" t="s">
-        <v>121</v>
+        <v>32</v>
       </c>
       <c r="I51" s="28"/>
       <c r="S51" s="5"/>
@@ -8460,7 +8460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:AD48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
@@ -10404,7 +10404,7 @@
       </c>
       <c r="Z16" s="12">
         <f>generator_costs!AG16</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA16" s="30">
         <f>generator_costs!AH16</f>
@@ -10526,7 +10526,7 @@
       </c>
       <c r="Z17" s="12">
         <f>generator_costs!AG17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA17" s="30">
         <f>generator_costs!AH17</f>
@@ -14351,15 +14351,15 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="24" t="s">
-        <v>125</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="24" t="s">
-        <v>126</v>
+        <v>37</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>127</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="24" customFormat="1">
@@ -14387,7 +14387,7 @@
         <v>3.3</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="E5" s="24"/>
     </row>

</xml_diff>

<commit_message>
- redefined hydro indexing to look much more like all other generators (NONPUMPED_HYDRO_AVAILABLE_HOURS and such) - disaggregated hydro by plant in build_existing_plants_table.sql -- this change doesn't make it to the model yet - droped a bunch of params in existing_plants.tab in favor of including them in generator_info.tab - got rid of parts of windsun.dat
</commit_message>
<xml_diff>
--- a/DatabasePrep/GeneratorInfo/generator_costs.xlsx
+++ b/DatabasePrep/GeneratorInfo/generator_costs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="33560" windowHeight="21580" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="33560" windowHeight="19480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="generator_costs" sheetId="1" r:id="rId1"/>
@@ -24,189 +24,43 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="148">
   <si>
-    <t>ReEDs Sheet, also new wind params used for fixed O+M, forced outage rate</t>
+    <t>Wind</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>ReEDs Sheet, 75 CapEx of non-cogen</t>
+    <t>CCGT_CCS_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Geothermal_EP</t>
+    <t>Gas_Combustion_Turbine_Cogen_CCS_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>ReEDs Sheet, nukes run for 40 years at least, so the 30 year ReEDs lifetime was changed to 40, also the cost declination rate was set to 0.55% as nukes don't really obey the laws of mass production because they aren't mass produced</t>
+    <t>Coal_Steam_Turbine_Cogen_CCS_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>CCGT</t>
-  </si>
-  <si>
-    <t>ReEDs Sheet</t>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine</t>
-  </si>
-  <si>
-    <t>CCGT_CCS</t>
+    <t>Gas_Steam_Turbine_Cogen_CCS_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Gas_Combustion_Turbine_CCS</t>
+    <t>CCGT_Cogen_CCS_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Bio_Gas_CCS</t>
+    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, EIA says minimum learning by 2025 is 20%, so this is a 1.1% declination rate, capital cost multipulier from EIA,http://graysharboroceanenergy.com/Documents/LIPA%20Offshore%20Wind%20rept.pdf for total outage rate of 3%, distributed by guess</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Biomass_IGCC_CCS</t>
+    <t>Cost Declination Rate (%/yr)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Coal_IGCC_CCS</t>
+    <t>Resultant Capital Costs ($2007/MW) in Investment Period Years</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Coal_Steam_Turbine_CCS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_CCS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>overnight_cost_$2007</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, cost declination rate assumed to be between ST and other techs (@1%).  EIA has minimum learning by 2025 as 10%, so this is roughly consistent</t>
-  </si>
-  <si>
-    <t>storage</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Offshore_Wind</t>
-  </si>
-  <si>
-    <t>Bio_Gas</t>
-  </si>
-  <si>
-    <t>year_1_cost_fraction</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_2_cost_fraction</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_3_cost_fraction</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Battery_Storage</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Storage</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>tech_name_again</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bio_Solid_CCS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biomass_Steam_Turbine</t>
-  </si>
-  <si>
-    <t>Hydro_NonPumped</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hydro_Pumped</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Water</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Water</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, cost declination rate assumed to be that of a gas steam turbine</t>
-  </si>
-  <si>
-    <t>Biomass_IGCC</t>
-  </si>
-  <si>
-    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to coal IGCC</t>
-  </si>
-  <si>
-    <t>Coal_IGCC</t>
-  </si>
-  <si>
-    <t>can_build_new</t>
-  </si>
-  <si>
-    <t>forced_outage_rate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>scheduled_outage_rate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CapEx from SAM with Solar Field area = 600000m^2, construction cost mulitplier and yearly cost fraction from ReEDs sheet, cost declination rate and fixed OM from DOE solar program costs on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_CCS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to gas combustion turbine</t>
-  </si>
-  <si>
-    <t>CCGT_Cogen_EP</t>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine_CCS_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wind_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>DOE Solar Program Costs, took 2020 value for fixed O+M, 10% added to capital costs to go from utility to distributed, but also assumed a 5% declination rate, , outage rates from Mathias</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>overnight_cost</t>
+    <t>Concentrating_PV</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -214,118 +68,23 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Bio_Solid</t>
+    <t>(in 2010 $)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Gas_Combustion_Turbine_EP</t>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_EP</t>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_EP</t>
-  </si>
-  <si>
-    <t>CCGT_EP</t>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine_Cogen_EP</t>
-  </si>
-  <si>
-    <t>Gas_Internal_Combustion_Engine_EP</t>
+    <t>year</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Gas</t>
+    <t>$/Wp</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Gas_Internal_Combustion_Engine_Cogen_EP</t>
+    <t>CPV Consortium numbers (It's more or less SolFocus)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>note: we assume that cogen plants have 3/4 of the capital cost of a pure-electric plant, (to reflect shared infrastructure for cogen), but the same operating costs.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>dispatchable</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>cogen</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, took CoalOldScr costs</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, took OGS (Oil Gas Steam)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, set lifetime to 60 years</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ReEDs Sheet; also Sullivan et al (2008), NREL/CP-670-43510 Conference Paper for o&amp;m costs, declanation rate, etc; $1,200,000 taken as capital cost in 2010 rather than 2004 based on conversation with Hernandez, also The storage efficiency of the the storage phase of compressed air energy storage from Samir Succar and Robert H. Williams: Compressed Air Energy Storage: Theory, Resources, And Applications For Wind Power, p. 39
-</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCGT_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wind</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>price_and_dollar_year</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas</t>
-  </si>
-  <si>
-    <t>year_4_cost_fraction</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_5_cost_fraction</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_6_cost_fraction</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed_o_m_$2007</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>heat_rate_mbtu_per_mwh</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Commercial_PV</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>min_build_year</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine_Cogen_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_Cogen_EP</t>
+    <t>cost declination rate</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -514,43 +273,29 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Wind</t>
+    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to gas combustion turbine</t>
+  </si>
+  <si>
+    <t>CCGT_Cogen_EP</t>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_CCS_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>CCGT_CCS_EP</t>
+    <t>Wind_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Gas_Combustion_Turbine_Cogen_CCS_EP</t>
+    <t>Gas</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Coal_Steam_Turbine_Cogen_CCS_EP</t>
+    <t>DOE Solar Program Costs, took 2020 value for fixed O+M, 10% added to capital costs to go from utility to distributed, but also assumed a 5% declination rate, , outage rates from Mathias</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Gas_Steam_Turbine_Cogen_CCS_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCGT_Cogen_CCS_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, EIA says minimum learning by 2025 is 20%, so this is a 1.1% declination rate, capital cost multipulier from EIA,http://graysharboroceanenergy.com/Documents/LIPA%20Offshore%20Wind%20rept.pdf for total outage rate of 3%, distributed by guess</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cost Declination Rate (%/yr)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resultant Capital Costs ($2007/MW) in Investment Period Years</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Concentrating_PV</t>
+    <t>overnight_cost</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -558,23 +303,278 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>(in 2010 $)</t>
+    <t>Bio_Solid</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>year</t>
+    <t>Gas_Combustion_Turbine_EP</t>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_EP</t>
+  </si>
+  <si>
+    <t>Gas_Steam_Turbine_EP</t>
+  </si>
+  <si>
+    <t>CCGT_EP</t>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_Cogen_EP</t>
+  </si>
+  <si>
+    <t>Gas_Internal_Combustion_Engine_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>$/Wp</t>
+    <t>Gas</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>CPV Consortium numbers (It's more or less SolFocus)</t>
+    <t>Gas_Internal_Combustion_Engine_Cogen_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>cost declination rate</t>
+    <t>note: we assume that cogen plants have 3/4 of the capital cost of a pure-electric plant, (to reflect shared infrastructure for cogen), but the same operating costs.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dispatchable</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>cogen</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, took CoalOldScr costs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, took OGS (Oil Gas Steam)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, set lifetime to 60 years</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ReEDs Sheet; also Sullivan et al (2008), NREL/CP-670-43510 Conference Paper for o&amp;m costs, declanation rate, etc; $1,200,000 taken as capital cost in 2010 rather than 2004 based on conversation with Hernandez, also The storage efficiency of the the storage phase of compressed air energy storage from Samir Succar and Robert H. Williams: Compressed Air Energy Storage: Theory, Resources, And Applications For Wind Power, p. 39
+</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCGT_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>price_and_dollar_year</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>year_4_cost_fraction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_5_cost_fraction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_6_cost_fraction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed_o_m_$2007</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>heat_rate_mbtu_per_mwh</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commercial_PV</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>min_build_year</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_Cogen_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_Cogen_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, also new wind params used for fixed O+M, forced outage rate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, 75 CapEx of non-cogen</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Geothermal_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, nukes run for 40 years at least, so the 30 year ReEDs lifetime was changed to 40, also the cost declination rate was set to 0.55% as nukes don't really obey the laws of mass production because they aren't mass produced</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCGT</t>
+  </si>
+  <si>
+    <t>ReEDs Sheet</t>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine</t>
+  </si>
+  <si>
+    <t>CCGT_CCS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_CCS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Gas_CCS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biomass_IGCC_CCS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_IGCC_CCS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_CCS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_CCS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>overnight_cost_$2007</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, cost declination rate assumed to be between ST and other techs (@1%).  EIA has minimum learning by 2025 as 10%, so this is roughly consistent</t>
+  </si>
+  <si>
+    <t>storage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Offshore_Wind</t>
+  </si>
+  <si>
+    <t>Bio_Gas</t>
+  </si>
+  <si>
+    <t>year_1_cost_fraction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_2_cost_fraction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_3_cost_fraction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery_Storage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Storage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>tech_name_again</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Steam_Turbine_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Solid_CCS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biomass_Steam_Turbine</t>
+  </si>
+  <si>
+    <t>Hydro_NonPumped</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hydro_Pumped</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Water</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Water</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, cost declination rate assumed to be that of a gas steam turbine</t>
+  </si>
+  <si>
+    <t>Biomass_IGCC</t>
+  </si>
+  <si>
+    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to coal IGCC</t>
+  </si>
+  <si>
+    <t>Coal_IGCC</t>
+  </si>
+  <si>
+    <t>can_build_new</t>
+  </si>
+  <si>
+    <t>forced_outage_rate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>scheduled_outage_rate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CapEx from SAM with Solar Field area = 600000m^2, construction cost mulitplier and yearly cost fraction from ReEDs sheet, cost declination rate and fixed OM from DOE solar program costs on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_CCS</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -582,14 +582,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -634,7 +629,7 @@
   <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -656,7 +651,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1001,8 +996,8 @@
   <dimension ref="A1:AO104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z22" sqref="Z22"/>
+      <pane xSplit="2" topLeftCell="AF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AF50" sqref="AF50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1034,133 +1029,133 @@
   <sheetData>
     <row r="1" spans="1:41" s="33" customFormat="1">
       <c r="A1" s="34" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:41" s="33" customFormat="1"/>
     <row r="3" spans="1:41">
       <c r="A3" s="5" t="s">
-        <v>107</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>27</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L3" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" t="s">
         <v>119</v>
       </c>
-      <c r="F3" t="s">
+      <c r="N3" t="s">
+        <v>99</v>
+      </c>
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>53</v>
+      </c>
+      <c r="R3" t="s">
+        <v>100</v>
+      </c>
+      <c r="S3" t="s">
+        <v>50</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y3" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="H3" t="s">
-        <v>99</v>
-      </c>
-      <c r="I3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" t="s">
-        <v>128</v>
-      </c>
-      <c r="K3" t="s">
-        <v>129</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="Z3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF3" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG3" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ3" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK3" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AN3" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="M3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N3" t="s">
-        <v>75</v>
-      </c>
-      <c r="O3" t="s">
-        <v>90</v>
-      </c>
-      <c r="P3" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>118</v>
-      </c>
-      <c r="R3" t="s">
-        <v>76</v>
-      </c>
-      <c r="S3" t="s">
-        <v>115</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y3" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>95</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>96</v>
-      </c>
-      <c r="AF3" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG3" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>97</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ3" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="AK3" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AN3" s="12" t="s">
-        <v>25</v>
-      </c>
       <c r="AO3" t="s">
-        <v>106</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:41">
@@ -1168,7 +1163,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="C4" s="5">
         <v>2007</v>
@@ -1177,7 +1172,7 @@
         <v>2010</v>
       </c>
       <c r="E4" t="s">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="F4">
         <v>2004</v>
@@ -1289,7 +1284,7 @@
         <v>CCGT</v>
       </c>
       <c r="AO4" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:41">
@@ -1297,7 +1292,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>111</v>
       </c>
       <c r="C5" s="5">
         <v>2007</v>
@@ -1306,7 +1301,7 @@
         <v>2010</v>
       </c>
       <c r="E5" t="s">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="F5">
         <v>2004</v>
@@ -1418,7 +1413,7 @@
         <v>Gas_Combustion_Turbine</v>
       </c>
       <c r="AO5" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:41" s="22" customFormat="1">
@@ -1426,7 +1421,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>141</v>
+        <v>9</v>
       </c>
       <c r="C6" s="22">
         <v>2007</v>
@@ -1435,7 +1430,7 @@
         <v>2010</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>142</v>
+        <v>10</v>
       </c>
       <c r="F6" s="22">
         <v>2010</v>
@@ -1548,7 +1543,7 @@
         <v>Concentrating_PV</v>
       </c>
       <c r="AO6" s="22" t="s">
-        <v>146</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:41">
@@ -1556,7 +1551,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="C7" s="5">
         <v>2007</v>
@@ -1565,7 +1560,7 @@
         <v>2010</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="F7">
         <v>2004</v>
@@ -1677,7 +1672,7 @@
         <v>Wind</v>
       </c>
       <c r="AO7" t="s">
-        <v>91</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:41">
@@ -1685,7 +1680,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
       <c r="C8" s="5">
         <v>2007</v>
@@ -1694,7 +1689,7 @@
         <v>2010</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="F8">
         <v>2004</v>
@@ -1806,7 +1801,7 @@
         <v>Offshore_Wind</v>
       </c>
       <c r="AO8" t="s">
-        <v>138</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:41">
@@ -1814,7 +1809,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>102</v>
+        <v>37</v>
       </c>
       <c r="C9" s="5">
         <v>2007</v>
@@ -1823,7 +1818,7 @@
         <v>2010</v>
       </c>
       <c r="E9" t="s">
-        <v>109</v>
+        <v>44</v>
       </c>
       <c r="F9">
         <v>2009</v>
@@ -1936,7 +1931,7 @@
         <v>Residential_PV</v>
       </c>
       <c r="AO9" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:41" s="11" customFormat="1">
@@ -1944,7 +1939,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>125</v>
+        <v>60</v>
       </c>
       <c r="C10" s="11">
         <v>2007</v>
@@ -1953,7 +1948,7 @@
         <v>2012</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="F10" s="11">
         <v>2010</v>
@@ -2065,7 +2060,7 @@
         <v>CSP_Trough_6h_Storage</v>
       </c>
       <c r="AO10" s="11" t="s">
-        <v>123</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:41">
@@ -2073,7 +2068,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="C11" s="5">
         <v>2007</v>
@@ -2082,7 +2077,7 @@
         <v>2010</v>
       </c>
       <c r="E11" t="s">
-        <v>110</v>
+        <v>45</v>
       </c>
       <c r="F11">
         <v>2007</v>
@@ -2194,7 +2189,7 @@
         <v>Bio_Gas</v>
       </c>
       <c r="AO11" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:41">
@@ -2202,7 +2197,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>134</v>
       </c>
       <c r="C12" s="5">
         <v>2007</v>
@@ -2211,7 +2206,7 @@
         <v>2010</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="F12">
         <v>2004</v>
@@ -2323,7 +2318,7 @@
         <v>Biomass_Steam_Turbine</v>
       </c>
       <c r="AO12" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:41">
@@ -2331,7 +2326,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="C13" s="5">
         <v>2007</v>
@@ -2340,7 +2335,7 @@
         <v>2012</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="F13">
         <v>2007</v>
@@ -2452,7 +2447,7 @@
         <v>Biomass_IGCC</v>
       </c>
       <c r="AO13" t="s">
-        <v>36</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:41">
@@ -2460,7 +2455,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>142</v>
       </c>
       <c r="C14" s="5">
         <v>2007</v>
@@ -2469,7 +2464,7 @@
         <v>2010</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="F14">
         <v>2004</v>
@@ -2581,7 +2576,7 @@
         <v>Coal_IGCC</v>
       </c>
       <c r="AO14" t="s">
-        <v>111</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:41">
@@ -2589,7 +2584,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>112</v>
+        <v>47</v>
       </c>
       <c r="C15" s="5">
         <v>2007</v>
@@ -2598,7 +2593,7 @@
         <v>2010</v>
       </c>
       <c r="E15" t="s">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="F15">
         <v>2004</v>
@@ -2710,7 +2705,7 @@
         <v>Coal_Steam_Turbine</v>
       </c>
       <c r="AO15" t="s">
-        <v>111</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:41">
@@ -2718,7 +2713,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>113</v>
+        <v>48</v>
       </c>
       <c r="C16" s="5">
         <v>2007</v>
@@ -2727,7 +2722,7 @@
         <v>2010</v>
       </c>
       <c r="E16" t="s">
-        <v>89</v>
+        <v>24</v>
       </c>
       <c r="F16">
         <v>2004</v>
@@ -2839,7 +2834,7 @@
         <v>Nuclear</v>
       </c>
       <c r="AO16" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:41">
@@ -2847,7 +2842,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>114</v>
+        <v>49</v>
       </c>
       <c r="C17" s="5">
         <v>2007</v>
@@ -2856,7 +2851,7 @@
         <v>2010</v>
       </c>
       <c r="E17" t="s">
-        <v>103</v>
+        <v>38</v>
       </c>
       <c r="F17">
         <v>2004</v>
@@ -2968,7 +2963,7 @@
         <v>Geothermal</v>
       </c>
       <c r="AO17" t="s">
-        <v>15</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:41">
@@ -2976,7 +2971,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="C18" s="5">
         <v>2007</v>
@@ -2985,7 +2980,7 @@
         <v>2010</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>32</v>
+        <v>137</v>
       </c>
       <c r="F18" s="5">
         <v>2007</v>
@@ -3097,7 +3092,7 @@
         <v>Hydro_NonPumped</v>
       </c>
       <c r="AO18" s="5" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:41">
@@ -3105,7 +3100,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="C19" s="5">
         <v>2007</v>
@@ -3114,7 +3109,7 @@
         <v>2010</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="F19" s="33">
         <v>2007</v>
@@ -3226,7 +3221,7 @@
         <v>Hydro_Pumped</v>
       </c>
       <c r="AO19" s="5" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:41" s="18" customFormat="1">
@@ -3234,7 +3229,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="C20" s="18">
         <v>2007</v>
@@ -3243,7 +3238,7 @@
         <v>2000</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="F20" s="18">
         <v>2007</v>
@@ -3355,7 +3350,7 @@
         <v>Gas_Combustion_Turbine_EP</v>
       </c>
       <c r="AO20" s="33" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:41" s="5" customFormat="1">
@@ -3363,7 +3358,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
       <c r="C21">
         <v>2007</v>
@@ -3372,7 +3367,7 @@
         <v>2000</v>
       </c>
       <c r="E21" t="s">
-        <v>83</v>
+        <v>18</v>
       </c>
       <c r="F21" s="33">
         <v>2007</v>
@@ -3484,7 +3479,7 @@
         <v>Coal_Steam_Turbine_EP</v>
       </c>
       <c r="AO21" s="33" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:41" s="5" customFormat="1">
@@ -3492,7 +3487,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>27</v>
+        <v>132</v>
       </c>
       <c r="C22" s="33">
         <v>2007</v>
@@ -3501,7 +3496,7 @@
         <v>2000</v>
       </c>
       <c r="E22" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F22" s="33">
         <v>2007</v>
@@ -3613,7 +3608,7 @@
         <v>Gas_Steam_Turbine_EP</v>
       </c>
       <c r="AO22" s="33" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:41" s="5" customFormat="1">
@@ -3621,7 +3616,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="C23" s="33">
         <v>2007</v>
@@ -3630,7 +3625,7 @@
         <v>2000</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F23" s="33">
         <v>2007</v>
@@ -3742,7 +3737,7 @@
         <v>CCGT_EP</v>
       </c>
       <c r="AO23" s="33" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:41" s="5" customFormat="1">
@@ -3750,7 +3745,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="C24" s="33">
         <v>2007</v>
@@ -3759,7 +3754,7 @@
         <v>2000</v>
       </c>
       <c r="E24" t="s">
-        <v>114</v>
+        <v>49</v>
       </c>
       <c r="F24" s="33">
         <v>2007</v>
@@ -3871,7 +3866,7 @@
         <v>Geothermal_EP</v>
       </c>
       <c r="AO24" s="33" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:41" s="5" customFormat="1">
@@ -3879,7 +3874,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>131</v>
+        <v>66</v>
       </c>
       <c r="C25" s="33">
         <v>2007</v>
@@ -3888,7 +3883,7 @@
         <v>2000</v>
       </c>
       <c r="E25" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="F25" s="33">
         <v>2007</v>
@@ -4000,7 +3995,7 @@
         <v>Nuclear_EP</v>
       </c>
       <c r="AO25" s="33" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:41" s="18" customFormat="1">
@@ -4008,7 +4003,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="C26" s="33">
         <v>2007</v>
@@ -4017,7 +4012,7 @@
         <v>2000</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="F26" s="33">
         <v>2007</v>
@@ -4129,7 +4124,7 @@
         <v>Wind_EP</v>
       </c>
       <c r="AO26" s="33" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:41" s="33" customFormat="1">
@@ -4137,7 +4132,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C27" s="33">
         <v>2007</v>
@@ -4146,7 +4141,7 @@
         <v>2000</v>
       </c>
       <c r="E27" s="33" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="F27" s="33">
         <v>2007</v>
@@ -4258,7 +4253,7 @@
         <v>Gas_Internal_Combustion_Engine_EP</v>
       </c>
       <c r="AO27" s="33" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:41" s="8" customFormat="1">
@@ -4266,7 +4261,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="C28" s="8">
         <v>2007</v>
@@ -4275,7 +4270,7 @@
         <v>2010</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="F28" s="8">
         <v>2009</v>
@@ -4387,7 +4382,7 @@
         <v>Commercial_PV</v>
       </c>
       <c r="AO28" s="9" t="s">
-        <v>100</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:41" s="8" customFormat="1">
@@ -4395,7 +4390,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>127</v>
+        <v>62</v>
       </c>
       <c r="C29" s="8">
         <v>2007</v>
@@ -4404,7 +4399,7 @@
         <v>2010</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="F29" s="8">
         <v>2009</v>
@@ -4516,7 +4511,7 @@
         <v>Central_PV</v>
       </c>
       <c r="AO29" s="9" t="s">
-        <v>100</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:41" s="5" customFormat="1">
@@ -4524,7 +4519,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>124</v>
+        <v>59</v>
       </c>
       <c r="C30" s="5">
         <v>2007</v>
@@ -4533,7 +4528,7 @@
         <v>2010</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="F30" s="5">
         <v>2010</v>
@@ -4645,7 +4640,7 @@
         <v>CSP_Trough_No_Storage</v>
       </c>
       <c r="AO30" s="9" t="s">
-        <v>41</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:41" s="9" customFormat="1" ht="15" customHeight="1">
@@ -4653,7 +4648,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>104</v>
+        <v>39</v>
       </c>
       <c r="C31" s="9">
         <v>2007</v>
@@ -4662,7 +4657,7 @@
         <v>2010</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>105</v>
+        <v>40</v>
       </c>
       <c r="F31" s="9">
         <v>2010</v>
@@ -4774,7 +4769,7 @@
         <v>Compressed_Air_Energy_Storage</v>
       </c>
       <c r="AO31" s="32" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:41" s="19" customFormat="1">
@@ -4782,7 +4777,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="C32" s="33">
         <v>2007</v>
@@ -4791,7 +4786,7 @@
         <v>2000</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="F32" s="19">
         <v>2007</v>
@@ -4908,7 +4903,7 @@
         <v>Gas_Combustion_Turbine_Cogen_EP</v>
       </c>
       <c r="AO32" s="33" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:41" s="19" customFormat="1">
@@ -4916,7 +4911,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="C33" s="33">
         <v>2007</v>
@@ -4925,7 +4920,7 @@
         <v>2000</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>83</v>
+        <v>18</v>
       </c>
       <c r="F33" s="33">
         <v>2007</v>
@@ -5042,7 +5037,7 @@
         <v>Coal_Steam_Turbine_Cogen_EP</v>
       </c>
       <c r="AO33" s="33" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:41" s="19" customFormat="1">
@@ -5050,7 +5045,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="C34" s="33">
         <v>2007</v>
@@ -5059,7 +5054,7 @@
         <v>2000</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F34" s="33">
         <v>2007</v>
@@ -5176,7 +5171,7 @@
         <v>Gas_Steam_Turbine_Cogen_EP</v>
       </c>
       <c r="AO34" s="33" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:41" s="19" customFormat="1">
@@ -5184,7 +5179,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="C35" s="33">
         <v>2007</v>
@@ -5193,7 +5188,7 @@
         <v>2000</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F35" s="33">
         <v>2007</v>
@@ -5310,7 +5305,7 @@
         <v>CCGT_Cogen_EP</v>
       </c>
       <c r="AO35" s="33" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:41" s="23" customFormat="1">
@@ -5318,7 +5313,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>22</v>
+        <v>127</v>
       </c>
       <c r="C36" s="23">
         <v>2007</v>
@@ -5327,7 +5322,7 @@
         <v>2010</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="F36" s="23">
         <v>2004</v>
@@ -5439,7 +5434,7 @@
         <v>Battery_Storage</v>
       </c>
       <c r="AO36" s="23" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:41" s="26" customFormat="1">
@@ -5447,7 +5442,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
       <c r="C37" s="26">
         <v>2007</v>
@@ -5456,7 +5451,7 @@
         <v>2014</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="F37" s="26">
         <v>2004</v>
@@ -5573,7 +5568,7 @@
         <v>CCGT_CCS</v>
       </c>
       <c r="AO37" s="33" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:41" s="26" customFormat="1">
@@ -5581,7 +5576,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="C38" s="26">
         <v>2007</v>
@@ -5590,7 +5585,7 @@
         <v>2014</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="F38" s="26">
         <v>2004</v>
@@ -5708,7 +5703,7 @@
         <v>Gas_Combustion_Turbine_CCS</v>
       </c>
       <c r="AO38" s="33" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:41" s="26" customFormat="1">
@@ -5716,7 +5711,7 @@
         <v>36</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="C39" s="26">
         <v>2007</v>
@@ -5725,7 +5720,7 @@
         <v>2014</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="F39" s="26">
         <v>2004</v>
@@ -5843,7 +5838,7 @@
         <v>Bio_Gas_CCS</v>
       </c>
       <c r="AO39" s="33" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:41" s="26" customFormat="1">
@@ -5851,7 +5846,7 @@
         <v>37</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="C40" s="26">
         <v>2007</v>
@@ -5860,7 +5855,7 @@
         <v>2014</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
       <c r="F40" s="26">
         <v>2004</v>
@@ -5978,7 +5973,7 @@
         <v>Biomass_IGCC_CCS</v>
       </c>
       <c r="AO40" s="33" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:41" s="26" customFormat="1">
@@ -5986,7 +5981,7 @@
         <v>38</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
       <c r="C41" s="26">
         <v>2007</v>
@@ -5995,7 +5990,7 @@
         <v>2014</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>42</v>
+        <v>147</v>
       </c>
       <c r="F41" s="26">
         <v>2004</v>
@@ -6083,7 +6078,7 @@
         <v>1</v>
       </c>
       <c r="AF41" s="33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG41" s="33">
         <v>0</v>
@@ -6111,7 +6106,7 @@
         <v>Coal_IGCC_CCS</v>
       </c>
       <c r="AO41" s="33" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:41" s="26" customFormat="1">
@@ -6119,7 +6114,7 @@
         <v>39</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="C42" s="26">
         <v>2007</v>
@@ -6128,7 +6123,7 @@
         <v>2014</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>42</v>
+        <v>147</v>
       </c>
       <c r="F42" s="26">
         <v>2004</v>
@@ -6218,7 +6213,7 @@
         <v>1</v>
       </c>
       <c r="AF42" s="33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG42" s="33">
         <v>0</v>
@@ -6246,7 +6241,7 @@
         <v>Coal_Steam_Turbine_CCS</v>
       </c>
       <c r="AO42" s="33" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:41" s="33" customFormat="1">
@@ -6254,7 +6249,7 @@
         <v>40</v>
       </c>
       <c r="B43" s="33" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="C43" s="33">
         <v>2007</v>
@@ -6263,7 +6258,7 @@
         <v>2000</v>
       </c>
       <c r="E43" s="33" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F43" s="33">
         <v>2007</v>
@@ -6379,7 +6374,7 @@
         <v>Gas_Internal_Combustion_Engine_Cogen_EP</v>
       </c>
       <c r="AO43" s="33" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:41" s="28" customFormat="1">
@@ -6387,7 +6382,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C44" s="28">
         <v>2007</v>
@@ -6396,7 +6391,7 @@
         <v>2014</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="F44" s="28">
         <v>2004</v>
@@ -6508,10 +6503,10 @@
         <v>0</v>
       </c>
       <c r="AN44" s="28" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="AO44" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:41" s="28" customFormat="1">
@@ -6519,7 +6514,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>121</v>
+        <v>56</v>
       </c>
       <c r="C45" s="28">
         <v>2007</v>
@@ -6528,7 +6523,7 @@
         <v>2014</v>
       </c>
       <c r="E45" s="30" t="s">
-        <v>42</v>
+        <v>147</v>
       </c>
       <c r="F45" s="28">
         <v>2004</v>
@@ -6639,10 +6634,10 @@
         <v>0</v>
       </c>
       <c r="AN45" s="28" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="AO45" s="33" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:41" s="28" customFormat="1">
@@ -6650,7 +6645,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>122</v>
+        <v>57</v>
       </c>
       <c r="C46" s="28">
         <v>2007</v>
@@ -6659,7 +6654,7 @@
         <v>2014</v>
       </c>
       <c r="E46" s="30" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="F46" s="28">
         <v>2004</v>
@@ -6771,10 +6766,10 @@
         <v>0</v>
       </c>
       <c r="AN46" s="28" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="AO46" s="33" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:41" s="28" customFormat="1">
@@ -6782,7 +6777,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="28" t="s">
-        <v>133</v>
+        <v>1</v>
       </c>
       <c r="C47" s="28">
         <v>2007</v>
@@ -6791,7 +6786,7 @@
         <v>2014</v>
       </c>
       <c r="E47" s="30" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="F47" s="28">
         <v>2004</v>
@@ -6902,10 +6897,10 @@
         <v>0</v>
       </c>
       <c r="AN47" s="28" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="AO47" s="33" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:41" s="28" customFormat="1">
@@ -6913,7 +6908,7 @@
         <v>45</v>
       </c>
       <c r="B48" s="28" t="s">
-        <v>134</v>
+        <v>2</v>
       </c>
       <c r="C48" s="28">
         <v>2007</v>
@@ -6922,7 +6917,7 @@
         <v>2014</v>
       </c>
       <c r="E48" s="30" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="F48" s="28">
         <v>2004</v>
@@ -7036,10 +7031,10 @@
         <v>0</v>
       </c>
       <c r="AN48" s="28" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="AO48" s="33" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:41" s="28" customFormat="1">
@@ -7047,7 +7042,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="28" t="s">
-        <v>135</v>
+        <v>3</v>
       </c>
       <c r="C49" s="28">
         <v>2007</v>
@@ -7056,7 +7051,7 @@
         <v>2014</v>
       </c>
       <c r="E49" s="30" t="s">
-        <v>42</v>
+        <v>147</v>
       </c>
       <c r="F49" s="28">
         <v>2004</v>
@@ -7170,10 +7165,10 @@
         <v>0</v>
       </c>
       <c r="AN49" s="28" t="s">
-        <v>116</v>
+        <v>51</v>
       </c>
       <c r="AO49" s="33" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:41" s="28" customFormat="1">
@@ -7181,7 +7176,7 @@
         <v>47</v>
       </c>
       <c r="B50" s="28" t="s">
-        <v>136</v>
+        <v>4</v>
       </c>
       <c r="C50" s="28">
         <v>2007</v>
@@ -7190,7 +7185,7 @@
         <v>2014</v>
       </c>
       <c r="E50" s="30" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="F50" s="28">
         <v>2004</v>
@@ -7304,10 +7299,10 @@
         <v>0</v>
       </c>
       <c r="AN50" s="28" t="s">
-        <v>117</v>
+        <v>52</v>
       </c>
       <c r="AO50" s="33" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:41" s="28" customFormat="1">
@@ -7315,7 +7310,7 @@
         <v>48</v>
       </c>
       <c r="B51" s="28" t="s">
-        <v>137</v>
+        <v>5</v>
       </c>
       <c r="C51" s="28">
         <v>2007</v>
@@ -7324,7 +7319,7 @@
         <v>2014</v>
       </c>
       <c r="E51" s="30" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="F51" s="28">
         <v>2004</v>
@@ -7438,10 +7433,10 @@
         <v>0</v>
       </c>
       <c r="AN51" s="28" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="AO51" s="33" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:41" s="5" customFormat="1">
@@ -7606,7 +7601,6 @@
       <c r="A104" s="33"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -12675,7 +12669,7 @@
       </c>
       <c r="Y39" s="33">
         <f>generator_costs!AF41</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z39" s="33">
         <f>generator_costs!AG41</f>
@@ -12805,7 +12799,7 @@
       </c>
       <c r="Y40" s="33">
         <f>generator_costs!AF42</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z40" s="33">
         <f>generator_costs!AG42</f>
@@ -14019,7 +14013,6 @@
       <c r="A53" s="33"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -14042,7 +14035,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="6" t="s">
-        <v>140</v>
+        <v>8</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -14053,7 +14046,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>2010</v>
@@ -14071,7 +14064,7 @@
         <v>2026</v>
       </c>
       <c r="G2" t="s">
-        <v>139</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -15515,7 +15508,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -15538,15 +15530,15 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="22" t="s">
-        <v>143</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="22" t="s">
-        <v>144</v>
+        <v>12</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>145</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="22" customFormat="1">
@@ -15574,7 +15566,7 @@
         <v>3.3</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>147</v>
+        <v>15</v>
       </c>
       <c r="E5" s="22"/>
     </row>
@@ -15727,7 +15719,6 @@
       <c r="E21" s="22"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
- made unified sets AVAILABLE_VINTAGES and AVAILABLE_HOURS, which encompass every existing and new plant - hydro and existing plant costs changed to be brought calculated alongside new plants - hydro aggregated to the load area level gets a start year of 2000 for this intermediate code - added pumped hydro storage params to generator_costs.csv
- added discount_to_base_year to simplify financials

- took out InstallGenTotal from the main model because it was taking too long to compile (solveout step of compliation)
-- instead added Installed_To_Date to basicstats.run
</commit_message>
<xml_diff>
--- a/DatabasePrep/GeneratorInfo/generator_costs.xlsx
+++ b/DatabasePrep/GeneratorInfo/generator_costs.xlsx
@@ -22,71 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="148">
-  <si>
-    <t>Wind</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCGT_CCS_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine_Cogen_CCS_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_Cogen_CCS_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_Cogen_CCS_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCGT_Cogen_CCS_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, EIA says minimum learning by 2025 is 20%, so this is a 1.1% declination rate, capital cost multipulier from EIA,http://graysharboroceanenergy.com/Documents/LIPA%20Offshore%20Wind%20rept.pdf for total outage rate of 3%, distributed by guess</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cost Declination Rate (%/yr)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resultant Capital Costs ($2007/MW) in Investment Period Years</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Concentrating_PV</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Solar</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(in 2010 $)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>year</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>$/Wp</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CPV Consortium numbers (It's more or less SolFocus)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>cost declination rate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="149">
   <si>
     <t>Gas_Steam_Turbine_Cogen_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -205,74 +141,6 @@
     <t>Nuclear</t>
   </si>
   <si>
-    <t>Geothermal</t>
-  </si>
-  <si>
-    <t>construction_time_years</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_Cogen_EP</t>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_Cogen_EP</t>
-  </si>
-  <si>
-    <t>connect_cost_generic_$2007_per_mw</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>fuel</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_CCS_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_CCS_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CapEx from SAM with Solar Field area = 800000m^2 and 6h TES, construction cost mulitplier and yearly cost fraction from CSP on ReEDs sheet- it's unclear how much these change with storage... assumed to be the same here, cost declination rate and fixed OM from Mark Mehos estimate on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSP_Trough_No_Storage</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSP_Trough_6h_Storage</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wind</t>
-  </si>
-  <si>
-    <t>Central_PV</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>construction_cost_multipulier</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed_o_m</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>var_o_m</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nuclear_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to gas combustion turbine</t>
   </si>
   <si>
@@ -358,67 +226,67 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">ReEDs Sheet; also Sullivan et al (2008), NREL/CP-670-43510 Conference Paper for o&amp;m costs, declanation rate, etc; $1,200,000 taken as capital cost in 2010 rather than 2004 based on conversation with Hernandez, also The storage efficiency of the the storage phase of compressed air energy storage from Samir Succar and Robert H. Williams: Compressed Air Energy Storage: Theory, Resources, And Applications For Wind Power, p. 39
-</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCGT_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Wind</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>price_and_dollar_year</t>
+    <t>CCGT_CCS_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Gas</t>
-  </si>
-  <si>
-    <t>year_4_cost_fraction</t>
+    <t>Gas_Combustion_Turbine_Cogen_CCS_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>year_5_cost_fraction</t>
+    <t>Coal_Steam_Turbine_Cogen_CCS_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>year_6_cost_fraction</t>
+    <t>Gas_Steam_Turbine_Cogen_CCS_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>fixed_o_m_$2007</t>
+    <t>CCGT_Cogen_CCS_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>heat_rate_mbtu_per_mwh</t>
+    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, EIA says minimum learning by 2025 is 20%, so this is a 1.1% declination rate, capital cost multipulier from EIA,http://graysharboroceanenergy.com/Documents/LIPA%20Offshore%20Wind%20rept.pdf for total outage rate of 3%, distributed by guess</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Commercial_PV</t>
+    <t>Cost Declination Rate (%/yr)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>min_build_year</t>
+    <t>Resultant Capital Costs ($2007/MW) in Investment Period Years</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Gas_Combustion_Turbine_Cogen_EP</t>
+    <t>Concentrating_PV</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Coal_Steam_Turbine_Cogen_EP</t>
+    <t>Solar</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>ReEDs Sheet, also new wind params used for fixed O+M, forced outage rate</t>
+    <t>(in 2010 $)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>year</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>$/Wp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPV Consortium numbers (It's more or less SolFocus)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>cost declination rate</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -516,6 +384,74 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>Geothermal</t>
+  </si>
+  <si>
+    <t>construction_time_years</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_Cogen_EP</t>
+  </si>
+  <si>
+    <t>Gas_Steam_Turbine_Cogen_EP</t>
+  </si>
+  <si>
+    <t>connect_cost_generic_$2007_per_mw</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>fuel</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_CCS_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Steam_Turbine_CCS_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CapEx from SAM with Solar Field area = 800000m^2 and 6h TES, construction cost mulitplier and yearly cost fraction from CSP on ReEDs sheet- it's unclear how much these change with storage... assumed to be the same here, cost declination rate and fixed OM from Mark Mehos estimate on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSP_Trough_No_Storage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSP_Trough_6h_Storage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Central_PV</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>construction_cost_multipulier</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed_o_m</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>var_o_m</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nuclear_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>Coal_Steam_Turbine_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -577,14 +513,83 @@
     <t>Coal_CCS</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>ReEDs Sheet, storage effiency from Samir Succar and Robert H. Williams: Compressed Air Energy Storage: Theory, Resources, And Applications For Wind Power, p. 39</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ReEDs Sheet; also Sullivan et al (2008), NREL/CP-670-43510 Conference Paper for o&amp;m costs, declanation rate, etc; $1,200,000 taken as capital cost in 2010 rather than 2004 based on conversation with Hernandez, also The storage efficiency of the the storage phase of compressed air energy storage from Samir Succar and Robert H. Williams: Compressed Air Energy Storage: Theory, Resources, And Applications For Wind Power, p. 39
+</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCGT_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>price_and_dollar_year</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>year_4_cost_fraction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_5_cost_fraction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_6_cost_fraction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed_o_m_$2007</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>heat_rate_mbtu_per_mwh</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commercial_PV</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>min_build_year</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_Cogen_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_Cogen_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, also new wind params used for fixed O+M, forced outage rate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -629,7 +634,7 @@
   <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -651,7 +656,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -996,8 +1001,8 @@
   <dimension ref="A1:AO104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AF1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AF50" sqref="AF50"/>
+      <pane xSplit="2" topLeftCell="AG1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AM19" sqref="AM19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1029,133 +1034,133 @@
   <sheetData>
     <row r="1" spans="1:41" s="33" customFormat="1">
       <c r="A1" s="34" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:41" s="33" customFormat="1"/>
     <row r="3" spans="1:41">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" t="s">
+        <v>111</v>
+      </c>
+      <c r="K3" t="s">
+        <v>112</v>
+      </c>
+      <c r="L3" t="s">
+        <v>113</v>
+      </c>
+      <c r="M3" t="s">
+        <v>85</v>
+      </c>
+      <c r="N3" t="s">
+        <v>142</v>
+      </c>
+      <c r="O3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>101</v>
+      </c>
+      <c r="R3" t="s">
+        <v>143</v>
+      </c>
+      <c r="S3" t="s">
+        <v>98</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L3" t="s">
-        <v>65</v>
-      </c>
-      <c r="M3" t="s">
-        <v>119</v>
-      </c>
-      <c r="N3" t="s">
-        <v>99</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="AA3" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF3" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG3" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ3" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK3" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN3" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="AO3" t="s">
         <v>25</v>
-      </c>
-      <c r="P3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>53</v>
-      </c>
-      <c r="R3" t="s">
-        <v>100</v>
-      </c>
-      <c r="S3" t="s">
-        <v>50</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="Y3" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>145</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF3" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG3" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>143</v>
-      </c>
-      <c r="AJ3" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK3" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>20</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>21</v>
-      </c>
-      <c r="AN3" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:41">
@@ -1163,7 +1168,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="C4" s="5">
         <v>2007</v>
@@ -1172,7 +1177,7 @@
         <v>2010</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="F4">
         <v>2004</v>
@@ -1284,7 +1289,7 @@
         <v>CCGT</v>
       </c>
       <c r="AO4" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:41">
@@ -1292,7 +1297,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="C5" s="5">
         <v>2007</v>
@@ -1301,7 +1306,7 @@
         <v>2010</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="F5">
         <v>2004</v>
@@ -1413,7 +1418,7 @@
         <v>Gas_Combustion_Turbine</v>
       </c>
       <c r="AO5" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:41" s="22" customFormat="1">
@@ -1421,7 +1426,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="C6" s="22">
         <v>2007</v>
@@ -1430,7 +1435,7 @@
         <v>2010</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="F6" s="22">
         <v>2010</v>
@@ -1543,7 +1548,7 @@
         <v>Concentrating_PV</v>
       </c>
       <c r="AO6" s="22" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:41">
@@ -1551,7 +1556,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="C7" s="5">
         <v>2007</v>
@@ -1560,7 +1565,7 @@
         <v>2010</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
       <c r="F7">
         <v>2004</v>
@@ -1672,7 +1677,7 @@
         <v>Wind</v>
       </c>
       <c r="AO7" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:41">
@@ -1680,7 +1685,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="C8" s="5">
         <v>2007</v>
@@ -1689,7 +1694,7 @@
         <v>2010</v>
       </c>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
       <c r="F8">
         <v>2004</v>
@@ -1801,7 +1806,7 @@
         <v>Offshore_Wind</v>
       </c>
       <c r="AO8" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:41">
@@ -1809,7 +1814,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C9" s="5">
         <v>2007</v>
@@ -1818,7 +1823,7 @@
         <v>2010</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="F9">
         <v>2009</v>
@@ -1931,7 +1936,7 @@
         <v>Residential_PV</v>
       </c>
       <c r="AO9" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:41" s="11" customFormat="1">
@@ -1939,7 +1944,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="C10" s="11">
         <v>2007</v>
@@ -1948,7 +1953,7 @@
         <v>2012</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="F10" s="11">
         <v>2010</v>
@@ -2060,7 +2065,7 @@
         <v>CSP_Trough_6h_Storage</v>
       </c>
       <c r="AO10" s="11" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:41">
@@ -2068,7 +2073,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="C11" s="5">
         <v>2007</v>
@@ -2077,7 +2082,7 @@
         <v>2010</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="F11">
         <v>2007</v>
@@ -2189,7 +2194,7 @@
         <v>Bio_Gas</v>
       </c>
       <c r="AO11" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:41">
@@ -2197,7 +2202,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="C12" s="5">
         <v>2007</v>
@@ -2206,7 +2211,7 @@
         <v>2010</v>
       </c>
       <c r="E12" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="F12">
         <v>2004</v>
@@ -2318,7 +2323,7 @@
         <v>Biomass_Steam_Turbine</v>
       </c>
       <c r="AO12" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:41">
@@ -2326,7 +2331,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="C13" s="5">
         <v>2007</v>
@@ -2335,7 +2340,7 @@
         <v>2012</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="F13">
         <v>2007</v>
@@ -2447,7 +2452,7 @@
         <v>Biomass_IGCC</v>
       </c>
       <c r="AO13" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:41">
@@ -2455,7 +2460,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C14" s="5">
         <v>2007</v>
@@ -2464,7 +2469,7 @@
         <v>2010</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F14">
         <v>2004</v>
@@ -2576,7 +2581,7 @@
         <v>Coal_IGCC</v>
       </c>
       <c r="AO14" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:41">
@@ -2584,7 +2589,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C15" s="5">
         <v>2007</v>
@@ -2593,7 +2598,7 @@
         <v>2010</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F15">
         <v>2004</v>
@@ -2705,7 +2710,7 @@
         <v>Coal_Steam_Turbine</v>
       </c>
       <c r="AO15" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:41">
@@ -2713,7 +2718,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C16" s="5">
         <v>2007</v>
@@ -2722,7 +2727,7 @@
         <v>2010</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F16">
         <v>2004</v>
@@ -2834,7 +2839,7 @@
         <v>Nuclear</v>
       </c>
       <c r="AO16" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:41">
@@ -2842,7 +2847,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="C17" s="5">
         <v>2007</v>
@@ -2851,7 +2856,7 @@
         <v>2010</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="F17">
         <v>2004</v>
@@ -2963,7 +2968,7 @@
         <v>Geothermal</v>
       </c>
       <c r="AO17" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:41">
@@ -2971,7 +2976,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="C18" s="5">
         <v>2007</v>
@@ -2980,7 +2985,7 @@
         <v>2010</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="F18" s="5">
         <v>2007</v>
@@ -3092,7 +3097,7 @@
         <v>Hydro_NonPumped</v>
       </c>
       <c r="AO18" s="5" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:41">
@@ -3100,7 +3105,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="C19" s="5">
         <v>2007</v>
@@ -3109,7 +3114,7 @@
         <v>2010</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F19" s="33">
         <v>2007</v>
@@ -3211,17 +3216,17 @@
         <v>0</v>
       </c>
       <c r="AL19">
-        <v>0</v>
+        <v>0.74</v>
       </c>
       <c r="AM19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN19" s="22" t="str">
         <f t="shared" si="3"/>
         <v>Hydro_Pumped</v>
       </c>
-      <c r="AO19" s="5" t="s">
-        <v>110</v>
+      <c r="AO19" s="33" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:41" s="18" customFormat="1">
@@ -3229,7 +3234,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>92</v>
+        <v>135</v>
       </c>
       <c r="C20" s="18">
         <v>2007</v>
@@ -3238,7 +3243,7 @@
         <v>2000</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="F20" s="18">
         <v>2007</v>
@@ -3350,7 +3355,7 @@
         <v>Gas_Combustion_Turbine_EP</v>
       </c>
       <c r="AO20" s="33" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:41" s="5" customFormat="1">
@@ -3358,7 +3363,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="C21">
         <v>2007</v>
@@ -3367,7 +3372,7 @@
         <v>2000</v>
       </c>
       <c r="E21" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="F21" s="33">
         <v>2007</v>
@@ -3479,7 +3484,7 @@
         <v>Coal_Steam_Turbine_EP</v>
       </c>
       <c r="AO21" s="33" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:41" s="5" customFormat="1">
@@ -3487,7 +3492,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="C22" s="33">
         <v>2007</v>
@@ -3496,7 +3501,7 @@
         <v>2000</v>
       </c>
       <c r="E22" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="F22" s="33">
         <v>2007</v>
@@ -3608,7 +3613,7 @@
         <v>Gas_Steam_Turbine_EP</v>
       </c>
       <c r="AO22" s="33" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:41" s="5" customFormat="1">
@@ -3616,7 +3621,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
       <c r="C23" s="33">
         <v>2007</v>
@@ -3625,7 +3630,7 @@
         <v>2000</v>
       </c>
       <c r="E23" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="F23" s="33">
         <v>2007</v>
@@ -3737,7 +3742,7 @@
         <v>CCGT_EP</v>
       </c>
       <c r="AO23" s="33" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:41" s="5" customFormat="1">
@@ -3745,7 +3750,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="C24" s="33">
         <v>2007</v>
@@ -3754,7 +3759,7 @@
         <v>2000</v>
       </c>
       <c r="E24" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="F24" s="33">
         <v>2007</v>
@@ -3866,7 +3871,7 @@
         <v>Geothermal_EP</v>
       </c>
       <c r="AO24" s="33" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:41" s="5" customFormat="1">
@@ -3874,7 +3879,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>66</v>
+        <v>114</v>
       </c>
       <c r="C25" s="33">
         <v>2007</v>
@@ -3883,7 +3888,7 @@
         <v>2000</v>
       </c>
       <c r="E25" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="F25" s="33">
         <v>2007</v>
@@ -3995,7 +4000,7 @@
         <v>Nuclear_EP</v>
       </c>
       <c r="AO25" s="33" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:41" s="18" customFormat="1">
@@ -4003,7 +4008,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="C26" s="33">
         <v>2007</v>
@@ -4012,7 +4017,7 @@
         <v>2000</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="F26" s="33">
         <v>2007</v>
@@ -4124,7 +4129,7 @@
         <v>Wind_EP</v>
       </c>
       <c r="AO26" s="33" t="s">
-        <v>105</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:41" s="33" customFormat="1">
@@ -4132,7 +4137,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="C27" s="33">
         <v>2007</v>
@@ -4141,7 +4146,7 @@
         <v>2000</v>
       </c>
       <c r="E27" s="33" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="F27" s="33">
         <v>2007</v>
@@ -4253,7 +4258,7 @@
         <v>Gas_Internal_Combustion_Engine_EP</v>
       </c>
       <c r="AO27" s="33" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:41" s="8" customFormat="1">
@@ -4261,7 +4266,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="C28" s="8">
         <v>2007</v>
@@ -4270,7 +4275,7 @@
         <v>2010</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="F28" s="8">
         <v>2009</v>
@@ -4382,7 +4387,7 @@
         <v>Commercial_PV</v>
       </c>
       <c r="AO28" s="9" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:41" s="8" customFormat="1">
@@ -4390,7 +4395,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="C29" s="8">
         <v>2007</v>
@@ -4399,7 +4404,7 @@
         <v>2010</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="F29" s="8">
         <v>2009</v>
@@ -4511,7 +4516,7 @@
         <v>Central_PV</v>
       </c>
       <c r="AO29" s="9" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:41" s="5" customFormat="1">
@@ -4519,7 +4524,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="C30" s="5">
         <v>2007</v>
@@ -4528,7 +4533,7 @@
         <v>2010</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="F30" s="5">
         <v>2010</v>
@@ -4640,7 +4645,7 @@
         <v>CSP_Trough_No_Storage</v>
       </c>
       <c r="AO30" s="9" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:41" s="9" customFormat="1" ht="15" customHeight="1">
@@ -4648,7 +4653,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C31" s="9">
         <v>2007</v>
@@ -4657,7 +4662,7 @@
         <v>2010</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="F31" s="9">
         <v>2010</v>
@@ -4769,7 +4774,7 @@
         <v>Compressed_Air_Energy_Storage</v>
       </c>
       <c r="AO31" s="32" t="s">
-        <v>90</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:41" s="19" customFormat="1">
@@ -4777,7 +4782,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="C32" s="33">
         <v>2007</v>
@@ -4786,7 +4791,7 @@
         <v>2000</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="F32" s="19">
         <v>2007</v>
@@ -4903,7 +4908,7 @@
         <v>Gas_Combustion_Turbine_Cogen_EP</v>
       </c>
       <c r="AO32" s="33" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:41" s="19" customFormat="1">
@@ -4911,7 +4916,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>104</v>
+        <v>147</v>
       </c>
       <c r="C33" s="33">
         <v>2007</v>
@@ -4920,7 +4925,7 @@
         <v>2000</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="F33" s="33">
         <v>2007</v>
@@ -5037,7 +5042,7 @@
         <v>Coal_Steam_Turbine_Cogen_EP</v>
       </c>
       <c r="AO33" s="33" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:41" s="19" customFormat="1">
@@ -5045,7 +5050,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C34" s="33">
         <v>2007</v>
@@ -5054,7 +5059,7 @@
         <v>2000</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="F34" s="33">
         <v>2007</v>
@@ -5171,7 +5176,7 @@
         <v>Gas_Steam_Turbine_Cogen_EP</v>
       </c>
       <c r="AO34" s="33" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:41" s="19" customFormat="1">
@@ -5179,7 +5184,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C35" s="33">
         <v>2007</v>
@@ -5188,7 +5193,7 @@
         <v>2000</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="F35" s="33">
         <v>2007</v>
@@ -5305,7 +5310,7 @@
         <v>CCGT_Cogen_EP</v>
       </c>
       <c r="AO35" s="33" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:41" s="23" customFormat="1">
@@ -5313,7 +5318,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="C36" s="23">
         <v>2007</v>
@@ -5322,7 +5327,7 @@
         <v>2010</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="F36" s="23">
         <v>2004</v>
@@ -5434,7 +5439,7 @@
         <v>Battery_Storage</v>
       </c>
       <c r="AO36" s="23" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:41" s="26" customFormat="1">
@@ -5442,7 +5447,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="C37" s="26">
         <v>2007</v>
@@ -5451,7 +5456,7 @@
         <v>2014</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="F37" s="26">
         <v>2004</v>
@@ -5568,7 +5573,7 @@
         <v>CCGT_CCS</v>
       </c>
       <c r="AO37" s="33" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:41" s="26" customFormat="1">
@@ -5576,7 +5581,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="C38" s="26">
         <v>2007</v>
@@ -5585,7 +5590,7 @@
         <v>2014</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="F38" s="26">
         <v>2004</v>
@@ -5703,7 +5708,7 @@
         <v>Gas_Combustion_Turbine_CCS</v>
       </c>
       <c r="AO38" s="33" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:41" s="26" customFormat="1">
@@ -5711,7 +5716,7 @@
         <v>36</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="C39" s="26">
         <v>2007</v>
@@ -5720,7 +5725,7 @@
         <v>2014</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="F39" s="26">
         <v>2004</v>
@@ -5838,7 +5843,7 @@
         <v>Bio_Gas_CCS</v>
       </c>
       <c r="AO39" s="33" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:41" s="26" customFormat="1">
@@ -5846,7 +5851,7 @@
         <v>37</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="C40" s="26">
         <v>2007</v>
@@ -5855,7 +5860,7 @@
         <v>2014</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="F40" s="26">
         <v>2004</v>
@@ -5973,7 +5978,7 @@
         <v>Biomass_IGCC_CCS</v>
       </c>
       <c r="AO40" s="33" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:41" s="26" customFormat="1">
@@ -5981,7 +5986,7 @@
         <v>38</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="C41" s="26">
         <v>2007</v>
@@ -5990,7 +5995,7 @@
         <v>2014</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="F41" s="26">
         <v>2004</v>
@@ -6106,7 +6111,7 @@
         <v>Coal_IGCC_CCS</v>
       </c>
       <c r="AO41" s="33" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:41" s="26" customFormat="1">
@@ -6114,7 +6119,7 @@
         <v>39</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="C42" s="26">
         <v>2007</v>
@@ -6123,7 +6128,7 @@
         <v>2014</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="F42" s="26">
         <v>2004</v>
@@ -6241,7 +6246,7 @@
         <v>Coal_Steam_Turbine_CCS</v>
       </c>
       <c r="AO42" s="33" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:41" s="33" customFormat="1">
@@ -6249,7 +6254,7 @@
         <v>40</v>
       </c>
       <c r="B43" s="33" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="C43" s="33">
         <v>2007</v>
@@ -6258,7 +6263,7 @@
         <v>2000</v>
       </c>
       <c r="E43" s="33" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="F43" s="33">
         <v>2007</v>
@@ -6374,7 +6379,7 @@
         <v>Gas_Internal_Combustion_Engine_Cogen_EP</v>
       </c>
       <c r="AO43" s="33" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:41" s="28" customFormat="1">
@@ -6382,7 +6387,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="C44" s="28">
         <v>2007</v>
@@ -6391,7 +6396,7 @@
         <v>2014</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="F44" s="28">
         <v>2004</v>
@@ -6503,10 +6508,10 @@
         <v>0</v>
       </c>
       <c r="AN44" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO44" t="s">
         <v>76</v>
-      </c>
-      <c r="AO44" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:41" s="28" customFormat="1">
@@ -6514,7 +6519,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="C45" s="28">
         <v>2007</v>
@@ -6523,7 +6528,7 @@
         <v>2014</v>
       </c>
       <c r="E45" s="30" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="F45" s="28">
         <v>2004</v>
@@ -6634,10 +6639,10 @@
         <v>0</v>
       </c>
       <c r="AN45" s="28" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="AO45" s="33" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:41" s="28" customFormat="1">
@@ -6645,7 +6650,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="C46" s="28">
         <v>2007</v>
@@ -6654,7 +6659,7 @@
         <v>2014</v>
       </c>
       <c r="E46" s="30" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="F46" s="28">
         <v>2004</v>
@@ -6766,10 +6771,10 @@
         <v>0</v>
       </c>
       <c r="AN46" s="28" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="AO46" s="33" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:41" s="28" customFormat="1">
@@ -6777,7 +6782,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="28" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C47" s="28">
         <v>2007</v>
@@ -6786,7 +6791,7 @@
         <v>2014</v>
       </c>
       <c r="E47" s="30" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="F47" s="28">
         <v>2004</v>
@@ -6897,10 +6902,10 @@
         <v>0</v>
       </c>
       <c r="AN47" s="28" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="AO47" s="33" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:41" s="28" customFormat="1">
@@ -6908,7 +6913,7 @@
         <v>45</v>
       </c>
       <c r="B48" s="28" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="C48" s="28">
         <v>2007</v>
@@ -6917,7 +6922,7 @@
         <v>2014</v>
       </c>
       <c r="E48" s="30" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="F48" s="28">
         <v>2004</v>
@@ -7031,10 +7036,10 @@
         <v>0</v>
       </c>
       <c r="AN48" s="28" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="AO48" s="33" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:41" s="28" customFormat="1">
@@ -7042,7 +7047,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="28" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C49" s="28">
         <v>2007</v>
@@ -7051,7 +7056,7 @@
         <v>2014</v>
       </c>
       <c r="E49" s="30" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="F49" s="28">
         <v>2004</v>
@@ -7165,10 +7170,10 @@
         <v>0</v>
       </c>
       <c r="AN49" s="28" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="AO49" s="33" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:41" s="28" customFormat="1">
@@ -7176,7 +7181,7 @@
         <v>47</v>
       </c>
       <c r="B50" s="28" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="C50" s="28">
         <v>2007</v>
@@ -7185,7 +7190,7 @@
         <v>2014</v>
       </c>
       <c r="E50" s="30" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="F50" s="28">
         <v>2004</v>
@@ -7299,10 +7304,10 @@
         <v>0</v>
       </c>
       <c r="AN50" s="28" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="AO50" s="33" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:41" s="28" customFormat="1">
@@ -7310,7 +7315,7 @@
         <v>48</v>
       </c>
       <c r="B51" s="28" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C51" s="28">
         <v>2007</v>
@@ -7319,7 +7324,7 @@
         <v>2014</v>
       </c>
       <c r="E51" s="30" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="F51" s="28">
         <v>2004</v>
@@ -7433,10 +7438,10 @@
         <v>0</v>
       </c>
       <c r="AN51" s="28" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="AO51" s="33" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:41" s="5" customFormat="1">
@@ -9833,11 +9838,11 @@
       </c>
       <c r="AE17" s="33">
         <f>generator_costs!AL19</f>
-        <v>0</v>
+        <v>0.74</v>
       </c>
       <c r="AF17" s="33">
         <f>generator_costs!AM19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:32">
@@ -14035,7 +14040,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="6" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -14046,7 +14051,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>2010</v>
@@ -14064,7 +14069,7 @@
         <v>2026</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -15530,15 +15535,15 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="22" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="22" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="22" customFormat="1">
@@ -15566,7 +15571,7 @@
         <v>3.3</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E5" s="22"/>
     </row>

</xml_diff>

<commit_message>
-- gave pumped hydro the 'storage' flag in generator_info -- merged nonpumped hydro and pumped hydro watershed electron dispatch -- added support to include pid in results printout for pumped hydro -- simplified storage record results
</commit_message>
<xml_diff>
--- a/DatabasePrep/GeneratorInfo/generator_costs.xlsx
+++ b/DatabasePrep/GeneratorInfo/generator_costs.xlsx
@@ -23,6 +23,386 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="149">
+  <si>
+    <t>CapEx from SAM with Solar Field area = 600000m^2, construction cost mulitplier and yearly cost fraction from ReEDs sheet, cost declination rate and fixed OM from DOE solar program costs on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_CCS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, storage effiency from Samir Succar and Robert H. Williams: Compressed Air Energy Storage: Theory, Resources, And Applications For Wind Power, p. 39</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ReEDs Sheet; also Sullivan et al (2008), NREL/CP-670-43510 Conference Paper for o&amp;m costs, declanation rate, etc; $1,200,000 taken as capital cost in 2010 rather than 2004 based on conversation with Hernandez, also The storage efficiency of the the storage phase of compressed air energy storage from Samir Succar and Robert H. Williams: Compressed Air Energy Storage: Theory, Resources, And Applications For Wind Power, p. 39
+</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCGT_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>price_and_dollar_year</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>year_4_cost_fraction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_5_cost_fraction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_6_cost_fraction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed_o_m_$2007</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>heat_rate_mbtu_per_mwh</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commercial_PV</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>min_build_year</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_Cogen_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_Cogen_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, also new wind params used for fixed O+M, forced outage rate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, cost declination rate assumed to be between ST and other techs (@1%).  EIA has minimum learning by 2025 as 10%, so this is roughly consistent</t>
+  </si>
+  <si>
+    <t>storage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Offshore_Wind</t>
+  </si>
+  <si>
+    <t>Bio_Gas</t>
+  </si>
+  <si>
+    <t>year_1_cost_fraction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_2_cost_fraction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_3_cost_fraction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery_Storage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Storage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>tech_name_again</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Geothermal</t>
+  </si>
+  <si>
+    <t>construction_time_years</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_Cogen_EP</t>
+  </si>
+  <si>
+    <t>Gas_Steam_Turbine_Cogen_EP</t>
+  </si>
+  <si>
+    <t>connect_cost_generic_$2007_per_mw</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>fuel</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_CCS_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Steam_Turbine_CCS_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CapEx from SAM with Solar Field area = 800000m^2 and 6h TES, construction cost mulitplier and yearly cost fraction from CSP on ReEDs sheet- it's unclear how much these change with storage... assumed to be the same here, cost declination rate and fixed OM from Mark Mehos estimate on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSP_Trough_No_Storage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSP_Trough_6h_Storage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Central_PV</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>construction_cost_multipulier</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed_o_m</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>var_o_m</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nuclear_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Steam_Turbine_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Solid_CCS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biomass_Steam_Turbine</t>
+  </si>
+  <si>
+    <t>Hydro_NonPumped</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hydro_Pumped</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Water</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Water</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, cost declination rate assumed to be that of a gas steam turbine</t>
+  </si>
+  <si>
+    <t>Biomass_IGCC</t>
+  </si>
+  <si>
+    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to coal IGCC</t>
+  </si>
+  <si>
+    <t>Coal_IGCC</t>
+  </si>
+  <si>
+    <t>can_build_new</t>
+  </si>
+  <si>
+    <t>forced_outage_rate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>scheduled_outage_rate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>note: we assume that cogen plants have 3/4 of the capital cost of a pure-electric plant, (to reflect shared infrastructure for cogen), but the same operating costs.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dispatchable</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>cogen</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, took CoalOldScr costs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, took OGS (Oil Gas Steam)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, set lifetime to 60 years</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCGT_CCS_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_Cogen_CCS_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_Cogen_CCS_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Steam_Turbine_Cogen_CCS_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCGT_Cogen_CCS_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, EIA says minimum learning by 2025 is 20%, so this is a 1.1% declination rate, capital cost multipulier from EIA,http://graysharboroceanenergy.com/Documents/LIPA%20Offshore%20Wind%20rept.pdf for total outage rate of 3%, distributed by guess</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cost Declination Rate (%/yr)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resultant Capital Costs ($2007/MW) in Investment Period Years</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Concentrating_PV</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Solar</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(in 2010 $)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>year</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>$/Wp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPV Consortium numbers (It's more or less SolFocus)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>cost declination rate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, 75 CapEx of non-cogen</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Geothermal_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, nukes run for 40 years at least, so the 30 year ReEDs lifetime was changed to 40, also the cost declination rate was set to 0.55% as nukes don't really obey the laws of mass production because they aren't mass produced</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCGT</t>
+  </si>
+  <si>
+    <t>ReEDs Sheet</t>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine</t>
+  </si>
+  <si>
+    <t>CCGT_CCS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_CCS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Gas_CCS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biomass_IGCC_CCS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_IGCC_CCS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_CCS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_CCS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>overnight_cost_$2007</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
   <si>
     <t>Gas_Steam_Turbine_Cogen_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -201,395 +581,18 @@
     <t>Gas_Internal_Combustion_Engine_Cogen_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
-  <si>
-    <t>note: we assume that cogen plants have 3/4 of the capital cost of a pure-electric plant, (to reflect shared infrastructure for cogen), but the same operating costs.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>dispatchable</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>cogen</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, took CoalOldScr costs</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, took OGS (Oil Gas Steam)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, set lifetime to 60 years</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wind</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCGT_CCS_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine_Cogen_CCS_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_Cogen_CCS_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_Cogen_CCS_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCGT_Cogen_CCS_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, EIA says minimum learning by 2025 is 20%, so this is a 1.1% declination rate, capital cost multipulier from EIA,http://graysharboroceanenergy.com/Documents/LIPA%20Offshore%20Wind%20rept.pdf for total outage rate of 3%, distributed by guess</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cost Declination Rate (%/yr)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resultant Capital Costs ($2007/MW) in Investment Period Years</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Concentrating_PV</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Solar</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(in 2010 $)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>year</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>$/Wp</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CPV Consortium numbers (It's more or less SolFocus)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>cost declination rate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, 75 CapEx of non-cogen</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Geothermal_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, nukes run for 40 years at least, so the 30 year ReEDs lifetime was changed to 40, also the cost declination rate was set to 0.55% as nukes don't really obey the laws of mass production because they aren't mass produced</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCGT</t>
-  </si>
-  <si>
-    <t>ReEDs Sheet</t>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine</t>
-  </si>
-  <si>
-    <t>CCGT_CCS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine_CCS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bio_Gas_CCS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biomass_IGCC_CCS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_IGCC_CCS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_CCS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_CCS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>overnight_cost_$2007</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, cost declination rate assumed to be between ST and other techs (@1%).  EIA has minimum learning by 2025 as 10%, so this is roughly consistent</t>
-  </si>
-  <si>
-    <t>storage</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Offshore_Wind</t>
-  </si>
-  <si>
-    <t>Bio_Gas</t>
-  </si>
-  <si>
-    <t>year_1_cost_fraction</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_2_cost_fraction</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_3_cost_fraction</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Battery_Storage</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Storage</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>tech_name_again</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Geothermal</t>
-  </si>
-  <si>
-    <t>construction_time_years</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_Cogen_EP</t>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_Cogen_EP</t>
-  </si>
-  <si>
-    <t>connect_cost_generic_$2007_per_mw</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>fuel</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_CCS_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_CCS_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CapEx from SAM with Solar Field area = 800000m^2 and 6h TES, construction cost mulitplier and yearly cost fraction from CSP on ReEDs sheet- it's unclear how much these change with storage... assumed to be the same here, cost declination rate and fixed OM from Mark Mehos estimate on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSP_Trough_No_Storage</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSP_Trough_6h_Storage</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wind</t>
-  </si>
-  <si>
-    <t>Central_PV</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>construction_cost_multipulier</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed_o_m</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>var_o_m</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nuclear_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bio_Solid_CCS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biomass_Steam_Turbine</t>
-  </si>
-  <si>
-    <t>Hydro_NonPumped</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hydro_Pumped</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Water</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Water</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, cost declination rate assumed to be that of a gas steam turbine</t>
-  </si>
-  <si>
-    <t>Biomass_IGCC</t>
-  </si>
-  <si>
-    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to coal IGCC</t>
-  </si>
-  <si>
-    <t>Coal_IGCC</t>
-  </si>
-  <si>
-    <t>can_build_new</t>
-  </si>
-  <si>
-    <t>forced_outage_rate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>scheduled_outage_rate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CapEx from SAM with Solar Field area = 600000m^2, construction cost mulitplier and yearly cost fraction from ReEDs sheet, cost declination rate and fixed OM from DOE solar program costs on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_CCS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, storage effiency from Samir Succar and Robert H. Williams: Compressed Air Energy Storage: Theory, Resources, And Applications For Wind Power, p. 39</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ReEDs Sheet; also Sullivan et al (2008), NREL/CP-670-43510 Conference Paper for o&amp;m costs, declanation rate, etc; $1,200,000 taken as capital cost in 2010 rather than 2004 based on conversation with Hernandez, also The storage efficiency of the the storage phase of compressed air energy storage from Samir Succar and Robert H. Williams: Compressed Air Energy Storage: Theory, Resources, And Applications For Wind Power, p. 39
-</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCGT_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wind</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>price_and_dollar_year</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas</t>
-  </si>
-  <si>
-    <t>year_4_cost_fraction</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_5_cost_fraction</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_6_cost_fraction</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed_o_m_$2007</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>heat_rate_mbtu_per_mwh</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Commercial_PV</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>min_build_year</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine_Cogen_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_Cogen_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, also new wind params used for fixed O+M, forced outage rate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="6">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -634,7 +637,7 @@
   <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -656,7 +659,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1002,7 +1005,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane xSplit="2" topLeftCell="AG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AM19" sqref="AM19"/>
+      <selection pane="topRight" activeCell="AK24" sqref="AK24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1034,133 +1037,133 @@
   <sheetData>
     <row r="1" spans="1:41" s="33" customFormat="1">
       <c r="A1" s="34" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:41" s="33" customFormat="1"/>
     <row r="3" spans="1:41">
       <c r="A3" s="5" t="s">
-        <v>26</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I3" t="s">
+        <v>138</v>
+      </c>
+      <c r="J3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" t="s">
+        <v>98</v>
+      </c>
+      <c r="N3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>108</v>
+      </c>
+      <c r="P3" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S3" t="s">
+        <v>31</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E3" t="s">
-        <v>102</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="11" t="s">
+      <c r="Z3" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF3" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG3" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ3" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" t="s">
-        <v>111</v>
-      </c>
-      <c r="K3" t="s">
-        <v>112</v>
-      </c>
-      <c r="L3" t="s">
-        <v>113</v>
-      </c>
-      <c r="M3" t="s">
-        <v>85</v>
-      </c>
-      <c r="N3" t="s">
-        <v>142</v>
-      </c>
-      <c r="O3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>101</v>
-      </c>
-      <c r="R3" t="s">
-        <v>143</v>
-      </c>
-      <c r="S3" t="s">
-        <v>98</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="Y3" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>128</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>129</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF3" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG3" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ3" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="AK3" s="15" t="s">
-        <v>87</v>
-      </c>
       <c r="AL3" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="AM3" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="AN3" s="12" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="AO3" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:41">
@@ -1168,7 +1171,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C4" s="5">
         <v>2007</v>
@@ -1177,7 +1180,7 @@
         <v>2010</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="F4">
         <v>2004</v>
@@ -1289,7 +1292,7 @@
         <v>CCGT</v>
       </c>
       <c r="AO4" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:41">
@@ -1297,7 +1300,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="C5" s="5">
         <v>2007</v>
@@ -1306,7 +1309,7 @@
         <v>2010</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="F5">
         <v>2004</v>
@@ -1418,7 +1421,7 @@
         <v>Gas_Combustion_Turbine</v>
       </c>
       <c r="AO5" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:41" s="22" customFormat="1">
@@ -1426,7 +1429,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="C6" s="22">
         <v>2007</v>
@@ -1435,7 +1438,7 @@
         <v>2010</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="F6" s="22">
         <v>2010</v>
@@ -1548,7 +1551,7 @@
         <v>Concentrating_PV</v>
       </c>
       <c r="AO6" s="22" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:41">
@@ -1556,7 +1559,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="C7" s="5">
         <v>2007</v>
@@ -1565,7 +1568,7 @@
         <v>2010</v>
       </c>
       <c r="E7" t="s">
-        <v>136</v>
+        <v>6</v>
       </c>
       <c r="F7">
         <v>2004</v>
@@ -1677,7 +1680,7 @@
         <v>Wind</v>
       </c>
       <c r="AO7" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:41">
@@ -1685,7 +1688,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="C8" s="5">
         <v>2007</v>
@@ -1694,7 +1697,7 @@
         <v>2010</v>
       </c>
       <c r="E8" t="s">
-        <v>136</v>
+        <v>6</v>
       </c>
       <c r="F8">
         <v>2004</v>
@@ -1806,7 +1809,7 @@
         <v>Offshore_Wind</v>
       </c>
       <c r="AO8" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:41">
@@ -1814,7 +1817,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>21</v>
+        <v>120</v>
       </c>
       <c r="C9" s="5">
         <v>2007</v>
@@ -1823,7 +1826,7 @@
         <v>2010</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>127</v>
       </c>
       <c r="F9">
         <v>2009</v>
@@ -1936,7 +1939,7 @@
         <v>Residential_PV</v>
       </c>
       <c r="AO9" t="s">
-        <v>38</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:41" s="11" customFormat="1">
@@ -1944,7 +1947,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="C10" s="11">
         <v>2007</v>
@@ -1953,7 +1956,7 @@
         <v>2012</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="F10" s="11">
         <v>2010</v>
@@ -2065,7 +2068,7 @@
         <v>CSP_Trough_6h_Storage</v>
       </c>
       <c r="AO10" s="11" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:41">
@@ -2073,7 +2076,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5">
         <v>2007</v>
@@ -2082,7 +2085,7 @@
         <v>2010</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="F11">
         <v>2007</v>
@@ -2194,7 +2197,7 @@
         <v>Bio_Gas</v>
       </c>
       <c r="AO11" t="s">
-        <v>33</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:41">
@@ -2202,7 +2205,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="C12" s="5">
         <v>2007</v>
@@ -2211,7 +2214,7 @@
         <v>2010</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>140</v>
       </c>
       <c r="F12">
         <v>2004</v>
@@ -2323,7 +2326,7 @@
         <v>Biomass_Steam_Turbine</v>
       </c>
       <c r="AO12" t="s">
-        <v>123</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:41">
@@ -2331,7 +2334,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>124</v>
+        <v>57</v>
       </c>
       <c r="C13" s="5">
         <v>2007</v>
@@ -2340,7 +2343,7 @@
         <v>2012</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>140</v>
       </c>
       <c r="F13">
         <v>2007</v>
@@ -2452,7 +2455,7 @@
         <v>Biomass_IGCC</v>
       </c>
       <c r="AO13" t="s">
-        <v>125</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:41">
@@ -2460,7 +2463,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>126</v>
+        <v>59</v>
       </c>
       <c r="C14" s="5">
         <v>2007</v>
@@ -2469,7 +2472,7 @@
         <v>2010</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="F14">
         <v>2004</v>
@@ -2581,7 +2584,7 @@
         <v>Coal_IGCC</v>
       </c>
       <c r="AO14" t="s">
-        <v>30</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:41">
@@ -2589,7 +2592,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>130</v>
       </c>
       <c r="C15" s="5">
         <v>2007</v>
@@ -2598,7 +2601,7 @@
         <v>2010</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="F15">
         <v>2004</v>
@@ -2710,7 +2713,7 @@
         <v>Coal_Steam_Turbine</v>
       </c>
       <c r="AO15" t="s">
-        <v>30</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:41">
@@ -2718,7 +2721,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>131</v>
       </c>
       <c r="C16" s="5">
         <v>2007</v>
@@ -2727,7 +2730,7 @@
         <v>2010</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="F16">
         <v>2004</v>
@@ -2839,7 +2842,7 @@
         <v>Nuclear</v>
       </c>
       <c r="AO16" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:41">
@@ -2847,7 +2850,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="C17" s="5">
         <v>2007</v>
@@ -2856,7 +2859,7 @@
         <v>2010</v>
       </c>
       <c r="E17" t="s">
-        <v>22</v>
+        <v>121</v>
       </c>
       <c r="F17">
         <v>2004</v>
@@ -2968,7 +2971,7 @@
         <v>Geothermal</v>
       </c>
       <c r="AO17" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:41">
@@ -2976,7 +2979,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>119</v>
+        <v>52</v>
       </c>
       <c r="C18" s="5">
         <v>2007</v>
@@ -2985,7 +2988,7 @@
         <v>2010</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="F18" s="5">
         <v>2007</v>
@@ -3097,7 +3100,7 @@
         <v>Hydro_NonPumped</v>
       </c>
       <c r="AO18" s="5" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:41">
@@ -3105,7 +3108,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>120</v>
+        <v>53</v>
       </c>
       <c r="C19" s="5">
         <v>2007</v>
@@ -3114,7 +3117,7 @@
         <v>2010</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>122</v>
+        <v>55</v>
       </c>
       <c r="F19" s="33">
         <v>2007</v>
@@ -3213,7 +3216,7 @@
         <v>0</v>
       </c>
       <c r="AK19" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL19">
         <v>0.74</v>
@@ -3226,7 +3229,7 @@
         <v>Hydro_Pumped</v>
       </c>
       <c r="AO19" s="33" t="s">
-        <v>132</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:41" s="18" customFormat="1">
@@ -3234,7 +3237,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>135</v>
+        <v>5</v>
       </c>
       <c r="C20" s="18">
         <v>2007</v>
@@ -3243,7 +3246,7 @@
         <v>2000</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>37</v>
+        <v>136</v>
       </c>
       <c r="F20" s="18">
         <v>2007</v>
@@ -3355,7 +3358,7 @@
         <v>Gas_Combustion_Turbine_EP</v>
       </c>
       <c r="AO20" s="33" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:41" s="5" customFormat="1">
@@ -3363,7 +3366,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>115</v>
+        <v>48</v>
       </c>
       <c r="C21">
         <v>2007</v>
@@ -3372,7 +3375,7 @@
         <v>2000</v>
       </c>
       <c r="E21" t="s">
-        <v>2</v>
+        <v>101</v>
       </c>
       <c r="F21" s="33">
         <v>2007</v>
@@ -3484,7 +3487,7 @@
         <v>Coal_Steam_Turbine_EP</v>
       </c>
       <c r="AO21" s="33" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:41" s="5" customFormat="1">
@@ -3492,7 +3495,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="C22" s="33">
         <v>2007</v>
@@ -3501,7 +3504,7 @@
         <v>2000</v>
       </c>
       <c r="E22" t="s">
-        <v>138</v>
+        <v>8</v>
       </c>
       <c r="F22" s="33">
         <v>2007</v>
@@ -3613,7 +3616,7 @@
         <v>Gas_Steam_Turbine_EP</v>
       </c>
       <c r="AO22" s="33" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:41" s="5" customFormat="1">
@@ -3621,7 +3624,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>134</v>
+        <v>4</v>
       </c>
       <c r="C23" s="33">
         <v>2007</v>
@@ -3630,7 +3633,7 @@
         <v>2000</v>
       </c>
       <c r="E23" t="s">
-        <v>138</v>
+        <v>8</v>
       </c>
       <c r="F23" s="33">
         <v>2007</v>
@@ -3742,7 +3745,7 @@
         <v>CCGT_EP</v>
       </c>
       <c r="AO23" s="33" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:41" s="5" customFormat="1">
@@ -3750,7 +3753,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="C24" s="33">
         <v>2007</v>
@@ -3759,7 +3762,7 @@
         <v>2000</v>
       </c>
       <c r="E24" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="F24" s="33">
         <v>2007</v>
@@ -3871,7 +3874,7 @@
         <v>Geothermal_EP</v>
       </c>
       <c r="AO24" s="33" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:41" s="5" customFormat="1">
@@ -3879,7 +3882,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="C25" s="33">
         <v>2007</v>
@@ -3888,7 +3891,7 @@
         <v>2000</v>
       </c>
       <c r="E25" t="s">
-        <v>3</v>
+        <v>102</v>
       </c>
       <c r="F25" s="33">
         <v>2007</v>
@@ -4000,7 +4003,7 @@
         <v>Nuclear_EP</v>
       </c>
       <c r="AO25" s="33" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:41" s="18" customFormat="1">
@@ -4008,7 +4011,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>36</v>
+        <v>135</v>
       </c>
       <c r="C26" s="33">
         <v>2007</v>
@@ -4017,7 +4020,7 @@
         <v>2000</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="F26" s="33">
         <v>2007</v>
@@ -4129,7 +4132,7 @@
         <v>Wind_EP</v>
       </c>
       <c r="AO26" s="33" t="s">
-        <v>148</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:41" s="33" customFormat="1">
@@ -4137,7 +4140,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>47</v>
+        <v>146</v>
       </c>
       <c r="C27" s="33">
         <v>2007</v>
@@ -4146,7 +4149,7 @@
         <v>2000</v>
       </c>
       <c r="E27" s="33" t="s">
-        <v>48</v>
+        <v>147</v>
       </c>
       <c r="F27" s="33">
         <v>2007</v>
@@ -4258,7 +4261,7 @@
         <v>Gas_Internal_Combustion_Engine_EP</v>
       </c>
       <c r="AO27" s="33" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:41" s="8" customFormat="1">
@@ -4266,7 +4269,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="C28" s="8">
         <v>2007</v>
@@ -4275,7 +4278,7 @@
         <v>2010</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="F28" s="8">
         <v>2009</v>
@@ -4387,7 +4390,7 @@
         <v>Commercial_PV</v>
       </c>
       <c r="AO28" s="9" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:41" s="8" customFormat="1">
@@ -4395,7 +4398,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="C29" s="8">
         <v>2007</v>
@@ -4404,7 +4407,7 @@
         <v>2010</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="F29" s="8">
         <v>2009</v>
@@ -4516,7 +4519,7 @@
         <v>Central_PV</v>
       </c>
       <c r="AO29" s="9" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:41" s="5" customFormat="1">
@@ -4524,7 +4527,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="C30" s="5">
         <v>2007</v>
@@ -4533,7 +4536,7 @@
         <v>2010</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="F30" s="5">
         <v>2010</v>
@@ -4645,7 +4648,7 @@
         <v>CSP_Trough_No_Storage</v>
       </c>
       <c r="AO30" s="9" t="s">
-        <v>130</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:41" s="9" customFormat="1" ht="15" customHeight="1">
@@ -4653,7 +4656,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>23</v>
+        <v>122</v>
       </c>
       <c r="C31" s="9">
         <v>2007</v>
@@ -4662,7 +4665,7 @@
         <v>2010</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>24</v>
+        <v>123</v>
       </c>
       <c r="F31" s="9">
         <v>2010</v>
@@ -4774,7 +4777,7 @@
         <v>Compressed_Air_Energy_Storage</v>
       </c>
       <c r="AO31" s="32" t="s">
-        <v>133</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:41" s="19" customFormat="1">
@@ -4782,7 +4785,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>146</v>
+        <v>16</v>
       </c>
       <c r="C32" s="33">
         <v>2007</v>
@@ -4791,7 +4794,7 @@
         <v>2000</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>37</v>
+        <v>136</v>
       </c>
       <c r="F32" s="19">
         <v>2007</v>
@@ -4908,7 +4911,7 @@
         <v>Gas_Combustion_Turbine_Cogen_EP</v>
       </c>
       <c r="AO32" s="33" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:41" s="19" customFormat="1">
@@ -4916,7 +4919,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>147</v>
+        <v>17</v>
       </c>
       <c r="C33" s="33">
         <v>2007</v>
@@ -4925,7 +4928,7 @@
         <v>2000</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>2</v>
+        <v>101</v>
       </c>
       <c r="F33" s="33">
         <v>2007</v>
@@ -5042,7 +5045,7 @@
         <v>Coal_Steam_Turbine_Cogen_EP</v>
       </c>
       <c r="AO33" s="33" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:41" s="19" customFormat="1">
@@ -5050,7 +5053,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="C34" s="33">
         <v>2007</v>
@@ -5059,7 +5062,7 @@
         <v>2000</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>138</v>
+        <v>8</v>
       </c>
       <c r="F34" s="33">
         <v>2007</v>
@@ -5176,7 +5179,7 @@
         <v>Gas_Steam_Turbine_Cogen_EP</v>
       </c>
       <c r="AO34" s="33" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:41" s="19" customFormat="1">
@@ -5184,7 +5187,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C35" s="33">
         <v>2007</v>
@@ -5193,7 +5196,7 @@
         <v>2000</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>138</v>
+        <v>8</v>
       </c>
       <c r="F35" s="33">
         <v>2007</v>
@@ -5310,7 +5313,7 @@
         <v>CCGT_Cogen_EP</v>
       </c>
       <c r="AO35" s="33" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:41" s="23" customFormat="1">
@@ -5318,7 +5321,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="C36" s="23">
         <v>2007</v>
@@ -5327,7 +5330,7 @@
         <v>2010</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="F36" s="23">
         <v>2004</v>
@@ -5439,7 +5442,7 @@
         <v>Battery_Storage</v>
       </c>
       <c r="AO36" s="23" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:41" s="26" customFormat="1">
@@ -5447,7 +5450,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="C37" s="26">
         <v>2007</v>
@@ -5456,7 +5459,7 @@
         <v>2014</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="F37" s="26">
         <v>2004</v>
@@ -5573,7 +5576,7 @@
         <v>CCGT_CCS</v>
       </c>
       <c r="AO37" s="33" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:41" s="26" customFormat="1">
@@ -5581,7 +5584,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="C38" s="26">
         <v>2007</v>
@@ -5590,7 +5593,7 @@
         <v>2014</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="F38" s="26">
         <v>2004</v>
@@ -5708,7 +5711,7 @@
         <v>Gas_Combustion_Turbine_CCS</v>
       </c>
       <c r="AO38" s="33" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:41" s="26" customFormat="1">
@@ -5716,7 +5719,7 @@
         <v>36</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="C39" s="26">
         <v>2007</v>
@@ -5725,7 +5728,7 @@
         <v>2014</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="F39" s="26">
         <v>2004</v>
@@ -5843,7 +5846,7 @@
         <v>Bio_Gas_CCS</v>
       </c>
       <c r="AO39" s="33" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:41" s="26" customFormat="1">
@@ -5851,7 +5854,7 @@
         <v>37</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C40" s="26">
         <v>2007</v>
@@ -5860,7 +5863,7 @@
         <v>2014</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>117</v>
+        <v>50</v>
       </c>
       <c r="F40" s="26">
         <v>2004</v>
@@ -5978,7 +5981,7 @@
         <v>Biomass_IGCC_CCS</v>
       </c>
       <c r="AO40" s="33" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:41" s="26" customFormat="1">
@@ -5986,7 +5989,7 @@
         <v>38</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="C41" s="26">
         <v>2007</v>
@@ -5995,7 +5998,7 @@
         <v>2014</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
       <c r="F41" s="26">
         <v>2004</v>
@@ -6111,7 +6114,7 @@
         <v>Coal_IGCC_CCS</v>
       </c>
       <c r="AO41" s="33" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:41" s="26" customFormat="1">
@@ -6119,7 +6122,7 @@
         <v>39</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="C42" s="26">
         <v>2007</v>
@@ -6128,7 +6131,7 @@
         <v>2014</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
       <c r="F42" s="26">
         <v>2004</v>
@@ -6246,7 +6249,7 @@
         <v>Coal_Steam_Turbine_CCS</v>
       </c>
       <c r="AO42" s="33" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:41" s="33" customFormat="1">
@@ -6254,7 +6257,7 @@
         <v>40</v>
       </c>
       <c r="B43" s="33" t="s">
-        <v>49</v>
+        <v>148</v>
       </c>
       <c r="C43" s="33">
         <v>2007</v>
@@ -6263,7 +6266,7 @@
         <v>2000</v>
       </c>
       <c r="E43" s="33" t="s">
-        <v>138</v>
+        <v>8</v>
       </c>
       <c r="F43" s="33">
         <v>2007</v>
@@ -6379,7 +6382,7 @@
         <v>Gas_Internal_Combustion_Engine_Cogen_EP</v>
       </c>
       <c r="AO43" s="33" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:41" s="28" customFormat="1">
@@ -6387,7 +6390,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>35</v>
+        <v>134</v>
       </c>
       <c r="C44" s="28">
         <v>2007</v>
@@ -6396,7 +6399,7 @@
         <v>2014</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="F44" s="28">
         <v>2004</v>
@@ -6508,10 +6511,10 @@
         <v>0</v>
       </c>
       <c r="AN44" s="28" t="s">
-        <v>42</v>
+        <v>141</v>
       </c>
       <c r="AO44" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:41" s="28" customFormat="1">
@@ -6519,7 +6522,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="C45" s="28">
         <v>2007</v>
@@ -6528,7 +6531,7 @@
         <v>2014</v>
       </c>
       <c r="E45" s="30" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
       <c r="F45" s="28">
         <v>2004</v>
@@ -6639,10 +6642,10 @@
         <v>0</v>
       </c>
       <c r="AN45" s="28" t="s">
-        <v>43</v>
+        <v>142</v>
       </c>
       <c r="AO45" s="33" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:41" s="28" customFormat="1">
@@ -6650,7 +6653,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="C46" s="28">
         <v>2007</v>
@@ -6659,7 +6662,7 @@
         <v>2014</v>
       </c>
       <c r="E46" s="30" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="F46" s="28">
         <v>2004</v>
@@ -6771,10 +6774,10 @@
         <v>0</v>
       </c>
       <c r="AN46" s="28" t="s">
-        <v>44</v>
+        <v>143</v>
       </c>
       <c r="AO46" s="33" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="47" spans="1:41" s="28" customFormat="1">
@@ -6782,7 +6785,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="28" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="C47" s="28">
         <v>2007</v>
@@ -6791,7 +6794,7 @@
         <v>2014</v>
       </c>
       <c r="E47" s="30" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="F47" s="28">
         <v>2004</v>
@@ -6902,10 +6905,10 @@
         <v>0</v>
       </c>
       <c r="AN47" s="28" t="s">
-        <v>45</v>
+        <v>144</v>
       </c>
       <c r="AO47" s="33" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:41" s="28" customFormat="1">
@@ -6913,7 +6916,7 @@
         <v>45</v>
       </c>
       <c r="B48" s="28" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C48" s="28">
         <v>2007</v>
@@ -6922,7 +6925,7 @@
         <v>2014</v>
       </c>
       <c r="E48" s="30" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="F48" s="28">
         <v>2004</v>
@@ -7036,10 +7039,10 @@
         <v>0</v>
       </c>
       <c r="AN48" s="28" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
       <c r="AO48" s="33" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:41" s="28" customFormat="1">
@@ -7047,7 +7050,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="28" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C49" s="28">
         <v>2007</v>
@@ -7056,7 +7059,7 @@
         <v>2014</v>
       </c>
       <c r="E49" s="30" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
       <c r="F49" s="28">
         <v>2004</v>
@@ -7170,10 +7173,10 @@
         <v>0</v>
       </c>
       <c r="AN49" s="28" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="AO49" s="33" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:41" s="28" customFormat="1">
@@ -7181,7 +7184,7 @@
         <v>47</v>
       </c>
       <c r="B50" s="28" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C50" s="28">
         <v>2007</v>
@@ -7190,7 +7193,7 @@
         <v>2014</v>
       </c>
       <c r="E50" s="30" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="F50" s="28">
         <v>2004</v>
@@ -7304,10 +7307,10 @@
         <v>0</v>
       </c>
       <c r="AN50" s="28" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="AO50" s="33" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:41" s="28" customFormat="1">
@@ -7315,7 +7318,7 @@
         <v>48</v>
       </c>
       <c r="B51" s="28" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C51" s="28">
         <v>2007</v>
@@ -7324,7 +7327,7 @@
         <v>2014</v>
       </c>
       <c r="E51" s="30" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="F51" s="28">
         <v>2004</v>
@@ -7438,10 +7441,10 @@
         <v>0</v>
       </c>
       <c r="AN51" s="28" t="s">
-        <v>34</v>
+        <v>133</v>
       </c>
       <c r="AO51" s="33" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:41" s="5" customFormat="1">
@@ -7606,6 +7609,7 @@
       <c r="A104" s="33"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -9834,7 +9838,7 @@
       </c>
       <c r="AD17" s="33">
         <f>generator_costs!AK19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE17" s="33">
         <f>generator_costs!AL19</f>
@@ -14018,6 +14022,7 @@
       <c r="A53" s="33"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -14040,7 +14045,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="6" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -14051,7 +14056,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>110</v>
       </c>
       <c r="B2">
         <v>2010</v>
@@ -14069,7 +14074,7 @@
         <v>2026</v>
       </c>
       <c r="G2" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -15513,6 +15518,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -15535,15 +15541,15 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="22" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="22" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="22" customFormat="1">
@@ -15571,7 +15577,7 @@
         <v>3.3</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="E5" s="22"/>
     </row>
@@ -15724,6 +15730,7 @@
       <c r="E21" s="22"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
- added constraints Mexican_Export_Limit and Mexican_Export_Limit_Reserve, which restrict the amount of power exported from Mexico, as it was gettin a bit crazy - the above restriction also allows nuclear to be built in mexico to serve their own load
- derated DispatchHydro to be consistent with the deration of other generation capacity in the model

- updated csp declination rates and fixed O&M to be from the same source (NREL/Black and Veatch) as many other of our capital costs
</commit_message>
<xml_diff>
--- a/DatabasePrep/GeneratorInfo/generator_costs.xlsx
+++ b/DatabasePrep/GeneratorInfo/generator_costs.xlsx
@@ -24,15 +24,11 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="149">
   <si>
-    <t>CapEx from SAM with Solar Field area = 600000m^2, construction cost mulitplier and yearly cost fraction from ReEDs sheet, cost declination rate and fixed OM from DOE solar program costs on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
+    <t>CapEx from SAM with Solar Field area = 600000m^2, construction cost mulitplier and yearly cost fraction from ReEDs sheet, cost declination rate and fixed OM from Black and Veach on ReEDs sheet.  Most places put VarOM at 0, so this was done here</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Coal_CCS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, storage effiency from Samir Succar and Robert H. Williams: Compressed Air Energy Storage: Theory, Resources, And Applications For Wind Power, p. 39</t>
+    <t>CapEx from SAM with Solar Field area = 800000m^2 and 6h TES, construction cost mulitplier and yearly cost fraction from CSP on ReEDs sheet- it's unclear how much these change with storage... assumed to be the same here, cost declination rate and fixed OM from Black and Veach ReEDs sheet.  Most places put VarOM at 0, so this was done here</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -154,61 +150,6 @@
     <t>Gas_Steam_Turbine_Cogen_EP</t>
   </si>
   <si>
-    <t>connect_cost_generic_$2007_per_mw</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>fuel</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_CCS_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_CCS_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CapEx from SAM with Solar Field area = 800000m^2 and 6h TES, construction cost mulitplier and yearly cost fraction from CSP on ReEDs sheet- it's unclear how much these change with storage... assumed to be the same here, cost declination rate and fixed OM from Mark Mehos estimate on ReEDs sheet - took 2020 fixed OM value.  Most places put VarOM at 0, so this was done here</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSP_Trough_No_Storage</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSP_Trough_6h_Storage</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wind</t>
-  </si>
-  <si>
-    <t>Central_PV</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>construction_cost_multipulier</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed_o_m</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>var_o_m</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nuclear_EP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Coal_Steam_Turbine_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -311,51 +252,11 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, EIA says minimum learning by 2025 is 20%, so this is a 1.1% declination rate, capital cost multipulier from EIA,http://graysharboroceanenergy.com/Documents/LIPA%20Offshore%20Wind%20rept.pdf for total outage rate of 3%, distributed by guess</t>
+    <t>Coal_CCS</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Cost Declination Rate (%/yr)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resultant Capital Costs ($2007/MW) in Investment Period Years</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Concentrating_PV</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Solar</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(in 2010 $)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>year</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>$/Wp</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>CPV Consortium numbers (It's more or less SolFocus)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>cost declination rate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet, 75 CapEx of non-cogen</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Geothermal_EP</t>
+    <t>ReEDs Sheet, storage effiency from Samir Succar and Robert H. Williams: Compressed Air Energy Storage: Theory, Resources, And Applications For Wind Power, p. 39</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -472,6 +373,57 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>connect_cost_generic_$2007_per_mw</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>fuel</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_CCS_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Steam_Turbine_CCS_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSP_Trough_No_Storage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSP_Trough_6h_Storage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Central_PV</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>construction_cost_multipulier</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed_o_m</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>var_o_m</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nuclear_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>interest_between_price_year_and_cost_year</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -581,18 +533,68 @@
     <t>Gas_Internal_Combustion_Engine_Cogen_EP</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>Black and Veatch for REFutures (12-02-09 update) (onReEDs sheet) for capital cost, EIA says minimum learning by 2025 is 20%, so this is a 1.1% declination rate, capital cost multipulier from EIA,http://graysharboroceanenergy.com/Documents/LIPA%20Offshore%20Wind%20rept.pdf for total outage rate of 3%, distributed by guess</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cost Declination Rate (%/yr)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resultant Capital Costs ($2007/MW) in Investment Period Years</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Concentrating_PV</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Solar</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(in 2010 $)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>year</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>$/Wp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPV Consortium numbers (It's more or less SolFocus)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>cost declination rate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet, 75 CapEx of non-cogen</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Geothermal_EP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="8">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -637,7 +639,7 @@
   <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -659,7 +661,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1004,8 +1006,8 @@
   <dimension ref="A1:AO104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AK24" sqref="AK24"/>
+      <pane xSplit="2" topLeftCell="AL1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AO11" sqref="AO11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1037,133 +1039,133 @@
   <sheetData>
     <row r="1" spans="1:41" s="33" customFormat="1">
       <c r="A1" s="34" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:41" s="33" customFormat="1"/>
     <row r="3" spans="1:41">
       <c r="A3" s="5" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="F3" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="H3" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="I3" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="J3" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="K3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L3" t="s">
+        <v>105</v>
+      </c>
+      <c r="M3" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P3" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>94</v>
+      </c>
+      <c r="R3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S3" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF3" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG3" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI3" t="s">
         <v>45</v>
       </c>
-      <c r="L3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" t="s">
-        <v>98</v>
-      </c>
-      <c r="N3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O3" t="s">
-        <v>108</v>
-      </c>
-      <c r="P3" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>34</v>
-      </c>
-      <c r="R3" t="s">
-        <v>13</v>
-      </c>
-      <c r="S3" t="s">
-        <v>31</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC3" t="s">
+      <c r="AJ3" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AO3" t="s">
         <v>112</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>113</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>114</v>
-      </c>
-      <c r="AF3" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG3" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>115</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ3" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="AK3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AN3" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:41">
@@ -1171,7 +1173,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="C4" s="5">
         <v>2007</v>
@@ -1180,7 +1182,7 @@
         <v>2010</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="F4">
         <v>2004</v>
@@ -1292,7 +1294,7 @@
         <v>CCGT</v>
       </c>
       <c r="AO4" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:41">
@@ -1300,7 +1302,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="C5" s="5">
         <v>2007</v>
@@ -1309,7 +1311,7 @@
         <v>2010</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="F5">
         <v>2004</v>
@@ -1421,7 +1423,7 @@
         <v>Gas_Combustion_Turbine</v>
       </c>
       <c r="AO5" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:41" s="22" customFormat="1">
@@ -1429,7 +1431,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>78</v>
+        <v>140</v>
       </c>
       <c r="C6" s="22">
         <v>2007</v>
@@ -1438,7 +1440,7 @@
         <v>2010</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>79</v>
+        <v>141</v>
       </c>
       <c r="F6" s="22">
         <v>2010</v>
@@ -1551,7 +1553,7 @@
         <v>Concentrating_PV</v>
       </c>
       <c r="AO6" s="22" t="s">
-        <v>83</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:41">
@@ -1559,7 +1561,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>101</v>
       </c>
       <c r="C7" s="5">
         <v>2007</v>
@@ -1568,7 +1570,7 @@
         <v>2010</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7">
         <v>2004</v>
@@ -1680,7 +1682,7 @@
         <v>Wind</v>
       </c>
       <c r="AO7" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:41">
@@ -1688,7 +1690,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="5">
         <v>2007</v>
@@ -1697,7 +1699,7 @@
         <v>2010</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8">
         <v>2004</v>
@@ -1809,7 +1811,7 @@
         <v>Offshore_Wind</v>
       </c>
       <c r="AO8" t="s">
-        <v>75</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:41">
@@ -1817,7 +1819,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C9" s="5">
         <v>2007</v>
@@ -1826,7 +1828,7 @@
         <v>2010</v>
       </c>
       <c r="E9" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="F9">
         <v>2009</v>
@@ -1939,7 +1941,7 @@
         <v>Residential_PV</v>
       </c>
       <c r="AO9" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:41" s="11" customFormat="1">
@@ -1947,7 +1949,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="C10" s="11">
         <v>2007</v>
@@ -1956,7 +1958,7 @@
         <v>2012</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="F10" s="11">
         <v>2010</v>
@@ -1974,25 +1976,25 @@
         <v>1.05</v>
       </c>
       <c r="K10" s="11">
-        <v>47820</v>
+        <v>49906</v>
       </c>
       <c r="L10" s="11">
         <v>0</v>
       </c>
       <c r="M10" s="21">
         <f t="shared" si="0"/>
-        <v>7935139.1551307421</v>
+        <v>7098171.79151126</v>
       </c>
       <c r="N10" s="11">
         <f t="shared" ref="N10" si="4">K10*G10</f>
-        <v>46146.299999999996</v>
+        <v>48159.29</v>
       </c>
       <c r="O10" s="11">
         <f t="shared" ref="O10" si="5">L10*G10</f>
         <v>0</v>
       </c>
       <c r="P10" s="11">
-        <v>-4.4999999999999998E-2</v>
+        <v>-8.8500000000000002E-3</v>
       </c>
       <c r="Q10" s="11">
         <v>65639</v>
@@ -2067,8 +2069,8 @@
         <f t="shared" si="3"/>
         <v>CSP_Trough_6h_Storage</v>
       </c>
-      <c r="AO10" s="11" t="s">
-        <v>39</v>
+      <c r="AO10" s="33" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:41">
@@ -2076,7 +2078,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="5">
         <v>2007</v>
@@ -2085,7 +2087,7 @@
         <v>2010</v>
       </c>
       <c r="E11" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="F11">
         <v>2007</v>
@@ -2197,7 +2199,7 @@
         <v>Bio_Gas</v>
       </c>
       <c r="AO11" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:41">
@@ -2205,7 +2207,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="C12" s="5">
         <v>2007</v>
@@ -2214,7 +2216,7 @@
         <v>2010</v>
       </c>
       <c r="E12" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="F12">
         <v>2004</v>
@@ -2326,7 +2328,7 @@
         <v>Biomass_Steam_Turbine</v>
       </c>
       <c r="AO12" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:41">
@@ -2334,7 +2336,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C13" s="5">
         <v>2007</v>
@@ -2343,7 +2345,7 @@
         <v>2012</v>
       </c>
       <c r="E13" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="F13">
         <v>2007</v>
@@ -2455,7 +2457,7 @@
         <v>Biomass_IGCC</v>
       </c>
       <c r="AO13" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:41">
@@ -2463,7 +2465,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C14" s="5">
         <v>2007</v>
@@ -2472,7 +2474,7 @@
         <v>2010</v>
       </c>
       <c r="E14" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="F14">
         <v>2004</v>
@@ -2584,7 +2586,7 @@
         <v>Coal_IGCC</v>
       </c>
       <c r="AO14" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:41">
@@ -2592,7 +2594,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C15" s="5">
         <v>2007</v>
@@ -2601,7 +2603,7 @@
         <v>2010</v>
       </c>
       <c r="E15" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="F15">
         <v>2004</v>
@@ -2713,7 +2715,7 @@
         <v>Coal_Steam_Turbine</v>
       </c>
       <c r="AO15" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:41">
@@ -2721,7 +2723,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C16" s="5">
         <v>2007</v>
@@ -2730,7 +2732,7 @@
         <v>2010</v>
       </c>
       <c r="E16" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="F16">
         <v>2004</v>
@@ -2842,7 +2844,7 @@
         <v>Nuclear</v>
       </c>
       <c r="AO16" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:41">
@@ -2850,7 +2852,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="5">
         <v>2007</v>
@@ -2859,7 +2861,7 @@
         <v>2010</v>
       </c>
       <c r="E17" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="F17">
         <v>2004</v>
@@ -2971,7 +2973,7 @@
         <v>Geothermal</v>
       </c>
       <c r="AO17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:41">
@@ -2979,7 +2981,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C18" s="5">
         <v>2007</v>
@@ -2988,7 +2990,7 @@
         <v>2010</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="F18" s="5">
         <v>2007</v>
@@ -3100,7 +3102,7 @@
         <v>Hydro_NonPumped</v>
       </c>
       <c r="AO18" s="5" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:41">
@@ -3108,7 +3110,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C19" s="5">
         <v>2007</v>
@@ -3117,7 +3119,7 @@
         <v>2010</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F19" s="33">
         <v>2007</v>
@@ -3229,7 +3231,7 @@
         <v>Hydro_Pumped</v>
       </c>
       <c r="AO19" s="33" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:41" s="18" customFormat="1">
@@ -3237,7 +3239,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" s="18">
         <v>2007</v>
@@ -3246,7 +3248,7 @@
         <v>2000</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="F20" s="18">
         <v>2007</v>
@@ -3358,7 +3360,7 @@
         <v>Gas_Combustion_Turbine_EP</v>
       </c>
       <c r="AO20" s="33" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:41" s="5" customFormat="1">
@@ -3366,7 +3368,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="C21">
         <v>2007</v>
@@ -3375,7 +3377,7 @@
         <v>2000</v>
       </c>
       <c r="E21" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="F21" s="33">
         <v>2007</v>
@@ -3487,7 +3489,7 @@
         <v>Coal_Steam_Turbine_EP</v>
       </c>
       <c r="AO21" s="33" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:41" s="5" customFormat="1">
@@ -3495,7 +3497,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="C22" s="33">
         <v>2007</v>
@@ -3504,7 +3506,7 @@
         <v>2000</v>
       </c>
       <c r="E22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" s="33">
         <v>2007</v>
@@ -3616,7 +3618,7 @@
         <v>Gas_Steam_Turbine_EP</v>
       </c>
       <c r="AO22" s="33" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:41" s="5" customFormat="1">
@@ -3624,7 +3626,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C23" s="33">
         <v>2007</v>
@@ -3633,7 +3635,7 @@
         <v>2000</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" s="33">
         <v>2007</v>
@@ -3745,7 +3747,7 @@
         <v>CCGT_EP</v>
       </c>
       <c r="AO23" s="33" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:41" s="5" customFormat="1">
@@ -3753,7 +3755,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>86</v>
+        <v>148</v>
       </c>
       <c r="C24" s="33">
         <v>2007</v>
@@ -3762,7 +3764,7 @@
         <v>2000</v>
       </c>
       <c r="E24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F24" s="33">
         <v>2007</v>
@@ -3874,7 +3876,7 @@
         <v>Geothermal_EP</v>
       </c>
       <c r="AO24" s="33" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:41" s="5" customFormat="1">
@@ -3882,7 +3884,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="C25" s="33">
         <v>2007</v>
@@ -3891,7 +3893,7 @@
         <v>2000</v>
       </c>
       <c r="E25" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="F25" s="33">
         <v>2007</v>
@@ -4003,7 +4005,7 @@
         <v>Nuclear_EP</v>
       </c>
       <c r="AO25" s="33" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:41" s="18" customFormat="1">
@@ -4011,7 +4013,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="C26" s="33">
         <v>2007</v>
@@ -4020,7 +4022,7 @@
         <v>2000</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="F26" s="33">
         <v>2007</v>
@@ -4132,7 +4134,7 @@
         <v>Wind_EP</v>
       </c>
       <c r="AO26" s="33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:41" s="33" customFormat="1">
@@ -4140,7 +4142,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C27" s="33">
         <v>2007</v>
@@ -4149,7 +4151,7 @@
         <v>2000</v>
       </c>
       <c r="E27" s="33" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="F27" s="33">
         <v>2007</v>
@@ -4261,7 +4263,7 @@
         <v>Gas_Internal_Combustion_Engine_EP</v>
       </c>
       <c r="AO27" s="33" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:41" s="8" customFormat="1">
@@ -4269,7 +4271,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" s="8">
         <v>2007</v>
@@ -4278,7 +4280,7 @@
         <v>2010</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="F28" s="8">
         <v>2009</v>
@@ -4390,7 +4392,7 @@
         <v>Commercial_PV</v>
       </c>
       <c r="AO28" s="9" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:41" s="8" customFormat="1">
@@ -4398,7 +4400,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>43</v>
+        <v>102</v>
       </c>
       <c r="C29" s="8">
         <v>2007</v>
@@ -4407,7 +4409,7 @@
         <v>2010</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="F29" s="8">
         <v>2009</v>
@@ -4519,7 +4521,7 @@
         <v>Central_PV</v>
       </c>
       <c r="AO29" s="9" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:41" s="5" customFormat="1">
@@ -4527,7 +4529,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C30" s="5">
         <v>2007</v>
@@ -4536,7 +4538,7 @@
         <v>2010</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="F30" s="5">
         <v>2010</v>
@@ -4553,26 +4555,26 @@
       <c r="J30" s="5">
         <v>1.05</v>
       </c>
-      <c r="K30" s="5">
-        <v>44370</v>
+      <c r="K30" s="33">
+        <v>49906</v>
       </c>
       <c r="L30" s="9">
         <v>0</v>
       </c>
       <c r="M30" s="21">
         <f>I30*J30*G30/(1+P30)^(H30-2007)</f>
-        <v>4624269.4583522985</v>
+        <v>4401886.3331025699</v>
       </c>
       <c r="N30" s="11">
         <f t="shared" si="1"/>
-        <v>42817.049999999996</v>
+        <v>48159.29</v>
       </c>
       <c r="O30" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P30" s="9">
-        <v>-2.5000000000000001E-2</v>
+        <v>-8.8500000000000002E-3</v>
       </c>
       <c r="Q30" s="9">
         <v>65639</v>
@@ -4647,7 +4649,7 @@
         <f t="shared" si="6"/>
         <v>CSP_Trough_No_Storage</v>
       </c>
-      <c r="AO30" s="9" t="s">
+      <c r="AO30" s="33" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4656,7 +4658,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C31" s="9">
         <v>2007</v>
@@ -4665,7 +4667,7 @@
         <v>2010</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="F31" s="9">
         <v>2010</v>
@@ -4777,7 +4779,7 @@
         <v>Compressed_Air_Energy_Storage</v>
       </c>
       <c r="AO31" s="32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:41" s="19" customFormat="1">
@@ -4785,7 +4787,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C32" s="33">
         <v>2007</v>
@@ -4794,7 +4796,7 @@
         <v>2000</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="F32" s="19">
         <v>2007</v>
@@ -4911,7 +4913,7 @@
         <v>Gas_Combustion_Turbine_Cogen_EP</v>
       </c>
       <c r="AO32" s="33" t="s">
-        <v>85</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:41" s="19" customFormat="1">
@@ -4919,7 +4921,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C33" s="33">
         <v>2007</v>
@@ -4928,7 +4930,7 @@
         <v>2000</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="F33" s="33">
         <v>2007</v>
@@ -5045,7 +5047,7 @@
         <v>Coal_Steam_Turbine_Cogen_EP</v>
       </c>
       <c r="AO33" s="33" t="s">
-        <v>85</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:41" s="19" customFormat="1">
@@ -5053,7 +5055,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="C34" s="33">
         <v>2007</v>
@@ -5062,7 +5064,7 @@
         <v>2000</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" s="33">
         <v>2007</v>
@@ -5179,7 +5181,7 @@
         <v>Gas_Steam_Turbine_Cogen_EP</v>
       </c>
       <c r="AO34" s="33" t="s">
-        <v>85</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:41" s="19" customFormat="1">
@@ -5187,7 +5189,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="C35" s="33">
         <v>2007</v>
@@ -5196,7 +5198,7 @@
         <v>2000</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" s="33">
         <v>2007</v>
@@ -5313,7 +5315,7 @@
         <v>CCGT_Cogen_EP</v>
       </c>
       <c r="AO35" s="33" t="s">
-        <v>85</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:41" s="23" customFormat="1">
@@ -5321,7 +5323,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C36" s="23">
         <v>2007</v>
@@ -5330,7 +5332,7 @@
         <v>2010</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F36" s="23">
         <v>2004</v>
@@ -5442,7 +5444,7 @@
         <v>Battery_Storage</v>
       </c>
       <c r="AO36" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:41" s="26" customFormat="1">
@@ -5450,7 +5452,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="C37" s="26">
         <v>2007</v>
@@ -5459,7 +5461,7 @@
         <v>2014</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="F37" s="26">
         <v>2004</v>
@@ -5576,7 +5578,7 @@
         <v>CCGT_CCS</v>
       </c>
       <c r="AO37" s="33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:41" s="26" customFormat="1">
@@ -5584,7 +5586,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="C38" s="26">
         <v>2007</v>
@@ -5593,7 +5595,7 @@
         <v>2014</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="F38" s="26">
         <v>2004</v>
@@ -5711,7 +5713,7 @@
         <v>Gas_Combustion_Turbine_CCS</v>
       </c>
       <c r="AO38" s="33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:41" s="26" customFormat="1">
@@ -5719,7 +5721,7 @@
         <v>36</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="C39" s="26">
         <v>2007</v>
@@ -5728,7 +5730,7 @@
         <v>2014</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="F39" s="26">
         <v>2004</v>
@@ -5846,7 +5848,7 @@
         <v>Bio_Gas_CCS</v>
       </c>
       <c r="AO39" s="33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:41" s="26" customFormat="1">
@@ -5854,7 +5856,7 @@
         <v>37</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="C40" s="26">
         <v>2007</v>
@@ -5863,7 +5865,7 @@
         <v>2014</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F40" s="26">
         <v>2004</v>
@@ -5981,7 +5983,7 @@
         <v>Biomass_IGCC_CCS</v>
       </c>
       <c r="AO40" s="33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:41" s="26" customFormat="1">
@@ -5989,7 +5991,7 @@
         <v>38</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="C41" s="26">
         <v>2007</v>
@@ -5998,7 +6000,7 @@
         <v>2014</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="F41" s="26">
         <v>2004</v>
@@ -6114,7 +6116,7 @@
         <v>Coal_IGCC_CCS</v>
       </c>
       <c r="AO41" s="33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:41" s="26" customFormat="1">
@@ -6122,7 +6124,7 @@
         <v>39</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="C42" s="26">
         <v>2007</v>
@@ -6131,7 +6133,7 @@
         <v>2014</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="F42" s="26">
         <v>2004</v>
@@ -6249,7 +6251,7 @@
         <v>Coal_Steam_Turbine_CCS</v>
       </c>
       <c r="AO42" s="33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:41" s="33" customFormat="1">
@@ -6257,7 +6259,7 @@
         <v>40</v>
       </c>
       <c r="B43" s="33" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C43" s="33">
         <v>2007</v>
@@ -6266,7 +6268,7 @@
         <v>2000</v>
       </c>
       <c r="E43" s="33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" s="33">
         <v>2007</v>
@@ -6382,7 +6384,7 @@
         <v>Gas_Internal_Combustion_Engine_Cogen_EP</v>
       </c>
       <c r="AO43" s="33" t="s">
-        <v>85</v>
+        <v>147</v>
       </c>
     </row>
     <row r="44" spans="1:41" s="28" customFormat="1">
@@ -6390,7 +6392,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C44" s="28">
         <v>2007</v>
@@ -6399,7 +6401,7 @@
         <v>2014</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="F44" s="28">
         <v>2004</v>
@@ -6511,10 +6513,10 @@
         <v>0</v>
       </c>
       <c r="AN44" s="28" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="AO44" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:41" s="28" customFormat="1">
@@ -6522,7 +6524,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="C45" s="28">
         <v>2007</v>
@@ -6531,7 +6533,7 @@
         <v>2014</v>
       </c>
       <c r="E45" s="30" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="F45" s="28">
         <v>2004</v>
@@ -6642,10 +6644,10 @@
         <v>0</v>
       </c>
       <c r="AN45" s="28" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="AO45" s="33" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:41" s="28" customFormat="1">
@@ -6653,7 +6655,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="C46" s="28">
         <v>2007</v>
@@ -6662,7 +6664,7 @@
         <v>2014</v>
       </c>
       <c r="E46" s="30" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="F46" s="28">
         <v>2004</v>
@@ -6774,10 +6776,10 @@
         <v>0</v>
       </c>
       <c r="AN46" s="28" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="AO46" s="33" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:41" s="28" customFormat="1">
@@ -6785,7 +6787,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="28" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C47" s="28">
         <v>2007</v>
@@ -6794,7 +6796,7 @@
         <v>2014</v>
       </c>
       <c r="E47" s="30" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="F47" s="28">
         <v>2004</v>
@@ -6905,10 +6907,10 @@
         <v>0</v>
       </c>
       <c r="AN47" s="28" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="AO47" s="33" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:41" s="28" customFormat="1">
@@ -6916,7 +6918,7 @@
         <v>45</v>
       </c>
       <c r="B48" s="28" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C48" s="28">
         <v>2007</v>
@@ -6925,7 +6927,7 @@
         <v>2014</v>
       </c>
       <c r="E48" s="30" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="F48" s="28">
         <v>2004</v>
@@ -7039,10 +7041,10 @@
         <v>0</v>
       </c>
       <c r="AN48" s="28" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="AO48" s="33" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:41" s="28" customFormat="1">
@@ -7050,7 +7052,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="28" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C49" s="28">
         <v>2007</v>
@@ -7059,7 +7061,7 @@
         <v>2014</v>
       </c>
       <c r="E49" s="30" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="F49" s="28">
         <v>2004</v>
@@ -7173,10 +7175,10 @@
         <v>0</v>
       </c>
       <c r="AN49" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AO49" s="33" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:41" s="28" customFormat="1">
@@ -7184,7 +7186,7 @@
         <v>47</v>
       </c>
       <c r="B50" s="28" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C50" s="28">
         <v>2007</v>
@@ -7193,7 +7195,7 @@
         <v>2014</v>
       </c>
       <c r="E50" s="30" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="F50" s="28">
         <v>2004</v>
@@ -7307,10 +7309,10 @@
         <v>0</v>
       </c>
       <c r="AN50" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AO50" s="33" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:41" s="28" customFormat="1">
@@ -7318,7 +7320,7 @@
         <v>48</v>
       </c>
       <c r="B51" s="28" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C51" s="28">
         <v>2007</v>
@@ -7327,7 +7329,7 @@
         <v>2014</v>
       </c>
       <c r="E51" s="30" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="F51" s="28">
         <v>2004</v>
@@ -7441,10 +7443,10 @@
         <v>0</v>
       </c>
       <c r="AN51" s="28" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="AO51" s="33" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:41" s="5" customFormat="1">
@@ -7609,7 +7611,6 @@
       <c r="A104" s="33"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -7624,7 +7625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:AF53"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
@@ -8572,11 +8573,11 @@
       </c>
       <c r="F8" s="33">
         <f>generator_costs!M10</f>
-        <v>7935139.1551307421</v>
+        <v>7098171.79151126</v>
       </c>
       <c r="G8" s="33">
         <f>generator_costs!N10</f>
-        <v>46146.299999999996</v>
+        <v>48159.29</v>
       </c>
       <c r="H8" s="33">
         <f>generator_costs!O10</f>
@@ -8584,7 +8585,7 @@
       </c>
       <c r="I8" s="33">
         <f>generator_costs!P10</f>
-        <v>-4.4999999999999998E-2</v>
+        <v>-8.8500000000000002E-3</v>
       </c>
       <c r="J8" s="33">
         <f>generator_costs!Q10</f>
@@ -11172,11 +11173,11 @@
       </c>
       <c r="F28" s="33">
         <f>generator_costs!M30</f>
-        <v>4624269.4583522985</v>
+        <v>4401886.3331025699</v>
       </c>
       <c r="G28" s="33">
         <f>generator_costs!N30</f>
-        <v>42817.049999999996</v>
+        <v>48159.29</v>
       </c>
       <c r="H28" s="33">
         <f>generator_costs!O30</f>
@@ -11184,7 +11185,7 @@
       </c>
       <c r="I28" s="33">
         <f>generator_costs!P30</f>
-        <v>-2.5000000000000001E-2</v>
+        <v>-8.8500000000000002E-3</v>
       </c>
       <c r="J28" s="33">
         <f>generator_costs!Q30</f>
@@ -14022,7 +14023,6 @@
       <c r="A53" s="33"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -14045,7 +14045,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="6" t="s">
-        <v>77</v>
+        <v>139</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -14056,7 +14056,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="B2">
         <v>2010</v>
@@ -14074,7 +14074,7 @@
         <v>2026</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -14268,23 +14268,23 @@
       </c>
       <c r="C9" s="1">
         <f>generator_costs!$M10*(1+generator_costs!$P10)^(C$2-2007)/1000000</f>
-        <v>5.7488125543358102</v>
+        <v>6.6699442382837946</v>
       </c>
       <c r="D9" s="1">
         <f>generator_costs!$M10*(1+generator_costs!$P10)^(D$2-2007)/1000000</f>
-        <v>4.78180249863897</v>
+        <v>6.4369442002129151</v>
       </c>
       <c r="E9" s="1">
         <f>generator_costs!$M10*(1+generator_costs!$P10)^(E$2-2007)/1000000</f>
-        <v>3.9774535906105353</v>
+        <v>6.2120835132072854</v>
       </c>
       <c r="F9" s="1">
         <f>generator_costs!$M10*(1+generator_costs!$P10)^(F$2-2007)/1000000</f>
-        <v>3.3084045336384098</v>
+        <v>5.9950778466877699</v>
       </c>
       <c r="G9" s="2">
         <f>-generator_costs!P10*100</f>
-        <v>4.5</v>
+        <v>0.88500000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -14868,23 +14868,23 @@
       </c>
       <c r="C29" s="1">
         <f>generator_costs!$M30*(1+generator_costs!$P30)^(C$2-2007)/1000000</f>
-        <v>3.8732492243935535</v>
+        <v>4.1363237249582836</v>
       </c>
       <c r="D29" s="1">
         <f>generator_costs!$M30*(1+generator_costs!$P30)^(D$2-2007)/1000000</f>
-        <v>3.5002084214571272</v>
+        <v>3.991830225318961</v>
       </c>
       <c r="E29" s="1">
         <f>generator_costs!$M30*(1+generator_costs!$P30)^(E$2-2007)/1000000</f>
-        <v>3.1630959651344517</v>
+        <v>3.852384292752796</v>
       </c>
       <c r="F29" s="1">
         <f>generator_costs!$M30*(1+generator_costs!$P30)^(F$2-2007)/1000000</f>
-        <v>2.8584515205768017</v>
+        <v>3.7178096014498263</v>
       </c>
       <c r="G29" s="2">
         <f>-generator_costs!P30*100</f>
-        <v>2.5</v>
+        <v>0.88500000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -15518,7 +15518,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -15541,15 +15540,15 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="22" t="s">
-        <v>80</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="22" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>82</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="22" customFormat="1">
@@ -15577,7 +15576,7 @@
         <v>3.3</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>84</v>
+        <v>146</v>
       </c>
       <c r="E5" s="22"/>
     </row>
@@ -15730,7 +15729,6 @@
       <c r="E21" s="22"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
-BIO SUPPLY CURVE: -changed data sources for supply curve -added producer surplus onto the biomass supply curve -the amount of solid biomass available now changes by period -added canada and mexico biomass and biogas -changed min_build_year of Biomass_IGCC to 2011 (from 2016)
</commit_message>
<xml_diff>
--- a/DatabasePrep/GeneratorInfo/generator_costs.xlsx
+++ b/DatabasePrep/GeneratorInfo/generator_costs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-37540" yWindow="1960" windowWidth="34400" windowHeight="22000" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="21580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="generator_costs" sheetId="1" r:id="rId1"/>
@@ -25,89 +25,570 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="212">
   <si>
-    <t>We assumed that the capital cost and fixed cost for adding a CCS system increase by the same amount (per W) as for Coal IGCC;  we assumed CCS biomass IGCC heat rate increases by the same percentage relative to non-CCS biomass IGCC as CCS to non-CCS coal IGCC heat rates; we also assume that there's an adder per MWh for variable costs -- we assume that the difference in variable cost scales with the difference in heat rates</t>
+    <t>CEC COG Model Version 2.02-4-5-10; we chose the fluidized bed biomass technology because it's more advanced</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>CCGT_Cogen_CCS</t>
+    <t>intermittent</t>
+  </si>
+  <si>
+    <t>resource_limited</t>
+  </si>
+  <si>
+    <t>baseload</t>
+  </si>
+  <si>
+    <t>min_build_capacity</t>
+  </si>
+  <si>
+    <t>$year_of_costs</t>
+  </si>
+  <si>
+    <t>cost_for_which_year?</t>
+  </si>
+  <si>
+    <t>connect_cost_generic_$2007_per_mw</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Gas_Combustion_Turbine_Cogen_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bio_Gas_Internal_Combustion_Engine_Cogen_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bio_Solid_Steam_Turbine_Cogen_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bio_Gas_Steam_Turbine_EP</t>
-  </si>
-  <si>
-    <t>"Updated Capital Cost Estimates for Electricity Generation Plants," US EIA, November 2010; construction cost breakdown comes from the ReEDs Sheet; outage rates are the same as hydro</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>We assume that a combustion turbine will never run at part load lower than 50 percent, so the 10-min ramp rate used to calculate the heat rate penalty is 0.5 rather than 1.</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sources</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Heat rate curve</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Extra Fuel D</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Extra Fuel (Sp)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Percent of full load</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Spinning reserve provided</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Steam</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Combustion</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>note: we assume that cogen plants have 3/4 of the capital cost and fixed cost of a pure-electric plant, (to reflect shared infrastructure for cogen), but the same variable operating costs.</t>
+    <t>fuel</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>Gas</t>
-  </si>
-  <si>
-    <t>interest_between_price_year_and_cost_year</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Residential_PV</t>
+    <t>Capital and fixed cost equal to cost for Bio_Solid_Steam_Turbine_Cogen plus the difference between Coal_Steam_Turbine_Cogen_CCS and Coal_Steam_Turbine_Cogen; overnight cost change like Coal_Steam_Turbine_Cogen_CCS; other params like Bio_Solid_Steam_Turbine_Cogen</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>technology_id</t>
+    <t>Costs are same as Bio_Solid_Steam_Turbine_Cogen_CCS; flags same as Bio_Liquid_Steam_Turbine_Cogen</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>We assumed that the capital cost and fixed cost for adding a CCS system increase by the same amount (per W) as for CCGT; we assumed CCS combustion turbine heat rate increases by the same percentage relative to non-CCS combustion turbines as CCS to non-CCS CCGT heat rates; we also assume that there's an adder per MWh for variable costs -- we assume that the difference in variable cost scales with the difference in heat rates</t>
+    <t>Uranium</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>var_o_m_$2007</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>technology</t>
+  </si>
+  <si>
+    <t>overnight_cost_change</t>
+  </si>
+  <si>
+    <t>Structure and Performance of Six European Wholesale Electricity Markets in 2003, 2004, and 2005. Appendix I. DG Comp. Presented to DG Comp 26th February 2007</t>
+  </si>
+  <si>
+    <t>Ramp rates</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>WWSIS, p. 174</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Part load relative heat rate</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heat rate penalty</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Updated Capital Cost Estimates for Electricity Generation Plants," US EIA, November 2010; chose the dual unit rather than the single unit costs because if we're installing CCS, we're likley installing a lot; the lifetime, construction time, construction cost breakdown, and outage rates are the same as Coal Steam Turbine</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as new Biogas</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as existing combustion turbines, 75% capital cost and fixed cost</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as existing coal steam turbines, 75% capital cost and fixed cost</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as existing gas steam turbines, 75% capital cost and fixed cost</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as existing CCGT, 75% capital cost and fixed cost</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as existing Gas Internal Combustion Engine, 75% capital cost and fixed cost</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Everything but costs same as gas steam turbine; captial and fixed costs are assumed to be the gas steam turbine cost plus the difference between biogas and gas combustion turbine</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as new biomass steam turbine</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Updated Capital Cost Estimates for Electricity Generation Plants," US EIA, November 2010; we assume the same lifetime, construction time, construction cost breakdown, and outage rates as for Coal IGCC</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CEC COG Model Version 2.02-4-5-10</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CEC COG Model Version 2.02-4-5-10; we chose the binary geothermal plants because they are more advanced</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Updated Capital Cost Estimates for Electricity Generation Plants," US EIA, November 2010; construction cost breakdown comes from the ReEDs Sheet; outage rates are from the CEC COG Model</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Offshore_Wind</t>
+  </si>
+  <si>
+    <t>Bio_Gas</t>
+  </si>
+  <si>
+    <t>year_1_cost_fraction</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_2_cost_fraction</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_3_cost_fraction</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery_Storage</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Storage</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CEC COG Model Version 2.02-4-5-10; we picked dual flash as the existing geothermal technology</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as new nuclear</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>can_build_new</t>
+  </si>
+  <si>
+    <t>forced_outage_rate</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>scheduled_outage_rate</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReEDs Sheet</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>tech_name_again</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Geothermal</t>
+  </si>
+  <si>
+    <t>DistillateFuelOil_Internal_Combustion_Engine_EP</t>
+  </si>
+  <si>
+    <t>DistillateFuelOil_Combustion_Turbine_EP</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>DistillateFuelOil</t>
+  </si>
+  <si>
+    <t>Compressed_Air_Energy_Storage</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-min ramp rate</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to coal IGCC</t>
+  </si>
+  <si>
+    <t>Coal_IGCC</t>
+  </si>
+  <si>
+    <t>Same as new Biogas, 75% capital cost and fixed cost</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as new biomass steam turbine, 75% capital cost and fixed cost</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as new coal steam turbines, 75% capital cost and fixed cost</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as gas combustion turbines, 75% capital cost and fixed cost</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as gas combustion turbine CCS; 75% capital cost and fixed cost</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as Gas_Internal_Combustion_Engine_Cogen_EP (which already includes the 75% of capital and fixed costs)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Steam_Turbine_Cogen_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as Gas_Combustion_Turbine_Cogen_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Capital and fixed cost equal to 75% of Gas_Steam_Turbine_EP + difference between CCGT_CCS and CCGT, other flags like Gas_Steam_Turbine_Cogen (except ccs)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as new Biogas_CCS, 75% capital cost and fixed cost</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Capital and fixed cost equal to 75% of Coal_Steam_Turbine_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data_Source</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as existing Gas Combustion Turbine</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Geothermal_EP</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Internal_Combustion_Engine_Cogen_EP</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCGT_Cogen_EP</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>storage_efficiency</t>
+  </si>
+  <si>
+    <t>max_store_rate</t>
+  </si>
+  <si>
+    <t>ccs</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPV Consortium numbers (It's more or less SolFocus)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>cost declination rate</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Liquid_Steam_Turbine_Cogen_EP</t>
+  </si>
+  <si>
+    <t>Bio_Solid_Steam_Turbine_EP</t>
+  </si>
+  <si>
+    <t>Bio_Solid_Steam_Turbine_Cogen_EP</t>
+  </si>
+  <si>
+    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to gas combustion turbine</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>heat_rate_penalty_spinning_reserve</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCGT</t>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine</t>
+  </si>
+  <si>
+    <t>CCGT_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Gas_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biomass_IGCC_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_IGCC_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>overnight_cost_$2007</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Steam_Turbine_Cogen_EP</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Updated Capital Cost Estimates for Electricity Generation Plants," US EIA, November 2010; the lifetime, construction time, construction cost breakdown, and outage rates are the same as CCGT</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_spinning_reserve_fraction_of_capacity</t>
+  </si>
+  <si>
+    <t>Bio_Liquid</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CEC COG Model Version 2.02-4-5-10; we picked the advanced combustion turbine as the new technology</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Updated Capital Cost Estimates for Electricity Generation Plants," US EIA, November 2010; the lifetime, construction time, construction cost breakdown, and outage rates are the same as Coal IGCC</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>We assumed that the capital cost and fixed cost for adding a CCS system increase by the same amount (per W) as for gas combustion turbine; as biogas contains 50% pre-combustion CO2, we assumed that the biogas-CCS heat rate was the biogas non-CCS heat rate plus double the difference between CCS to non-CCS combustion turbine heat rates; we also assume a similar multiplier to variable costs</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as CCGT_CCS; 75% capital cost and fixed cost</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biomass_Steam_Turbine</t>
+  </si>
+  <si>
+    <t>Hydro_NonPumped</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hydro_Pumped</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Water</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Water</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biomass_IGCC</t>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_Cogen_EP</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>storage</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ReEDs Sheet; also Sullivan et al (2008), NREL/CP-670-43510 Conference Paper for o&amp;m costs, declanation rate, etc; $1,200,000 taken as capital cost in 2010 rather than 2004 based on conversation with Hernandez, also The storage efficiency of the the storage phase of compressed air energy storage from Samir Succar and Robert H. Williams: Compressed Air Energy Storage: Theory, Resources, And Applications For Wind Power, p. 39
+</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCGT_EP</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Combustion_Turbine_EP</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wind</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>price_and_dollar_year</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CEC COG Model Version 2.02-4-5-10; we picked the advanced CCGT technology (H Frame) for the new CCGT plants</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CEC COG Model Version 2.02-4-5-10; we picked the duct firing CCGT turbine for the existing CCGT technology</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Solar</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Solid</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>construction_time_years</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_EP</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Steam_Turbine_EP</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Solid_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_age_years</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Solar</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Gas</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine</t>
+  </si>
+  <si>
+    <t>Nuclear</t>
+  </si>
+  <si>
+    <t>Wind_EP</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>overnight_cost</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Liquid_Steam_Turbine_Cogen_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_Steam_Turbine_Cogen_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_Internal_Combustion_Engine_Cogen_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Gas_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Liquid_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bio_Solid_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coal_CCS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gas</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CEC COG Model Version 2.02-4-5-10</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CEC COG Model Version 2.02-4-5-10; the overnight cost is adjusted from the non-storage CSP overnight-cost based on the difference in the storage and non-storage CSP from the Solar Advisor Model; the construction time of 1 year is probably too low</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CEC COG Model Version 2.02-4-5-10</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>dispatchable</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>cogen</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as new CCGT, 75% capital cost and fixed cost</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>all dispatch data from TEPPC_Generator_Categories</t>
+  </si>
+  <si>
+    <t>year</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>$/Wp</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -272,570 +753,89 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">ReEDs Sheet; also Sullivan et al (2008), NREL/CP-670-43510 Conference Paper for o&amp;m costs, declanation rate, etc; $1,200,000 taken as capital cost in 2010 rather than 2004 based on conversation with Hernandez, also The storage efficiency of the the storage phase of compressed air energy storage from Samir Succar and Robert H. Williams: Compressed Air Energy Storage: Theory, Resources, And Applications For Wind Power, p. 39
-</t>
+    <t>We assumed that the capital cost and fixed cost for adding a CCS system increase by the same amount (per W) as for Coal IGCC;  we assumed CCS biomass IGCC heat rate increases by the same percentage relative to non-CCS biomass IGCC as CCS to non-CCS coal IGCC heat rates; we also assume that there's an adder per MWh for variable costs -- we assume that the difference in variable cost scales with the difference in heat rates</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>CCGT_EP</t>
+    <t>CCGT_Cogen_CCS</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Gas_Combustion_Turbine_EP</t>
+    <t>Gas_Combustion_Turbine_Cogen_CCS</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Wind</t>
+    <t>Bio_Gas_Internal_Combustion_Engine_Cogen_CCS</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>price_and_dollar_year</t>
+    <t>Bio_Solid_Steam_Turbine_Cogen_CCS</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>CEC COG Model Version 2.02-4-5-10; we picked the advanced CCGT technology (H Frame) for the new CCGT plants</t>
+    <t>Bio_Gas_Steam_Turbine_EP</t>
+  </si>
+  <si>
+    <t>"Updated Capital Cost Estimates for Electricity Generation Plants," US EIA, November 2010; construction cost breakdown comes from the ReEDs Sheet; outage rates are the same as hydro</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>CEC COG Model Version 2.02-4-5-10; we picked the duct firing CCGT turbine for the existing CCGT technology</t>
+    <t>We assume that a combustion turbine will never run at part load lower than 50 percent, so the 10-min ramp rate used to calculate the heat rate penalty is 0.5 rather than 1.</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Solar</t>
+    <t>Sources</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Bio_Solid</t>
+    <t>Heat rate curve</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>construction_time_years</t>
+    <t>Extra Fuel D</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Coal_Steam_Turbine_EP</t>
+    <t>Extra Fuel (Sp)</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Gas_Steam_Turbine_EP</t>
+    <t>Percent of full load</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Bio_Solid_CCS</t>
+    <t>Spinning reserve provided</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>max_age_years</t>
+    <t>Steam</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Solar</t>
+    <t>Combustion</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Bio_Gas</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine</t>
-  </si>
-  <si>
-    <t>Nuclear</t>
-  </si>
-  <si>
-    <t>Wind_EP</t>
+    <t>note: we assume that cogen plants have 3/4 of the capital cost and fixed cost of a pure-electric plant, (to reflect shared infrastructure for cogen), but the same variable operating costs.</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>Gas</t>
+  </si>
+  <si>
+    <t>interest_between_price_year_and_cost_year</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>overnight_cost</t>
+    <t>Residential_PV</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Bio_Liquid_Steam_Turbine_Cogen_CCS</t>
+    <t>technology_id</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Coal_Steam_Turbine_Cogen_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Internal_Combustion_Engine_Cogen_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bio_Gas_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bio_Liquid_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bio_Solid_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>CEC COG Model Version 2.02-4-5-10</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>CEC COG Model Version 2.02-4-5-10; the overnight cost is adjusted from the non-storage CSP overnight-cost based on the difference in the storage and non-storage CSP from the Solar Advisor Model; the construction time of 1 year is probably too low</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>CEC COG Model Version 2.02-4-5-10</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>dispatchable</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>cogen</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Same as new CCGT, 75% capital cost and fixed cost</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>all dispatch data from TEPPC_Generator_Categories</t>
-  </si>
-  <si>
-    <t>year</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>$/Wp</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>CPV Consortium numbers (It's more or less SolFocus)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>cost declination rate</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bio_Liquid_Steam_Turbine_Cogen_EP</t>
-  </si>
-  <si>
-    <t>Bio_Solid_Steam_Turbine_EP</t>
-  </si>
-  <si>
-    <t>Bio_Solid_Steam_Turbine_Cogen_EP</t>
-  </si>
-  <si>
-    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to gas combustion turbine</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>heat_rate_penalty_spinning_reserve</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCGT</t>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine</t>
-  </si>
-  <si>
-    <t>CCGT_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Combustion_Turbine_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bio_Gas_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biomass_IGCC_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_IGCC_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>overnight_cost_$2007</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_Cogen_EP</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>"Updated Capital Cost Estimates for Electricity Generation Plants," US EIA, November 2010; the lifetime, construction time, construction cost breakdown, and outage rates are the same as CCGT</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_spinning_reserve_fraction_of_capacity</t>
-  </si>
-  <si>
-    <t>Bio_Liquid</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>CEC COG Model Version 2.02-4-5-10; we picked the advanced combustion turbine as the new technology</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>"Updated Capital Cost Estimates for Electricity Generation Plants," US EIA, November 2010; the lifetime, construction time, construction cost breakdown, and outage rates are the same as Coal IGCC</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>We assumed that the capital cost and fixed cost for adding a CCS system increase by the same amount (per W) as for gas combustion turbine; as biogas contains 50% pre-combustion CO2, we assumed that the biogas-CCS heat rate was the biogas non-CCS heat rate plus double the difference between CCS to non-CCS combustion turbine heat rates; we also assume a similar multiplier to variable costs</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Same as CCGT_CCS; 75% capital cost and fixed cost</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biomass_Steam_Turbine</t>
-  </si>
-  <si>
-    <t>Hydro_NonPumped</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hydro_Pumped</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Water</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Water</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biomass_IGCC</t>
-  </si>
-  <si>
-    <t>Coal_Steam_Turbine_Cogen_EP</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>storage</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Offshore_Wind</t>
-  </si>
-  <si>
-    <t>Bio_Gas</t>
-  </si>
-  <si>
-    <t>year_1_cost_fraction</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_2_cost_fraction</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>year_3_cost_fraction</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Battery_Storage</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Storage</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>CEC COG Model Version 2.02-4-5-10; we picked dual flash as the existing geothermal technology</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Same as new nuclear</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>can_build_new</t>
-  </si>
-  <si>
-    <t>forced_outage_rate</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>scheduled_outage_rate</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReEDs Sheet</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>tech_name_again</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Geothermal</t>
-  </si>
-  <si>
-    <t>DistillateFuelOil_Internal_Combustion_Engine_EP</t>
-  </si>
-  <si>
-    <t>DistillateFuelOil_Combustion_Turbine_EP</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>DistillateFuelOil</t>
-  </si>
-  <si>
-    <t>Compressed_Air_Energy_Storage</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-min ramp rate</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>EIA, cost declination rate, construction time, lifetime, outage rates assumed to be equal to coal IGCC</t>
-  </si>
-  <si>
-    <t>Coal_IGCC</t>
-  </si>
-  <si>
-    <t>Same as new Biogas, 75% capital cost and fixed cost</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Same as new biomass steam turbine, 75% capital cost and fixed cost</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Same as new coal steam turbines, 75% capital cost and fixed cost</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Same as gas combustion turbines, 75% capital cost and fixed cost</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Same as gas combustion turbine CCS; 75% capital cost and fixed cost</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Same as Gas_Internal_Combustion_Engine_Cogen_EP (which already includes the 75% of capital and fixed costs)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Steam_Turbine_Cogen_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Same as Gas_Combustion_Turbine_Cogen_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Capital and fixed cost equal to 75% of Gas_Steam_Turbine_EP + difference between CCGT_CCS and CCGT, other flags like Gas_Steam_Turbine_Cogen (except ccs)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Same as new Biogas_CCS, 75% capital cost and fixed cost</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Capital and fixed cost equal to 75% of Coal_Steam_Turbine_CCS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data_Source</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Same as existing Gas Combustion Turbine</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Geothermal_EP</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas_Internal_Combustion_Engine_Cogen_EP</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>CCGT_Cogen_EP</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>storage_efficiency</t>
-  </si>
-  <si>
-    <t>max_store_rate</t>
-  </si>
-  <si>
-    <t>ccs</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coal</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Uranium</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>var_o_m_$2007</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>technology</t>
-  </si>
-  <si>
-    <t>overnight_cost_change</t>
-  </si>
-  <si>
-    <t>Structure and Performance of Six European Wholesale Electricity Markets in 2003, 2004, and 2005. Appendix I. DG Comp. Presented to DG Comp 26th February 2007</t>
-  </si>
-  <si>
-    <t>Ramp rates</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>WWSIS, p. 174</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Part load relative heat rate</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Heat rate penalty</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>"Updated Capital Cost Estimates for Electricity Generation Plants," US EIA, November 2010; chose the dual unit rather than the single unit costs because if we're installing CCS, we're likley installing a lot; the lifetime, construction time, construction cost breakdown, and outage rates are the same as Coal Steam Turbine</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Same as new Biogas</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Same as existing combustion turbines, 75% capital cost and fixed cost</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Same as existing coal steam turbines, 75% capital cost and fixed cost</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Same as existing gas steam turbines, 75% capital cost and fixed cost</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Same as existing CCGT, 75% capital cost and fixed cost</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Same as existing Gas Internal Combustion Engine, 75% capital cost and fixed cost</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Everything but costs same as gas steam turbine; captial and fixed costs are assumed to be the gas steam turbine cost plus the difference between biogas and gas combustion turbine</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Same as new biomass steam turbine</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>"Updated Capital Cost Estimates for Electricity Generation Plants," US EIA, November 2010; we assume the same lifetime, construction time, construction cost breakdown, and outage rates as for Coal IGCC</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>CEC COG Model Version 2.02-4-5-10</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>CEC COG Model Version 2.02-4-5-10; we chose the binary geothermal plants because they are more advanced</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>"Updated Capital Cost Estimates for Electricity Generation Plants," US EIA, November 2010; construction cost breakdown comes from the ReEDs Sheet; outage rates are from the CEC COG Model</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>CEC COG Model Version 2.02-4-5-10; we chose the fluidized bed biomass technology because it's more advanced</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>intermittent</t>
-  </si>
-  <si>
-    <t>resource_limited</t>
-  </si>
-  <si>
-    <t>baseload</t>
-  </si>
-  <si>
-    <t>min_build_capacity</t>
-  </si>
-  <si>
-    <t>$year_of_costs</t>
-  </si>
-  <si>
-    <t>cost_for_which_year?</t>
-  </si>
-  <si>
-    <t>connect_cost_generic_$2007_per_mw</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>fuel</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gas</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Capital and fixed cost equal to cost for Bio_Solid_Steam_Turbine_Cogen plus the difference between Coal_Steam_Turbine_Cogen_CCS and Coal_Steam_Turbine_Cogen; overnight cost change like Coal_Steam_Turbine_Cogen_CCS; other params like Bio_Solid_Steam_Turbine_Cogen</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Costs are same as Bio_Solid_Steam_Turbine_Cogen_CCS; flags same as Bio_Liquid_Steam_Turbine_Cogen</t>
+    <t>We assumed that the capital cost and fixed cost for adding a CCS system increase by the same amount (per W) as for CCGT; we assumed CCS combustion turbine heat rate increases by the same percentage relative to non-CCS combustion turbines as CCS to non-CCS CCGT heat rates; we also assume that there's an adder per MWh for variable costs -- we assume that the difference in variable cost scales with the difference in heat rates</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -843,17 +843,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="10">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  <numFmts count="4">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.0000"/>
-    <numFmt numFmtId="172" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -934,7 +928,7 @@
   <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -955,7 +949,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -965,15 +959,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -2029,25 +2023,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="536636344"/>
-        <c:axId val="536638568"/>
+        <c:axId val="541458712"/>
+        <c:axId val="69297432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="536636344"/>
+        <c:axId val="541458712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="536638568"/>
+        <c:crossAx val="69297432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="536638568"/>
+        <c:axId val="69297432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2055,7 +2049,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="536636344"/>
+        <c:crossAx val="541458712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3076,11 +3070,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="475233256"/>
-        <c:axId val="541021384"/>
+        <c:axId val="541220328"/>
+        <c:axId val="541223400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="475233256"/>
+        <c:axId val="541220328"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1.0"/>
@@ -3089,12 +3083,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541021384"/>
+        <c:crossAx val="541223400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="541021384"/>
+        <c:axId val="541223400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3102,7 +3096,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="475233256"/>
+        <c:crossAx val="541220328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3461,11 +3455,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="536507784"/>
-        <c:axId val="536184344"/>
+        <c:axId val="541896872"/>
+        <c:axId val="541899944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="536507784"/>
+        <c:axId val="541896872"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1.0"/>
@@ -3474,12 +3468,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="536184344"/>
+        <c:crossAx val="541899944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="536184344"/>
+        <c:axId val="541899944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3487,7 +3481,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="536507784"/>
+        <c:crossAx val="541896872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3923,10 +3917,10 @@
   <dimension ref="A1:AQ114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N29" sqref="N29"/>
+      <selection pane="bottomRight" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -3960,144 +3954,144 @@
   <sheetData>
     <row r="1" spans="1:43" s="29" customFormat="1">
       <c r="A1" s="30" t="s">
-        <v>16</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:43" s="29" customFormat="1">
       <c r="A2" s="30" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:43" s="29" customFormat="1"/>
     <row r="4" spans="1:43">
       <c r="A4" s="5" t="s">
-        <v>20</v>
+        <v>210</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J4" t="s">
+        <v>160</v>
+      </c>
+      <c r="K4" t="s">
+        <v>161</v>
+      </c>
+      <c r="L4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M4" t="s">
+        <v>182</v>
+      </c>
+      <c r="N4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>183</v>
+      </c>
+      <c r="R4" t="s">
+        <v>119</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="W4" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="X4" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE4" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF4" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI4" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="AJ4" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK4" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AN4" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="AO4" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="AP4" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ4" s="29" t="s">
         <v>67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" t="s">
-        <v>208</v>
-      </c>
-      <c r="F4" t="s">
-        <v>205</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
-        <v>206</v>
-      </c>
-      <c r="I4" t="s">
-        <v>83</v>
-      </c>
-      <c r="J4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" t="s">
-        <v>119</v>
-      </c>
-      <c r="M4" t="s">
-        <v>55</v>
-      </c>
-      <c r="N4" t="s">
-        <v>179</v>
-      </c>
-      <c r="O4" t="s">
-        <v>181</v>
-      </c>
-      <c r="P4" t="s">
-        <v>207</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>56</v>
-      </c>
-      <c r="R4" t="s">
-        <v>72</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="T4" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="W4" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="X4" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y4" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>146</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>147</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>201</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>202</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>203</v>
-      </c>
-      <c r="AE4" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="AF4" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>204</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>145</v>
-      </c>
-      <c r="AI4" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ4" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="AK4" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>174</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>175</v>
-      </c>
-      <c r="AN4" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="AO4" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="AP4" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="AQ4" s="29" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:43">
@@ -4105,7 +4099,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="C5" s="5">
         <v>2007</v>
@@ -4114,7 +4108,7 @@
         <v>2011</v>
       </c>
       <c r="E5" t="s">
-        <v>209</v>
+        <v>9</v>
       </c>
       <c r="F5">
         <v>2009</v>
@@ -4232,7 +4226,7 @@
         <v>CCGT</v>
       </c>
       <c r="AQ5" s="29" t="s">
-        <v>68</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:43">
@@ -4383,7 +4377,7 @@
         <v>CCGT_Cogen</v>
       </c>
       <c r="AQ6" s="29" t="s">
-        <v>98</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:43">
@@ -4391,7 +4385,7 @@
         <v>110</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>1</v>
+        <v>191</v>
       </c>
       <c r="C7" s="5">
         <v>2007</v>
@@ -4400,7 +4394,7 @@
         <v>2016</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="L7">
         <f>0.75*L8</f>
@@ -4505,7 +4499,7 @@
         <v>CCGT_Cogen_CCS</v>
       </c>
       <c r="AQ7" s="29" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:43" s="25" customFormat="1">
@@ -4513,7 +4507,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="C8" s="25">
         <v>2007</v>
@@ -4522,7 +4516,7 @@
         <v>2016</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="F8" s="25">
         <v>2010</v>
@@ -4650,7 +4644,7 @@
         <v>CCGT_CCS</v>
       </c>
       <c r="AQ8" s="29" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:43" s="5" customFormat="1">
@@ -4658,7 +4652,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="C9" s="29">
         <v>2007</v>
@@ -4787,7 +4781,7 @@
         <v>CCGT_EP</v>
       </c>
       <c r="AQ9" s="29" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:43" s="19" customFormat="1">
@@ -4795,7 +4789,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>173</v>
+        <v>71</v>
       </c>
       <c r="C10" s="29">
         <v>2007</v>
@@ -4940,7 +4934,7 @@
         <v>CCGT_Cogen_EP</v>
       </c>
       <c r="AQ10" s="29" t="s">
-        <v>192</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:43">
@@ -4948,7 +4942,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="C11" s="5">
         <v>2007</v>
@@ -4957,7 +4951,7 @@
         <v>2011</v>
       </c>
       <c r="E11" t="s">
-        <v>209</v>
+        <v>9</v>
       </c>
       <c r="F11">
         <v>2009</v>
@@ -5075,7 +5069,7 @@
         <v>Gas_Combustion_Turbine</v>
       </c>
       <c r="AQ11" s="29" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:43">
@@ -5225,7 +5219,7 @@
         <v>Gas_Combustion_Turbine_Cogen</v>
       </c>
       <c r="AQ12" s="29" t="s">
-        <v>161</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:43">
@@ -5233,7 +5227,7 @@
         <v>111</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>2</v>
+        <v>192</v>
       </c>
       <c r="C13" s="5">
         <v>2007</v>
@@ -5242,7 +5236,7 @@
         <v>2016</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="L13">
         <f>0.75*L14</f>
@@ -5346,7 +5340,7 @@
         <v>Gas_Combustion_Turbine_Cogen_CCS</v>
       </c>
       <c r="AQ13" s="29" t="s">
-        <v>162</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:43" s="25" customFormat="1">
@@ -5354,7 +5348,7 @@
         <v>35</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="C14" s="25">
         <v>2007</v>
@@ -5363,7 +5357,7 @@
         <v>2016</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="L14" s="29">
         <f>L11+(L8-L5)</f>
@@ -5475,7 +5469,7 @@
         <v>Gas_Combustion_Turbine_CCS</v>
       </c>
       <c r="AQ14" s="29" t="s">
-        <v>21</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:43" s="18" customFormat="1">
@@ -5483,7 +5477,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="C15" s="18">
         <v>2007</v>
@@ -5617,7 +5611,7 @@
         <v>Gas_Combustion_Turbine_EP</v>
       </c>
       <c r="AQ15" s="46" t="s">
-        <v>62</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:43" s="19" customFormat="1">
@@ -5625,7 +5619,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>59</v>
+        <v>186</v>
       </c>
       <c r="C16" s="29">
         <v>2007</v>
@@ -5635,7 +5629,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="F16" s="19">
         <f>F15</f>
@@ -5770,7 +5764,7 @@
         <v>Gas_Combustion_Turbine_Cogen_EP</v>
       </c>
       <c r="AQ16" s="29" t="s">
-        <v>189</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:43">
@@ -5909,7 +5903,7 @@
         <v>Gas_Internal_Combustion_Engine_Cogen</v>
       </c>
       <c r="AQ17" s="29" t="s">
-        <v>163</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:43" s="29" customFormat="1">
@@ -5917,7 +5911,7 @@
         <v>112</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>86</v>
+        <v>133</v>
       </c>
       <c r="C18" s="29">
         <v>2007</v>
@@ -5926,7 +5920,7 @@
         <v>2016</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="L18" s="29">
         <f>L13</f>
@@ -6045,7 +6039,7 @@
         <v>Gas_Internal_Combustion_Engine_Cogen_CCS</v>
       </c>
       <c r="AQ18" s="29" t="s">
-        <v>165</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:43" s="29" customFormat="1">
@@ -6053,7 +6047,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>43</v>
+        <v>170</v>
       </c>
       <c r="C19" s="29">
         <v>2007</v>
@@ -6200,7 +6194,7 @@
         <v>Gas_Internal_Combustion_Engine_EP</v>
       </c>
       <c r="AQ19" s="29" t="s">
-        <v>39</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:43" s="29" customFormat="1">
@@ -6208,7 +6202,7 @@
         <v>40</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>172</v>
+        <v>70</v>
       </c>
       <c r="C20" s="29">
         <v>2007</v>
@@ -6353,7 +6347,7 @@
         <v>Gas_Internal_Combustion_Engine_Cogen_EP</v>
       </c>
       <c r="AQ20" s="29" t="s">
-        <v>193</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:43">
@@ -6512,7 +6506,7 @@
         <v>113</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>164</v>
+        <v>62</v>
       </c>
       <c r="C22" s="5">
         <v>2007</v>
@@ -6521,7 +6515,7 @@
         <v>2016</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="L22" s="29">
         <f>0.75*(L23+(L8-L5))</f>
@@ -6635,7 +6629,7 @@
         <v>Gas_Steam_Turbine_Cogen_CCS</v>
       </c>
       <c r="AQ22" s="29" t="s">
-        <v>166</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:43" s="5" customFormat="1">
@@ -6643,7 +6637,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="C23" s="29">
         <v>2007</v>
@@ -6652,7 +6646,7 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>207</v>
       </c>
       <c r="F23" s="29">
         <v>2007</v>
@@ -6770,7 +6764,7 @@
         <v>Gas_Steam_Turbine_EP</v>
       </c>
       <c r="AQ23" s="29" t="s">
-        <v>42</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:43" s="19" customFormat="1">
@@ -6778,7 +6772,7 @@
         <v>31</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="C24" s="29">
         <v>2007</v>
@@ -6924,7 +6918,7 @@
         <v>Gas_Steam_Turbine_Cogen_EP</v>
       </c>
       <c r="AQ24" s="29" t="s">
-        <v>191</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:43">
@@ -6932,7 +6926,7 @@
         <v>60</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>152</v>
+        <v>50</v>
       </c>
       <c r="C25" s="24">
         <f>C15</f>
@@ -6943,7 +6937,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>153</v>
+        <v>51</v>
       </c>
       <c r="F25" s="24">
         <f t="shared" ref="F25:K25" si="33">F15</f>
@@ -7091,7 +7085,7 @@
         <v>DistillateFuelOil_Combustion_Turbine_EP</v>
       </c>
       <c r="AQ25" s="29" t="s">
-        <v>170</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:43">
@@ -7099,7 +7093,7 @@
         <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>151</v>
+        <v>49</v>
       </c>
       <c r="C26" s="29">
         <f>C19</f>
@@ -7110,7 +7104,7 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>153</v>
+        <v>51</v>
       </c>
       <c r="F26" s="29">
         <f t="shared" ref="F26:K26" si="35">F19</f>
@@ -7258,7 +7252,7 @@
         <v>DistillateFuelOil_Internal_Combustion_Engine_EP</v>
       </c>
       <c r="AQ26" s="29" t="s">
-        <v>170</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:43">
@@ -7266,7 +7260,7 @@
         <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>137</v>
+        <v>35</v>
       </c>
       <c r="C27" s="5">
         <v>2007</v>
@@ -7275,7 +7269,7 @@
         <v>2011</v>
       </c>
       <c r="E27" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="F27">
         <v>2007</v>
@@ -7393,7 +7387,7 @@
         <v>Bio_Gas</v>
       </c>
       <c r="AQ27" s="29" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:43" s="25" customFormat="1">
@@ -7401,7 +7395,7 @@
         <v>36</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="C28" s="25">
         <v>2007</v>
@@ -7410,7 +7404,7 @@
         <v>2016</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="I28" s="26"/>
       <c r="L28" s="29">
@@ -7513,7 +7507,7 @@
         <v>Bio_Gas_CCS</v>
       </c>
       <c r="AQ28" s="29" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:43">
@@ -7661,7 +7655,7 @@
         <v>114</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>3</v>
+        <v>193</v>
       </c>
       <c r="C30" s="5">
         <v>2007</v>
@@ -7670,7 +7664,7 @@
         <v>2016</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
       <c r="L30">
         <f>0.75*L28</f>
@@ -7788,7 +7782,7 @@
         <v>Bio_Gas_Internal_Combustion_Engine_Cogen_CCS</v>
       </c>
       <c r="AQ30" s="29" t="s">
-        <v>167</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:43" s="29" customFormat="1">
@@ -7796,7 +7790,7 @@
         <v>80</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>40</v>
+        <v>167</v>
       </c>
       <c r="C31" s="24">
         <f t="shared" ref="C31:K31" si="40">C27</f>
@@ -7952,7 +7946,7 @@
         <v>Bio_Gas_Internal_Combustion_Engine_EP</v>
       </c>
       <c r="AQ31" s="24" t="s">
-        <v>188</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:43" s="29" customFormat="1">
@@ -7960,7 +7954,7 @@
         <v>81</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>41</v>
+        <v>168</v>
       </c>
       <c r="C32" s="29">
         <f>C31</f>
@@ -8118,7 +8112,7 @@
         <v>Bio_Gas_Internal_Combustion_Engine_Cogen_EP</v>
       </c>
       <c r="AQ32" s="29" t="s">
-        <v>158</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:43" s="29" customFormat="1">
@@ -8126,7 +8120,7 @@
         <v>82</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>5</v>
+        <v>195</v>
       </c>
       <c r="C33" s="29">
         <f>C23</f>
@@ -8260,7 +8254,7 @@
         <v>Bio_Gas_Steam_Turbine_EP</v>
       </c>
       <c r="AQ33" s="29" t="s">
-        <v>194</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:43">
@@ -8408,7 +8402,7 @@
         <v>115</v>
       </c>
       <c r="B35" s="29" t="s">
-        <v>84</v>
+        <v>131</v>
       </c>
       <c r="C35" s="5">
         <v>2007</v>
@@ -8417,7 +8411,7 @@
         <v>2016</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="L35">
         <f>L41</f>
@@ -8536,7 +8530,7 @@
         <v>Bio_Liquid_Steam_Turbine_Cogen_CCS</v>
       </c>
       <c r="AQ35" s="29" t="s">
-        <v>211</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:43">
@@ -8544,7 +8538,7 @@
         <v>85</v>
       </c>
       <c r="B36" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="C36" s="5">
         <f>C33</f>
@@ -8555,7 +8549,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="F36" s="29"/>
       <c r="G36" s="29"/>
@@ -8684,7 +8678,7 @@
         <v>Bio_Liquid_Steam_Turbine_Cogen_EP</v>
       </c>
       <c r="AQ36" s="29" t="s">
-        <v>159</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:43">
@@ -8692,16 +8686,16 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="C37" s="5">
         <v>2007</v>
       </c>
       <c r="D37" s="5">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="E37" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="F37">
         <v>2009</v>
@@ -8819,7 +8813,7 @@
         <v>Biomass_IGCC</v>
       </c>
       <c r="AQ37" t="s">
-        <v>156</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:43" s="25" customFormat="1">
@@ -8827,7 +8821,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="C38" s="25">
         <v>2007</v>
@@ -8836,7 +8830,7 @@
         <v>2016</v>
       </c>
       <c r="E38" s="25" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="I38" s="26"/>
       <c r="K38" s="26"/>
@@ -8941,7 +8935,7 @@
         <v>Biomass_IGCC_CCS</v>
       </c>
       <c r="AQ38" s="29" t="s">
-        <v>0</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:43">
@@ -8949,7 +8943,7 @@
         <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C39" s="5">
         <v>2007</v>
@@ -8958,7 +8952,7 @@
         <v>2011</v>
       </c>
       <c r="E39" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="F39">
         <v>2009</v>
@@ -9076,7 +9070,7 @@
         <v>Biomass_Steam_Turbine</v>
       </c>
       <c r="AQ39" s="29" t="s">
-        <v>200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:43">
@@ -9224,7 +9218,7 @@
         <v>116</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>4</v>
+        <v>194</v>
       </c>
       <c r="C41" s="5">
         <v>2007</v>
@@ -9233,7 +9227,7 @@
         <v>2016</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="L41">
         <f>L40+(L47-L46)</f>
@@ -9351,7 +9345,7 @@
         <v>Bio_Solid_Steam_Turbine_Cogen_CCS</v>
       </c>
       <c r="AQ41" s="29" t="s">
-        <v>210</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:43">
@@ -9359,7 +9353,7 @@
         <v>90</v>
       </c>
       <c r="B42" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="C42" s="29">
         <f>C33</f>
@@ -9370,7 +9364,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="29" t="s">
-        <v>51</v>
+        <v>178</v>
       </c>
       <c r="F42" s="29"/>
       <c r="G42" s="29"/>
@@ -9499,7 +9493,7 @@
         <v>Bio_Solid_Steam_Turbine_EP</v>
       </c>
       <c r="AQ42" s="29" t="s">
-        <v>195</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:43">
@@ -9507,7 +9501,7 @@
         <v>91</v>
       </c>
       <c r="B43" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="C43" s="29">
         <f>C36</f>
@@ -9518,7 +9512,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="29" t="s">
-        <v>51</v>
+        <v>178</v>
       </c>
       <c r="F43" s="29"/>
       <c r="G43" s="29"/>
@@ -9648,7 +9642,7 @@
         <v>Bio_Solid_Steam_Turbine_Cogen_EP</v>
       </c>
       <c r="AQ43" s="29" t="s">
-        <v>159</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:43">
@@ -9656,7 +9650,7 @@
         <v>12</v>
       </c>
       <c r="B44" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="C44" s="5">
         <v>2007</v>
@@ -9665,7 +9659,7 @@
         <v>2011</v>
       </c>
       <c r="E44" t="s">
-        <v>177</v>
+        <v>75</v>
       </c>
       <c r="F44">
         <v>2010</v>
@@ -9783,7 +9777,7 @@
         <v>Coal_Steam_Turbine</v>
       </c>
       <c r="AQ44" s="29" t="s">
-        <v>196</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:43" s="25" customFormat="1">
@@ -9791,7 +9785,7 @@
         <v>39</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="C45" s="25">
         <v>2007</v>
@@ -9800,7 +9794,7 @@
         <v>2016</v>
       </c>
       <c r="E45" s="25" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="F45" s="25">
         <v>2010</v>
@@ -9929,7 +9923,7 @@
         <v>Coal_Steam_Turbine_CCS</v>
       </c>
       <c r="AQ45" s="29" t="s">
-        <v>187</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:43">
@@ -10079,7 +10073,7 @@
         <v>Coal_Steam_Turbine_Cogen</v>
       </c>
       <c r="AQ46" s="29" t="s">
-        <v>160</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:43">
@@ -10087,7 +10081,7 @@
         <v>117</v>
       </c>
       <c r="B47" s="29" t="s">
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="C47" s="5">
         <v>2007</v>
@@ -10096,7 +10090,7 @@
         <v>2016</v>
       </c>
       <c r="E47" s="29" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
       <c r="L47">
         <f>0.75*L45</f>
@@ -10214,7 +10208,7 @@
         <v>Coal_Steam_Turbine_Cogen_CCS</v>
       </c>
       <c r="AQ47" s="29" t="s">
-        <v>168</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:43" s="5" customFormat="1">
@@ -10222,7 +10216,7 @@
         <v>18</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="C48">
         <v>2007</v>
@@ -10376,7 +10370,7 @@
         <v>30</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="C49" s="29">
         <v>2007</v>
@@ -10522,7 +10516,7 @@
         <v>Coal_Steam_Turbine_Cogen_EP</v>
       </c>
       <c r="AQ49" s="29" t="s">
-        <v>190</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:43">
@@ -10530,7 +10524,7 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>157</v>
+        <v>55</v>
       </c>
       <c r="C50" s="5">
         <v>2007</v>
@@ -10539,7 +10533,7 @@
         <v>2011</v>
       </c>
       <c r="E50" t="s">
-        <v>177</v>
+        <v>75</v>
       </c>
       <c r="F50">
         <v>2010</v>
@@ -10657,7 +10651,7 @@
         <v>Coal_IGCC</v>
       </c>
       <c r="AQ50" s="29" t="s">
-        <v>50</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:43" s="25" customFormat="1">
@@ -10665,7 +10659,7 @@
         <v>38</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="C51" s="25">
         <v>2007</v>
@@ -10674,7 +10668,7 @@
         <v>2016</v>
       </c>
       <c r="E51" s="25" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="F51" s="25">
         <v>2010</v>
@@ -10802,7 +10796,7 @@
         <v>Coal_IGCC_CCS</v>
       </c>
       <c r="AQ51" s="29" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:43">
@@ -10810,7 +10804,7 @@
         <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="C52" s="5">
         <v>2007</v>
@@ -10819,7 +10813,7 @@
         <v>2011</v>
       </c>
       <c r="E52" t="s">
-        <v>178</v>
+        <v>12</v>
       </c>
       <c r="F52">
         <v>2009</v>
@@ -10937,7 +10931,7 @@
         <v>Nuclear</v>
       </c>
       <c r="AQ52" s="29" t="s">
-        <v>197</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:43" s="5" customFormat="1">
@@ -10945,7 +10939,7 @@
         <v>22</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>35</v>
+        <v>162</v>
       </c>
       <c r="C53" s="29">
         <v>2007</v>
@@ -11090,7 +11084,7 @@
         <v>Nuclear_EP</v>
       </c>
       <c r="AQ53" s="29" t="s">
-        <v>144</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:43">
@@ -11098,7 +11092,7 @@
         <v>14</v>
       </c>
       <c r="B54" t="s">
-        <v>150</v>
+        <v>48</v>
       </c>
       <c r="C54" s="5">
         <v>2007</v>
@@ -11107,7 +11101,7 @@
         <v>2011</v>
       </c>
       <c r="E54" t="s">
-        <v>37</v>
+        <v>164</v>
       </c>
       <c r="F54">
         <v>2009</v>
@@ -11225,7 +11219,7 @@
         <v>Geothermal</v>
       </c>
       <c r="AQ54" s="29" t="s">
-        <v>198</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:43" s="5" customFormat="1">
@@ -11233,7 +11227,7 @@
         <v>21</v>
       </c>
       <c r="B55" s="29" t="s">
-        <v>171</v>
+        <v>69</v>
       </c>
       <c r="C55" s="29">
         <v>2007</v>
@@ -11242,7 +11236,7 @@
         <v>0</v>
       </c>
       <c r="E55" t="s">
-        <v>150</v>
+        <v>48</v>
       </c>
       <c r="F55" s="29">
         <v>2009</v>
@@ -11361,7 +11355,7 @@
         <v>Geothermal_EP</v>
       </c>
       <c r="AQ55" s="29" t="s">
-        <v>143</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:43">
@@ -11369,7 +11363,7 @@
         <v>6</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>19</v>
+        <v>209</v>
       </c>
       <c r="C56" s="5">
         <v>2007</v>
@@ -11378,7 +11372,7 @@
         <v>2011</v>
       </c>
       <c r="E56" t="s">
-        <v>77</v>
+        <v>124</v>
       </c>
       <c r="F56">
         <v>2009</v>
@@ -11497,7 +11491,7 @@
         <v>Residential_PV</v>
       </c>
       <c r="AQ56" s="29" t="s">
-        <v>22</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:43" s="8" customFormat="1">
@@ -11505,7 +11499,7 @@
         <v>25</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>57</v>
+        <v>184</v>
       </c>
       <c r="C57" s="8">
         <v>2007</v>
@@ -11514,7 +11508,7 @@
         <v>2011</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="F57" s="8">
         <v>2009</v>
@@ -11632,7 +11626,7 @@
         <v>Commercial_PV</v>
       </c>
       <c r="AQ57" s="29" t="s">
-        <v>49</v>
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:43" s="8" customFormat="1">
@@ -11640,7 +11634,7 @@
         <v>26</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="C58" s="8">
         <v>2007</v>
@@ -11649,7 +11643,7 @@
         <v>2011</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="F58" s="8">
         <v>2009</v>
@@ -11767,7 +11761,7 @@
         <v>Central_PV</v>
       </c>
       <c r="AQ58" s="29" t="s">
-        <v>49</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:43" s="21" customFormat="1">
@@ -11775,7 +11769,7 @@
         <v>3</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>46</v>
+        <v>173</v>
       </c>
       <c r="C59" s="21">
         <v>2007</v>
@@ -11784,7 +11778,7 @@
         <v>2011</v>
       </c>
       <c r="E59" s="21" t="s">
-        <v>47</v>
+        <v>174</v>
       </c>
       <c r="F59" s="21">
         <v>2010</v>
@@ -11903,7 +11897,7 @@
         <v>Concentrating_PV</v>
       </c>
       <c r="AQ59" s="21" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:43" s="5" customFormat="1">
@@ -11911,7 +11905,7 @@
         <v>27</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>29</v>
+        <v>156</v>
       </c>
       <c r="C60" s="5">
         <v>2007</v>
@@ -11920,7 +11914,7 @@
         <v>2011</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="F60" s="5">
         <v>2009</v>
@@ -12038,7 +12032,7 @@
         <v>CSP_Trough_No_Storage</v>
       </c>
       <c r="AQ60" s="29" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61" spans="1:43" s="11" customFormat="1">
@@ -12046,7 +12040,7 @@
         <v>7</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>30</v>
+        <v>157</v>
       </c>
       <c r="C61" s="11">
         <v>2007</v>
@@ -12055,7 +12049,7 @@
         <v>2012</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="F61" s="11">
         <v>2009</v>
@@ -12174,7 +12168,7 @@
         <v>CSP_Trough_6h_Storage</v>
       </c>
       <c r="AQ61" s="29" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="1:43">
@@ -12182,7 +12176,7 @@
         <v>5</v>
       </c>
       <c r="B62" t="s">
-        <v>136</v>
+        <v>34</v>
       </c>
       <c r="C62" s="5">
         <v>2007</v>
@@ -12191,7 +12185,7 @@
         <v>2011</v>
       </c>
       <c r="E62" t="s">
-        <v>66</v>
+        <v>113</v>
       </c>
       <c r="F62">
         <v>2009</v>
@@ -12309,7 +12303,7 @@
         <v>Offshore_Wind</v>
       </c>
       <c r="AQ62" s="29" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
     </row>
     <row r="63" spans="1:43">
@@ -12317,7 +12311,7 @@
         <v>4</v>
       </c>
       <c r="B63" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="C63" s="5">
         <v>2007</v>
@@ -12326,7 +12320,7 @@
         <v>2011</v>
       </c>
       <c r="E63" t="s">
-        <v>66</v>
+        <v>113</v>
       </c>
       <c r="F63">
         <v>2009</v>
@@ -12444,7 +12438,7 @@
         <v>Wind</v>
       </c>
       <c r="AQ63" s="29" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
     </row>
     <row r="64" spans="1:43" s="18" customFormat="1">
@@ -12452,7 +12446,7 @@
         <v>23</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="C64" s="29">
         <v>2007</v>
@@ -12596,7 +12590,7 @@
         <v>Wind_EP</v>
       </c>
       <c r="AQ64" s="29" t="s">
-        <v>38</v>
+        <v>165</v>
       </c>
     </row>
     <row r="65" spans="1:43">
@@ -12604,7 +12598,7 @@
         <v>15</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="C65" s="5">
         <v>2007</v>
@@ -12613,7 +12607,7 @@
         <v>0</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="F65" s="5">
         <v>2010</v>
@@ -12731,7 +12725,7 @@
         <v>Hydro_NonPumped</v>
       </c>
       <c r="AQ65" s="29" t="s">
-        <v>199</v>
+        <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:43">
@@ -12739,7 +12733,7 @@
         <v>16</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="C66" s="5">
         <v>2007</v>
@@ -12748,7 +12742,7 @@
         <v>0</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="F66" s="29">
         <v>2010</v>
@@ -12866,7 +12860,7 @@
         <v>Hydro_Pumped</v>
       </c>
       <c r="AQ66" s="29" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
     </row>
     <row r="67" spans="1:43" s="9" customFormat="1" ht="15" customHeight="1">
@@ -12874,7 +12868,7 @@
         <v>28</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>154</v>
+        <v>52</v>
       </c>
       <c r="C67" s="9">
         <v>2007</v>
@@ -12883,7 +12877,7 @@
         <v>2011</v>
       </c>
       <c r="E67" s="14" t="s">
-        <v>92</v>
+        <v>139</v>
       </c>
       <c r="F67" s="9">
         <v>2010</v>
@@ -13001,7 +12995,7 @@
         <v>Compressed_Air_Energy_Storage</v>
       </c>
       <c r="AQ67" s="28" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
     </row>
     <row r="68" spans="1:43" s="22" customFormat="1">
@@ -13009,7 +13003,7 @@
         <v>33</v>
       </c>
       <c r="B68" s="32" t="s">
-        <v>141</v>
+        <v>39</v>
       </c>
       <c r="C68" s="32">
         <v>2007</v>
@@ -13018,7 +13012,7 @@
         <v>2011</v>
       </c>
       <c r="E68" s="32" t="s">
-        <v>142</v>
+        <v>40</v>
       </c>
       <c r="F68" s="32">
         <v>2004</v>
@@ -13136,7 +13130,7 @@
         <v>Battery_Storage</v>
       </c>
       <c r="AQ68" s="32" t="s">
-        <v>148</v>
+        <v>46</v>
       </c>
     </row>
     <row r="78" spans="1:43">
@@ -18090,7 +18084,7 @@
       </c>
       <c r="D34" s="29">
         <f>generator_costs!D37</f>
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="E34" s="29" t="str">
         <f>generator_costs!E37</f>
@@ -22770,7 +22764,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="6" t="s">
-        <v>45</v>
+        <v>172</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -22781,7 +22775,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>2010</v>
@@ -22799,7 +22793,7 @@
         <v>2026</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -24505,15 +24499,15 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="21" t="s">
-        <v>48</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="21" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>101</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="21" customFormat="1">
@@ -24541,7 +24535,7 @@
         <v>3.3</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="E5" s="21"/>
     </row>
@@ -24725,25 +24719,25 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="33" t="s">
-        <v>60</v>
+        <v>187</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>61</v>
+        <v>188</v>
       </c>
       <c r="C1" s="33"/>
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
       <c r="F1" s="33" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
       <c r="G1" s="33" t="s">
-        <v>23</v>
+        <v>150</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>24</v>
+        <v>151</v>
       </c>
       <c r="I1" s="34" t="s">
-        <v>25</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -24763,7 +24757,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="35" t="s">
-        <v>26</v>
+        <v>153</v>
       </c>
       <c r="B3" s="35">
         <v>1.788</v>
@@ -24792,7 +24786,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="37" t="s">
-        <v>27</v>
+        <v>154</v>
       </c>
       <c r="B4" s="35">
         <v>1.276</v>
@@ -24820,7 +24814,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="37" t="s">
-        <v>28</v>
+        <v>155</v>
       </c>
       <c r="B5" s="35">
         <v>1.504</v>
@@ -24846,74 +24840,74 @@
         <v>8.6999999999999744E-2</v>
       </c>
       <c r="I5" s="35" t="s">
-        <v>7</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="34" t="s">
-        <v>8</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="37" t="s">
-        <v>9</v>
+        <v>199</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>182</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="35" t="s">
-        <v>183</v>
+        <v>17</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>184</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="C12" s="35" t="s">
-        <v>185</v>
+        <v>19</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>186</v>
+        <v>20</v>
       </c>
       <c r="J12" s="35" t="s">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="K12" s="35" t="s">
-        <v>11</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="37" t="s">
-        <v>12</v>
+        <v>202</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>13</v>
+        <v>203</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>26</v>
+        <v>153</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>15</v>
+        <v>205</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>26</v>
+        <v>153</v>
       </c>
       <c r="G13" s="37" t="s">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="H13" s="37" t="s">
-        <v>15</v>
+        <v>205</v>
       </c>
       <c r="J13" s="37" t="s">
-        <v>26</v>
+        <v>153</v>
       </c>
       <c r="K13" s="37" t="s">
-        <v>26</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:11">

</xml_diff>